<commit_message>
Update PD parameters of norepi.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -2122,7 +2122,7 @@
     <t>Direct Copy from Epi</t>
   </si>
   <si>
-    <t>0.00095 ug/mL</t>
+    <t>0.0038 ug/mL</t>
   </si>
 </sst>
 </file>
@@ -4668,7 +4668,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="AO30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AP43" sqref="AP43"/>
+      <selection pane="bottomRight" activeCell="AP38" sqref="AP38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Correct O2/CO2 compound concentrations (different for each compound)
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\physiology\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B3FC1F36-D223-4AB9-852A-EDA4AD820FCC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{847AC547-9CB8-4C1B-9949-A3244C58E6F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="555" windowWidth="15090" windowHeight="7350" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4661" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4661" uniqueCount="701">
   <si>
     <t>Name</t>
   </si>
@@ -2136,6 +2136,12 @@
   </si>
   <si>
     <t>Approximated using the product of Figure 2 solubility values at 37C and density</t>
+  </si>
+  <si>
+    <t>0.0314 g/L</t>
+  </si>
+  <si>
+    <t>0.921 g/L</t>
   </si>
 </sst>
 </file>
@@ -23482,8 +23488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -23663,7 +23669,7 @@
         <v>698</v>
       </c>
       <c r="F8" s="79" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c r="G8" s="79"/>
       <c r="H8" s="79"/>
@@ -23728,7 +23734,7 @@
         <v>698</v>
       </c>
       <c r="F11" s="79" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
       <c r="G11" s="79"/>
       <c r="H11" s="79"/>

</xml_diff>

<commit_message>
Added more reference information for Saline and Blood compound O2 and CO2 references.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\physiology\engine\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{847AC547-9CB8-4C1B-9949-A3244C58E6F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7A2330BD-46FA-4131-9F32-60ABECB6E214}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="555" windowWidth="15090" windowHeight="7350" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="555" windowWidth="15090" windowHeight="7350" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4661" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4669" uniqueCount="705">
   <si>
     <t>Name</t>
   </si>
@@ -2142,6 +2142,18 @@
   </si>
   <si>
     <t>0.921 g/L</t>
+  </si>
+  <si>
+    <t>Solubility = 0.023 mL/mL</t>
+  </si>
+  <si>
+    <t>Solubility = 0.022 mL/mL</t>
+  </si>
+  <si>
+    <t>Solubility = 0.55 mL/mL</t>
+  </si>
+  <si>
+    <t>Solubility = 0.5 mL/mL</t>
   </si>
 </sst>
 </file>
@@ -4682,7 +4694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:FB74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -23488,8 +23500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -23498,7 +23510,8 @@
     <col min="2" max="2" width="37" style="1" customWidth="1"/>
     <col min="3" max="5" width="37" style="28" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="37" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="37" style="28" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="8" width="37" style="28" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="36.7109375" style="28" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="10" max="10" width="8.85546875" style="1" collapsed="1"/>
     <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
@@ -23654,14 +23667,16 @@
       <c r="H7" s="79"/>
       <c r="I7" s="79"/>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B8" s="79" t="s">
         <v>695</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="79" t="s">
+        <v>701</v>
+      </c>
       <c r="D8" s="79" t="s">
         <v>697</v>
       </c>
@@ -23671,9 +23686,15 @@
       <c r="F8" s="79" t="s">
         <v>699</v>
       </c>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="79"/>
+      <c r="G8" s="79" t="s">
+        <v>702</v>
+      </c>
+      <c r="H8" s="79" t="s">
+        <v>697</v>
+      </c>
+      <c r="I8" s="180" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
@@ -23726,7 +23747,9 @@
       <c r="B11" s="79" t="s">
         <v>696</v>
       </c>
-      <c r="C11" s="79"/>
+      <c r="C11" s="79" t="s">
+        <v>703</v>
+      </c>
       <c r="D11" s="79" t="s">
         <v>697</v>
       </c>
@@ -23736,9 +23759,15 @@
       <c r="F11" s="79" t="s">
         <v>700</v>
       </c>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="79"/>
+      <c r="G11" s="79" t="s">
+        <v>704</v>
+      </c>
+      <c r="H11" s="79" t="s">
+        <v>697</v>
+      </c>
+      <c r="I11" s="180" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>

</xml_diff>

<commit_message>
Added packed red blood cells to compound substances.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulseHemorrhage\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7A2330BD-46FA-4131-9F32-60ABECB6E214}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434EA094-AD6F-47A7-9D3A-91D2F69EF27E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="555" windowWidth="15090" windowHeight="7350" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4669" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4704" uniqueCount="708">
   <si>
     <t>Name</t>
   </si>
@@ -2154,6 +2154,15 @@
   </si>
   <si>
     <t>Solubility = 0.5 mL/mL</t>
+  </si>
+  <si>
+    <t>5.513 g/dL</t>
+  </si>
+  <si>
+    <t>16.5 g/dL</t>
+  </si>
+  <si>
+    <t>PackedRBC</t>
   </si>
 </sst>
 </file>
@@ -23501,7 +23510,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -23512,11 +23521,11 @@
     <col min="6" max="6" width="37" style="1" customWidth="1" collapsed="1"/>
     <col min="7" max="8" width="37" style="28" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="36.7109375" style="28" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="8.85546875" style="1" collapsed="1"/>
+    <col min="10" max="10" width="37" style="28" customWidth="1" collapsed="1"/>
     <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
@@ -23544,8 +23553,11 @@
       <c r="I1" s="80" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="80" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>53</v>
       </c>
@@ -23561,8 +23573,11 @@
       <c r="G2" s="77"/>
       <c r="H2" s="77"/>
       <c r="I2" s="77"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="77" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="82" t="s">
         <v>2</v>
@@ -23588,8 +23603,11 @@
       <c r="I3" s="80" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>61</v>
       </c>
@@ -23605,8 +23623,11 @@
       <c r="G4" s="79"/>
       <c r="H4" s="79"/>
       <c r="I4" s="79"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="79" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>54</v>
       </c>
@@ -23622,8 +23643,11 @@
       <c r="G5" s="79"/>
       <c r="H5" s="79"/>
       <c r="I5" s="79"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="79" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="82" t="s">
         <v>2</v>
@@ -23649,8 +23673,11 @@
       <c r="I6" s="80" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>61</v>
       </c>
@@ -23666,8 +23693,11 @@
       <c r="G7" s="79"/>
       <c r="H7" s="79"/>
       <c r="I7" s="79"/>
-    </row>
-    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="J7" s="79" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>54</v>
       </c>
@@ -23695,8 +23725,11 @@
       <c r="I8" s="180" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="79" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="82" t="s">
         <v>2</v>
@@ -23722,8 +23755,11 @@
       <c r="I9" s="80" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>61</v>
       </c>
@@ -23739,8 +23775,11 @@
       <c r="G10" s="79"/>
       <c r="H10" s="79"/>
       <c r="I10" s="79"/>
-    </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J10" s="79" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
@@ -23768,8 +23807,11 @@
       <c r="I11" s="180" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="79" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="82" t="s">
         <v>2</v>
@@ -23795,8 +23837,11 @@
       <c r="I12" s="80" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>61</v>
       </c>
@@ -23810,8 +23855,11 @@
       <c r="G13" s="79"/>
       <c r="H13" s="79"/>
       <c r="I13" s="79"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="79" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>54</v>
       </c>
@@ -23825,8 +23873,11 @@
       <c r="G14" s="79"/>
       <c r="H14" s="79"/>
       <c r="I14" s="79"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="79" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="82" t="s">
         <v>2</v>
@@ -23852,8 +23903,11 @@
       <c r="I15" s="80" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>61</v>
       </c>
@@ -23867,8 +23921,11 @@
       <c r="G16" s="79"/>
       <c r="H16" s="79"/>
       <c r="I16" s="79"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="79" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>54</v>
       </c>
@@ -23882,8 +23939,11 @@
       <c r="G17" s="79"/>
       <c r="H17" s="79"/>
       <c r="I17" s="79"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="79" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="81"/>
       <c r="B18" s="82" t="s">
         <v>2</v>
@@ -23909,8 +23969,11 @@
       <c r="I18" s="80" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="78" t="s">
         <v>61</v>
       </c>
@@ -23924,8 +23987,11 @@
       <c r="G19" s="79"/>
       <c r="H19" s="79"/>
       <c r="I19" s="79"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="79" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="78" t="s">
         <v>54</v>
       </c>
@@ -23939,8 +24005,11 @@
       <c r="G20" s="79"/>
       <c r="H20" s="79"/>
       <c r="I20" s="79"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="79" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="81"/>
       <c r="B21" s="82" t="s">
         <v>2</v>
@@ -23966,8 +24035,11 @@
       <c r="I21" s="80" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
         <v>61</v>
       </c>
@@ -23981,8 +24053,11 @@
       <c r="G22" s="79"/>
       <c r="H22" s="79"/>
       <c r="I22" s="79"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="79" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="78" t="s">
         <v>54</v>
       </c>
@@ -23996,8 +24071,11 @@
       <c r="G23" s="79"/>
       <c r="H23" s="79"/>
       <c r="I23" s="79"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="79" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="81"/>
       <c r="B24" s="82" t="s">
         <v>2</v>
@@ -24023,8 +24101,11 @@
       <c r="I24" s="80" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="78" t="s">
         <v>61</v>
       </c>
@@ -24038,8 +24119,11 @@
       <c r="G25" s="79"/>
       <c r="H25" s="79"/>
       <c r="I25" s="79"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="79" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="78" t="s">
         <v>54</v>
       </c>
@@ -24053,8 +24137,11 @@
       <c r="G26" s="79"/>
       <c r="H26" s="79"/>
       <c r="I26" s="79"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="79" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="81"/>
       <c r="B27" s="82" t="s">
         <v>2</v>
@@ -24080,8 +24167,11 @@
       <c r="I27" s="80" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="78" t="s">
         <v>61</v>
       </c>
@@ -24095,8 +24185,11 @@
       <c r="G28" s="79"/>
       <c r="H28" s="79"/>
       <c r="I28" s="79"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="79" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="78" t="s">
         <v>54</v>
       </c>
@@ -24110,8 +24203,11 @@
       <c r="G29" s="79"/>
       <c r="H29" s="79"/>
       <c r="I29" s="79"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="79" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="81"/>
       <c r="B30" s="82" t="s">
         <v>2</v>
@@ -24137,8 +24233,11 @@
       <c r="I30" s="80" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="78" t="s">
         <v>61</v>
       </c>
@@ -24152,8 +24251,11 @@
       <c r="G31" s="79"/>
       <c r="H31" s="79"/>
       <c r="I31" s="79"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="79" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="78" t="s">
         <v>54</v>
       </c>
@@ -24167,8 +24269,11 @@
       <c r="G32" s="79"/>
       <c r="H32" s="79"/>
       <c r="I32" s="79"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="79" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="81"/>
       <c r="B33" s="82" t="s">
         <v>2</v>
@@ -24194,8 +24299,11 @@
       <c r="I33" s="80" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="78" t="s">
         <v>61</v>
       </c>
@@ -24209,8 +24317,11 @@
       <c r="G34" s="79"/>
       <c r="H34" s="79"/>
       <c r="I34" s="79"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="79" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="78" t="s">
         <v>54</v>
       </c>
@@ -24224,6 +24335,9 @@
       <c r="G35" s="79"/>
       <c r="H35" s="79"/>
       <c r="I35" s="79"/>
+      <c r="J35" s="79" t="s">
+        <v>306</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated minimum baseline respiration rate to be 8 instead of 12. Small tweak to respiration rate in system validation spreadsheet.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\IngMarPublicMaster\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3311F783-79FC-4488-8A86-0679AC047763}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0CB34D-A05F-41F1-B228-CEDB69022BAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9780" yWindow="8385" windowWidth="32205" windowHeight="16845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4704" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4704" uniqueCount="709">
   <si>
     <t>Name</t>
   </si>
@@ -2171,6 +2171,9 @@
   </si>
   <si>
     <t>PackedRBC</t>
+  </si>
+  <si>
+    <t>8 bpm</t>
   </si>
 </sst>
 </file>
@@ -3645,7 +3648,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomRight" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4402,7 +4405,7 @@
         <v>293</v>
       </c>
       <c r="I16" s="157" t="s">
-        <v>292</v>
+        <v>708</v>
       </c>
       <c r="J16" s="156" t="s">
         <v>71</v>
@@ -4435,7 +4438,7 @@
         <v>71</v>
       </c>
       <c r="T16" s="156" t="s">
-        <v>292</v>
+        <v>708</v>
       </c>
       <c r="U16" s="157" t="s">
         <v>293</v>

</xml_diff>

<commit_message>
C# and Java for new Respiratory Actions/Conditions (with stabs criteria)
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\IngMarPublicMaster\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\Pulse\engine-ingmar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0CB34D-A05F-41F1-B228-CEDB69022BAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1764AFFB-EF35-432F-9A9E-74F1136AB1D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -23,12 +23,11 @@
     <sheet name="Configuration" sheetId="12" r:id="rId8"/>
     <sheet name="Tissue" sheetId="13" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4704" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4776" uniqueCount="711">
   <si>
     <t>Name</t>
   </si>
@@ -2174,6 +2173,12 @@
   </si>
   <si>
     <t>8 bpm</t>
+  </si>
+  <si>
+    <t>AcuteRespiratoryDistressSyndrome</t>
+  </si>
+  <si>
+    <t>Sepsis</t>
   </si>
 </sst>
 </file>
@@ -3644,7 +3649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -25741,10 +25746,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F174"/>
+  <dimension ref="A1:F206"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="B160" sqref="B160:B163"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26176,7 +26181,7 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34" t="s">
-        <v>161</v>
+        <v>709</v>
       </c>
       <c r="B31" s="35" t="s">
         <v>145</v>
@@ -26398,7 +26403,7 @@
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="34" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B47" s="35" t="s">
         <v>145</v>
@@ -26620,7 +26625,7 @@
     </row>
     <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="34" t="s">
-        <v>627</v>
+        <v>163</v>
       </c>
       <c r="B63" s="35" t="s">
         <v>145</v>
@@ -26841,22 +26846,22 @@
       <c r="F78" s="43"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="39" t="s">
-        <v>276</v>
-      </c>
-      <c r="B79" s="40" t="s">
+      <c r="A79" s="34" t="s">
+        <v>627</v>
+      </c>
+      <c r="B79" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="C79" s="40" t="s">
+      <c r="C79" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="D79" s="40" t="s">
+      <c r="D79" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="E79" s="40" t="s">
+      <c r="E79" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="F79" s="40" t="s">
+      <c r="F79" s="35" t="s">
         <v>2</v>
       </c>
     </row>
@@ -26875,7 +26880,7 @@
       <c r="F80" s="45"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="44" t="s">
+      <c r="A81" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B81" s="49">
@@ -26884,12 +26889,12 @@
       <c r="C81" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="D81" s="44"/>
-      <c r="E81" s="45"/>
-      <c r="F81" s="45"/>
+      <c r="D81" s="46"/>
+      <c r="E81" s="47"/>
+      <c r="F81" s="47"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="44" t="s">
+      <c r="A82" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B82" s="49">
@@ -26898,9 +26903,9 @@
       <c r="C82" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D82" s="44"/>
-      <c r="E82" s="45"/>
-      <c r="F82" s="45"/>
+      <c r="D82" s="46"/>
+      <c r="E82" s="47"/>
+      <c r="F82" s="47"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="46" t="s">
@@ -27039,16 +27044,16 @@
       <c r="F92" s="38"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="41" t="s">
+      <c r="A93" s="36" t="s">
         <v>158</v>
       </c>
       <c r="B93" s="41" t="s">
         <v>603</v>
       </c>
-      <c r="C93" s="42"/>
-      <c r="D93" s="42"/>
-      <c r="E93" s="43"/>
-      <c r="F93" s="43"/>
+      <c r="C93" s="37"/>
+      <c r="D93" s="37"/>
+      <c r="E93" s="38"/>
+      <c r="F93" s="38"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="48" t="s">
@@ -27064,7 +27069,7 @@
     </row>
     <row r="95" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="39" t="s">
-        <v>188</v>
+        <v>276</v>
       </c>
       <c r="B95" s="40" t="s">
         <v>145</v>
@@ -27125,7 +27130,7 @@
       <c r="F98" s="45"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="44" t="s">
+      <c r="A99" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B99" s="49">
@@ -27134,9 +27139,9 @@
       <c r="C99" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="D99" s="44"/>
-      <c r="E99" s="45"/>
-      <c r="F99" s="45"/>
+      <c r="D99" s="46"/>
+      <c r="E99" s="47"/>
+      <c r="F99" s="47"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="46" t="s">
@@ -27286,7 +27291,7 @@
     </row>
     <row r="111" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="39" t="s">
-        <v>273</v>
+        <v>188</v>
       </c>
       <c r="B111" s="40" t="s">
         <v>145</v>
@@ -27319,7 +27324,7 @@
       <c r="F112" s="45"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="46" t="s">
+      <c r="A113" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B113" s="49">
@@ -27328,12 +27333,12 @@
       <c r="C113" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="D113" s="46"/>
-      <c r="E113" s="47"/>
-      <c r="F113" s="47"/>
+      <c r="D113" s="44"/>
+      <c r="E113" s="45"/>
+      <c r="F113" s="45"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="46" t="s">
+      <c r="A114" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B114" s="49">
@@ -27342,12 +27347,12 @@
       <c r="C114" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D114" s="46"/>
-      <c r="E114" s="47"/>
-      <c r="F114" s="47"/>
+      <c r="D114" s="44"/>
+      <c r="E114" s="45"/>
+      <c r="F114" s="45"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="46" t="s">
+      <c r="A115" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B115" s="49">
@@ -27356,9 +27361,9 @@
       <c r="C115" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="D115" s="46"/>
-      <c r="E115" s="47"/>
-      <c r="F115" s="47"/>
+      <c r="D115" s="44"/>
+      <c r="E115" s="45"/>
+      <c r="F115" s="45"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="46" t="s">
@@ -27508,7 +27513,7 @@
     </row>
     <row r="127" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="39" t="s">
-        <v>287</v>
+        <v>710</v>
       </c>
       <c r="B127" s="40" t="s">
         <v>145</v>
@@ -27541,7 +27546,7 @@
       <c r="F128" s="45"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="46" t="s">
+      <c r="A129" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B129" s="49">
@@ -27550,12 +27555,12 @@
       <c r="C129" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="D129" s="46"/>
-      <c r="E129" s="47"/>
-      <c r="F129" s="47"/>
+      <c r="D129" s="44"/>
+      <c r="E129" s="45"/>
+      <c r="F129" s="45"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="46" t="s">
+      <c r="A130" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B130" s="49">
@@ -27564,12 +27569,12 @@
       <c r="C130" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D130" s="46"/>
-      <c r="E130" s="47"/>
-      <c r="F130" s="47"/>
+      <c r="D130" s="44"/>
+      <c r="E130" s="45"/>
+      <c r="F130" s="45"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="46" t="s">
+      <c r="A131" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B131" s="49">
@@ -27578,9 +27583,9 @@
       <c r="C131" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="D131" s="46"/>
-      <c r="E131" s="47"/>
-      <c r="F131" s="47"/>
+      <c r="D131" s="44"/>
+      <c r="E131" s="45"/>
+      <c r="F131" s="45"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="46" t="s">
@@ -27729,22 +27734,22 @@
       <c r="F142" s="43"/>
     </row>
     <row r="143" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="34" t="s">
-        <v>326</v>
-      </c>
-      <c r="B143" s="35" t="s">
+      <c r="A143" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="B143" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="C143" s="35" t="s">
+      <c r="C143" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="D143" s="35" t="s">
+      <c r="D143" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="E143" s="35" t="s">
+      <c r="E143" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="F143" s="35" t="s">
+      <c r="F143" s="40" t="s">
         <v>2</v>
       </c>
     </row>
@@ -27927,16 +27932,16 @@
       <c r="F156" s="38"/>
     </row>
     <row r="157" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="36" t="s">
+      <c r="A157" s="41" t="s">
         <v>158</v>
       </c>
       <c r="B157" s="41" t="s">
         <v>603</v>
       </c>
-      <c r="C157" s="37"/>
-      <c r="D157" s="37"/>
-      <c r="E157" s="38"/>
-      <c r="F157" s="38"/>
+      <c r="C157" s="42"/>
+      <c r="D157" s="42"/>
+      <c r="E157" s="43"/>
+      <c r="F157" s="43"/>
     </row>
     <row r="158" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="48" t="s">
@@ -27952,7 +27957,7 @@
     </row>
     <row r="159" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="39" t="s">
-        <v>678</v>
+        <v>287</v>
       </c>
       <c r="B159" s="40" t="s">
         <v>145</v>
@@ -27985,7 +27990,7 @@
       <c r="F160" s="45"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161" s="44" t="s">
+      <c r="A161" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B161" s="49">
@@ -27994,12 +27999,12 @@
       <c r="C161" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="D161" s="44"/>
-      <c r="E161" s="45"/>
-      <c r="F161" s="45"/>
+      <c r="D161" s="46"/>
+      <c r="E161" s="47"/>
+      <c r="F161" s="47"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A162" s="44" t="s">
+      <c r="A162" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B162" s="49">
@@ -28008,12 +28013,12 @@
       <c r="C162" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D162" s="44"/>
-      <c r="E162" s="45"/>
-      <c r="F162" s="45"/>
+      <c r="D162" s="46"/>
+      <c r="E162" s="47"/>
+      <c r="F162" s="47"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" s="44" t="s">
+      <c r="A163" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B163" s="49">
@@ -28022,9 +28027,9 @@
       <c r="C163" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="D163" s="44"/>
-      <c r="E163" s="45"/>
-      <c r="F163" s="45"/>
+      <c r="D163" s="46"/>
+      <c r="E163" s="47"/>
+      <c r="F163" s="47"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="46" t="s">
@@ -28171,6 +28176,450 @@
       <c r="D174" s="42"/>
       <c r="E174" s="43"/>
       <c r="F174" s="43"/>
+    </row>
+    <row r="175" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="34" t="s">
+        <v>326</v>
+      </c>
+      <c r="B175" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="C175" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="D175" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="E175" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="F175" s="35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B176" s="49">
+        <v>4</v>
+      </c>
+      <c r="C176" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="D176" s="44"/>
+      <c r="E176" s="45"/>
+      <c r="F176" s="45"/>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B177" s="49">
+        <v>4</v>
+      </c>
+      <c r="C177" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="D177" s="46"/>
+      <c r="E177" s="47"/>
+      <c r="F177" s="47"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B178" s="49">
+        <v>4</v>
+      </c>
+      <c r="C178" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="D178" s="46"/>
+      <c r="E178" s="47"/>
+      <c r="F178" s="47"/>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B179" s="49">
+        <v>4</v>
+      </c>
+      <c r="C179" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="D179" s="46"/>
+      <c r="E179" s="47"/>
+      <c r="F179" s="47"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B180" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C180" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="D180" s="46"/>
+      <c r="E180" s="47"/>
+      <c r="F180" s="47"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B181" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C181" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="D181" s="46"/>
+      <c r="E181" s="47"/>
+      <c r="F181" s="47"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B182" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C182" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="D182" s="46"/>
+      <c r="E182" s="47"/>
+      <c r="F182" s="47"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B183" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C183" s="46" t="s">
+        <v>601</v>
+      </c>
+      <c r="D183" s="46"/>
+      <c r="E183" s="47"/>
+      <c r="F183" s="47"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B184" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C184" s="46" t="s">
+        <v>602</v>
+      </c>
+      <c r="D184" s="46"/>
+      <c r="E184" s="47"/>
+      <c r="F184" s="47"/>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B185" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C185" s="46" t="s">
+        <v>274</v>
+      </c>
+      <c r="D185" s="46"/>
+      <c r="E185" s="47"/>
+      <c r="F185" s="47"/>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B186" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C186" s="46" t="s">
+        <v>275</v>
+      </c>
+      <c r="D186" s="46"/>
+      <c r="E186" s="47"/>
+      <c r="F186" s="47"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="B187" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C187" s="37"/>
+      <c r="D187" s="37"/>
+      <c r="E187" s="38"/>
+      <c r="F187" s="38"/>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="B188" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="C188" s="37"/>
+      <c r="D188" s="37"/>
+      <c r="E188" s="38"/>
+      <c r="F188" s="38"/>
+    </row>
+    <row r="189" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="B189" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="C189" s="37"/>
+      <c r="D189" s="37"/>
+      <c r="E189" s="38"/>
+      <c r="F189" s="38"/>
+    </row>
+    <row r="190" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="B190" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C190" s="42"/>
+      <c r="D190" s="42"/>
+      <c r="E190" s="43"/>
+      <c r="F190" s="43"/>
+    </row>
+    <row r="191" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="39" t="s">
+        <v>678</v>
+      </c>
+      <c r="B191" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="C191" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="D191" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="E191" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="F191" s="40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B192" s="49">
+        <v>4</v>
+      </c>
+      <c r="C192" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="D192" s="44"/>
+      <c r="E192" s="45"/>
+      <c r="F192" s="45"/>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B193" s="49">
+        <v>4</v>
+      </c>
+      <c r="C193" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="D193" s="44"/>
+      <c r="E193" s="45"/>
+      <c r="F193" s="45"/>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B194" s="49">
+        <v>4</v>
+      </c>
+      <c r="C194" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="D194" s="44"/>
+      <c r="E194" s="45"/>
+      <c r="F194" s="45"/>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B195" s="49">
+        <v>4</v>
+      </c>
+      <c r="C195" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="D195" s="44"/>
+      <c r="E195" s="45"/>
+      <c r="F195" s="45"/>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B196" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C196" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="D196" s="46"/>
+      <c r="E196" s="47"/>
+      <c r="F196" s="47"/>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B197" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C197" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="D197" s="46"/>
+      <c r="E197" s="47"/>
+      <c r="F197" s="47"/>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B198" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C198" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="D198" s="46"/>
+      <c r="E198" s="47"/>
+      <c r="F198" s="47"/>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B199" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C199" s="46" t="s">
+        <v>601</v>
+      </c>
+      <c r="D199" s="46"/>
+      <c r="E199" s="47"/>
+      <c r="F199" s="47"/>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B200" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C200" s="46" t="s">
+        <v>602</v>
+      </c>
+      <c r="D200" s="46"/>
+      <c r="E200" s="47"/>
+      <c r="F200" s="47"/>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B201" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C201" s="46" t="s">
+        <v>274</v>
+      </c>
+      <c r="D201" s="46"/>
+      <c r="E201" s="47"/>
+      <c r="F201" s="47"/>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B202" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C202" s="46" t="s">
+        <v>275</v>
+      </c>
+      <c r="D202" s="46"/>
+      <c r="E202" s="47"/>
+      <c r="F202" s="47"/>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="B203" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C203" s="37"/>
+      <c r="D203" s="37"/>
+      <c r="E203" s="38"/>
+      <c r="F203" s="38"/>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="B204" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="C204" s="37"/>
+      <c r="D204" s="37"/>
+      <c r="E204" s="38"/>
+      <c r="F204" s="38"/>
+    </row>
+    <row r="205" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A205" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="B205" s="41" t="s">
+        <v>603</v>
+      </c>
+      <c r="C205" s="42"/>
+      <c r="D205" s="42"/>
+      <c r="E205" s="43"/>
+      <c r="F205" s="43"/>
+    </row>
+    <row r="206" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="B206" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C206" s="42"/>
+      <c r="D206" s="42"/>
+      <c r="E206" s="43"/>
+      <c r="F206" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Pulmonary Fibrosis condition
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\IngMarPublicMaster\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anusham2\Desktop\Engine\Source\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE5492B-5F43-43CC-8B87-80139E5E2DC2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17490" yWindow="8685" windowWidth="23175" windowHeight="19425" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17490" yWindow="8685" windowWidth="23175" windowHeight="19425" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <sheet name="Configuration" sheetId="12" r:id="rId8"/>
     <sheet name="Tissue" sheetId="13" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2176,13 +2175,13 @@
     <t>AcuteRespiratoryDistressSyndrome</t>
   </si>
   <si>
-    <t>Sepsis</t>
+    <t>PulmonaryFibrosis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -3400,23 +3399,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3452,23 +3434,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3644,7 +3609,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4714,7 +4679,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FB74"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -23520,7 +23485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24360,7 +24325,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25450,7 +25415,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25608,7 +25573,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25743,11 +25708,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="A186" sqref="A186:XFD186"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28444,7 +28409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28906,7 +28871,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N105"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Reivew and updates to ensure everything is as it should be
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22ABA4DB-2572-4FA9-BB75-08D00D1C35CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063337D2-BDB7-4FD7-9D4F-D6E8CB22CA5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="850" yWindow="2450" windowWidth="28970" windowHeight="10590" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21360" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4750" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4784" uniqueCount="711">
   <si>
     <t>Name</t>
   </si>
@@ -2179,6 +2179,9 @@
   </si>
   <si>
     <t>InitialEnvironmentalConditions</t>
+  </si>
+  <si>
+    <t>PulmonaryShunt</t>
   </si>
 </sst>
 </file>
@@ -25746,10 +25749,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:F193"/>
+  <dimension ref="A1:F208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="A139" sqref="A139"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A195" sqref="A195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26569,7 +26572,7 @@
     </row>
     <row r="59" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="34" t="s">
-        <v>162</v>
+        <v>625</v>
       </c>
       <c r="B59" s="35" t="s">
         <v>145</v>
@@ -26776,22 +26779,22 @@
       <c r="F73" s="43"/>
     </row>
     <row r="74" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="34" t="s">
-        <v>625</v>
-      </c>
-      <c r="B74" s="35" t="s">
+      <c r="A74" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="B74" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="C74" s="35" t="s">
+      <c r="C74" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="D74" s="35" t="s">
+      <c r="D74" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="E74" s="35" t="s">
+      <c r="E74" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="F74" s="35" t="s">
+      <c r="F74" s="40" t="s">
         <v>2</v>
       </c>
     </row>
@@ -26810,7 +26813,7 @@
       <c r="F75" s="45"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" s="46" t="s">
+      <c r="A76" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B76" s="49">
@@ -26819,12 +26822,12 @@
       <c r="C76" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="D76" s="46"/>
-      <c r="E76" s="47"/>
-      <c r="F76" s="47"/>
+      <c r="D76" s="44"/>
+      <c r="E76" s="45"/>
+      <c r="F76" s="45"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77" s="46" t="s">
+      <c r="A77" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B77" s="49">
@@ -26833,9 +26836,9 @@
       <c r="C77" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D77" s="46"/>
-      <c r="E77" s="47"/>
-      <c r="F77" s="47"/>
+      <c r="D77" s="44"/>
+      <c r="E77" s="45"/>
+      <c r="F77" s="45"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="46" t="s">
@@ -26960,16 +26963,16 @@
       <c r="F86" s="38"/>
     </row>
     <row r="87" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="36" t="s">
+      <c r="A87" s="41" t="s">
         <v>157</v>
       </c>
       <c r="B87" s="41" t="s">
         <v>601</v>
       </c>
-      <c r="C87" s="37"/>
-      <c r="D87" s="37"/>
-      <c r="E87" s="38"/>
-      <c r="F87" s="38"/>
+      <c r="C87" s="42"/>
+      <c r="D87" s="42"/>
+      <c r="E87" s="43"/>
+      <c r="F87" s="43"/>
     </row>
     <row r="88" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="48" t="s">
@@ -26984,22 +26987,22 @@
       <c r="F88" s="43"/>
     </row>
     <row r="89" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="39" t="s">
-        <v>274</v>
-      </c>
-      <c r="B89" s="40" t="s">
+      <c r="A89" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="B89" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="C89" s="40" t="s">
+      <c r="C89" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="D89" s="40" t="s">
+      <c r="D89" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="E89" s="40" t="s">
+      <c r="E89" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="F89" s="40" t="s">
+      <c r="F89" s="35" t="s">
         <v>2</v>
       </c>
     </row>
@@ -27018,7 +27021,7 @@
       <c r="F90" s="45"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A91" s="44" t="s">
+      <c r="A91" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B91" s="49">
@@ -27027,12 +27030,12 @@
       <c r="C91" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="D91" s="44"/>
-      <c r="E91" s="45"/>
-      <c r="F91" s="45"/>
+      <c r="D91" s="46"/>
+      <c r="E91" s="47"/>
+      <c r="F91" s="47"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92" s="44" t="s">
+      <c r="A92" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B92" s="49">
@@ -27041,9 +27044,9 @@
       <c r="C92" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D92" s="44"/>
-      <c r="E92" s="45"/>
-      <c r="F92" s="45"/>
+      <c r="D92" s="46"/>
+      <c r="E92" s="47"/>
+      <c r="F92" s="47"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="46" t="s">
@@ -27168,16 +27171,16 @@
       <c r="F101" s="38"/>
     </row>
     <row r="102" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="41" t="s">
+      <c r="A102" s="36" t="s">
         <v>157</v>
       </c>
       <c r="B102" s="41" t="s">
         <v>601</v>
       </c>
-      <c r="C102" s="42"/>
-      <c r="D102" s="42"/>
-      <c r="E102" s="43"/>
-      <c r="F102" s="43"/>
+      <c r="C102" s="37"/>
+      <c r="D102" s="37"/>
+      <c r="E102" s="38"/>
+      <c r="F102" s="38"/>
     </row>
     <row r="103" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="48" t="s">
@@ -27192,22 +27195,22 @@
       <c r="F103" s="43"/>
     </row>
     <row r="104" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="B104" s="40" t="s">
+      <c r="A104" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="B104" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="C104" s="40" t="s">
+      <c r="C104" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="D104" s="40" t="s">
+      <c r="D104" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="E104" s="40" t="s">
+      <c r="E104" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="F104" s="40" t="s">
+      <c r="F104" s="35" t="s">
         <v>2</v>
       </c>
     </row>
@@ -27226,7 +27229,7 @@
       <c r="F105" s="45"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A106" s="44" t="s">
+      <c r="A106" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B106" s="49">
@@ -27235,12 +27238,12 @@
       <c r="C106" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="D106" s="44"/>
-      <c r="E106" s="45"/>
-      <c r="F106" s="45"/>
+      <c r="D106" s="46"/>
+      <c r="E106" s="47"/>
+      <c r="F106" s="47"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A107" s="44" t="s">
+      <c r="A107" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B107" s="49">
@@ -27249,12 +27252,12 @@
       <c r="C107" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D107" s="44"/>
-      <c r="E107" s="45"/>
-      <c r="F107" s="45"/>
+      <c r="D107" s="46"/>
+      <c r="E107" s="47"/>
+      <c r="F107" s="47"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A108" s="44" t="s">
+      <c r="A108" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B108" s="49">
@@ -27263,9 +27266,9 @@
       <c r="C108" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="D108" s="44"/>
-      <c r="E108" s="45"/>
-      <c r="F108" s="45"/>
+      <c r="D108" s="46"/>
+      <c r="E108" s="47"/>
+      <c r="F108" s="47"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="46" t="s">
@@ -27376,16 +27379,16 @@
       <c r="F116" s="38"/>
     </row>
     <row r="117" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="41" t="s">
+      <c r="A117" s="36" t="s">
         <v>157</v>
       </c>
       <c r="B117" s="41" t="s">
         <v>601</v>
       </c>
-      <c r="C117" s="42"/>
-      <c r="D117" s="42"/>
-      <c r="E117" s="43"/>
-      <c r="F117" s="43"/>
+      <c r="C117" s="37"/>
+      <c r="D117" s="37"/>
+      <c r="E117" s="38"/>
+      <c r="F117" s="38"/>
     </row>
     <row r="118" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A118" s="48" t="s">
@@ -27401,7 +27404,7 @@
     </row>
     <row r="119" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A119" s="39" t="s">
-        <v>708</v>
+        <v>285</v>
       </c>
       <c r="B119" s="40" t="s">
         <v>145</v>
@@ -27434,7 +27437,7 @@
       <c r="F120" s="45"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A121" s="44" t="s">
+      <c r="A121" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B121" s="49">
@@ -27443,12 +27446,12 @@
       <c r="C121" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="D121" s="44"/>
-      <c r="E121" s="45"/>
-      <c r="F121" s="45"/>
+      <c r="D121" s="46"/>
+      <c r="E121" s="47"/>
+      <c r="F121" s="47"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A122" s="44" t="s">
+      <c r="A122" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B122" s="49">
@@ -27457,12 +27460,12 @@
       <c r="C122" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D122" s="44"/>
-      <c r="E122" s="45"/>
-      <c r="F122" s="45"/>
+      <c r="D122" s="46"/>
+      <c r="E122" s="47"/>
+      <c r="F122" s="47"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A123" s="44" t="s">
+      <c r="A123" s="46" t="s">
         <v>144</v>
       </c>
       <c r="B123" s="49">
@@ -27471,9 +27474,9 @@
       <c r="C123" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="D123" s="44"/>
-      <c r="E123" s="45"/>
-      <c r="F123" s="45"/>
+      <c r="D123" s="46"/>
+      <c r="E123" s="47"/>
+      <c r="F123" s="47"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="46" t="s">
@@ -27609,7 +27612,7 @@
     </row>
     <row r="134" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A134" s="39" t="s">
-        <v>709</v>
+        <v>676</v>
       </c>
       <c r="B134" s="40" t="s">
         <v>145</v>
@@ -27642,7 +27645,7 @@
       <c r="F135" s="45"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A136" s="46" t="s">
+      <c r="A136" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B136" s="49">
@@ -27651,12 +27654,12 @@
       <c r="C136" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="D136" s="46"/>
-      <c r="E136" s="47"/>
-      <c r="F136" s="47"/>
+      <c r="D136" s="44"/>
+      <c r="E136" s="45"/>
+      <c r="F136" s="45"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A137" s="46" t="s">
+      <c r="A137" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B137" s="49">
@@ -27665,12 +27668,12 @@
       <c r="C137" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D137" s="46"/>
-      <c r="E137" s="47"/>
-      <c r="F137" s="47"/>
+      <c r="D137" s="44"/>
+      <c r="E137" s="45"/>
+      <c r="F137" s="45"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A138" s="46" t="s">
+      <c r="A138" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B138" s="49">
@@ -27679,9 +27682,9 @@
       <c r="C138" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="D138" s="46"/>
-      <c r="E138" s="47"/>
-      <c r="F138" s="47"/>
+      <c r="D138" s="44"/>
+      <c r="E138" s="45"/>
+      <c r="F138" s="45"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" s="46" t="s">
@@ -27817,7 +27820,7 @@
     </row>
     <row r="149" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A149" s="39" t="s">
-        <v>285</v>
+        <v>709</v>
       </c>
       <c r="B149" s="40" t="s">
         <v>145</v>
@@ -28024,22 +28027,22 @@
       <c r="F163" s="43"/>
     </row>
     <row r="164" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A164" s="34" t="s">
-        <v>324</v>
-      </c>
-      <c r="B164" s="35" t="s">
+      <c r="A164" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="B164" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="C164" s="35" t="s">
+      <c r="C164" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="D164" s="35" t="s">
+      <c r="D164" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="E164" s="35" t="s">
+      <c r="E164" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="F164" s="35" t="s">
+      <c r="F164" s="40" t="s">
         <v>2</v>
       </c>
     </row>
@@ -28058,7 +28061,7 @@
       <c r="F165" s="45"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A166" s="46" t="s">
+      <c r="A166" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B166" s="49">
@@ -28067,12 +28070,12 @@
       <c r="C166" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="D166" s="46"/>
-      <c r="E166" s="47"/>
-      <c r="F166" s="47"/>
+      <c r="D166" s="44"/>
+      <c r="E166" s="45"/>
+      <c r="F166" s="45"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A167" s="46" t="s">
+      <c r="A167" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B167" s="49">
@@ -28081,12 +28084,12 @@
       <c r="C167" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="D167" s="46"/>
-      <c r="E167" s="47"/>
-      <c r="F167" s="47"/>
+      <c r="D167" s="44"/>
+      <c r="E167" s="45"/>
+      <c r="F167" s="45"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A168" s="46" t="s">
+      <c r="A168" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B168" s="49">
@@ -28095,9 +28098,9 @@
       <c r="C168" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="D168" s="46"/>
-      <c r="E168" s="47"/>
-      <c r="F168" s="47"/>
+      <c r="D168" s="44"/>
+      <c r="E168" s="45"/>
+      <c r="F168" s="45"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" s="46" t="s">
@@ -28208,16 +28211,16 @@
       <c r="F176" s="38"/>
     </row>
     <row r="177" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A177" s="36" t="s">
+      <c r="A177" s="41" t="s">
         <v>157</v>
       </c>
       <c r="B177" s="41" t="s">
         <v>601</v>
       </c>
-      <c r="C177" s="37"/>
-      <c r="D177" s="37"/>
-      <c r="E177" s="38"/>
-      <c r="F177" s="38"/>
+      <c r="C177" s="42"/>
+      <c r="D177" s="42"/>
+      <c r="E177" s="43"/>
+      <c r="F177" s="43"/>
     </row>
     <row r="178" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A178" s="48" t="s">
@@ -28233,7 +28236,7 @@
     </row>
     <row r="179" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A179" s="39" t="s">
-        <v>676</v>
+        <v>708</v>
       </c>
       <c r="B179" s="40" t="s">
         <v>145</v>
@@ -28438,6 +28441,214 @@
       <c r="D193" s="42"/>
       <c r="E193" s="43"/>
       <c r="F193" s="43"/>
+    </row>
+    <row r="194" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A194" s="39" t="s">
+        <v>710</v>
+      </c>
+      <c r="B194" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="C194" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="D194" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="E194" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="F194" s="40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A195" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B195" s="49">
+        <v>4</v>
+      </c>
+      <c r="C195" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="D195" s="44"/>
+      <c r="E195" s="45"/>
+      <c r="F195" s="45"/>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A196" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B196" s="49">
+        <v>4</v>
+      </c>
+      <c r="C196" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="D196" s="44"/>
+      <c r="E196" s="45"/>
+      <c r="F196" s="45"/>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A197" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B197" s="49">
+        <v>4</v>
+      </c>
+      <c r="C197" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="D197" s="44"/>
+      <c r="E197" s="45"/>
+      <c r="F197" s="45"/>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A198" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B198" s="49">
+        <v>4</v>
+      </c>
+      <c r="C198" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="D198" s="44"/>
+      <c r="E198" s="45"/>
+      <c r="F198" s="45"/>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A199" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B199" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C199" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="D199" s="46"/>
+      <c r="E199" s="47"/>
+      <c r="F199" s="47"/>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A200" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B200" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C200" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="D200" s="46"/>
+      <c r="E200" s="47"/>
+      <c r="F200" s="47"/>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A201" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B201" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C201" s="46" t="s">
+        <v>599</v>
+      </c>
+      <c r="D201" s="46"/>
+      <c r="E201" s="47"/>
+      <c r="F201" s="47"/>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A202" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B202" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C202" s="46" t="s">
+        <v>600</v>
+      </c>
+      <c r="D202" s="46"/>
+      <c r="E202" s="47"/>
+      <c r="F202" s="47"/>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A203" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B203" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C203" s="46" t="s">
+        <v>272</v>
+      </c>
+      <c r="D203" s="46"/>
+      <c r="E203" s="47"/>
+      <c r="F203" s="47"/>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A204" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B204" s="49">
+        <v>0.25</v>
+      </c>
+      <c r="C204" s="46" t="s">
+        <v>273</v>
+      </c>
+      <c r="D204" s="46"/>
+      <c r="E204" s="47"/>
+      <c r="F204" s="47"/>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A205" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B205" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="C205" s="37"/>
+      <c r="D205" s="37"/>
+      <c r="E205" s="38"/>
+      <c r="F205" s="38"/>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A206" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="B206" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C206" s="37"/>
+      <c r="D206" s="37"/>
+      <c r="E206" s="38"/>
+      <c r="F206" s="38"/>
+    </row>
+    <row r="207" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A207" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="B207" s="41" t="s">
+        <v>601</v>
+      </c>
+      <c r="C207" s="42"/>
+      <c r="D207" s="42"/>
+      <c r="E207" s="43"/>
+      <c r="F207" s="43"/>
+    </row>
+    <row r="208" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A208" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="B208" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="C208" s="42"/>
+      <c r="D208" s="42"/>
+      <c r="E208" s="43"/>
+      <c r="F208" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
References update, validation spreadsheet updates for etomidate.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngineStable\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EB554D-DB9A-4EDA-8765-AAE38F24C194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA918807-551C-4568-B979-BA422DC7DA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4780,7 +4780,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="CT18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="DF42" sqref="DF42"/>
+      <selection pane="bottomRight" activeCell="DF46" sqref="DF46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -15942,7 +15942,7 @@
       <c r="DD45" s="115"/>
       <c r="DE45" s="115"/>
       <c r="DF45" s="115">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="DG45" s="115"/>
       <c r="DH45" s="111" t="s">

</xml_diff>

<commit_message>
Move norepi updates to new model
co-author Rachel Clipp
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngineStable\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA918807-551C-4568-B979-BA422DC7DA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CE20E3-9173-4BF0-8C89-99757C299AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5071" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5074" uniqueCount="735">
   <si>
     <t>Name</t>
   </si>
@@ -2240,6 +2240,21 @@
   </si>
   <si>
     <t>0.01 ug/mL</t>
+  </si>
+  <si>
+    <t>https://go.drugbank.com/drugs/DB00368</t>
+  </si>
+  <si>
+    <t>169.18 g/mol</t>
+  </si>
+  <si>
+    <t>de Vera et al</t>
+  </si>
+  <si>
+    <t>https://drugcentral.org/drugcard/1960</t>
+  </si>
+  <si>
+    <t>55.0 mL/min kg</t>
   </si>
 </sst>
 </file>
@@ -4777,10 +4792,10 @@
   <dimension ref="A1:FF75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="CT18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AH21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="DF46" sqref="DF46"/>
+      <selection pane="bottomRight" activeCell="AP39" sqref="AP39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -7054,7 +7069,7 @@
       <c r="AN8" s="106"/>
       <c r="AO8" s="106"/>
       <c r="AP8" s="103" t="s">
-        <v>120</v>
+        <v>731</v>
       </c>
       <c r="AQ8" s="106"/>
       <c r="AR8" s="106"/>
@@ -9342,10 +9357,12 @@
       <c r="AN18" s="106"/>
       <c r="AO18" s="106"/>
       <c r="AP18" s="103">
-        <v>0.88</v>
+        <v>0.75</v>
       </c>
       <c r="AQ18" s="106"/>
-      <c r="AR18" s="106"/>
+      <c r="AR18" s="106" t="s">
+        <v>732</v>
+      </c>
       <c r="AS18" s="106"/>
       <c r="AT18" s="88">
         <v>1</v>
@@ -9973,7 +9990,7 @@
       <c r="AN21" s="106"/>
       <c r="AO21" s="106"/>
       <c r="AP21" s="103" t="s">
-        <v>665</v>
+        <v>734</v>
       </c>
       <c r="AQ21" s="106"/>
       <c r="AR21" s="106"/>
@@ -12536,10 +12553,14 @@
       <c r="AN30" s="106"/>
       <c r="AO30" s="106"/>
       <c r="AP30" s="103">
-        <v>8.59</v>
-      </c>
-      <c r="AQ30" s="106"/>
-      <c r="AR30" s="106"/>
+        <v>9.41</v>
+      </c>
+      <c r="AQ30" s="106">
+        <v>9.41</v>
+      </c>
+      <c r="AR30" s="106" t="s">
+        <v>733</v>
+      </c>
       <c r="AS30" s="106"/>
       <c r="AT30" s="92"/>
       <c r="AU30" s="92"/>
@@ -12731,7 +12752,7 @@
       <c r="AN31" s="106"/>
       <c r="AO31" s="106"/>
       <c r="AP31" s="103" t="s">
-        <v>262</v>
+        <v>114</v>
       </c>
       <c r="AQ31" s="106"/>
       <c r="AR31" s="106"/>
@@ -13121,7 +13142,7 @@
       <c r="AO33" s="106"/>
       <c r="AP33" s="103">
         <f>AP18</f>
-        <v>0.88</v>
+        <v>0.75</v>
       </c>
       <c r="AQ33" s="106"/>
       <c r="AR33" s="106"/>
@@ -13429,7 +13450,7 @@
       <c r="AN34" s="106"/>
       <c r="AO34" s="106"/>
       <c r="AP34" s="103" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="AQ34" s="106"/>
       <c r="AR34" s="106"/>
@@ -13620,10 +13641,14 @@
       <c r="AN35" s="106"/>
       <c r="AO35" s="106"/>
       <c r="AP35" s="103">
-        <v>-1.37</v>
-      </c>
-      <c r="AQ35" s="106"/>
-      <c r="AR35" s="106"/>
+        <v>-1.24</v>
+      </c>
+      <c r="AQ35" s="106">
+        <v>-1.24</v>
+      </c>
+      <c r="AR35" s="106" t="s">
+        <v>730</v>
+      </c>
       <c r="AS35" s="106"/>
       <c r="AT35" s="92"/>
       <c r="AU35" s="92"/>
@@ -15022,7 +15047,7 @@
       <c r="AN41" s="114"/>
       <c r="AO41" s="114"/>
       <c r="AP41" s="114">
-        <v>-0.15</v>
+        <v>-0.2</v>
       </c>
       <c r="AQ41" s="114"/>
       <c r="AR41" s="114"/>
@@ -16264,7 +16289,7 @@
       <c r="AN47" s="114"/>
       <c r="AO47" s="114"/>
       <c r="AP47" s="114">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="AQ47" s="114"/>
       <c r="AR47" s="114"/>

</xml_diff>

<commit_message>
Added Phenylephrine to the drug library with validation at 4 infusion rates for plasma concentration, heart rate, and systolic and diastolic pressure
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngineStable\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CE20E3-9173-4BF0-8C89-99757C299AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670570FB-B379-4ACE-BAF4-6C357FCF6A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5074" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5157" uniqueCount="746">
   <si>
     <t>Name</t>
   </si>
@@ -2255,6 +2255,39 @@
   </si>
   <si>
     <t>55.0 mL/min kg</t>
+  </si>
+  <si>
+    <t>Phenylephrine</t>
+  </si>
+  <si>
+    <t>167.205 g/mol</t>
+  </si>
+  <si>
+    <t>https://go.drugbank.com/drugs/DB00388</t>
+  </si>
+  <si>
+    <t>2100 mL/min</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>no info available so used Epi</t>
+  </si>
+  <si>
+    <t>no info available</t>
+  </si>
+  <si>
+    <t>3800 mL/min kg</t>
+  </si>
+  <si>
+    <t>45 mL/min kg</t>
+  </si>
+  <si>
+    <t>190 mL/min kg</t>
+  </si>
+  <si>
+    <t>0.018 ug/mL</t>
   </si>
 </sst>
 </file>
@@ -4789,13 +4822,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:FF75"/>
+  <dimension ref="A1:FJ75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AH21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="DF21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AP39" sqref="AP39"/>
+      <selection pane="bottomRight" activeCell="ED28" sqref="ED28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -4930,26 +4963,30 @@
     <col min="142" max="142" width="13.42578125" style="53" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="143" max="143" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="144" max="144" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="145" max="145" width="11.42578125" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="146" max="146" width="14.42578125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="145" max="145" width="11.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="146" max="146" width="13.42578125" style="53" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="147" max="147" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="148" max="148" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="149" max="149" width="11.42578125" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="150" max="150" width="21.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="150" max="150" width="14.42578125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="151" max="151" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="152" max="152" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="153" max="153" width="11.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="154" max="154" width="15.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="153" max="153" width="11.42578125" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="154" max="154" width="21.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="155" max="155" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="156" max="156" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="157" max="157" width="15.5703125" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="158" max="158" width="45.42578125" style="102" customWidth="1" collapsed="1"/>
-    <col min="159" max="161" width="23" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="162" max="162" width="9.140625" style="28" collapsed="1"/>
-    <col min="163" max="16384" width="9.140625" style="28"/>
+    <col min="157" max="157" width="11.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="158" max="158" width="15.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="159" max="159" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="160" max="160" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="161" max="161" width="15.5703125" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="162" max="162" width="45.42578125" style="102" customWidth="1" collapsed="1"/>
+    <col min="163" max="165" width="23" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="166" max="166" width="9.140625" style="28" collapsed="1"/>
+    <col min="167" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="59"/>
       <c r="B1" s="54"/>
       <c r="C1" s="99" t="s">
@@ -5311,7 +5348,7 @@
       <c r="EO1" s="108" t="s">
         <v>364</v>
       </c>
-      <c r="EP1" s="67"/>
+      <c r="EP1" s="68"/>
       <c r="EQ1" s="108" t="s">
         <v>362</v>
       </c>
@@ -5341,18 +5378,28 @@
       <c r="FA1" s="108" t="s">
         <v>364</v>
       </c>
-      <c r="FB1" s="158"/>
-      <c r="FC1" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD1" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE1" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="2" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB1" s="67"/>
+      <c r="FC1" s="108" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD1" s="108" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE1" s="108" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF1" s="158"/>
+      <c r="FG1" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH1" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI1" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="2" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>0</v>
       </c>
@@ -5765,79 +5812,91 @@
         <v>48</v>
       </c>
       <c r="EH2" s="100" t="s">
+        <v>735</v>
+      </c>
+      <c r="EI2" s="100" t="s">
+        <v>735</v>
+      </c>
+      <c r="EJ2" s="100" t="s">
+        <v>735</v>
+      </c>
+      <c r="EK2" s="100" t="s">
+        <v>735</v>
+      </c>
+      <c r="EL2" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="EI2" s="100" t="s">
+      <c r="EM2" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="EJ2" s="100" t="s">
+      <c r="EN2" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="EK2" s="100" t="s">
+      <c r="EO2" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="EL2" s="100" t="s">
+      <c r="EP2" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="EM2" s="100" t="s">
+      <c r="EQ2" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="EN2" s="100" t="s">
+      <c r="ER2" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="EO2" s="100" t="s">
+      <c r="ES2" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="EP2" s="100" t="s">
+      <c r="ET2" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="EQ2" s="100" t="s">
+      <c r="EU2" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="ER2" s="100" t="s">
+      <c r="EV2" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="ES2" s="100" t="s">
+      <c r="EW2" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="ET2" s="100" t="s">
+      <c r="EX2" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="EU2" s="100" t="s">
+      <c r="EY2" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="EV2" s="100" t="s">
+      <c r="EZ2" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="EW2" s="100" t="s">
+      <c r="FA2" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="EX2" s="100" t="s">
+      <c r="FB2" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="EY2" s="100" t="s">
+      <c r="FC2" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="EZ2" s="100" t="s">
+      <c r="FD2" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="FA2" s="100" t="s">
+      <c r="FE2" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="FB2" s="100" t="s">
+      <c r="FF2" s="100" t="s">
         <v>668</v>
       </c>
-      <c r="FC2" s="100" t="s">
+      <c r="FG2" s="100" t="s">
         <v>668</v>
       </c>
-      <c r="FD2" s="100" t="s">
+      <c r="FH2" s="100" t="s">
         <v>668</v>
       </c>
-      <c r="FE2" s="100" t="s">
+      <c r="FI2" s="100" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="3" spans="1:161" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:165" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
         <v>341</v>
       </c>
@@ -6241,8 +6300,18 @@
       <c r="FE3" s="109" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="4" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FF3" s="57"/>
+      <c r="FG3" s="109" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH3" s="109" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI3" s="109" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>1</v>
       </c>
@@ -6482,14 +6551,20 @@
       <c r="EY4" s="111"/>
       <c r="EZ4" s="111"/>
       <c r="FA4" s="111"/>
-      <c r="FB4" s="160" t="s">
+      <c r="FB4" s="111" t="s">
+        <v>17</v>
+      </c>
+      <c r="FC4" s="111"/>
+      <c r="FD4" s="111"/>
+      <c r="FE4" s="111"/>
+      <c r="FF4" s="160" t="s">
         <v>631</v>
       </c>
-      <c r="FC4" s="160"/>
-      <c r="FD4" s="160"/>
-      <c r="FE4" s="160"/>
-    </row>
-    <row r="5" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FG4" s="160"/>
+      <c r="FH4" s="160"/>
+      <c r="FI4" s="160"/>
+    </row>
+    <row r="5" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>10</v>
       </c>
@@ -6665,12 +6740,16 @@
       <c r="EY5" s="111"/>
       <c r="EZ5" s="111"/>
       <c r="FA5" s="111"/>
-      <c r="FB5" s="160"/>
-      <c r="FC5" s="160"/>
-      <c r="FD5" s="160"/>
-      <c r="FE5" s="160"/>
-    </row>
-    <row r="6" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB5" s="111"/>
+      <c r="FC5" s="111"/>
+      <c r="FD5" s="111"/>
+      <c r="FE5" s="111"/>
+      <c r="FF5" s="160"/>
+      <c r="FG5" s="160"/>
+      <c r="FH5" s="160"/>
+      <c r="FI5" s="160"/>
+    </row>
+    <row r="6" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>553</v>
       </c>
@@ -6832,12 +6911,16 @@
       <c r="EY6" s="111"/>
       <c r="EZ6" s="111"/>
       <c r="FA6" s="111"/>
-      <c r="FB6" s="160"/>
-      <c r="FC6" s="160"/>
-      <c r="FD6" s="160"/>
-      <c r="FE6" s="160"/>
-    </row>
-    <row r="7" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB6" s="111"/>
+      <c r="FC6" s="111"/>
+      <c r="FD6" s="111"/>
+      <c r="FE6" s="111"/>
+      <c r="FF6" s="160"/>
+      <c r="FG6" s="160"/>
+      <c r="FH6" s="160"/>
+      <c r="FI6" s="160"/>
+    </row>
+    <row r="7" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>554</v>
       </c>
@@ -6999,12 +7082,16 @@
       <c r="EY7" s="111"/>
       <c r="EZ7" s="111"/>
       <c r="FA7" s="111"/>
-      <c r="FB7" s="160"/>
-      <c r="FC7" s="160"/>
-      <c r="FD7" s="160"/>
-      <c r="FE7" s="160"/>
-    </row>
-    <row r="8" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB7" s="111"/>
+      <c r="FC7" s="111"/>
+      <c r="FD7" s="111"/>
+      <c r="FE7" s="111"/>
+      <c r="FF7" s="160"/>
+      <c r="FG7" s="160"/>
+      <c r="FH7" s="160"/>
+      <c r="FI7" s="160"/>
+    </row>
+    <row r="8" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>43</v>
       </c>
@@ -7215,41 +7302,49 @@
       <c r="EF8" s="111"/>
       <c r="EG8" s="111"/>
       <c r="EH8" s="111" t="s">
-        <v>129</v>
+        <v>736</v>
       </c>
       <c r="EI8" s="111"/>
-      <c r="EJ8" s="111"/>
+      <c r="EJ8" s="111" t="s">
+        <v>737</v>
+      </c>
       <c r="EK8" s="111"/>
       <c r="EL8" s="111" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="EM8" s="111"/>
       <c r="EN8" s="111"/>
       <c r="EO8" s="111"/>
       <c r="EP8" s="111" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="EQ8" s="111"/>
       <c r="ER8" s="111"/>
       <c r="ES8" s="111"/>
       <c r="ET8" s="111" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="EU8" s="111"/>
       <c r="EV8" s="111"/>
       <c r="EW8" s="111"/>
       <c r="EX8" s="111" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="EY8" s="111"/>
       <c r="EZ8" s="111"/>
       <c r="FA8" s="111"/>
-      <c r="FB8" s="160"/>
-      <c r="FC8" s="160"/>
-      <c r="FD8" s="160"/>
-      <c r="FE8" s="160"/>
-    </row>
-    <row r="9" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB8" s="111" t="s">
+        <v>118</v>
+      </c>
+      <c r="FC8" s="111"/>
+      <c r="FD8" s="111"/>
+      <c r="FE8" s="111"/>
+      <c r="FF8" s="160"/>
+      <c r="FG8" s="160"/>
+      <c r="FH8" s="160"/>
+      <c r="FI8" s="160"/>
+    </row>
+    <row r="9" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
         <v>716</v>
       </c>
@@ -7419,12 +7514,16 @@
       <c r="EY9" s="111"/>
       <c r="EZ9" s="111"/>
       <c r="FA9" s="111"/>
-      <c r="FB9" s="160"/>
-      <c r="FC9" s="160"/>
-      <c r="FD9" s="160"/>
-      <c r="FE9" s="160"/>
-    </row>
-    <row r="10" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB9" s="111"/>
+      <c r="FC9" s="111"/>
+      <c r="FD9" s="111"/>
+      <c r="FE9" s="111"/>
+      <c r="FF9" s="160"/>
+      <c r="FG9" s="160"/>
+      <c r="FH9" s="160"/>
+      <c r="FI9" s="160"/>
+    </row>
+    <row r="10" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
         <v>76</v>
       </c>
@@ -7596,12 +7695,16 @@
       <c r="EY10" s="111"/>
       <c r="EZ10" s="111"/>
       <c r="FA10" s="111"/>
-      <c r="FB10" s="160"/>
-      <c r="FC10" s="160"/>
-      <c r="FD10" s="160"/>
-      <c r="FE10" s="160"/>
-    </row>
-    <row r="11" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB10" s="111"/>
+      <c r="FC10" s="111"/>
+      <c r="FD10" s="111"/>
+      <c r="FE10" s="111"/>
+      <c r="FF10" s="160"/>
+      <c r="FG10" s="160"/>
+      <c r="FH10" s="160"/>
+      <c r="FI10" s="160"/>
+    </row>
+    <row r="11" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>75</v>
       </c>
@@ -7779,12 +7882,16 @@
       <c r="EY11" s="111"/>
       <c r="EZ11" s="111"/>
       <c r="FA11" s="111"/>
-      <c r="FB11" s="160"/>
-      <c r="FC11" s="160"/>
-      <c r="FD11" s="160"/>
-      <c r="FE11" s="160"/>
-    </row>
-    <row r="12" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB11" s="111"/>
+      <c r="FC11" s="111"/>
+      <c r="FD11" s="111"/>
+      <c r="FE11" s="111"/>
+      <c r="FF11" s="160"/>
+      <c r="FG11" s="160"/>
+      <c r="FH11" s="160"/>
+      <c r="FI11" s="160"/>
+    </row>
+    <row r="12" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="80" t="s">
         <v>337</v>
       </c>
@@ -8150,7 +8257,7 @@
       <c r="EO12" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP12" s="112"/>
+      <c r="EP12" s="70"/>
       <c r="EQ12" s="110" t="s">
         <v>362</v>
       </c>
@@ -8180,18 +8287,28 @@
       <c r="FA12" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB12" s="158"/>
-      <c r="FC12" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD12" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE12" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="13" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB12" s="112"/>
+      <c r="FC12" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD12" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE12" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF12" s="158"/>
+      <c r="FG12" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH12" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI12" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="64" t="s">
         <v>671</v>
       </c>
@@ -8350,17 +8467,21 @@
       <c r="EV13" s="115"/>
       <c r="EW13" s="115"/>
       <c r="EX13" s="115"/>
-      <c r="EY13" s="157"/>
-      <c r="EZ13" s="157"/>
-      <c r="FA13" s="157"/>
-      <c r="FB13" s="160">
+      <c r="EY13" s="115"/>
+      <c r="EZ13" s="115"/>
+      <c r="FA13" s="115"/>
+      <c r="FB13" s="115"/>
+      <c r="FC13" s="157"/>
+      <c r="FD13" s="157"/>
+      <c r="FE13" s="157"/>
+      <c r="FF13" s="160">
         <v>0</v>
       </c>
-      <c r="FC13" s="166"/>
-      <c r="FD13" s="166"/>
-      <c r="FE13" s="166"/>
-    </row>
-    <row r="14" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FG13" s="166"/>
+      <c r="FH13" s="166"/>
+      <c r="FI13" s="166"/>
+    </row>
+    <row r="14" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="64" t="s">
         <v>658</v>
       </c>
@@ -8519,17 +8640,21 @@
       <c r="EV14" s="115"/>
       <c r="EW14" s="115"/>
       <c r="EX14" s="115"/>
-      <c r="EY14" s="157"/>
-      <c r="EZ14" s="157"/>
-      <c r="FA14" s="157"/>
-      <c r="FB14" s="160">
+      <c r="EY14" s="115"/>
+      <c r="EZ14" s="115"/>
+      <c r="FA14" s="115"/>
+      <c r="FB14" s="115"/>
+      <c r="FC14" s="157"/>
+      <c r="FD14" s="157"/>
+      <c r="FE14" s="157"/>
+      <c r="FF14" s="160">
         <v>0.5</v>
       </c>
-      <c r="FC14" s="166"/>
-      <c r="FD14" s="166"/>
-      <c r="FE14" s="166"/>
-    </row>
-    <row r="15" spans="1:161" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="FG14" s="166"/>
+      <c r="FH14" s="166"/>
+      <c r="FI14" s="166"/>
+    </row>
+    <row r="15" spans="1:165" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="64" t="s">
         <v>627</v>
       </c>
@@ -8688,17 +8813,21 @@
       <c r="EV15" s="115"/>
       <c r="EW15" s="115"/>
       <c r="EX15" s="115"/>
-      <c r="EY15" s="157"/>
-      <c r="EZ15" s="157"/>
-      <c r="FA15" s="157"/>
-      <c r="FB15" s="164" t="s">
+      <c r="EY15" s="115"/>
+      <c r="EZ15" s="115"/>
+      <c r="FA15" s="115"/>
+      <c r="FB15" s="115"/>
+      <c r="FC15" s="157"/>
+      <c r="FD15" s="157"/>
+      <c r="FE15" s="157"/>
+      <c r="FF15" s="164" t="s">
         <v>628</v>
       </c>
-      <c r="FC15" s="162"/>
-      <c r="FD15" s="162"/>
-      <c r="FE15" s="162"/>
-    </row>
-    <row r="16" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FG15" s="162"/>
+      <c r="FH15" s="162"/>
+      <c r="FI15" s="162"/>
+    </row>
+    <row r="16" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="80" t="s">
         <v>338</v>
       </c>
@@ -9064,7 +9193,7 @@
       <c r="EO16" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP16" s="112"/>
+      <c r="EP16" s="70"/>
       <c r="EQ16" s="110" t="s">
         <v>362</v>
       </c>
@@ -9094,18 +9223,28 @@
       <c r="FA16" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB16" s="158"/>
-      <c r="FC16" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD16" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE16" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="17" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB16" s="112"/>
+      <c r="FC16" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD16" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE16" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF16" s="158"/>
+      <c r="FG16" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH16" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI16" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="17" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
         <v>96</v>
       </c>
@@ -9288,29 +9427,35 @@
       <c r="EN17" s="111"/>
       <c r="EO17" s="111"/>
       <c r="EP17" s="111">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="EQ17" s="111"/>
       <c r="ER17" s="111"/>
       <c r="ES17" s="111"/>
       <c r="ET17" s="111">
-        <v>0.31</v>
+        <v>0.02</v>
       </c>
       <c r="EU17" s="111"/>
       <c r="EV17" s="111"/>
       <c r="EW17" s="111"/>
       <c r="EX17" s="111">
-        <v>0</v>
+        <v>0.31</v>
       </c>
       <c r="EY17" s="111"/>
       <c r="EZ17" s="111"/>
       <c r="FA17" s="111"/>
-      <c r="FB17" s="160"/>
-      <c r="FC17" s="160"/>
-      <c r="FD17" s="160"/>
-      <c r="FE17" s="160"/>
-    </row>
-    <row r="18" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB17" s="111">
+        <v>0</v>
+      </c>
+      <c r="FC17" s="111"/>
+      <c r="FD17" s="111"/>
+      <c r="FE17" s="111"/>
+      <c r="FF17" s="160"/>
+      <c r="FG17" s="160"/>
+      <c r="FH17" s="160"/>
+      <c r="FI17" s="160"/>
+    </row>
+    <row r="18" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="62" t="s">
         <v>92</v>
       </c>
@@ -9495,41 +9640,47 @@
       <c r="EF18" s="111"/>
       <c r="EG18" s="111"/>
       <c r="EH18" s="111">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="EI18" s="111"/>
       <c r="EJ18" s="111"/>
       <c r="EK18" s="111"/>
       <c r="EL18" s="111">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="EM18" s="111"/>
       <c r="EN18" s="111"/>
       <c r="EO18" s="111"/>
       <c r="EP18" s="111">
-        <v>0.03</v>
+        <v>0.25</v>
       </c>
       <c r="EQ18" s="111"/>
       <c r="ER18" s="111"/>
       <c r="ES18" s="111"/>
       <c r="ET18" s="111">
-        <v>0.7</v>
+        <v>0.03</v>
       </c>
       <c r="EU18" s="111"/>
       <c r="EV18" s="111"/>
       <c r="EW18" s="111"/>
       <c r="EX18" s="111">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="EY18" s="111"/>
       <c r="EZ18" s="111"/>
       <c r="FA18" s="111"/>
-      <c r="FB18" s="160"/>
-      <c r="FC18" s="160"/>
-      <c r="FD18" s="160"/>
-      <c r="FE18" s="160"/>
-    </row>
-    <row r="19" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB18" s="111">
+        <v>0.8</v>
+      </c>
+      <c r="FC18" s="111"/>
+      <c r="FD18" s="111"/>
+      <c r="FE18" s="111"/>
+      <c r="FF18" s="160"/>
+      <c r="FG18" s="160"/>
+      <c r="FH18" s="160"/>
+      <c r="FI18" s="160"/>
+    </row>
+    <row r="19" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="62" t="s">
         <v>94</v>
       </c>
@@ -9704,41 +9855,51 @@
       <c r="EF19" s="111"/>
       <c r="EG19" s="111"/>
       <c r="EH19" s="111" t="s">
-        <v>99</v>
-      </c>
-      <c r="EI19" s="111"/>
-      <c r="EJ19" s="111"/>
+        <v>742</v>
+      </c>
+      <c r="EI19" s="111" t="s">
+        <v>738</v>
+      </c>
+      <c r="EJ19" s="111" t="s">
+        <v>737</v>
+      </c>
       <c r="EK19" s="111"/>
       <c r="EL19" s="111" t="s">
-        <v>263</v>
+        <v>99</v>
       </c>
       <c r="EM19" s="111"/>
       <c r="EN19" s="111"/>
       <c r="EO19" s="111"/>
       <c r="EP19" s="111" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="EQ19" s="111"/>
       <c r="ER19" s="111"/>
       <c r="ES19" s="111"/>
       <c r="ET19" s="111" t="s">
-        <v>361</v>
+        <v>264</v>
       </c>
       <c r="EU19" s="111"/>
       <c r="EV19" s="111"/>
       <c r="EW19" s="111"/>
       <c r="EX19" s="111" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="EY19" s="111"/>
       <c r="EZ19" s="111"/>
       <c r="FA19" s="111"/>
-      <c r="FB19" s="160"/>
-      <c r="FC19" s="160"/>
-      <c r="FD19" s="160"/>
-      <c r="FE19" s="160"/>
-    </row>
-    <row r="20" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB19" s="111" t="s">
+        <v>347</v>
+      </c>
+      <c r="FC19" s="111"/>
+      <c r="FD19" s="111"/>
+      <c r="FE19" s="111"/>
+      <c r="FF19" s="160"/>
+      <c r="FG19" s="160"/>
+      <c r="FH19" s="160"/>
+      <c r="FI19" s="160"/>
+    </row>
+    <row r="20" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="62" t="s">
         <v>379</v>
       </c>
@@ -9909,41 +10070,47 @@
       <c r="EF20" s="111"/>
       <c r="EG20" s="111"/>
       <c r="EH20" s="111" t="s">
-        <v>130</v>
+        <v>743</v>
       </c>
       <c r="EI20" s="111"/>
       <c r="EJ20" s="111"/>
       <c r="EK20" s="111"/>
       <c r="EL20" s="111" t="s">
-        <v>358</v>
+        <v>130</v>
       </c>
       <c r="EM20" s="111"/>
       <c r="EN20" s="111"/>
       <c r="EO20" s="111"/>
       <c r="EP20" s="111" t="s">
-        <v>265</v>
+        <v>358</v>
       </c>
       <c r="EQ20" s="111"/>
       <c r="ER20" s="111"/>
       <c r="ES20" s="111"/>
       <c r="ET20" s="111" t="s">
-        <v>360</v>
+        <v>265</v>
       </c>
       <c r="EU20" s="111"/>
       <c r="EV20" s="111"/>
       <c r="EW20" s="111"/>
       <c r="EX20" s="111" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="EY20" s="111"/>
       <c r="EZ20" s="111"/>
       <c r="FA20" s="111"/>
-      <c r="FB20" s="160"/>
-      <c r="FC20" s="160"/>
-      <c r="FD20" s="160"/>
-      <c r="FE20" s="160"/>
-    </row>
-    <row r="21" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB20" s="111" t="s">
+        <v>347</v>
+      </c>
+      <c r="FC20" s="111"/>
+      <c r="FD20" s="111"/>
+      <c r="FE20" s="111"/>
+      <c r="FF20" s="160"/>
+      <c r="FG20" s="160"/>
+      <c r="FH20" s="160"/>
+      <c r="FI20" s="160"/>
+    </row>
+    <row r="21" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="62" t="s">
         <v>95</v>
       </c>
@@ -10122,41 +10289,47 @@
       <c r="EF21" s="111"/>
       <c r="EG21" s="111"/>
       <c r="EH21" s="111" t="s">
-        <v>268</v>
+        <v>744</v>
       </c>
       <c r="EI21" s="111"/>
       <c r="EJ21" s="111"/>
       <c r="EK21" s="111"/>
       <c r="EL21" s="111" t="s">
-        <v>359</v>
+        <v>268</v>
       </c>
       <c r="EM21" s="111"/>
       <c r="EN21" s="111"/>
       <c r="EO21" s="111"/>
       <c r="EP21" s="111" t="s">
-        <v>269</v>
+        <v>359</v>
       </c>
       <c r="EQ21" s="111"/>
       <c r="ER21" s="111"/>
       <c r="ES21" s="111"/>
       <c r="ET21" s="111" t="s">
-        <v>353</v>
+        <v>269</v>
       </c>
       <c r="EU21" s="111"/>
       <c r="EV21" s="111"/>
       <c r="EW21" s="111"/>
       <c r="EX21" s="111" t="s">
-        <v>382</v>
+        <v>353</v>
       </c>
       <c r="EY21" s="111"/>
       <c r="EZ21" s="111"/>
       <c r="FA21" s="111"/>
-      <c r="FB21" s="160"/>
-      <c r="FC21" s="160"/>
-      <c r="FD21" s="160"/>
-      <c r="FE21" s="160"/>
-    </row>
-    <row r="22" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB21" s="111" t="s">
+        <v>382</v>
+      </c>
+      <c r="FC21" s="111"/>
+      <c r="FD21" s="111"/>
+      <c r="FE21" s="111"/>
+      <c r="FF21" s="160"/>
+      <c r="FG21" s="160"/>
+      <c r="FH21" s="160"/>
+      <c r="FI21" s="160"/>
+    </row>
+    <row r="22" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="81" t="s">
         <v>336</v>
       </c>
@@ -10522,7 +10695,7 @@
       <c r="EO22" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP22" s="112"/>
+      <c r="EP22" s="70"/>
       <c r="EQ22" s="110" t="s">
         <v>362</v>
       </c>
@@ -10552,18 +10725,28 @@
       <c r="FA22" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB22" s="158"/>
-      <c r="FC22" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD22" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE22" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="23" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB22" s="112"/>
+      <c r="FC22" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD22" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE22" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF22" s="158"/>
+      <c r="FG22" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH22" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI22" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="23" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="82" t="s">
         <v>332</v>
       </c>
@@ -10679,7 +10862,7 @@
       <c r="CZ23" s="111"/>
       <c r="DA23" s="111"/>
       <c r="DB23" s="111" t="str">
-        <f t="shared" ref="DB23:EX23" si="0">DB20</f>
+        <f t="shared" ref="DB23:FB23" si="0">DB20</f>
         <v>0 mL/min kg</v>
       </c>
       <c r="DC23" s="111">
@@ -10807,24 +10990,24 @@
         <v>0</v>
       </c>
       <c r="EH23" s="111" t="str">
+        <f t="shared" ref="EH23:EK23" si="2">EH20</f>
+        <v>45 mL/min kg</v>
+      </c>
+      <c r="EI23" s="111">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="EJ23" s="111">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="EK23" s="111">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="EL23" s="111" t="str">
         <f t="shared" si="0"/>
         <v>7.2 mL/min kg</v>
-      </c>
-      <c r="EI23" s="111">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="EJ23" s="111">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="EK23" s="111">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="EL23" s="111" t="str">
-        <f t="shared" si="0"/>
-        <v>0.72 mL/min kg</v>
       </c>
       <c r="EM23" s="111">
         <f t="shared" si="0"/>
@@ -10840,7 +11023,7 @@
       </c>
       <c r="EP23" s="111" t="str">
         <f t="shared" si="0"/>
-        <v>1.3 mL/min kg</v>
+        <v>0.72 mL/min kg</v>
       </c>
       <c r="EQ23" s="111">
         <f t="shared" si="0"/>
@@ -10856,7 +11039,7 @@
       </c>
       <c r="ET23" s="111" t="str">
         <f t="shared" si="0"/>
-        <v>2.2 mL/min kg</v>
+        <v>1.3 mL/min kg</v>
       </c>
       <c r="EU23" s="111">
         <f t="shared" si="0"/>
@@ -10872,17 +11055,33 @@
       </c>
       <c r="EX23" s="111" t="str">
         <f t="shared" si="0"/>
+        <v>2.2 mL/min kg</v>
+      </c>
+      <c r="EY23" s="111">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="EZ23" s="111">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="FA23" s="111">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="FB23" s="111" t="str">
+        <f t="shared" si="0"/>
         <v>0.0 mL/min kg</v>
       </c>
-      <c r="EY23" s="111"/>
-      <c r="EZ23" s="111"/>
-      <c r="FA23" s="111"/>
-      <c r="FB23" s="160"/>
-      <c r="FC23" s="160"/>
-      <c r="FD23" s="160"/>
-      <c r="FE23" s="160"/>
-    </row>
-    <row r="24" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FC23" s="111"/>
+      <c r="FD23" s="111"/>
+      <c r="FE23" s="111"/>
+      <c r="FF23" s="160"/>
+      <c r="FG23" s="160"/>
+      <c r="FH23" s="160"/>
+      <c r="FI23" s="160"/>
+    </row>
+    <row r="24" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="81" t="s">
         <v>331</v>
       </c>
@@ -11248,7 +11447,7 @@
       <c r="EO24" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP24" s="112"/>
+      <c r="EP24" s="70"/>
       <c r="EQ24" s="110" t="s">
         <v>362</v>
       </c>
@@ -11278,18 +11477,28 @@
       <c r="FA24" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB24" s="158"/>
-      <c r="FC24" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD24" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE24" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="25" spans="1:161" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FB24" s="112"/>
+      <c r="FC24" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD24" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE24" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF24" s="158"/>
+      <c r="FG24" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH24" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI24" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="25" spans="1:165" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="82" t="s">
         <v>333</v>
       </c>
@@ -11477,12 +11686,16 @@
       <c r="EY25" s="111"/>
       <c r="EZ25" s="111"/>
       <c r="FA25" s="111"/>
-      <c r="FB25" s="160"/>
-      <c r="FC25" s="160"/>
-      <c r="FD25" s="160"/>
-      <c r="FE25" s="160"/>
-    </row>
-    <row r="26" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB25" s="111"/>
+      <c r="FC25" s="111"/>
+      <c r="FD25" s="111"/>
+      <c r="FE25" s="111"/>
+      <c r="FF25" s="160"/>
+      <c r="FG25" s="160"/>
+      <c r="FH25" s="160"/>
+      <c r="FI25" s="160"/>
+    </row>
+    <row r="26" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="82" t="s">
         <v>380</v>
       </c>
@@ -11670,12 +11883,16 @@
       <c r="EY26" s="111"/>
       <c r="EZ26" s="111"/>
       <c r="FA26" s="111"/>
-      <c r="FB26" s="160"/>
-      <c r="FC26" s="160"/>
-      <c r="FD26" s="160"/>
-      <c r="FE26" s="160"/>
-    </row>
-    <row r="27" spans="1:161" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FB26" s="111"/>
+      <c r="FC26" s="111"/>
+      <c r="FD26" s="111"/>
+      <c r="FE26" s="111"/>
+      <c r="FF26" s="160"/>
+      <c r="FG26" s="160"/>
+      <c r="FH26" s="160"/>
+      <c r="FI26" s="160"/>
+    </row>
+    <row r="27" spans="1:165" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="82" t="s">
         <v>334</v>
       </c>
@@ -11881,12 +12098,16 @@
       <c r="EY27" s="111"/>
       <c r="EZ27" s="111"/>
       <c r="FA27" s="111"/>
-      <c r="FB27" s="160"/>
-      <c r="FC27" s="160"/>
-      <c r="FD27" s="160"/>
-      <c r="FE27" s="160"/>
-    </row>
-    <row r="28" spans="1:161" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FB27" s="111"/>
+      <c r="FC27" s="111"/>
+      <c r="FD27" s="111"/>
+      <c r="FE27" s="111"/>
+      <c r="FF27" s="160"/>
+      <c r="FG27" s="160"/>
+      <c r="FH27" s="160"/>
+      <c r="FI27" s="160"/>
+    </row>
+    <row r="28" spans="1:165" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="82" t="s">
         <v>335</v>
       </c>
@@ -12094,12 +12315,16 @@
       <c r="EY28" s="111"/>
       <c r="EZ28" s="111"/>
       <c r="FA28" s="111"/>
-      <c r="FB28" s="160"/>
-      <c r="FC28" s="160"/>
-      <c r="FD28" s="160"/>
-      <c r="FE28" s="160"/>
-    </row>
-    <row r="29" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB28" s="111"/>
+      <c r="FC28" s="111"/>
+      <c r="FD28" s="111"/>
+      <c r="FE28" s="111"/>
+      <c r="FF28" s="160"/>
+      <c r="FG28" s="160"/>
+      <c r="FH28" s="160"/>
+      <c r="FI28" s="160"/>
+    </row>
+    <row r="29" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="80" t="s">
         <v>339</v>
       </c>
@@ -12465,7 +12690,7 @@
       <c r="EO29" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP29" s="112"/>
+      <c r="EP29" s="70"/>
       <c r="EQ29" s="110" t="s">
         <v>362</v>
       </c>
@@ -12495,18 +12720,28 @@
       <c r="FA29" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB29" s="158"/>
-      <c r="FC29" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD29" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE29" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="30" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB29" s="112"/>
+      <c r="FC29" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD29" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE29" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF29" s="158"/>
+      <c r="FG29" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH29" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI29" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="30" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="62" t="s">
         <v>90</v>
       </c>
@@ -12671,41 +12906,49 @@
       <c r="EF30" s="111"/>
       <c r="EG30" s="111"/>
       <c r="EH30" s="111">
-        <v>5.78</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="EI30" s="111"/>
-      <c r="EJ30" s="111"/>
+      <c r="EJ30" s="111" t="s">
+        <v>737</v>
+      </c>
       <c r="EK30" s="111"/>
       <c r="EL30" s="111">
-        <v>12.58</v>
+        <v>5.78</v>
       </c>
       <c r="EM30" s="111"/>
       <c r="EN30" s="111"/>
       <c r="EO30" s="111"/>
       <c r="EP30" s="111">
-        <v>11.1</v>
+        <v>12.58</v>
       </c>
       <c r="EQ30" s="111"/>
       <c r="ER30" s="111"/>
       <c r="ES30" s="111"/>
       <c r="ET30" s="111">
-        <v>14.95</v>
+        <v>11.1</v>
       </c>
       <c r="EU30" s="111"/>
       <c r="EV30" s="111"/>
       <c r="EW30" s="111"/>
       <c r="EX30" s="111">
-        <v>1</v>
+        <v>14.95</v>
       </c>
       <c r="EY30" s="111"/>
       <c r="EZ30" s="111"/>
       <c r="FA30" s="111"/>
-      <c r="FB30" s="160"/>
-      <c r="FC30" s="160"/>
-      <c r="FD30" s="160"/>
-      <c r="FE30" s="160"/>
-    </row>
-    <row r="31" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB30" s="111">
+        <v>1</v>
+      </c>
+      <c r="FC30" s="111"/>
+      <c r="FD30" s="111"/>
+      <c r="FE30" s="111"/>
+      <c r="FF30" s="160"/>
+      <c r="FG30" s="160"/>
+      <c r="FH30" s="160"/>
+      <c r="FI30" s="160"/>
+    </row>
+    <row r="31" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="62" t="s">
         <v>113</v>
       </c>
@@ -12870,8 +13113,12 @@
       <c r="EH31" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="EI31" s="111"/>
-      <c r="EJ31" s="111"/>
+      <c r="EI31" s="111" t="s">
+        <v>739</v>
+      </c>
+      <c r="EJ31" s="111" t="s">
+        <v>741</v>
+      </c>
       <c r="EK31" s="111"/>
       <c r="EL31" s="111" t="s">
         <v>114</v>
@@ -12897,12 +13144,18 @@
       <c r="EY31" s="111"/>
       <c r="EZ31" s="111"/>
       <c r="FA31" s="111"/>
-      <c r="FB31" s="160"/>
-      <c r="FC31" s="160"/>
-      <c r="FD31" s="160"/>
-      <c r="FE31" s="160"/>
-    </row>
-    <row r="32" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB31" s="111" t="s">
+        <v>114</v>
+      </c>
+      <c r="FC31" s="111"/>
+      <c r="FD31" s="111"/>
+      <c r="FE31" s="111"/>
+      <c r="FF31" s="160"/>
+      <c r="FG31" s="160"/>
+      <c r="FH31" s="160"/>
+      <c r="FI31" s="160"/>
+    </row>
+    <row r="32" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="62" t="s">
         <v>93</v>
       </c>
@@ -13059,25 +13312,27 @@
       <c r="EF32" s="111"/>
       <c r="EG32" s="111"/>
       <c r="EH32" s="111">
-        <v>1.5640000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="EI32" s="111"/>
       <c r="EJ32" s="111"/>
-      <c r="EK32" s="111"/>
+      <c r="EK32" s="111" t="s">
+        <v>740</v>
+      </c>
       <c r="EL32" s="111">
-        <v>0.83</v>
+        <v>1.5640000000000001</v>
       </c>
       <c r="EM32" s="111"/>
       <c r="EN32" s="111"/>
       <c r="EO32" s="111"/>
       <c r="EP32" s="111">
-        <v>0.03</v>
+        <v>0.83</v>
       </c>
       <c r="EQ32" s="111"/>
       <c r="ER32" s="111"/>
       <c r="ES32" s="111"/>
       <c r="ET32" s="111">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="EU32" s="111"/>
       <c r="EV32" s="111"/>
@@ -13088,12 +13343,18 @@
       <c r="EY32" s="111"/>
       <c r="EZ32" s="111"/>
       <c r="FA32" s="111"/>
-      <c r="FB32" s="160"/>
-      <c r="FC32" s="160"/>
-      <c r="FD32" s="160"/>
-      <c r="FE32" s="160"/>
-    </row>
-    <row r="33" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB32" s="111">
+        <v>1</v>
+      </c>
+      <c r="FC32" s="111"/>
+      <c r="FD32" s="111"/>
+      <c r="FE32" s="111"/>
+      <c r="FF32" s="160"/>
+      <c r="FG32" s="160"/>
+      <c r="FH32" s="160"/>
+      <c r="FI32" s="160"/>
+    </row>
+    <row r="33" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="62" t="s">
         <v>92</v>
       </c>
@@ -13208,202 +13469,218 @@
       <c r="CZ33" s="111"/>
       <c r="DA33" s="111"/>
       <c r="DB33" s="111">
-        <f t="shared" ref="DB33:EW33" si="2">DB18</f>
+        <f t="shared" ref="DB33:FA33" si="3">DB18</f>
         <v>1</v>
       </c>
       <c r="DC33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DD33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DE33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DF33" s="111">
         <v>0.215</v>
       </c>
       <c r="DG33" s="111">
-        <f t="shared" ref="DG31:DI33" si="3">DG18</f>
+        <f t="shared" ref="DG33:DI33" si="4">DG18</f>
         <v>0.215</v>
       </c>
       <c r="DH33" s="111" t="str">
+        <f t="shared" si="4"/>
+        <v>Vanlersberghe2008Handbook</v>
+      </c>
+      <c r="DI33" s="111" t="str">
+        <f t="shared" si="4"/>
+        <v>p270</v>
+      </c>
+      <c r="DJ33" s="111">
         <f t="shared" si="3"/>
-        <v>Vanlersberghe2008Handbook</v>
-      </c>
-      <c r="DI33" s="111" t="str">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="DK33" s="111">
         <f t="shared" si="3"/>
-        <v>p270</v>
-      </c>
-      <c r="DJ33" s="111">
-        <f t="shared" si="2"/>
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="DK33" s="111">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="DL33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DM33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DN33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="DO33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DP33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DQ33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DR33" s="111"/>
       <c r="DS33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DT33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DU33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DV33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="DW33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DX33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DY33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DZ33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.65</v>
       </c>
       <c r="EA33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="EB33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="EC33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="ED33" s="111"/>
       <c r="EE33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="EF33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="EG33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="EH33" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="EH33:EK33" si="5">EH18</f>
+        <v>0.05</v>
+      </c>
+      <c r="EI33" s="111">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="EJ33" s="111">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="EK33" s="111">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="EL33" s="111">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="EI33" s="111">
-        <f t="shared" si="2"/>
+      <c r="EM33" s="111">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="EJ33" s="111">
-        <f t="shared" si="2"/>
+      <c r="EN33" s="111">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="EK33" s="111">
-        <f t="shared" si="2"/>
+      <c r="EO33" s="111">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="EL33" s="111">
-        <f t="shared" si="2"/>
+      <c r="EP33" s="111">
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="EM33" s="111">
-        <f t="shared" si="2"/>
+      <c r="EQ33" s="111">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="EN33" s="111">
-        <f t="shared" si="2"/>
+      <c r="ER33" s="111">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="EO33" s="111">
-        <f t="shared" si="2"/>
+      <c r="ES33" s="111">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="EP33" s="111">
-        <f t="shared" si="2"/>
+      <c r="ET33" s="111">
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
-      <c r="EQ33" s="111">
-        <f t="shared" si="2"/>
+      <c r="EU33" s="111">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="ER33" s="111">
-        <f t="shared" si="2"/>
+      <c r="EV33" s="111">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="ES33" s="111">
-        <f t="shared" si="2"/>
+      <c r="EW33" s="111">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="ET33" s="111">
-        <f t="shared" si="2"/>
+      <c r="EX33" s="111">
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="EU33" s="111">
-        <f t="shared" si="2"/>
+      <c r="EY33" s="111">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="EV33" s="111">
-        <f t="shared" si="2"/>
+      <c r="EZ33" s="111">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="EW33" s="111">
-        <f t="shared" si="2"/>
+      <c r="FA33" s="111">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="EX33" s="111">
+      <c r="FB33" s="111">
         <v>0.8</v>
       </c>
-      <c r="EY33" s="111"/>
-      <c r="EZ33" s="111"/>
-      <c r="FA33" s="111"/>
-      <c r="FB33" s="160"/>
-      <c r="FC33" s="160"/>
-      <c r="FD33" s="160"/>
-      <c r="FE33" s="160"/>
-    </row>
-    <row r="34" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FC33" s="111"/>
+      <c r="FD33" s="111"/>
+      <c r="FE33" s="111"/>
+      <c r="FF33" s="160"/>
+      <c r="FG33" s="160"/>
+      <c r="FH33" s="160"/>
+      <c r="FI33" s="160"/>
+    </row>
+    <row r="34" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="62" t="s">
         <v>89</v>
       </c>
@@ -13560,41 +13837,47 @@
       <c r="EF34" s="111"/>
       <c r="EG34" s="111"/>
       <c r="EH34" s="111" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="EI34" s="111"/>
       <c r="EJ34" s="111"/>
       <c r="EK34" s="111"/>
       <c r="EL34" s="111" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="EM34" s="111"/>
       <c r="EN34" s="111"/>
       <c r="EO34" s="111"/>
       <c r="EP34" s="111" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="EQ34" s="111"/>
       <c r="ER34" s="111"/>
       <c r="ES34" s="111"/>
       <c r="ET34" s="111" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="EU34" s="111"/>
       <c r="EV34" s="111"/>
       <c r="EW34" s="111"/>
       <c r="EX34" s="111" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="EY34" s="111"/>
       <c r="EZ34" s="111"/>
       <c r="FA34" s="111"/>
-      <c r="FB34" s="160"/>
-      <c r="FC34" s="160"/>
-      <c r="FD34" s="160"/>
-      <c r="FE34" s="160"/>
-    </row>
-    <row r="35" spans="1:161" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB34" s="111" t="s">
+        <v>116</v>
+      </c>
+      <c r="FC34" s="111"/>
+      <c r="FD34" s="111"/>
+      <c r="FE34" s="111"/>
+      <c r="FF34" s="160"/>
+      <c r="FG34" s="160"/>
+      <c r="FH34" s="160"/>
+      <c r="FI34" s="160"/>
+    </row>
+    <row r="35" spans="1:165" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="62" t="s">
         <v>91</v>
       </c>
@@ -13759,41 +14042,49 @@
       <c r="EF35" s="111"/>
       <c r="EG35" s="111"/>
       <c r="EH35" s="111">
-        <v>1.5640000000000001</v>
+        <v>-0.31</v>
       </c>
       <c r="EI35" s="111"/>
-      <c r="EJ35" s="111"/>
+      <c r="EJ35" s="111" t="s">
+        <v>737</v>
+      </c>
       <c r="EK35" s="111"/>
       <c r="EL35" s="111">
-        <v>1.46</v>
+        <v>1.5640000000000001</v>
       </c>
       <c r="EM35" s="111"/>
       <c r="EN35" s="111"/>
       <c r="EO35" s="111"/>
       <c r="EP35" s="111">
-        <v>3.79</v>
+        <v>1.46</v>
       </c>
       <c r="EQ35" s="111"/>
       <c r="ER35" s="111"/>
       <c r="ES35" s="111"/>
       <c r="ET35" s="111">
-        <v>2.77</v>
+        <v>3.79</v>
       </c>
       <c r="EU35" s="111"/>
       <c r="EV35" s="111"/>
       <c r="EW35" s="111"/>
       <c r="EX35" s="111">
-        <v>-1.5</v>
+        <v>2.77</v>
       </c>
       <c r="EY35" s="111"/>
       <c r="EZ35" s="111"/>
       <c r="FA35" s="111"/>
-      <c r="FB35" s="160"/>
-      <c r="FC35" s="160"/>
-      <c r="FD35" s="160"/>
-      <c r="FE35" s="160"/>
-    </row>
-    <row r="36" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB35" s="111">
+        <v>-1.5</v>
+      </c>
+      <c r="FC35" s="111"/>
+      <c r="FD35" s="111"/>
+      <c r="FE35" s="111"/>
+      <c r="FF35" s="160"/>
+      <c r="FG35" s="160"/>
+      <c r="FH35" s="160"/>
+      <c r="FI35" s="160"/>
+    </row>
+    <row r="36" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="80" t="s">
         <v>340</v>
       </c>
@@ -14159,7 +14450,7 @@
       <c r="EO36" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP36" s="112"/>
+      <c r="EP36" s="70"/>
       <c r="EQ36" s="110" t="s">
         <v>362</v>
       </c>
@@ -14189,18 +14480,28 @@
       <c r="FA36" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB36" s="158"/>
-      <c r="FC36" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD36" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE36" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="37" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB36" s="112"/>
+      <c r="FC36" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD36" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE36" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF36" s="158"/>
+      <c r="FG36" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH36" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI36" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="37" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="64" t="s">
         <v>323</v>
       </c>
@@ -14402,12 +14703,18 @@
       <c r="EY37" s="115"/>
       <c r="EZ37" s="115"/>
       <c r="FA37" s="115"/>
-      <c r="FB37" s="161"/>
-      <c r="FC37" s="161"/>
-      <c r="FD37" s="161"/>
-      <c r="FE37" s="161"/>
-    </row>
-    <row r="38" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB37" s="115">
+        <v>0</v>
+      </c>
+      <c r="FC37" s="115"/>
+      <c r="FD37" s="115"/>
+      <c r="FE37" s="115"/>
+      <c r="FF37" s="161"/>
+      <c r="FG37" s="161"/>
+      <c r="FH37" s="161"/>
+      <c r="FI37" s="161"/>
+    </row>
+    <row r="38" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="64" t="s">
         <v>324</v>
       </c>
@@ -14572,41 +14879,47 @@
       <c r="EF38" s="115"/>
       <c r="EG38" s="115"/>
       <c r="EH38" s="115">
-        <v>0.15</v>
+        <v>0.35</v>
       </c>
       <c r="EI38" s="115"/>
       <c r="EJ38" s="115"/>
       <c r="EK38" s="115"/>
       <c r="EL38" s="115">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="EM38" s="115"/>
       <c r="EN38" s="115"/>
       <c r="EO38" s="115"/>
       <c r="EP38" s="115">
-        <v>-0.35</v>
+        <v>0</v>
       </c>
       <c r="EQ38" s="115"/>
       <c r="ER38" s="115"/>
       <c r="ES38" s="115"/>
       <c r="ET38" s="115">
-        <v>0</v>
+        <v>-0.35</v>
       </c>
       <c r="EU38" s="115"/>
       <c r="EV38" s="115"/>
       <c r="EW38" s="115"/>
       <c r="EX38" s="115">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="EY38" s="115"/>
       <c r="EZ38" s="115"/>
       <c r="FA38" s="115"/>
-      <c r="FB38" s="161"/>
-      <c r="FC38" s="161"/>
-      <c r="FD38" s="161"/>
-      <c r="FE38" s="161"/>
-    </row>
-    <row r="39" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB38" s="115">
+        <v>-0.1</v>
+      </c>
+      <c r="FC38" s="115"/>
+      <c r="FD38" s="115"/>
+      <c r="FE38" s="115"/>
+      <c r="FF38" s="161"/>
+      <c r="FG38" s="161"/>
+      <c r="FH38" s="161"/>
+      <c r="FI38" s="161"/>
+    </row>
+    <row r="39" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="64" t="s">
         <v>325</v>
       </c>
@@ -14769,41 +15082,47 @@
       <c r="EF39" s="115"/>
       <c r="EG39" s="115"/>
       <c r="EH39" s="115" t="s">
-        <v>388</v>
+        <v>745</v>
       </c>
       <c r="EI39" s="115"/>
       <c r="EJ39" s="115"/>
       <c r="EK39" s="115"/>
       <c r="EL39" s="115" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="EM39" s="115"/>
       <c r="EN39" s="115"/>
       <c r="EO39" s="115"/>
       <c r="EP39" s="115" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="EQ39" s="115"/>
       <c r="ER39" s="115"/>
       <c r="ES39" s="115"/>
       <c r="ET39" s="115" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="EU39" s="115"/>
       <c r="EV39" s="115"/>
       <c r="EW39" s="115"/>
       <c r="EX39" s="115" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="EY39" s="115"/>
       <c r="EZ39" s="115"/>
       <c r="FA39" s="115"/>
-      <c r="FB39" s="161"/>
-      <c r="FC39" s="161"/>
-      <c r="FD39" s="161"/>
-      <c r="FE39" s="161"/>
-    </row>
-    <row r="40" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB39" s="115" t="s">
+        <v>392</v>
+      </c>
+      <c r="FC39" s="115"/>
+      <c r="FD39" s="115"/>
+      <c r="FE39" s="115"/>
+      <c r="FF39" s="161"/>
+      <c r="FG39" s="161"/>
+      <c r="FH39" s="161"/>
+      <c r="FI39" s="161"/>
+    </row>
+    <row r="40" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="64" t="s">
         <v>641</v>
       </c>
@@ -14995,12 +15314,18 @@
       <c r="EY40" s="115"/>
       <c r="EZ40" s="115"/>
       <c r="FA40" s="115"/>
-      <c r="FB40" s="161"/>
-      <c r="FC40" s="161"/>
-      <c r="FD40" s="161"/>
-      <c r="FE40" s="161"/>
-    </row>
-    <row r="41" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB40" s="115">
+        <v>1</v>
+      </c>
+      <c r="FC40" s="115"/>
+      <c r="FD40" s="115"/>
+      <c r="FE40" s="115"/>
+      <c r="FF40" s="161"/>
+      <c r="FG40" s="161"/>
+      <c r="FH40" s="161"/>
+      <c r="FI40" s="161"/>
+    </row>
+    <row r="41" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="64" t="s">
         <v>3</v>
       </c>
@@ -15165,13 +15490,13 @@
       <c r="EF41" s="115"/>
       <c r="EG41" s="115"/>
       <c r="EH41" s="115">
-        <v>0.45</v>
+        <v>-0.2</v>
       </c>
       <c r="EI41" s="115"/>
       <c r="EJ41" s="115"/>
       <c r="EK41" s="115"/>
       <c r="EL41" s="115">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="EM41" s="115"/>
       <c r="EN41" s="115"/>
@@ -15189,17 +15514,23 @@
       <c r="EV41" s="115"/>
       <c r="EW41" s="115"/>
       <c r="EX41" s="115">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="EY41" s="115"/>
       <c r="EZ41" s="115"/>
       <c r="FA41" s="115"/>
-      <c r="FB41" s="161"/>
-      <c r="FC41" s="161"/>
-      <c r="FD41" s="161"/>
-      <c r="FE41" s="161"/>
-    </row>
-    <row r="42" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB41" s="115">
+        <v>-0.1</v>
+      </c>
+      <c r="FC41" s="115"/>
+      <c r="FD41" s="115"/>
+      <c r="FE41" s="115"/>
+      <c r="FF41" s="161"/>
+      <c r="FG41" s="161"/>
+      <c r="FH41" s="161"/>
+      <c r="FI41" s="161"/>
+    </row>
+    <row r="42" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="64" t="s">
         <v>326</v>
       </c>
@@ -15380,7 +15711,7 @@
       <c r="ER42" s="115"/>
       <c r="ES42" s="115"/>
       <c r="ET42" s="115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EU42" s="115"/>
       <c r="EV42" s="115"/>
@@ -15391,12 +15722,18 @@
       <c r="EY42" s="115"/>
       <c r="EZ42" s="115"/>
       <c r="FA42" s="115"/>
-      <c r="FB42" s="161"/>
-      <c r="FC42" s="161"/>
-      <c r="FD42" s="161"/>
-      <c r="FE42" s="161"/>
-    </row>
-    <row r="43" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB42" s="115">
+        <v>1</v>
+      </c>
+      <c r="FC42" s="115"/>
+      <c r="FD42" s="115"/>
+      <c r="FE42" s="115"/>
+      <c r="FF42" s="161"/>
+      <c r="FG42" s="161"/>
+      <c r="FH42" s="161"/>
+      <c r="FI42" s="161"/>
+    </row>
+    <row r="43" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="64" t="s">
         <v>640</v>
       </c>
@@ -15595,19 +15932,17 @@
       <c r="EN43" s="115"/>
       <c r="EO43" s="115"/>
       <c r="EP43" s="115">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="EQ43" s="115"/>
-      <c r="ER43" s="115" t="s">
-        <v>652</v>
-      </c>
+      <c r="ER43" s="115"/>
       <c r="ES43" s="115"/>
       <c r="ET43" s="115">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="EU43" s="115"/>
       <c r="EV43" s="115" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="EW43" s="115"/>
       <c r="EX43" s="115">
@@ -15618,12 +15953,20 @@
         <v>650</v>
       </c>
       <c r="FA43" s="115"/>
-      <c r="FB43" s="161"/>
-      <c r="FC43" s="161"/>
-      <c r="FD43" s="161"/>
-      <c r="FE43" s="161"/>
-    </row>
-    <row r="44" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB43" s="115">
+        <v>0</v>
+      </c>
+      <c r="FC43" s="115"/>
+      <c r="FD43" s="115" t="s">
+        <v>650</v>
+      </c>
+      <c r="FE43" s="115"/>
+      <c r="FF43" s="161"/>
+      <c r="FG43" s="161"/>
+      <c r="FH43" s="161"/>
+      <c r="FI43" s="161"/>
+    </row>
+    <row r="44" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="64" t="s">
         <v>639</v>
       </c>
@@ -15841,12 +16184,18 @@
       <c r="EY44" s="115"/>
       <c r="EZ44" s="115"/>
       <c r="FA44" s="115"/>
-      <c r="FB44" s="161"/>
-      <c r="FC44" s="161"/>
-      <c r="FD44" s="161"/>
-      <c r="FE44" s="161"/>
-    </row>
-    <row r="45" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB44" s="115">
+        <v>0</v>
+      </c>
+      <c r="FC44" s="115"/>
+      <c r="FD44" s="115"/>
+      <c r="FE44" s="115"/>
+      <c r="FF44" s="161"/>
+      <c r="FG44" s="161"/>
+      <c r="FH44" s="161"/>
+      <c r="FI44" s="161"/>
+    </row>
+    <row r="45" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="64" t="s">
         <v>4</v>
       </c>
@@ -16011,25 +16360,25 @@
       <c r="EF45" s="115"/>
       <c r="EG45" s="115"/>
       <c r="EH45" s="115">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="EI45" s="115"/>
       <c r="EJ45" s="115"/>
       <c r="EK45" s="115"/>
       <c r="EL45" s="115">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EM45" s="115"/>
       <c r="EN45" s="115"/>
       <c r="EO45" s="115"/>
       <c r="EP45" s="115">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EQ45" s="115"/>
       <c r="ER45" s="115"/>
       <c r="ES45" s="115"/>
       <c r="ET45" s="115">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="EU45" s="115"/>
       <c r="EV45" s="115"/>
@@ -16040,12 +16389,18 @@
       <c r="EY45" s="115"/>
       <c r="EZ45" s="115"/>
       <c r="FA45" s="115"/>
-      <c r="FB45" s="161"/>
-      <c r="FC45" s="161"/>
-      <c r="FD45" s="161"/>
-      <c r="FE45" s="161"/>
-    </row>
-    <row r="46" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB45" s="115">
+        <v>0</v>
+      </c>
+      <c r="FC45" s="115"/>
+      <c r="FD45" s="115"/>
+      <c r="FE45" s="115"/>
+      <c r="FF45" s="161"/>
+      <c r="FG45" s="161"/>
+      <c r="FH45" s="161"/>
+      <c r="FI45" s="161"/>
+    </row>
+    <row r="46" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="64" t="s">
         <v>327</v>
       </c>
@@ -16220,13 +16575,13 @@
       <c r="EN46" s="115"/>
       <c r="EO46" s="115"/>
       <c r="EP46" s="115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EQ46" s="115"/>
       <c r="ER46" s="115"/>
       <c r="ES46" s="115"/>
       <c r="ET46" s="115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EU46" s="115"/>
       <c r="EV46" s="115"/>
@@ -16237,12 +16592,18 @@
       <c r="EY46" s="115"/>
       <c r="EZ46" s="115"/>
       <c r="FA46" s="115"/>
-      <c r="FB46" s="161"/>
-      <c r="FC46" s="161"/>
-      <c r="FD46" s="161"/>
-      <c r="FE46" s="161"/>
-    </row>
-    <row r="47" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB46" s="115">
+        <v>0</v>
+      </c>
+      <c r="FC46" s="115"/>
+      <c r="FD46" s="115"/>
+      <c r="FE46" s="115"/>
+      <c r="FF46" s="161"/>
+      <c r="FG46" s="161"/>
+      <c r="FH46" s="161"/>
+      <c r="FI46" s="161"/>
+    </row>
+    <row r="47" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="64" t="s">
         <v>328</v>
       </c>
@@ -16407,41 +16768,47 @@
       <c r="EF47" s="115"/>
       <c r="EG47" s="115"/>
       <c r="EH47" s="115">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="EI47" s="115"/>
       <c r="EJ47" s="115"/>
       <c r="EK47" s="115"/>
       <c r="EL47" s="115">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="EM47" s="115"/>
       <c r="EN47" s="115"/>
       <c r="EO47" s="115"/>
       <c r="EP47" s="115">
-        <v>-0.35</v>
+        <v>0</v>
       </c>
       <c r="EQ47" s="115"/>
       <c r="ER47" s="115"/>
       <c r="ES47" s="115"/>
       <c r="ET47" s="115">
-        <v>0</v>
+        <v>-0.35</v>
       </c>
       <c r="EU47" s="115"/>
       <c r="EV47" s="115"/>
       <c r="EW47" s="115"/>
       <c r="EX47" s="115">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="EY47" s="115"/>
       <c r="EZ47" s="115"/>
       <c r="FA47" s="115"/>
-      <c r="FB47" s="161"/>
-      <c r="FC47" s="161"/>
-      <c r="FD47" s="161"/>
-      <c r="FE47" s="161"/>
-    </row>
-    <row r="48" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB47" s="115">
+        <v>-0.1</v>
+      </c>
+      <c r="FC47" s="115"/>
+      <c r="FD47" s="115"/>
+      <c r="FE47" s="115"/>
+      <c r="FF47" s="161"/>
+      <c r="FG47" s="161"/>
+      <c r="FH47" s="161"/>
+      <c r="FI47" s="161"/>
+    </row>
+    <row r="48" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="64" t="s">
         <v>329</v>
       </c>
@@ -16616,13 +16983,13 @@
       <c r="EN48" s="115"/>
       <c r="EO48" s="115"/>
       <c r="EP48" s="115">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="EQ48" s="115"/>
       <c r="ER48" s="115"/>
       <c r="ES48" s="115"/>
       <c r="ET48" s="115">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="EU48" s="115"/>
       <c r="EV48" s="115"/>
@@ -16633,12 +17000,18 @@
       <c r="EY48" s="115"/>
       <c r="EZ48" s="115"/>
       <c r="FA48" s="115"/>
-      <c r="FB48" s="161"/>
-      <c r="FC48" s="161"/>
-      <c r="FD48" s="161"/>
-      <c r="FE48" s="161"/>
-    </row>
-    <row r="49" spans="1:161" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB48" s="115">
+        <v>0</v>
+      </c>
+      <c r="FC48" s="115"/>
+      <c r="FD48" s="115"/>
+      <c r="FE48" s="115"/>
+      <c r="FF48" s="161"/>
+      <c r="FG48" s="161"/>
+      <c r="FH48" s="161"/>
+      <c r="FI48" s="161"/>
+    </row>
+    <row r="49" spans="1:165" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="64" t="s">
         <v>637</v>
       </c>
@@ -16830,12 +17203,18 @@
       <c r="EY49" s="115"/>
       <c r="EZ49" s="115"/>
       <c r="FA49" s="115"/>
-      <c r="FB49" s="161"/>
-      <c r="FC49" s="161"/>
-      <c r="FD49" s="161"/>
-      <c r="FE49" s="161"/>
-    </row>
-    <row r="50" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB49" s="115">
+        <v>0</v>
+      </c>
+      <c r="FC49" s="115"/>
+      <c r="FD49" s="115"/>
+      <c r="FE49" s="115"/>
+      <c r="FF49" s="161"/>
+      <c r="FG49" s="161"/>
+      <c r="FH49" s="161"/>
+      <c r="FI49" s="161"/>
+    </row>
+    <row r="50" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="63" t="s">
         <v>608</v>
       </c>
@@ -17199,7 +17578,7 @@
       <c r="EO50" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP50" s="112"/>
+      <c r="EP50" s="70"/>
       <c r="EQ50" s="110" t="s">
         <v>362</v>
       </c>
@@ -17229,18 +17608,28 @@
       <c r="FA50" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB50" s="158"/>
-      <c r="FC50" s="158" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD50" s="158" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE50" s="158" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="51" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB50" s="112"/>
+      <c r="FC50" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD50" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE50" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF50" s="158"/>
+      <c r="FG50" s="158" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH50" s="158" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI50" s="158" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="51" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="65" t="s">
         <v>115</v>
       </c>
@@ -17394,7 +17783,7 @@
       <c r="EM51" s="113"/>
       <c r="EN51" s="113"/>
       <c r="EO51" s="113"/>
-      <c r="EP51" s="113"/>
+      <c r="EP51" s="71"/>
       <c r="EQ51" s="113"/>
       <c r="ER51" s="113"/>
       <c r="ES51" s="113"/>
@@ -17406,12 +17795,16 @@
       <c r="EY51" s="113"/>
       <c r="EZ51" s="113"/>
       <c r="FA51" s="113"/>
-      <c r="FB51" s="163"/>
-      <c r="FC51" s="163"/>
-      <c r="FD51" s="163"/>
-      <c r="FE51" s="163"/>
-    </row>
-    <row r="52" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB51" s="113"/>
+      <c r="FC51" s="113"/>
+      <c r="FD51" s="113"/>
+      <c r="FE51" s="113"/>
+      <c r="FF51" s="163"/>
+      <c r="FG51" s="163"/>
+      <c r="FH51" s="163"/>
+      <c r="FI51" s="163"/>
+    </row>
+    <row r="52" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="63" t="s">
         <v>605</v>
       </c>
@@ -17775,7 +18168,7 @@
       <c r="EO52" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP52" s="112"/>
+      <c r="EP52" s="70"/>
       <c r="EQ52" s="110" t="s">
         <v>362</v>
       </c>
@@ -17805,18 +18198,28 @@
       <c r="FA52" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB52" s="158"/>
-      <c r="FC52" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD52" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE52" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="53" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB52" s="112"/>
+      <c r="FC52" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD52" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE52" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF52" s="158"/>
+      <c r="FG52" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH52" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI52" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="53" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="65" t="s">
         <v>115</v>
       </c>
@@ -17970,7 +18373,7 @@
       <c r="EM53" s="113"/>
       <c r="EN53" s="113"/>
       <c r="EO53" s="113"/>
-      <c r="EP53" s="113"/>
+      <c r="EP53" s="71"/>
       <c r="EQ53" s="113"/>
       <c r="ER53" s="113"/>
       <c r="ES53" s="113"/>
@@ -17982,12 +18385,16 @@
       <c r="EY53" s="113"/>
       <c r="EZ53" s="113"/>
       <c r="FA53" s="113"/>
-      <c r="FB53" s="163"/>
-      <c r="FC53" s="163"/>
-      <c r="FD53" s="163"/>
-      <c r="FE53" s="163"/>
-    </row>
-    <row r="54" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB53" s="113"/>
+      <c r="FC53" s="113"/>
+      <c r="FD53" s="113"/>
+      <c r="FE53" s="113"/>
+      <c r="FF53" s="163"/>
+      <c r="FG53" s="163"/>
+      <c r="FH53" s="163"/>
+      <c r="FI53" s="163"/>
+    </row>
+    <row r="54" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="63" t="s">
         <v>604</v>
       </c>
@@ -18351,7 +18758,7 @@
       <c r="EO54" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP54" s="112"/>
+      <c r="EP54" s="70"/>
       <c r="EQ54" s="110" t="s">
         <v>362</v>
       </c>
@@ -18381,18 +18788,28 @@
       <c r="FA54" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB54" s="158"/>
-      <c r="FC54" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD54" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE54" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="55" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB54" s="112"/>
+      <c r="FC54" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD54" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE54" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF54" s="158"/>
+      <c r="FG54" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH54" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI54" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="55" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="65" t="s">
         <v>115</v>
       </c>
@@ -18546,7 +18963,7 @@
       <c r="EM55" s="113"/>
       <c r="EN55" s="113"/>
       <c r="EO55" s="113"/>
-      <c r="EP55" s="113"/>
+      <c r="EP55" s="71"/>
       <c r="EQ55" s="113"/>
       <c r="ER55" s="113"/>
       <c r="ES55" s="113"/>
@@ -18558,12 +18975,16 @@
       <c r="EY55" s="113"/>
       <c r="EZ55" s="113"/>
       <c r="FA55" s="113"/>
-      <c r="FB55" s="163"/>
-      <c r="FC55" s="163"/>
-      <c r="FD55" s="163"/>
-      <c r="FE55" s="163"/>
-    </row>
-    <row r="56" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB55" s="113"/>
+      <c r="FC55" s="113"/>
+      <c r="FD55" s="113"/>
+      <c r="FE55" s="113"/>
+      <c r="FF55" s="163"/>
+      <c r="FG55" s="163"/>
+      <c r="FH55" s="163"/>
+      <c r="FI55" s="163"/>
+    </row>
+    <row r="56" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="63" t="s">
         <v>609</v>
       </c>
@@ -18927,7 +19348,7 @@
       <c r="EO56" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP56" s="112"/>
+      <c r="EP56" s="70"/>
       <c r="EQ56" s="110" t="s">
         <v>362</v>
       </c>
@@ -18957,18 +19378,28 @@
       <c r="FA56" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB56" s="158"/>
-      <c r="FC56" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD56" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE56" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="57" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB56" s="112"/>
+      <c r="FC56" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD56" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE56" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF56" s="158"/>
+      <c r="FG56" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH56" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI56" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="57" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="65" t="s">
         <v>115</v>
       </c>
@@ -19122,7 +19553,7 @@
       <c r="EM57" s="113"/>
       <c r="EN57" s="113"/>
       <c r="EO57" s="113"/>
-      <c r="EP57" s="113"/>
+      <c r="EP57" s="71"/>
       <c r="EQ57" s="113"/>
       <c r="ER57" s="113"/>
       <c r="ES57" s="113"/>
@@ -19134,12 +19565,16 @@
       <c r="EY57" s="113"/>
       <c r="EZ57" s="113"/>
       <c r="FA57" s="113"/>
-      <c r="FB57" s="163"/>
-      <c r="FC57" s="163"/>
-      <c r="FD57" s="163"/>
-      <c r="FE57" s="163"/>
-    </row>
-    <row r="58" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB57" s="113"/>
+      <c r="FC57" s="113"/>
+      <c r="FD57" s="113"/>
+      <c r="FE57" s="113"/>
+      <c r="FF57" s="163"/>
+      <c r="FG57" s="163"/>
+      <c r="FH57" s="163"/>
+      <c r="FI57" s="163"/>
+    </row>
+    <row r="58" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="63" t="s">
         <v>614</v>
       </c>
@@ -19503,7 +19938,7 @@
       <c r="EO58" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP58" s="112"/>
+      <c r="EP58" s="70"/>
       <c r="EQ58" s="110" t="s">
         <v>362</v>
       </c>
@@ -19533,18 +19968,28 @@
       <c r="FA58" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB58" s="158"/>
-      <c r="FC58" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD58" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE58" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="59" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB58" s="112"/>
+      <c r="FC58" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD58" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE58" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF58" s="158"/>
+      <c r="FG58" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH58" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI58" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="59" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="65" t="s">
         <v>115</v>
       </c>
@@ -19698,7 +20143,7 @@
       <c r="EM59" s="113"/>
       <c r="EN59" s="113"/>
       <c r="EO59" s="113"/>
-      <c r="EP59" s="113"/>
+      <c r="EP59" s="71"/>
       <c r="EQ59" s="113"/>
       <c r="ER59" s="113"/>
       <c r="ES59" s="113"/>
@@ -19710,12 +20155,16 @@
       <c r="EY59" s="113"/>
       <c r="EZ59" s="113"/>
       <c r="FA59" s="113"/>
-      <c r="FB59" s="163"/>
-      <c r="FC59" s="163"/>
-      <c r="FD59" s="163"/>
-      <c r="FE59" s="163"/>
-    </row>
-    <row r="60" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB59" s="113"/>
+      <c r="FC59" s="113"/>
+      <c r="FD59" s="113"/>
+      <c r="FE59" s="113"/>
+      <c r="FF59" s="163"/>
+      <c r="FG59" s="163"/>
+      <c r="FH59" s="163"/>
+      <c r="FI59" s="163"/>
+    </row>
+    <row r="60" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="63" t="s">
         <v>615</v>
       </c>
@@ -20079,7 +20528,7 @@
       <c r="EO60" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP60" s="112"/>
+      <c r="EP60" s="70"/>
       <c r="EQ60" s="110" t="s">
         <v>362</v>
       </c>
@@ -20109,18 +20558,28 @@
       <c r="FA60" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB60" s="158"/>
-      <c r="FC60" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD60" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE60" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="61" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB60" s="112"/>
+      <c r="FC60" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD60" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE60" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF60" s="158"/>
+      <c r="FG60" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH60" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI60" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="61" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="65" t="s">
         <v>115</v>
       </c>
@@ -20274,7 +20733,7 @@
       <c r="EM61" s="113"/>
       <c r="EN61" s="113"/>
       <c r="EO61" s="113"/>
-      <c r="EP61" s="113"/>
+      <c r="EP61" s="71"/>
       <c r="EQ61" s="113"/>
       <c r="ER61" s="113"/>
       <c r="ES61" s="113"/>
@@ -20286,12 +20745,16 @@
       <c r="EY61" s="113"/>
       <c r="EZ61" s="113"/>
       <c r="FA61" s="113"/>
-      <c r="FB61" s="163"/>
-      <c r="FC61" s="163"/>
-      <c r="FD61" s="163"/>
-      <c r="FE61" s="163"/>
-    </row>
-    <row r="62" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB61" s="113"/>
+      <c r="FC61" s="113"/>
+      <c r="FD61" s="113"/>
+      <c r="FE61" s="113"/>
+      <c r="FF61" s="163"/>
+      <c r="FG61" s="163"/>
+      <c r="FH61" s="163"/>
+      <c r="FI61" s="163"/>
+    </row>
+    <row r="62" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="63" t="s">
         <v>611</v>
       </c>
@@ -20655,7 +21118,7 @@
       <c r="EO62" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP62" s="112"/>
+      <c r="EP62" s="70"/>
       <c r="EQ62" s="110" t="s">
         <v>362</v>
       </c>
@@ -20685,18 +21148,28 @@
       <c r="FA62" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB62" s="158"/>
-      <c r="FC62" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD62" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE62" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="63" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB62" s="112"/>
+      <c r="FC62" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD62" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE62" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF62" s="158"/>
+      <c r="FG62" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH62" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI62" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="63" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="65" t="s">
         <v>115</v>
       </c>
@@ -20850,7 +21323,7 @@
       <c r="EM63" s="113"/>
       <c r="EN63" s="113"/>
       <c r="EO63" s="113"/>
-      <c r="EP63" s="113"/>
+      <c r="EP63" s="71"/>
       <c r="EQ63" s="113"/>
       <c r="ER63" s="113"/>
       <c r="ES63" s="113"/>
@@ -20862,12 +21335,16 @@
       <c r="EY63" s="113"/>
       <c r="EZ63" s="113"/>
       <c r="FA63" s="113"/>
-      <c r="FB63" s="163"/>
-      <c r="FC63" s="163"/>
-      <c r="FD63" s="163"/>
-      <c r="FE63" s="163"/>
-    </row>
-    <row r="64" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB63" s="113"/>
+      <c r="FC63" s="113"/>
+      <c r="FD63" s="113"/>
+      <c r="FE63" s="113"/>
+      <c r="FF63" s="163"/>
+      <c r="FG63" s="163"/>
+      <c r="FH63" s="163"/>
+      <c r="FI63" s="163"/>
+    </row>
+    <row r="64" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="63" t="s">
         <v>606</v>
       </c>
@@ -21231,7 +21708,7 @@
       <c r="EO64" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP64" s="112"/>
+      <c r="EP64" s="70"/>
       <c r="EQ64" s="110" t="s">
         <v>362</v>
       </c>
@@ -21261,18 +21738,28 @@
       <c r="FA64" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB64" s="158"/>
-      <c r="FC64" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD64" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE64" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="65" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB64" s="112"/>
+      <c r="FC64" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD64" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE64" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF64" s="158"/>
+      <c r="FG64" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH64" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI64" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="65" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="65" t="s">
         <v>115</v>
       </c>
@@ -21426,7 +21913,7 @@
       <c r="EM65" s="113"/>
       <c r="EN65" s="113"/>
       <c r="EO65" s="113"/>
-      <c r="EP65" s="113"/>
+      <c r="EP65" s="71"/>
       <c r="EQ65" s="113"/>
       <c r="ER65" s="113"/>
       <c r="ES65" s="113"/>
@@ -21438,12 +21925,16 @@
       <c r="EY65" s="113"/>
       <c r="EZ65" s="113"/>
       <c r="FA65" s="113"/>
-      <c r="FB65" s="163"/>
-      <c r="FC65" s="163"/>
-      <c r="FD65" s="163"/>
-      <c r="FE65" s="163"/>
-    </row>
-    <row r="66" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB65" s="113"/>
+      <c r="FC65" s="113"/>
+      <c r="FD65" s="113"/>
+      <c r="FE65" s="113"/>
+      <c r="FF65" s="163"/>
+      <c r="FG65" s="163"/>
+      <c r="FH65" s="163"/>
+      <c r="FI65" s="163"/>
+    </row>
+    <row r="66" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="63" t="s">
         <v>603</v>
       </c>
@@ -21807,7 +22298,7 @@
       <c r="EO66" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP66" s="112"/>
+      <c r="EP66" s="70"/>
       <c r="EQ66" s="110" t="s">
         <v>362</v>
       </c>
@@ -21837,18 +22328,28 @@
       <c r="FA66" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB66" s="158"/>
-      <c r="FC66" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD66" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE66" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="67" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB66" s="112"/>
+      <c r="FC66" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD66" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE66" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF66" s="158"/>
+      <c r="FG66" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH66" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI66" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="67" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="65" t="s">
         <v>115</v>
       </c>
@@ -22002,7 +22503,7 @@
       <c r="EM67" s="113"/>
       <c r="EN67" s="113"/>
       <c r="EO67" s="113"/>
-      <c r="EP67" s="113"/>
+      <c r="EP67" s="71"/>
       <c r="EQ67" s="113"/>
       <c r="ER67" s="113"/>
       <c r="ES67" s="113"/>
@@ -22014,12 +22515,16 @@
       <c r="EY67" s="113"/>
       <c r="EZ67" s="113"/>
       <c r="FA67" s="113"/>
-      <c r="FB67" s="163"/>
-      <c r="FC67" s="163"/>
-      <c r="FD67" s="163"/>
-      <c r="FE67" s="163"/>
-    </row>
-    <row r="68" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB67" s="113"/>
+      <c r="FC67" s="113"/>
+      <c r="FD67" s="113"/>
+      <c r="FE67" s="113"/>
+      <c r="FF67" s="163"/>
+      <c r="FG67" s="163"/>
+      <c r="FH67" s="163"/>
+      <c r="FI67" s="163"/>
+    </row>
+    <row r="68" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="63" t="s">
         <v>612</v>
       </c>
@@ -22383,7 +22888,7 @@
       <c r="EO68" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP68" s="112"/>
+      <c r="EP68" s="70"/>
       <c r="EQ68" s="110" t="s">
         <v>362</v>
       </c>
@@ -22413,18 +22918,28 @@
       <c r="FA68" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB68" s="158"/>
-      <c r="FC68" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD68" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE68" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="69" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB68" s="112"/>
+      <c r="FC68" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD68" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE68" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF68" s="158"/>
+      <c r="FG68" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH68" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI68" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="69" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="65" t="s">
         <v>115</v>
       </c>
@@ -22578,7 +23093,7 @@
       <c r="EM69" s="113"/>
       <c r="EN69" s="113"/>
       <c r="EO69" s="113"/>
-      <c r="EP69" s="113"/>
+      <c r="EP69" s="71"/>
       <c r="EQ69" s="113"/>
       <c r="ER69" s="113"/>
       <c r="ES69" s="113"/>
@@ -22590,12 +23105,16 @@
       <c r="EY69" s="113"/>
       <c r="EZ69" s="113"/>
       <c r="FA69" s="113"/>
-      <c r="FB69" s="163"/>
-      <c r="FC69" s="163"/>
-      <c r="FD69" s="163"/>
-      <c r="FE69" s="163"/>
-    </row>
-    <row r="70" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB69" s="113"/>
+      <c r="FC69" s="113"/>
+      <c r="FD69" s="113"/>
+      <c r="FE69" s="113"/>
+      <c r="FF69" s="163"/>
+      <c r="FG69" s="163"/>
+      <c r="FH69" s="163"/>
+      <c r="FI69" s="163"/>
+    </row>
+    <row r="70" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="63" t="s">
         <v>613</v>
       </c>
@@ -22959,7 +23478,7 @@
       <c r="EO70" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP70" s="112"/>
+      <c r="EP70" s="70"/>
       <c r="EQ70" s="110" t="s">
         <v>362</v>
       </c>
@@ -22989,18 +23508,28 @@
       <c r="FA70" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB70" s="158"/>
-      <c r="FC70" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD70" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE70" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="71" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB70" s="112"/>
+      <c r="FC70" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD70" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE70" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF70" s="158"/>
+      <c r="FG70" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH70" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI70" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="71" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="65" t="s">
         <v>115</v>
       </c>
@@ -23154,7 +23683,7 @@
       <c r="EM71" s="113"/>
       <c r="EN71" s="113"/>
       <c r="EO71" s="113"/>
-      <c r="EP71" s="113"/>
+      <c r="EP71" s="71"/>
       <c r="EQ71" s="113"/>
       <c r="ER71" s="113"/>
       <c r="ES71" s="113"/>
@@ -23166,12 +23695,16 @@
       <c r="EY71" s="113"/>
       <c r="EZ71" s="113"/>
       <c r="FA71" s="113"/>
-      <c r="FB71" s="163"/>
-      <c r="FC71" s="163"/>
-      <c r="FD71" s="163"/>
-      <c r="FE71" s="163"/>
-    </row>
-    <row r="72" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB71" s="113"/>
+      <c r="FC71" s="113"/>
+      <c r="FD71" s="113"/>
+      <c r="FE71" s="113"/>
+      <c r="FF71" s="163"/>
+      <c r="FG71" s="163"/>
+      <c r="FH71" s="163"/>
+      <c r="FI71" s="163"/>
+    </row>
+    <row r="72" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="63" t="s">
         <v>607</v>
       </c>
@@ -23535,7 +24068,7 @@
       <c r="EO72" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP72" s="112"/>
+      <c r="EP72" s="70"/>
       <c r="EQ72" s="110" t="s">
         <v>362</v>
       </c>
@@ -23565,18 +24098,28 @@
       <c r="FA72" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB72" s="158"/>
-      <c r="FC72" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD72" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE72" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="73" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB72" s="112"/>
+      <c r="FC72" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD72" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE72" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF72" s="158"/>
+      <c r="FG72" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH72" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI72" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="73" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="65" t="s">
         <v>115</v>
       </c>
@@ -23730,7 +24273,7 @@
       <c r="EM73" s="113"/>
       <c r="EN73" s="113"/>
       <c r="EO73" s="113"/>
-      <c r="EP73" s="113"/>
+      <c r="EP73" s="71"/>
       <c r="EQ73" s="113"/>
       <c r="ER73" s="113"/>
       <c r="ES73" s="113"/>
@@ -23742,12 +24285,16 @@
       <c r="EY73" s="113"/>
       <c r="EZ73" s="113"/>
       <c r="FA73" s="113"/>
-      <c r="FB73" s="163"/>
-      <c r="FC73" s="163"/>
-      <c r="FD73" s="163"/>
-      <c r="FE73" s="163"/>
-    </row>
-    <row r="74" spans="1:161" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FB73" s="113"/>
+      <c r="FC73" s="113"/>
+      <c r="FD73" s="113"/>
+      <c r="FE73" s="113"/>
+      <c r="FF73" s="163"/>
+      <c r="FG73" s="163"/>
+      <c r="FH73" s="163"/>
+      <c r="FI73" s="163"/>
+    </row>
+    <row r="74" spans="1:165" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="63" t="s">
         <v>610</v>
       </c>
@@ -24111,7 +24658,7 @@
       <c r="EO74" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EP74" s="112"/>
+      <c r="EP74" s="70"/>
       <c r="EQ74" s="110" t="s">
         <v>362</v>
       </c>
@@ -24141,18 +24688,28 @@
       <c r="FA74" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FB74" s="158"/>
-      <c r="FC74" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FD74" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FE74" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="75" spans="1:161" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FB74" s="112"/>
+      <c r="FC74" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FD74" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FE74" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FF74" s="158"/>
+      <c r="FG74" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FH74" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FI74" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="75" spans="1:165" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="65" t="s">
         <v>115</v>
       </c>
@@ -24306,7 +24863,7 @@
       <c r="EM75" s="113"/>
       <c r="EN75" s="113"/>
       <c r="EO75" s="113"/>
-      <c r="EP75" s="113"/>
+      <c r="EP75" s="71"/>
       <c r="EQ75" s="113"/>
       <c r="ER75" s="113"/>
       <c r="ES75" s="113"/>
@@ -24318,10 +24875,14 @@
       <c r="EY75" s="113"/>
       <c r="EZ75" s="113"/>
       <c r="FA75" s="113"/>
-      <c r="FB75" s="163"/>
-      <c r="FC75" s="163"/>
-      <c r="FD75" s="163"/>
-      <c r="FE75" s="163"/>
+      <c r="FB75" s="113"/>
+      <c r="FC75" s="113"/>
+      <c r="FD75" s="113"/>
+      <c r="FE75" s="113"/>
+      <c r="FF75" s="163"/>
+      <c r="FG75" s="163"/>
+      <c r="FH75" s="163"/>
+      <c r="FI75" s="163"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes to make oversedation work - not validated
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngineStable\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D411D03-25E1-4609-A438-83E3A69BF9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0186F65E-CCA4-4640-B14B-EABA45A97E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="555" yWindow="1530" windowWidth="26655" windowHeight="11895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5243" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5318" uniqueCount="764">
   <si>
     <t>Name</t>
   </si>
@@ -2324,6 +2324,24 @@
   </si>
   <si>
     <t>0.0358 ug/mL</t>
+  </si>
+  <si>
+    <t>Overdose</t>
+  </si>
+  <si>
+    <t>321.28 g/mol</t>
+  </si>
+  <si>
+    <t>1.07 mL/min kg</t>
+  </si>
+  <si>
+    <t>0.92 mL/min kg</t>
+  </si>
+  <si>
+    <t>0.0558 ug/mL</t>
+  </si>
+  <si>
+    <t>Oversedation</t>
   </si>
 </sst>
 </file>
@@ -4858,13 +4876,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:FN75"/>
+  <dimension ref="A1:FR75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="DB36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="DB33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="EX42" sqref="EX42"/>
+      <selection pane="bottomRight" activeCell="EL36" sqref="EL36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -4996,37 +5014,41 @@
     <col min="139" max="139" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="140" max="140" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="141" max="141" width="11.42578125" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="142" max="142" width="13.42578125" style="53" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="142" max="142" width="14.42578125" style="102" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="143" max="143" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="144" max="144" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="145" max="145" width="11.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="146" max="146" width="13.42578125" style="53" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="146" max="146" width="14.85546875" style="53" bestFit="1" customWidth="1"/>
     <col min="147" max="147" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="148" max="148" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="149" max="149" width="11.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="150" max="150" width="13.42578125" style="53" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="151" max="151" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="152" max="152" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="153" max="153" width="11.42578125" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="154" max="154" width="14.42578125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="153" max="153" width="11.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="154" max="154" width="13.42578125" style="53" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="155" max="155" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="156" max="156" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="157" max="157" width="11.42578125" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="158" max="158" width="21.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="158" max="158" width="14.42578125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="159" max="159" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="160" max="160" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="161" max="161" width="11.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="162" max="162" width="15.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="161" max="161" width="11.42578125" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="162" max="162" width="21.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="163" max="163" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
     <col min="164" max="164" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="165" max="165" width="15.5703125" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="166" max="166" width="45.42578125" style="102" customWidth="1" collapsed="1"/>
-    <col min="167" max="169" width="23" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
-    <col min="170" max="170" width="9.140625" style="28" collapsed="1"/>
-    <col min="171" max="16384" width="9.140625" style="28"/>
+    <col min="165" max="165" width="11.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="166" max="166" width="15.5703125" style="102" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="167" max="167" width="15.85546875" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="168" max="168" width="16.7109375" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="169" max="169" width="15.5703125" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="170" max="170" width="45.42578125" style="102" customWidth="1" collapsed="1"/>
+    <col min="171" max="173" width="23" style="102" hidden="1" customWidth="1" outlineLevel="1" collapsed="1"/>
+    <col min="174" max="174" width="9.140625" style="28" collapsed="1"/>
+    <col min="175" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="59"/>
       <c r="B1" s="54"/>
       <c r="C1" s="99" t="s">
@@ -5378,7 +5400,7 @@
       <c r="EK1" s="108" t="s">
         <v>364</v>
       </c>
-      <c r="EL1" s="68"/>
+      <c r="EL1" s="108"/>
       <c r="EM1" s="108" t="s">
         <v>362</v>
       </c>
@@ -5408,7 +5430,7 @@
       <c r="EW1" s="108" t="s">
         <v>364</v>
       </c>
-      <c r="EX1" s="67"/>
+      <c r="EX1" s="68"/>
       <c r="EY1" s="108" t="s">
         <v>362</v>
       </c>
@@ -5438,18 +5460,28 @@
       <c r="FI1" s="108" t="s">
         <v>364</v>
       </c>
-      <c r="FJ1" s="158"/>
-      <c r="FK1" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL1" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM1" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="2" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ1" s="67"/>
+      <c r="FK1" s="108" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL1" s="108" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM1" s="108" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN1" s="158"/>
+      <c r="FO1" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP1" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ1" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="2" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>0</v>
       </c>
@@ -5874,91 +5906,103 @@
         <v>48</v>
       </c>
       <c r="EL2" s="100" t="s">
+        <v>763</v>
+      </c>
+      <c r="EM2" s="100" t="s">
+        <v>758</v>
+      </c>
+      <c r="EN2" s="100" t="s">
+        <v>758</v>
+      </c>
+      <c r="EO2" s="100" t="s">
+        <v>758</v>
+      </c>
+      <c r="EP2" s="100" t="s">
         <v>734</v>
       </c>
-      <c r="EM2" s="100" t="s">
+      <c r="EQ2" s="100" t="s">
         <v>734</v>
       </c>
-      <c r="EN2" s="100" t="s">
+      <c r="ER2" s="100" t="s">
         <v>734</v>
       </c>
-      <c r="EO2" s="100" t="s">
+      <c r="ES2" s="100" t="s">
         <v>734</v>
       </c>
-      <c r="EP2" s="100" t="s">
+      <c r="ET2" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="EQ2" s="100" t="s">
+      <c r="EU2" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="ER2" s="100" t="s">
+      <c r="EV2" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="ES2" s="100" t="s">
+      <c r="EW2" s="100" t="s">
         <v>197</v>
       </c>
-      <c r="ET2" s="100" t="s">
+      <c r="EX2" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="EU2" s="100" t="s">
+      <c r="EY2" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="EV2" s="100" t="s">
+      <c r="EZ2" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="EW2" s="100" t="s">
+      <c r="FA2" s="100" t="s">
         <v>198</v>
       </c>
-      <c r="EX2" s="100" t="s">
+      <c r="FB2" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="EY2" s="100" t="s">
+      <c r="FC2" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="EZ2" s="100" t="s">
+      <c r="FD2" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="FA2" s="100" t="s">
+      <c r="FE2" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="FB2" s="100" t="s">
+      <c r="FF2" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="FC2" s="100" t="s">
+      <c r="FG2" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="FD2" s="100" t="s">
+      <c r="FH2" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="FE2" s="100" t="s">
+      <c r="FI2" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="FF2" s="100" t="s">
+      <c r="FJ2" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="FG2" s="100" t="s">
+      <c r="FK2" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="FH2" s="100" t="s">
+      <c r="FL2" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="FI2" s="100" t="s">
+      <c r="FM2" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="FJ2" s="100" t="s">
+      <c r="FN2" s="100" t="s">
         <v>667</v>
       </c>
-      <c r="FK2" s="100" t="s">
+      <c r="FO2" s="100" t="s">
         <v>667</v>
       </c>
-      <c r="FL2" s="100" t="s">
+      <c r="FP2" s="100" t="s">
         <v>667</v>
       </c>
-      <c r="FM2" s="100" t="s">
+      <c r="FQ2" s="100" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="3" spans="1:169" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:173" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
         <v>341</v>
       </c>
@@ -6312,7 +6356,7 @@
       <c r="EK3" s="109" t="s">
         <v>364</v>
       </c>
-      <c r="EL3" s="57"/>
+      <c r="EL3" s="109"/>
       <c r="EM3" s="109" t="s">
         <v>362</v>
       </c>
@@ -6382,8 +6426,18 @@
       <c r="FM3" s="109" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="4" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FN3" s="57"/>
+      <c r="FO3" s="109" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP3" s="109" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ3" s="109" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>1</v>
       </c>
@@ -6635,14 +6689,20 @@
       <c r="FG4" s="111"/>
       <c r="FH4" s="111"/>
       <c r="FI4" s="111"/>
-      <c r="FJ4" s="160" t="s">
+      <c r="FJ4" s="111" t="s">
+        <v>17</v>
+      </c>
+      <c r="FK4" s="111"/>
+      <c r="FL4" s="111"/>
+      <c r="FM4" s="111"/>
+      <c r="FN4" s="160" t="s">
         <v>630</v>
       </c>
-      <c r="FK4" s="160"/>
-      <c r="FL4" s="160"/>
-      <c r="FM4" s="160"/>
-    </row>
-    <row r="5" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FO4" s="160"/>
+      <c r="FP4" s="160"/>
+      <c r="FQ4" s="160"/>
+    </row>
+    <row r="5" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>10</v>
       </c>
@@ -6826,12 +6886,16 @@
       <c r="FG5" s="111"/>
       <c r="FH5" s="111"/>
       <c r="FI5" s="111"/>
-      <c r="FJ5" s="160"/>
-      <c r="FK5" s="160"/>
-      <c r="FL5" s="160"/>
-      <c r="FM5" s="160"/>
-    </row>
-    <row r="6" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ5" s="111"/>
+      <c r="FK5" s="111"/>
+      <c r="FL5" s="111"/>
+      <c r="FM5" s="111"/>
+      <c r="FN5" s="160"/>
+      <c r="FO5" s="160"/>
+      <c r="FP5" s="160"/>
+      <c r="FQ5" s="160"/>
+    </row>
+    <row r="6" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
         <v>552</v>
       </c>
@@ -7001,12 +7065,16 @@
       <c r="FG6" s="111"/>
       <c r="FH6" s="111"/>
       <c r="FI6" s="111"/>
-      <c r="FJ6" s="160"/>
-      <c r="FK6" s="160"/>
-      <c r="FL6" s="160"/>
-      <c r="FM6" s="160"/>
-    </row>
-    <row r="7" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ6" s="111"/>
+      <c r="FK6" s="111"/>
+      <c r="FL6" s="111"/>
+      <c r="FM6" s="111"/>
+      <c r="FN6" s="160"/>
+      <c r="FO6" s="160"/>
+      <c r="FP6" s="160"/>
+      <c r="FQ6" s="160"/>
+    </row>
+    <row r="7" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>553</v>
       </c>
@@ -7176,12 +7244,16 @@
       <c r="FG7" s="111"/>
       <c r="FH7" s="111"/>
       <c r="FI7" s="111"/>
-      <c r="FJ7" s="160"/>
-      <c r="FK7" s="160"/>
-      <c r="FL7" s="160"/>
-      <c r="FM7" s="160"/>
-    </row>
-    <row r="8" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ7" s="111"/>
+      <c r="FK7" s="111"/>
+      <c r="FL7" s="111"/>
+      <c r="FM7" s="111"/>
+      <c r="FN7" s="160"/>
+      <c r="FO7" s="160"/>
+      <c r="FP7" s="160"/>
+      <c r="FQ7" s="160"/>
+    </row>
+    <row r="8" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="62" t="s">
         <v>43</v>
       </c>
@@ -7402,49 +7474,55 @@
       <c r="EJ8" s="111"/>
       <c r="EK8" s="111"/>
       <c r="EL8" s="111" t="s">
-        <v>735</v>
+        <v>759</v>
       </c>
       <c r="EM8" s="111"/>
-      <c r="EN8" s="111" t="s">
-        <v>736</v>
-      </c>
+      <c r="EN8" s="111"/>
       <c r="EO8" s="111"/>
       <c r="EP8" s="111" t="s">
-        <v>129</v>
+        <v>735</v>
       </c>
       <c r="EQ8" s="111"/>
-      <c r="ER8" s="111"/>
+      <c r="ER8" s="111" t="s">
+        <v>736</v>
+      </c>
       <c r="ES8" s="111"/>
       <c r="ET8" s="111" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="EU8" s="111"/>
       <c r="EV8" s="111"/>
       <c r="EW8" s="111"/>
       <c r="EX8" s="111" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="EY8" s="111"/>
       <c r="EZ8" s="111"/>
       <c r="FA8" s="111"/>
       <c r="FB8" s="111" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="FC8" s="111"/>
       <c r="FD8" s="111"/>
       <c r="FE8" s="111"/>
       <c r="FF8" s="111" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="FG8" s="111"/>
       <c r="FH8" s="111"/>
       <c r="FI8" s="111"/>
-      <c r="FJ8" s="160"/>
-      <c r="FK8" s="160"/>
-      <c r="FL8" s="160"/>
-      <c r="FM8" s="160"/>
-    </row>
-    <row r="9" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ8" s="111" t="s">
+        <v>118</v>
+      </c>
+      <c r="FK8" s="111"/>
+      <c r="FL8" s="111"/>
+      <c r="FM8" s="111"/>
+      <c r="FN8" s="160"/>
+      <c r="FO8" s="160"/>
+      <c r="FP8" s="160"/>
+      <c r="FQ8" s="160"/>
+    </row>
+    <row r="9" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
         <v>715</v>
       </c>
@@ -7622,12 +7700,16 @@
       <c r="FG9" s="111"/>
       <c r="FH9" s="111"/>
       <c r="FI9" s="111"/>
-      <c r="FJ9" s="160"/>
-      <c r="FK9" s="160"/>
-      <c r="FL9" s="160"/>
-      <c r="FM9" s="160"/>
-    </row>
-    <row r="10" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ9" s="111"/>
+      <c r="FK9" s="111"/>
+      <c r="FL9" s="111"/>
+      <c r="FM9" s="111"/>
+      <c r="FN9" s="160"/>
+      <c r="FO9" s="160"/>
+      <c r="FP9" s="160"/>
+      <c r="FQ9" s="160"/>
+    </row>
+    <row r="10" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
         <v>76</v>
       </c>
@@ -7807,12 +7889,16 @@
       <c r="FG10" s="111"/>
       <c r="FH10" s="111"/>
       <c r="FI10" s="111"/>
-      <c r="FJ10" s="160"/>
-      <c r="FK10" s="160"/>
-      <c r="FL10" s="160"/>
-      <c r="FM10" s="160"/>
-    </row>
-    <row r="11" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ10" s="111"/>
+      <c r="FK10" s="111"/>
+      <c r="FL10" s="111"/>
+      <c r="FM10" s="111"/>
+      <c r="FN10" s="160"/>
+      <c r="FO10" s="160"/>
+      <c r="FP10" s="160"/>
+      <c r="FQ10" s="160"/>
+    </row>
+    <row r="11" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>75</v>
       </c>
@@ -7998,12 +8084,16 @@
       <c r="FG11" s="111"/>
       <c r="FH11" s="111"/>
       <c r="FI11" s="111"/>
-      <c r="FJ11" s="160"/>
-      <c r="FK11" s="160"/>
-      <c r="FL11" s="160"/>
-      <c r="FM11" s="160"/>
-    </row>
-    <row r="12" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ11" s="111"/>
+      <c r="FK11" s="111"/>
+      <c r="FL11" s="111"/>
+      <c r="FM11" s="111"/>
+      <c r="FN11" s="160"/>
+      <c r="FO11" s="160"/>
+      <c r="FP11" s="160"/>
+      <c r="FQ11" s="160"/>
+    </row>
+    <row r="12" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="80" t="s">
         <v>337</v>
       </c>
@@ -8359,7 +8449,7 @@
       <c r="EK12" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL12" s="70"/>
+      <c r="EL12" s="110"/>
       <c r="EM12" s="110" t="s">
         <v>362</v>
       </c>
@@ -8389,7 +8479,7 @@
       <c r="EW12" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX12" s="112"/>
+      <c r="EX12" s="70"/>
       <c r="EY12" s="110" t="s">
         <v>362</v>
       </c>
@@ -8419,18 +8509,28 @@
       <c r="FI12" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ12" s="158"/>
-      <c r="FK12" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL12" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM12" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="13" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ12" s="112"/>
+      <c r="FK12" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL12" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM12" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN12" s="158"/>
+      <c r="FO12" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP12" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ12" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="64" t="s">
         <v>670</v>
       </c>
@@ -8597,17 +8697,21 @@
       <c r="FD13" s="115"/>
       <c r="FE13" s="115"/>
       <c r="FF13" s="115"/>
-      <c r="FG13" s="157"/>
-      <c r="FH13" s="157"/>
-      <c r="FI13" s="157"/>
-      <c r="FJ13" s="160">
+      <c r="FG13" s="115"/>
+      <c r="FH13" s="115"/>
+      <c r="FI13" s="115"/>
+      <c r="FJ13" s="115"/>
+      <c r="FK13" s="157"/>
+      <c r="FL13" s="157"/>
+      <c r="FM13" s="157"/>
+      <c r="FN13" s="160">
         <v>0</v>
       </c>
-      <c r="FK13" s="166"/>
-      <c r="FL13" s="166"/>
-      <c r="FM13" s="166"/>
-    </row>
-    <row r="14" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FO13" s="166"/>
+      <c r="FP13" s="166"/>
+      <c r="FQ13" s="166"/>
+    </row>
+    <row r="14" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="64" t="s">
         <v>657</v>
       </c>
@@ -8774,17 +8878,21 @@
       <c r="FD14" s="115"/>
       <c r="FE14" s="115"/>
       <c r="FF14" s="115"/>
-      <c r="FG14" s="157"/>
-      <c r="FH14" s="157"/>
-      <c r="FI14" s="157"/>
-      <c r="FJ14" s="160">
+      <c r="FG14" s="115"/>
+      <c r="FH14" s="115"/>
+      <c r="FI14" s="115"/>
+      <c r="FJ14" s="115"/>
+      <c r="FK14" s="157"/>
+      <c r="FL14" s="157"/>
+      <c r="FM14" s="157"/>
+      <c r="FN14" s="160">
         <v>0.5</v>
       </c>
-      <c r="FK14" s="166"/>
-      <c r="FL14" s="166"/>
-      <c r="FM14" s="166"/>
-    </row>
-    <row r="15" spans="1:169" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="FO14" s="166"/>
+      <c r="FP14" s="166"/>
+      <c r="FQ14" s="166"/>
+    </row>
+    <row r="15" spans="1:173" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="64" t="s">
         <v>626</v>
       </c>
@@ -8951,17 +9059,21 @@
       <c r="FD15" s="115"/>
       <c r="FE15" s="115"/>
       <c r="FF15" s="115"/>
-      <c r="FG15" s="157"/>
-      <c r="FH15" s="157"/>
-      <c r="FI15" s="157"/>
-      <c r="FJ15" s="164" t="s">
+      <c r="FG15" s="115"/>
+      <c r="FH15" s="115"/>
+      <c r="FI15" s="115"/>
+      <c r="FJ15" s="115"/>
+      <c r="FK15" s="157"/>
+      <c r="FL15" s="157"/>
+      <c r="FM15" s="157"/>
+      <c r="FN15" s="164" t="s">
         <v>627</v>
       </c>
-      <c r="FK15" s="162"/>
-      <c r="FL15" s="162"/>
-      <c r="FM15" s="162"/>
-    </row>
-    <row r="16" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FO15" s="162"/>
+      <c r="FP15" s="162"/>
+      <c r="FQ15" s="162"/>
+    </row>
+    <row r="16" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="80" t="s">
         <v>338</v>
       </c>
@@ -9317,7 +9429,7 @@
       <c r="EK16" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL16" s="70"/>
+      <c r="EL16" s="110"/>
       <c r="EM16" s="110" t="s">
         <v>362</v>
       </c>
@@ -9347,7 +9459,7 @@
       <c r="EW16" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX16" s="112"/>
+      <c r="EX16" s="70"/>
       <c r="EY16" s="110" t="s">
         <v>362</v>
       </c>
@@ -9377,18 +9489,28 @@
       <c r="FI16" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ16" s="158"/>
-      <c r="FK16" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL16" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM16" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="17" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ16" s="112"/>
+      <c r="FK16" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL16" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM16" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN16" s="158"/>
+      <c r="FO16" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP16" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ16" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="17" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="62" t="s">
         <v>96</v>
       </c>
@@ -9583,29 +9705,35 @@
       <c r="EV17" s="111"/>
       <c r="EW17" s="111"/>
       <c r="EX17" s="111">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="EY17" s="111"/>
       <c r="EZ17" s="111"/>
       <c r="FA17" s="111"/>
       <c r="FB17" s="111">
-        <v>0.31</v>
+        <v>0.02</v>
       </c>
       <c r="FC17" s="111"/>
       <c r="FD17" s="111"/>
       <c r="FE17" s="111"/>
       <c r="FF17" s="111">
-        <v>0</v>
+        <v>0.31</v>
       </c>
       <c r="FG17" s="111"/>
       <c r="FH17" s="111"/>
       <c r="FI17" s="111"/>
-      <c r="FJ17" s="160"/>
-      <c r="FK17" s="160"/>
-      <c r="FL17" s="160"/>
-      <c r="FM17" s="160"/>
-    </row>
-    <row r="18" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ17" s="111">
+        <v>0</v>
+      </c>
+      <c r="FK17" s="111"/>
+      <c r="FL17" s="111"/>
+      <c r="FM17" s="111"/>
+      <c r="FN17" s="160"/>
+      <c r="FO17" s="160"/>
+      <c r="FP17" s="160"/>
+      <c r="FQ17" s="160"/>
+    </row>
+    <row r="18" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="62" t="s">
         <v>92</v>
       </c>
@@ -9800,47 +9928,53 @@
       <c r="EJ18" s="111"/>
       <c r="EK18" s="111"/>
       <c r="EL18" s="111">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="EM18" s="111"/>
       <c r="EN18" s="111"/>
       <c r="EO18" s="111"/>
       <c r="EP18" s="111">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="EQ18" s="111"/>
       <c r="ER18" s="111"/>
       <c r="ES18" s="111"/>
       <c r="ET18" s="111">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="EU18" s="111"/>
       <c r="EV18" s="111"/>
       <c r="EW18" s="111"/>
       <c r="EX18" s="111">
-        <v>0.03</v>
+        <v>0.25</v>
       </c>
       <c r="EY18" s="111"/>
       <c r="EZ18" s="111"/>
       <c r="FA18" s="111"/>
       <c r="FB18" s="111">
-        <v>0.7</v>
+        <v>0.03</v>
       </c>
       <c r="FC18" s="111"/>
       <c r="FD18" s="111"/>
       <c r="FE18" s="111"/>
       <c r="FF18" s="111">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="FG18" s="111"/>
       <c r="FH18" s="111"/>
       <c r="FI18" s="111"/>
-      <c r="FJ18" s="160"/>
-      <c r="FK18" s="160"/>
-      <c r="FL18" s="160"/>
-      <c r="FM18" s="160"/>
-    </row>
-    <row r="19" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ18" s="111">
+        <v>0.8</v>
+      </c>
+      <c r="FK18" s="111"/>
+      <c r="FL18" s="111"/>
+      <c r="FM18" s="111"/>
+      <c r="FN18" s="160"/>
+      <c r="FO18" s="160"/>
+      <c r="FP18" s="160"/>
+      <c r="FQ18" s="160"/>
+    </row>
+    <row r="19" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="62" t="s">
         <v>94</v>
       </c>
@@ -10023,51 +10157,57 @@
       <c r="EJ19" s="111"/>
       <c r="EK19" s="111"/>
       <c r="EL19" s="111" t="s">
-        <v>741</v>
-      </c>
-      <c r="EM19" s="111" t="s">
-        <v>737</v>
-      </c>
-      <c r="EN19" s="111" t="s">
-        <v>736</v>
-      </c>
+        <v>760</v>
+      </c>
+      <c r="EM19" s="111"/>
+      <c r="EN19" s="111"/>
       <c r="EO19" s="111"/>
       <c r="EP19" s="111" t="s">
-        <v>99</v>
-      </c>
-      <c r="EQ19" s="111"/>
-      <c r="ER19" s="111"/>
+        <v>741</v>
+      </c>
+      <c r="EQ19" s="111" t="s">
+        <v>737</v>
+      </c>
+      <c r="ER19" s="111" t="s">
+        <v>736</v>
+      </c>
       <c r="ES19" s="111"/>
       <c r="ET19" s="111" t="s">
-        <v>263</v>
+        <v>99</v>
       </c>
       <c r="EU19" s="111"/>
       <c r="EV19" s="111"/>
       <c r="EW19" s="111"/>
       <c r="EX19" s="111" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="EY19" s="111"/>
       <c r="EZ19" s="111"/>
       <c r="FA19" s="111"/>
       <c r="FB19" s="111" t="s">
-        <v>361</v>
+        <v>264</v>
       </c>
       <c r="FC19" s="111"/>
       <c r="FD19" s="111"/>
       <c r="FE19" s="111"/>
       <c r="FF19" s="111" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="FG19" s="111"/>
       <c r="FH19" s="111"/>
       <c r="FI19" s="111"/>
-      <c r="FJ19" s="160"/>
-      <c r="FK19" s="160"/>
-      <c r="FL19" s="160"/>
-      <c r="FM19" s="160"/>
-    </row>
-    <row r="20" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ19" s="111" t="s">
+        <v>347</v>
+      </c>
+      <c r="FK19" s="111"/>
+      <c r="FL19" s="111"/>
+      <c r="FM19" s="111"/>
+      <c r="FN19" s="160"/>
+      <c r="FO19" s="160"/>
+      <c r="FP19" s="160"/>
+      <c r="FQ19" s="160"/>
+    </row>
+    <row r="20" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="62" t="s">
         <v>379</v>
       </c>
@@ -10244,47 +10384,53 @@
       <c r="EJ20" s="111"/>
       <c r="EK20" s="111"/>
       <c r="EL20" s="111" t="s">
-        <v>742</v>
+        <v>99</v>
       </c>
       <c r="EM20" s="111"/>
       <c r="EN20" s="111"/>
       <c r="EO20" s="111"/>
       <c r="EP20" s="111" t="s">
-        <v>130</v>
+        <v>742</v>
       </c>
       <c r="EQ20" s="111"/>
       <c r="ER20" s="111"/>
       <c r="ES20" s="111"/>
       <c r="ET20" s="111" t="s">
-        <v>358</v>
+        <v>130</v>
       </c>
       <c r="EU20" s="111"/>
       <c r="EV20" s="111"/>
       <c r="EW20" s="111"/>
       <c r="EX20" s="111" t="s">
-        <v>265</v>
+        <v>358</v>
       </c>
       <c r="EY20" s="111"/>
       <c r="EZ20" s="111"/>
       <c r="FA20" s="111"/>
       <c r="FB20" s="111" t="s">
-        <v>360</v>
+        <v>265</v>
       </c>
       <c r="FC20" s="111"/>
       <c r="FD20" s="111"/>
       <c r="FE20" s="111"/>
       <c r="FF20" s="111" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="FG20" s="111"/>
       <c r="FH20" s="111"/>
       <c r="FI20" s="111"/>
-      <c r="FJ20" s="160"/>
-      <c r="FK20" s="160"/>
-      <c r="FL20" s="160"/>
-      <c r="FM20" s="160"/>
-    </row>
-    <row r="21" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ20" s="111" t="s">
+        <v>347</v>
+      </c>
+      <c r="FK20" s="111"/>
+      <c r="FL20" s="111"/>
+      <c r="FM20" s="111"/>
+      <c r="FN20" s="160"/>
+      <c r="FO20" s="160"/>
+      <c r="FP20" s="160"/>
+      <c r="FQ20" s="160"/>
+    </row>
+    <row r="21" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="62" t="s">
         <v>95</v>
       </c>
@@ -10471,47 +10617,53 @@
       <c r="EJ21" s="111"/>
       <c r="EK21" s="111"/>
       <c r="EL21" s="111" t="s">
-        <v>743</v>
+        <v>761</v>
       </c>
       <c r="EM21" s="111"/>
       <c r="EN21" s="111"/>
       <c r="EO21" s="111"/>
       <c r="EP21" s="111" t="s">
-        <v>268</v>
+        <v>743</v>
       </c>
       <c r="EQ21" s="111"/>
       <c r="ER21" s="111"/>
       <c r="ES21" s="111"/>
       <c r="ET21" s="111" t="s">
-        <v>359</v>
+        <v>268</v>
       </c>
       <c r="EU21" s="111"/>
       <c r="EV21" s="111"/>
       <c r="EW21" s="111"/>
       <c r="EX21" s="111" t="s">
-        <v>269</v>
+        <v>359</v>
       </c>
       <c r="EY21" s="111"/>
       <c r="EZ21" s="111"/>
       <c r="FA21" s="111"/>
       <c r="FB21" s="111" t="s">
-        <v>353</v>
+        <v>269</v>
       </c>
       <c r="FC21" s="111"/>
       <c r="FD21" s="111"/>
       <c r="FE21" s="111"/>
       <c r="FF21" s="111" t="s">
-        <v>382</v>
+        <v>353</v>
       </c>
       <c r="FG21" s="111"/>
       <c r="FH21" s="111"/>
       <c r="FI21" s="111"/>
-      <c r="FJ21" s="160"/>
-      <c r="FK21" s="160"/>
-      <c r="FL21" s="160"/>
-      <c r="FM21" s="160"/>
-    </row>
-    <row r="22" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ21" s="111" t="s">
+        <v>382</v>
+      </c>
+      <c r="FK21" s="111"/>
+      <c r="FL21" s="111"/>
+      <c r="FM21" s="111"/>
+      <c r="FN21" s="160"/>
+      <c r="FO21" s="160"/>
+      <c r="FP21" s="160"/>
+      <c r="FQ21" s="160"/>
+    </row>
+    <row r="22" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="81" t="s">
         <v>336</v>
       </c>
@@ -10867,7 +11019,7 @@
       <c r="EK22" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL22" s="70"/>
+      <c r="EL22" s="110"/>
       <c r="EM22" s="110" t="s">
         <v>362</v>
       </c>
@@ -10897,7 +11049,7 @@
       <c r="EW22" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX22" s="112"/>
+      <c r="EX22" s="70"/>
       <c r="EY22" s="110" t="s">
         <v>362</v>
       </c>
@@ -10927,18 +11079,28 @@
       <c r="FI22" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ22" s="158"/>
-      <c r="FK22" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL22" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM22" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="23" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ22" s="112"/>
+      <c r="FK22" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL22" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM22" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN22" s="158"/>
+      <c r="FO22" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP22" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ22" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="23" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="82" t="s">
         <v>332</v>
       </c>
@@ -11054,7 +11216,7 @@
       <c r="CZ23" s="111"/>
       <c r="DA23" s="111"/>
       <c r="DB23" s="111" t="str">
-        <f t="shared" ref="DB23:FF23" si="0">DB20</f>
+        <f t="shared" ref="DB23:EH23" si="0">DB20</f>
         <v>0 mL/min kg</v>
       </c>
       <c r="DC23" s="111">
@@ -11070,19 +11232,19 @@
         <v>0</v>
       </c>
       <c r="DF23" s="111" t="str">
-        <f t="shared" ref="DF23:DI23" si="1">DF20</f>
+        <f t="shared" si="0"/>
         <v>0 mL/min kg</v>
       </c>
       <c r="DG23" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="DH23" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="DI23" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="DJ23" s="111" t="str">
@@ -11134,19 +11296,19 @@
         <v>0</v>
       </c>
       <c r="DV23" s="111" t="str">
-        <f t="shared" ref="DV23:DY23" si="2">DV20</f>
+        <f t="shared" si="0"/>
         <v>0.05 mL/min kg</v>
       </c>
       <c r="DW23" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="DX23" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="DY23" s="111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="DZ23" s="111" t="str">
@@ -11186,110 +11348,126 @@
         <v>0.5 mL/min kg</v>
       </c>
       <c r="EI23" s="111">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="DB23:FJ23" si="1">EI20</f>
         <v>0</v>
       </c>
       <c r="EJ23" s="111">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="EK23" s="111">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="EL23" s="111" t="str">
-        <f t="shared" ref="EL23:EO23" si="3">EL20</f>
+        <f t="shared" si="1"/>
+        <v>0 mL/min kg</v>
+      </c>
+      <c r="EM23" s="111">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="EN23" s="111">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="EO23" s="111">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="EP23" s="111" t="str">
+        <f t="shared" ref="EP23:ES23" si="2">EP20</f>
         <v>45 mL/min kg</v>
       </c>
-      <c r="EM23" s="111">
-        <f t="shared" si="3"/>
+      <c r="EQ23" s="111">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="EN23" s="111">
-        <f t="shared" si="3"/>
+      <c r="ER23" s="111">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="EO23" s="111">
-        <f t="shared" si="3"/>
+      <c r="ES23" s="111">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="EP23" s="111" t="str">
-        <f t="shared" si="0"/>
+      <c r="ET23" s="111" t="str">
+        <f t="shared" si="1"/>
         <v>7.2 mL/min kg</v>
       </c>
-      <c r="EQ23" s="111">
-        <f t="shared" si="0"/>
+      <c r="EU23" s="111">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="ER23" s="111">
-        <f t="shared" si="0"/>
+      <c r="EV23" s="111">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="ES23" s="111">
-        <f t="shared" si="0"/>
+      <c r="EW23" s="111">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="ET23" s="111" t="str">
-        <f t="shared" si="0"/>
+      <c r="EX23" s="111" t="str">
+        <f t="shared" si="1"/>
         <v>0.72 mL/min kg</v>
       </c>
-      <c r="EU23" s="111">
-        <f t="shared" si="0"/>
+      <c r="EY23" s="111">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="EV23" s="111">
-        <f t="shared" si="0"/>
+      <c r="EZ23" s="111">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="EW23" s="111">
-        <f t="shared" si="0"/>
+      <c r="FA23" s="111">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="EX23" s="111" t="str">
-        <f t="shared" si="0"/>
+      <c r="FB23" s="111" t="str">
+        <f t="shared" si="1"/>
         <v>1.3 mL/min kg</v>
       </c>
-      <c r="EY23" s="111">
-        <f t="shared" si="0"/>
+      <c r="FC23" s="111">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="EZ23" s="111">
-        <f t="shared" si="0"/>
+      <c r="FD23" s="111">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="FA23" s="111">
-        <f t="shared" si="0"/>
+      <c r="FE23" s="111">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="FB23" s="111" t="str">
-        <f t="shared" si="0"/>
+      <c r="FF23" s="111" t="str">
+        <f t="shared" si="1"/>
         <v>2.2 mL/min kg</v>
       </c>
-      <c r="FC23" s="111">
-        <f t="shared" si="0"/>
+      <c r="FG23" s="111">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="FD23" s="111">
-        <f t="shared" si="0"/>
+      <c r="FH23" s="111">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="FE23" s="111">
-        <f t="shared" si="0"/>
+      <c r="FI23" s="111">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="FF23" s="111" t="str">
-        <f t="shared" si="0"/>
+      <c r="FJ23" s="111" t="str">
+        <f t="shared" si="1"/>
         <v>0.0 mL/min kg</v>
       </c>
-      <c r="FG23" s="111"/>
-      <c r="FH23" s="111"/>
-      <c r="FI23" s="111"/>
-      <c r="FJ23" s="160"/>
-      <c r="FK23" s="160"/>
-      <c r="FL23" s="160"/>
-      <c r="FM23" s="160"/>
-    </row>
-    <row r="24" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FK23" s="111"/>
+      <c r="FL23" s="111"/>
+      <c r="FM23" s="111"/>
+      <c r="FN23" s="160"/>
+      <c r="FO23" s="160"/>
+      <c r="FP23" s="160"/>
+      <c r="FQ23" s="160"/>
+    </row>
+    <row r="24" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="81" t="s">
         <v>331</v>
       </c>
@@ -11645,7 +11823,7 @@
       <c r="EK24" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL24" s="70"/>
+      <c r="EL24" s="110"/>
       <c r="EM24" s="110" t="s">
         <v>362</v>
       </c>
@@ -11675,7 +11853,7 @@
       <c r="EW24" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX24" s="112"/>
+      <c r="EX24" s="70"/>
       <c r="EY24" s="110" t="s">
         <v>362</v>
       </c>
@@ -11705,18 +11883,28 @@
       <c r="FI24" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ24" s="158"/>
-      <c r="FK24" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL24" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM24" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="25" spans="1:169" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FJ24" s="112"/>
+      <c r="FK24" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL24" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM24" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN24" s="158"/>
+      <c r="FO24" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP24" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ24" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="25" spans="1:173" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="82" t="s">
         <v>333</v>
       </c>
@@ -11912,12 +12100,16 @@
       <c r="FG25" s="111"/>
       <c r="FH25" s="111"/>
       <c r="FI25" s="111"/>
-      <c r="FJ25" s="160"/>
-      <c r="FK25" s="160"/>
-      <c r="FL25" s="160"/>
-      <c r="FM25" s="160"/>
-    </row>
-    <row r="26" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ25" s="111"/>
+      <c r="FK25" s="111"/>
+      <c r="FL25" s="111"/>
+      <c r="FM25" s="111"/>
+      <c r="FN25" s="160"/>
+      <c r="FO25" s="160"/>
+      <c r="FP25" s="160"/>
+      <c r="FQ25" s="160"/>
+    </row>
+    <row r="26" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="82" t="s">
         <v>380</v>
       </c>
@@ -12113,12 +12305,16 @@
       <c r="FG26" s="111"/>
       <c r="FH26" s="111"/>
       <c r="FI26" s="111"/>
-      <c r="FJ26" s="160"/>
-      <c r="FK26" s="160"/>
-      <c r="FL26" s="160"/>
-      <c r="FM26" s="160"/>
-    </row>
-    <row r="27" spans="1:169" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FJ26" s="111"/>
+      <c r="FK26" s="111"/>
+      <c r="FL26" s="111"/>
+      <c r="FM26" s="111"/>
+      <c r="FN26" s="160"/>
+      <c r="FO26" s="160"/>
+      <c r="FP26" s="160"/>
+      <c r="FQ26" s="160"/>
+    </row>
+    <row r="27" spans="1:173" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="82" t="s">
         <v>334</v>
       </c>
@@ -12332,12 +12528,16 @@
       <c r="FG27" s="111"/>
       <c r="FH27" s="111"/>
       <c r="FI27" s="111"/>
-      <c r="FJ27" s="160"/>
-      <c r="FK27" s="160"/>
-      <c r="FL27" s="160"/>
-      <c r="FM27" s="160"/>
-    </row>
-    <row r="28" spans="1:169" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="FJ27" s="111"/>
+      <c r="FK27" s="111"/>
+      <c r="FL27" s="111"/>
+      <c r="FM27" s="111"/>
+      <c r="FN27" s="160"/>
+      <c r="FO27" s="160"/>
+      <c r="FP27" s="160"/>
+      <c r="FQ27" s="160"/>
+    </row>
+    <row r="28" spans="1:173" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="82" t="s">
         <v>335</v>
       </c>
@@ -12553,12 +12753,16 @@
       <c r="FG28" s="111"/>
       <c r="FH28" s="111"/>
       <c r="FI28" s="111"/>
-      <c r="FJ28" s="160"/>
-      <c r="FK28" s="160"/>
-      <c r="FL28" s="160"/>
-      <c r="FM28" s="160"/>
-    </row>
-    <row r="29" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ28" s="111"/>
+      <c r="FK28" s="111"/>
+      <c r="FL28" s="111"/>
+      <c r="FM28" s="111"/>
+      <c r="FN28" s="160"/>
+      <c r="FO28" s="160"/>
+      <c r="FP28" s="160"/>
+      <c r="FQ28" s="160"/>
+    </row>
+    <row r="29" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="80" t="s">
         <v>339</v>
       </c>
@@ -12914,7 +13118,7 @@
       <c r="EK29" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL29" s="70"/>
+      <c r="EL29" s="110"/>
       <c r="EM29" s="110" t="s">
         <v>362</v>
       </c>
@@ -12944,7 +13148,7 @@
       <c r="EW29" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX29" s="112"/>
+      <c r="EX29" s="70"/>
       <c r="EY29" s="110" t="s">
         <v>362</v>
       </c>
@@ -12974,18 +13178,28 @@
       <c r="FI29" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ29" s="158"/>
-      <c r="FK29" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL29" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM29" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="30" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ29" s="112"/>
+      <c r="FK29" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL29" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM29" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN29" s="158"/>
+      <c r="FO29" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP29" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ29" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="30" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="62" t="s">
         <v>90</v>
       </c>
@@ -13158,49 +13372,55 @@
       <c r="EJ30" s="111"/>
       <c r="EK30" s="111"/>
       <c r="EL30" s="111">
-        <v>8.9700000000000006</v>
+        <v>1.5</v>
       </c>
       <c r="EM30" s="111"/>
-      <c r="EN30" s="111" t="s">
-        <v>736</v>
-      </c>
+      <c r="EN30" s="111"/>
       <c r="EO30" s="111"/>
       <c r="EP30" s="111">
-        <v>5.78</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="EQ30" s="111"/>
-      <c r="ER30" s="111"/>
+      <c r="ER30" s="111" t="s">
+        <v>736</v>
+      </c>
       <c r="ES30" s="111"/>
       <c r="ET30" s="111">
-        <v>12.58</v>
+        <v>5.78</v>
       </c>
       <c r="EU30" s="111"/>
       <c r="EV30" s="111"/>
       <c r="EW30" s="111"/>
       <c r="EX30" s="111">
-        <v>11.1</v>
+        <v>12.58</v>
       </c>
       <c r="EY30" s="111"/>
       <c r="EZ30" s="111"/>
       <c r="FA30" s="111"/>
       <c r="FB30" s="111">
-        <v>14.95</v>
+        <v>11.1</v>
       </c>
       <c r="FC30" s="111"/>
       <c r="FD30" s="111"/>
       <c r="FE30" s="111"/>
       <c r="FF30" s="111">
-        <v>1</v>
+        <v>14.95</v>
       </c>
       <c r="FG30" s="111"/>
       <c r="FH30" s="111"/>
       <c r="FI30" s="111"/>
-      <c r="FJ30" s="160"/>
-      <c r="FK30" s="160"/>
-      <c r="FL30" s="160"/>
-      <c r="FM30" s="160"/>
-    </row>
-    <row r="31" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ30" s="111">
+        <v>1</v>
+      </c>
+      <c r="FK30" s="111"/>
+      <c r="FL30" s="111"/>
+      <c r="FM30" s="111"/>
+      <c r="FN30" s="160"/>
+      <c r="FO30" s="160"/>
+      <c r="FP30" s="160"/>
+      <c r="FQ30" s="160"/>
+    </row>
+    <row r="31" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="62" t="s">
         <v>113</v>
       </c>
@@ -13371,18 +13591,18 @@
       <c r="EL31" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="EM31" s="111" t="s">
-        <v>738</v>
-      </c>
-      <c r="EN31" s="111" t="s">
-        <v>740</v>
-      </c>
+      <c r="EM31" s="111"/>
+      <c r="EN31" s="111"/>
       <c r="EO31" s="111"/>
       <c r="EP31" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="EQ31" s="111"/>
-      <c r="ER31" s="111"/>
+      <c r="EQ31" s="111" t="s">
+        <v>738</v>
+      </c>
+      <c r="ER31" s="111" t="s">
+        <v>740</v>
+      </c>
       <c r="ES31" s="111"/>
       <c r="ET31" s="111" t="s">
         <v>114</v>
@@ -13408,12 +13628,18 @@
       <c r="FG31" s="111"/>
       <c r="FH31" s="111"/>
       <c r="FI31" s="111"/>
-      <c r="FJ31" s="160"/>
-      <c r="FK31" s="160"/>
-      <c r="FL31" s="160"/>
-      <c r="FM31" s="160"/>
-    </row>
-    <row r="32" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ31" s="111" t="s">
+        <v>114</v>
+      </c>
+      <c r="FK31" s="111"/>
+      <c r="FL31" s="111"/>
+      <c r="FM31" s="111"/>
+      <c r="FN31" s="160"/>
+      <c r="FO31" s="160"/>
+      <c r="FP31" s="160"/>
+      <c r="FQ31" s="160"/>
+    </row>
+    <row r="32" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="62" t="s">
         <v>93</v>
       </c>
@@ -13578,33 +13804,33 @@
       <c r="EJ32" s="111"/>
       <c r="EK32" s="111"/>
       <c r="EL32" s="111">
-        <v>0.6</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="EM32" s="111"/>
       <c r="EN32" s="111"/>
-      <c r="EO32" s="111" t="s">
-        <v>739</v>
-      </c>
+      <c r="EO32" s="111"/>
       <c r="EP32" s="111">
-        <v>1.5640000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="EQ32" s="111"/>
       <c r="ER32" s="111"/>
-      <c r="ES32" s="111"/>
+      <c r="ES32" s="111" t="s">
+        <v>739</v>
+      </c>
       <c r="ET32" s="111">
-        <v>0.83</v>
+        <v>1.5640000000000001</v>
       </c>
       <c r="EU32" s="111"/>
       <c r="EV32" s="111"/>
       <c r="EW32" s="111"/>
       <c r="EX32" s="111">
-        <v>0.03</v>
+        <v>0.83</v>
       </c>
       <c r="EY32" s="111"/>
       <c r="EZ32" s="111"/>
       <c r="FA32" s="111"/>
       <c r="FB32" s="111">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="FC32" s="111"/>
       <c r="FD32" s="111"/>
@@ -13615,12 +13841,18 @@
       <c r="FG32" s="111"/>
       <c r="FH32" s="111"/>
       <c r="FI32" s="111"/>
-      <c r="FJ32" s="160"/>
-      <c r="FK32" s="160"/>
-      <c r="FL32" s="160"/>
-      <c r="FM32" s="160"/>
-    </row>
-    <row r="33" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ32" s="111">
+        <v>1</v>
+      </c>
+      <c r="FK32" s="111"/>
+      <c r="FL32" s="111"/>
+      <c r="FM32" s="111"/>
+      <c r="FN32" s="160"/>
+      <c r="FO32" s="160"/>
+      <c r="FP32" s="160"/>
+      <c r="FQ32" s="160"/>
+    </row>
+    <row r="33" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="62" t="s">
         <v>92</v>
       </c>
@@ -13735,231 +13967,238 @@
       <c r="CZ33" s="111"/>
       <c r="DA33" s="111"/>
       <c r="DB33" s="111">
-        <f t="shared" ref="DB33:FE33" si="4">DB18</f>
+        <f t="shared" ref="DB33:EH33" si="3">DB18</f>
         <v>1</v>
       </c>
       <c r="DC33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DD33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DE33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DF33" s="111">
         <v>0.215</v>
       </c>
       <c r="DG33" s="111">
-        <f t="shared" ref="DG33:DI33" si="5">DG18</f>
+        <f t="shared" ref="DG33:DI33" si="4">DG18</f>
         <v>0.215</v>
       </c>
       <c r="DH33" s="111" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>Vanlersberghe2008Handbook</v>
       </c>
       <c r="DI33" s="111" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>p270</v>
       </c>
       <c r="DJ33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.33600000000000002</v>
       </c>
       <c r="DK33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DL33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DM33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DN33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="DO33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DP33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DQ33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DR33" s="111"/>
       <c r="DS33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DT33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DU33" s="111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="DV33" s="111"/>
       <c r="DW33" s="111" t="str">
-        <f t="shared" ref="DW33:DY33" si="6">DW18</f>
+        <f t="shared" ref="DW33:DY33" si="5">DW18</f>
         <v>8-12%</v>
       </c>
       <c r="DX33" s="111" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>Greenblatt1981Clinical</v>
       </c>
       <c r="DY33" s="111">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="DZ33" s="111">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="EA33" s="111">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="EB33" s="111">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="EC33" s="111">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="ED33" s="111">
+        <f t="shared" si="3"/>
+        <v>0.65</v>
+      </c>
+      <c r="EE33" s="111">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="EF33" s="111">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="EG33" s="111">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="EH33" s="111"/>
+      <c r="EI33" s="111">
+        <f t="shared" ref="DB33:FI33" si="6">EI18</f>
+        <v>0</v>
+      </c>
+      <c r="EJ33" s="111">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="DZ33" s="111">
-        <f t="shared" si="4"/>
+      <c r="EK33" s="111">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="EL33" s="111">
+        <f t="shared" ref="EL33:ES33" si="7">EL18</f>
+        <v>0.08</v>
+      </c>
+      <c r="EM33" s="111"/>
+      <c r="EN33" s="111"/>
+      <c r="EO33" s="111"/>
+      <c r="EP33" s="111">
+        <f t="shared" si="7"/>
         <v>0.05</v>
       </c>
-      <c r="EA33" s="111">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="EB33" s="111">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="EC33" s="111">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="ED33" s="111">
-        <f t="shared" si="4"/>
-        <v>0.65</v>
-      </c>
-      <c r="EE33" s="111">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="EF33" s="111">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="EG33" s="111">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="EH33" s="111"/>
-      <c r="EI33" s="111">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="EJ33" s="111">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="EK33" s="111">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="EL33" s="111">
-        <f t="shared" ref="EL33:EO33" si="7">EL18</f>
-        <v>0.05</v>
-      </c>
-      <c r="EM33" s="111">
+      <c r="EQ33" s="111">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="EN33" s="111">
+      <c r="ER33" s="111">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="EO33" s="111">
+      <c r="ES33" s="111">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="EP33" s="111">
-        <f t="shared" si="4"/>
+      <c r="ET33" s="111">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="EQ33" s="111">
-        <f t="shared" si="4"/>
+      <c r="EU33" s="111">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="ER33" s="111">
-        <f t="shared" si="4"/>
+      <c r="EV33" s="111">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="ES33" s="111">
-        <f t="shared" si="4"/>
+      <c r="EW33" s="111">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="ET33" s="111">
-        <f t="shared" si="4"/>
+      <c r="EX33" s="111">
+        <f t="shared" si="6"/>
         <v>0.25</v>
       </c>
-      <c r="EU33" s="111">
-        <f t="shared" si="4"/>
+      <c r="EY33" s="111">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="EV33" s="111">
-        <f t="shared" si="4"/>
+      <c r="EZ33" s="111">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="EW33" s="111">
-        <f t="shared" si="4"/>
+      <c r="FA33" s="111">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="EX33" s="111">
-        <f t="shared" si="4"/>
+      <c r="FB33" s="111">
+        <f t="shared" si="6"/>
         <v>0.03</v>
       </c>
-      <c r="EY33" s="111">
-        <f t="shared" si="4"/>
+      <c r="FC33" s="111">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="EZ33" s="111">
-        <f t="shared" si="4"/>
+      <c r="FD33" s="111">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="FA33" s="111">
-        <f t="shared" si="4"/>
+      <c r="FE33" s="111">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="FB33" s="111">
-        <f t="shared" si="4"/>
+      <c r="FF33" s="111">
+        <f t="shared" si="6"/>
         <v>0.7</v>
       </c>
-      <c r="FC33" s="111">
-        <f t="shared" si="4"/>
+      <c r="FG33" s="111">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="FD33" s="111">
-        <f t="shared" si="4"/>
+      <c r="FH33" s="111">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="FE33" s="111">
-        <f t="shared" si="4"/>
+      <c r="FI33" s="111">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="FF33" s="111">
+      <c r="FJ33" s="111">
         <v>0.8</v>
       </c>
-      <c r="FG33" s="111"/>
-      <c r="FH33" s="111"/>
-      <c r="FI33" s="111"/>
-      <c r="FJ33" s="160"/>
-      <c r="FK33" s="160"/>
-      <c r="FL33" s="160"/>
-      <c r="FM33" s="160"/>
-    </row>
-    <row r="34" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FK33" s="111"/>
+      <c r="FL33" s="111"/>
+      <c r="FM33" s="111"/>
+      <c r="FN33" s="160"/>
+      <c r="FO33" s="160"/>
+      <c r="FP33" s="160"/>
+      <c r="FQ33" s="160"/>
+    </row>
+    <row r="34" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="62" t="s">
         <v>89</v>
       </c>
@@ -14122,47 +14361,53 @@
       <c r="EJ34" s="111"/>
       <c r="EK34" s="111"/>
       <c r="EL34" s="111" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="EM34" s="111"/>
       <c r="EN34" s="111"/>
       <c r="EO34" s="111"/>
       <c r="EP34" s="111" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="EQ34" s="111"/>
       <c r="ER34" s="111"/>
       <c r="ES34" s="111"/>
       <c r="ET34" s="111" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="EU34" s="111"/>
       <c r="EV34" s="111"/>
       <c r="EW34" s="111"/>
       <c r="EX34" s="111" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="EY34" s="111"/>
       <c r="EZ34" s="111"/>
       <c r="FA34" s="111"/>
       <c r="FB34" s="111" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="FC34" s="111"/>
       <c r="FD34" s="111"/>
       <c r="FE34" s="111"/>
       <c r="FF34" s="111" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="FG34" s="111"/>
       <c r="FH34" s="111"/>
       <c r="FI34" s="111"/>
-      <c r="FJ34" s="160"/>
-      <c r="FK34" s="160"/>
-      <c r="FL34" s="160"/>
-      <c r="FM34" s="160"/>
-    </row>
-    <row r="35" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ34" s="111" t="s">
+        <v>116</v>
+      </c>
+      <c r="FK34" s="111"/>
+      <c r="FL34" s="111"/>
+      <c r="FM34" s="111"/>
+      <c r="FN34" s="160"/>
+      <c r="FO34" s="160"/>
+      <c r="FP34" s="160"/>
+      <c r="FQ34" s="160"/>
+    </row>
+    <row r="35" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="62" t="s">
         <v>91</v>
       </c>
@@ -14335,49 +14580,55 @@
       <c r="EJ35" s="111"/>
       <c r="EK35" s="111"/>
       <c r="EL35" s="111">
-        <v>-0.31</v>
+        <v>3.33</v>
       </c>
       <c r="EM35" s="111"/>
-      <c r="EN35" s="111" t="s">
-        <v>736</v>
-      </c>
+      <c r="EN35" s="111"/>
       <c r="EO35" s="111"/>
       <c r="EP35" s="111">
-        <v>1.5640000000000001</v>
+        <v>-0.31</v>
       </c>
       <c r="EQ35" s="111"/>
-      <c r="ER35" s="111"/>
+      <c r="ER35" s="111" t="s">
+        <v>736</v>
+      </c>
       <c r="ES35" s="111"/>
       <c r="ET35" s="111">
-        <v>1.46</v>
+        <v>1.5640000000000001</v>
       </c>
       <c r="EU35" s="111"/>
       <c r="EV35" s="111"/>
       <c r="EW35" s="111"/>
       <c r="EX35" s="111">
-        <v>3.79</v>
+        <v>1.46</v>
       </c>
       <c r="EY35" s="111"/>
       <c r="EZ35" s="111"/>
       <c r="FA35" s="111"/>
       <c r="FB35" s="111">
-        <v>2.77</v>
+        <v>3.79</v>
       </c>
       <c r="FC35" s="111"/>
       <c r="FD35" s="111"/>
       <c r="FE35" s="111"/>
       <c r="FF35" s="111">
-        <v>-1.5</v>
+        <v>2.77</v>
       </c>
       <c r="FG35" s="111"/>
       <c r="FH35" s="111"/>
       <c r="FI35" s="111"/>
-      <c r="FJ35" s="160"/>
-      <c r="FK35" s="160"/>
-      <c r="FL35" s="160"/>
-      <c r="FM35" s="160"/>
-    </row>
-    <row r="36" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ35" s="111">
+        <v>-1.5</v>
+      </c>
+      <c r="FK35" s="111"/>
+      <c r="FL35" s="111"/>
+      <c r="FM35" s="111"/>
+      <c r="FN35" s="160"/>
+      <c r="FO35" s="160"/>
+      <c r="FP35" s="160"/>
+      <c r="FQ35" s="160"/>
+    </row>
+    <row r="36" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="80" t="s">
         <v>340</v>
       </c>
@@ -14733,7 +14984,7 @@
       <c r="EK36" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL36" s="70"/>
+      <c r="EL36" s="110"/>
       <c r="EM36" s="110" t="s">
         <v>362</v>
       </c>
@@ -14763,7 +15014,7 @@
       <c r="EW36" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX36" s="112"/>
+      <c r="EX36" s="70"/>
       <c r="EY36" s="110" t="s">
         <v>362</v>
       </c>
@@ -14793,18 +15044,28 @@
       <c r="FI36" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ36" s="158"/>
-      <c r="FK36" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL36" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM36" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="37" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ36" s="112"/>
+      <c r="FK36" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL36" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM36" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN36" s="158"/>
+      <c r="FO36" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP36" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ36" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="37" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="64" t="s">
         <v>323</v>
       </c>
@@ -15018,12 +15279,18 @@
       <c r="FG37" s="115"/>
       <c r="FH37" s="115"/>
       <c r="FI37" s="115"/>
-      <c r="FJ37" s="161"/>
-      <c r="FK37" s="161"/>
-      <c r="FL37" s="161"/>
-      <c r="FM37" s="161"/>
-    </row>
-    <row r="38" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ37" s="115">
+        <v>0</v>
+      </c>
+      <c r="FK37" s="115"/>
+      <c r="FL37" s="115"/>
+      <c r="FM37" s="115"/>
+      <c r="FN37" s="161"/>
+      <c r="FO37" s="161"/>
+      <c r="FP37" s="161"/>
+      <c r="FQ37" s="161"/>
+    </row>
+    <row r="38" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="64" t="s">
         <v>324</v>
       </c>
@@ -15194,47 +15461,53 @@
       <c r="EJ38" s="115"/>
       <c r="EK38" s="115"/>
       <c r="EL38" s="115">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="EM38" s="115"/>
       <c r="EN38" s="115"/>
       <c r="EO38" s="115"/>
       <c r="EP38" s="115">
-        <v>0.15</v>
+        <v>0.35</v>
       </c>
       <c r="EQ38" s="115"/>
       <c r="ER38" s="115"/>
       <c r="ES38" s="115"/>
       <c r="ET38" s="115">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="EU38" s="115"/>
       <c r="EV38" s="115"/>
       <c r="EW38" s="115"/>
       <c r="EX38" s="115">
-        <v>-0.35</v>
+        <v>0</v>
       </c>
       <c r="EY38" s="115"/>
       <c r="EZ38" s="115"/>
       <c r="FA38" s="115"/>
       <c r="FB38" s="115">
-        <v>0</v>
+        <v>-0.35</v>
       </c>
       <c r="FC38" s="115"/>
       <c r="FD38" s="115"/>
       <c r="FE38" s="115"/>
       <c r="FF38" s="115">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="FG38" s="115"/>
       <c r="FH38" s="115"/>
       <c r="FI38" s="115"/>
-      <c r="FJ38" s="161"/>
-      <c r="FK38" s="161"/>
-      <c r="FL38" s="161"/>
-      <c r="FM38" s="161"/>
-    </row>
-    <row r="39" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ38" s="115">
+        <v>-0.1</v>
+      </c>
+      <c r="FK38" s="115"/>
+      <c r="FL38" s="115"/>
+      <c r="FM38" s="115"/>
+      <c r="FN38" s="161"/>
+      <c r="FO38" s="161"/>
+      <c r="FP38" s="161"/>
+      <c r="FQ38" s="161"/>
+    </row>
+    <row r="39" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="64" t="s">
         <v>325</v>
       </c>
@@ -15403,47 +15676,53 @@
       <c r="EJ39" s="115"/>
       <c r="EK39" s="115"/>
       <c r="EL39" s="115" t="s">
-        <v>744</v>
+        <v>762</v>
       </c>
       <c r="EM39" s="115"/>
       <c r="EN39" s="115"/>
       <c r="EO39" s="115"/>
       <c r="EP39" s="115" t="s">
-        <v>387</v>
+        <v>744</v>
       </c>
       <c r="EQ39" s="115"/>
       <c r="ER39" s="115"/>
       <c r="ES39" s="115"/>
       <c r="ET39" s="115" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="EU39" s="115"/>
       <c r="EV39" s="115"/>
       <c r="EW39" s="115"/>
       <c r="EX39" s="115" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="EY39" s="115"/>
       <c r="EZ39" s="115"/>
       <c r="FA39" s="115"/>
       <c r="FB39" s="115" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="FC39" s="115"/>
       <c r="FD39" s="115"/>
       <c r="FE39" s="115"/>
       <c r="FF39" s="115" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="FG39" s="115"/>
       <c r="FH39" s="115"/>
       <c r="FI39" s="115"/>
-      <c r="FJ39" s="161"/>
-      <c r="FK39" s="161"/>
-      <c r="FL39" s="161"/>
-      <c r="FM39" s="161"/>
-    </row>
-    <row r="40" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ39" s="115" t="s">
+        <v>391</v>
+      </c>
+      <c r="FK39" s="115"/>
+      <c r="FL39" s="115"/>
+      <c r="FM39" s="115"/>
+      <c r="FN39" s="161"/>
+      <c r="FO39" s="161"/>
+      <c r="FP39" s="161"/>
+      <c r="FQ39" s="161"/>
+    </row>
+    <row r="40" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="64" t="s">
         <v>640</v>
       </c>
@@ -15647,12 +15926,18 @@
       <c r="FG40" s="115"/>
       <c r="FH40" s="115"/>
       <c r="FI40" s="115"/>
-      <c r="FJ40" s="161"/>
-      <c r="FK40" s="161"/>
-      <c r="FL40" s="161"/>
-      <c r="FM40" s="161"/>
-    </row>
-    <row r="41" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ40" s="115">
+        <v>1</v>
+      </c>
+      <c r="FK40" s="115"/>
+      <c r="FL40" s="115"/>
+      <c r="FM40" s="115"/>
+      <c r="FN40" s="161"/>
+      <c r="FO40" s="161"/>
+      <c r="FP40" s="161"/>
+      <c r="FQ40" s="161"/>
+    </row>
+    <row r="41" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="64" t="s">
         <v>3</v>
       </c>
@@ -15823,47 +16108,53 @@
       <c r="EJ41" s="115"/>
       <c r="EK41" s="115"/>
       <c r="EL41" s="115">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="EM41" s="115"/>
       <c r="EN41" s="115"/>
       <c r="EO41" s="115"/>
       <c r="EP41" s="115">
-        <v>0.45</v>
+        <v>-0.2</v>
       </c>
       <c r="EQ41" s="115"/>
       <c r="ER41" s="115"/>
       <c r="ES41" s="115"/>
       <c r="ET41" s="115">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="EU41" s="115"/>
       <c r="EV41" s="115"/>
       <c r="EW41" s="115"/>
       <c r="EX41" s="115">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="EY41" s="115"/>
       <c r="EZ41" s="115"/>
       <c r="FA41" s="115"/>
       <c r="FB41" s="115">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="FC41" s="115"/>
       <c r="FD41" s="115"/>
       <c r="FE41" s="115"/>
       <c r="FF41" s="115">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="FG41" s="115"/>
       <c r="FH41" s="115"/>
       <c r="FI41" s="115"/>
-      <c r="FJ41" s="161"/>
-      <c r="FK41" s="161"/>
-      <c r="FL41" s="161"/>
-      <c r="FM41" s="161"/>
-    </row>
-    <row r="42" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ41" s="115">
+        <v>-0.1</v>
+      </c>
+      <c r="FK41" s="115"/>
+      <c r="FL41" s="115"/>
+      <c r="FM41" s="115"/>
+      <c r="FN41" s="161"/>
+      <c r="FO41" s="161"/>
+      <c r="FP41" s="161"/>
+      <c r="FQ41" s="161"/>
+    </row>
+    <row r="42" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="64" t="s">
         <v>326</v>
       </c>
@@ -16050,13 +16341,13 @@
       <c r="EV42" s="115"/>
       <c r="EW42" s="115"/>
       <c r="EX42" s="115">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="EY42" s="115"/>
       <c r="EZ42" s="115"/>
       <c r="FA42" s="115"/>
       <c r="FB42" s="115">
-        <v>1</v>
+        <v>-0.2</v>
       </c>
       <c r="FC42" s="115"/>
       <c r="FD42" s="115"/>
@@ -16067,12 +16358,18 @@
       <c r="FG42" s="115"/>
       <c r="FH42" s="115"/>
       <c r="FI42" s="115"/>
-      <c r="FJ42" s="161"/>
-      <c r="FK42" s="161"/>
-      <c r="FL42" s="161"/>
-      <c r="FM42" s="161"/>
-    </row>
-    <row r="43" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ42" s="115">
+        <v>1</v>
+      </c>
+      <c r="FK42" s="115"/>
+      <c r="FL42" s="115"/>
+      <c r="FM42" s="115"/>
+      <c r="FN42" s="161"/>
+      <c r="FO42" s="161"/>
+      <c r="FP42" s="161"/>
+      <c r="FQ42" s="161"/>
+    </row>
+    <row r="43" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="64" t="s">
         <v>639</v>
       </c>
@@ -16269,7 +16566,7 @@
         <v>648</v>
       </c>
       <c r="EL43" s="115">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="EM43" s="115"/>
       <c r="EN43" s="115"/>
@@ -16287,19 +16584,17 @@
       <c r="EV43" s="115"/>
       <c r="EW43" s="115"/>
       <c r="EX43" s="115">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="EY43" s="115"/>
-      <c r="EZ43" s="115" t="s">
-        <v>651</v>
-      </c>
+      <c r="EZ43" s="115"/>
       <c r="FA43" s="115"/>
       <c r="FB43" s="115">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="FC43" s="115"/>
       <c r="FD43" s="115" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="FE43" s="115"/>
       <c r="FF43" s="115">
@@ -16310,12 +16605,20 @@
         <v>649</v>
       </c>
       <c r="FI43" s="115"/>
-      <c r="FJ43" s="161"/>
-      <c r="FK43" s="161"/>
-      <c r="FL43" s="161"/>
-      <c r="FM43" s="161"/>
-    </row>
-    <row r="44" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ43" s="115">
+        <v>0</v>
+      </c>
+      <c r="FK43" s="115"/>
+      <c r="FL43" s="115" t="s">
+        <v>649</v>
+      </c>
+      <c r="FM43" s="115"/>
+      <c r="FN43" s="161"/>
+      <c r="FO43" s="161"/>
+      <c r="FP43" s="161"/>
+      <c r="FQ43" s="161"/>
+    </row>
+    <row r="44" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="64" t="s">
         <v>638</v>
       </c>
@@ -16545,12 +16848,18 @@
       <c r="FG44" s="115"/>
       <c r="FH44" s="115"/>
       <c r="FI44" s="115"/>
-      <c r="FJ44" s="161"/>
-      <c r="FK44" s="161"/>
-      <c r="FL44" s="161"/>
-      <c r="FM44" s="161"/>
-    </row>
-    <row r="45" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ44" s="115">
+        <v>0</v>
+      </c>
+      <c r="FK44" s="115"/>
+      <c r="FL44" s="115"/>
+      <c r="FM44" s="115"/>
+      <c r="FN44" s="161"/>
+      <c r="FO44" s="161"/>
+      <c r="FP44" s="161"/>
+      <c r="FQ44" s="161"/>
+    </row>
+    <row r="45" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="64" t="s">
         <v>4</v>
       </c>
@@ -16721,31 +17030,31 @@
       <c r="EJ45" s="115"/>
       <c r="EK45" s="115"/>
       <c r="EL45" s="115">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="EM45" s="115"/>
       <c r="EN45" s="115"/>
       <c r="EO45" s="115"/>
       <c r="EP45" s="115">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="EQ45" s="115"/>
       <c r="ER45" s="115"/>
       <c r="ES45" s="115"/>
       <c r="ET45" s="115">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="EU45" s="115"/>
       <c r="EV45" s="115"/>
       <c r="EW45" s="115"/>
       <c r="EX45" s="115">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="EY45" s="115"/>
       <c r="EZ45" s="115"/>
       <c r="FA45" s="115"/>
       <c r="FB45" s="115">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="FC45" s="115"/>
       <c r="FD45" s="115"/>
@@ -16756,12 +17065,18 @@
       <c r="FG45" s="115"/>
       <c r="FH45" s="115"/>
       <c r="FI45" s="115"/>
-      <c r="FJ45" s="161"/>
-      <c r="FK45" s="161"/>
-      <c r="FL45" s="161"/>
-      <c r="FM45" s="161"/>
-    </row>
-    <row r="46" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ45" s="115">
+        <v>0</v>
+      </c>
+      <c r="FK45" s="115"/>
+      <c r="FL45" s="115"/>
+      <c r="FM45" s="115"/>
+      <c r="FN45" s="161"/>
+      <c r="FO45" s="161"/>
+      <c r="FP45" s="161"/>
+      <c r="FQ45" s="161"/>
+    </row>
+    <row r="46" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="64" t="s">
         <v>327</v>
       </c>
@@ -16930,7 +17245,7 @@
       <c r="EJ46" s="115"/>
       <c r="EK46" s="115"/>
       <c r="EL46" s="115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EM46" s="115"/>
       <c r="EN46" s="115"/>
@@ -16948,13 +17263,13 @@
       <c r="EV46" s="115"/>
       <c r="EW46" s="115"/>
       <c r="EX46" s="115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EY46" s="115"/>
       <c r="EZ46" s="115"/>
       <c r="FA46" s="115"/>
       <c r="FB46" s="115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FC46" s="115"/>
       <c r="FD46" s="115"/>
@@ -16965,12 +17280,18 @@
       <c r="FG46" s="115"/>
       <c r="FH46" s="115"/>
       <c r="FI46" s="115"/>
-      <c r="FJ46" s="161"/>
-      <c r="FK46" s="161"/>
-      <c r="FL46" s="161"/>
-      <c r="FM46" s="161"/>
-    </row>
-    <row r="47" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ46" s="115">
+        <v>0</v>
+      </c>
+      <c r="FK46" s="115"/>
+      <c r="FL46" s="115"/>
+      <c r="FM46" s="115"/>
+      <c r="FN46" s="161"/>
+      <c r="FO46" s="161"/>
+      <c r="FP46" s="161"/>
+      <c r="FQ46" s="161"/>
+    </row>
+    <row r="47" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="64" t="s">
         <v>328</v>
       </c>
@@ -17141,47 +17462,53 @@
       <c r="EJ47" s="115"/>
       <c r="EK47" s="115"/>
       <c r="EL47" s="115">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="EM47" s="115"/>
       <c r="EN47" s="115"/>
       <c r="EO47" s="115"/>
       <c r="EP47" s="115">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="EQ47" s="115"/>
       <c r="ER47" s="115"/>
       <c r="ES47" s="115"/>
       <c r="ET47" s="115">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="EU47" s="115"/>
       <c r="EV47" s="115"/>
       <c r="EW47" s="115"/>
       <c r="EX47" s="115">
-        <v>-0.35</v>
+        <v>0</v>
       </c>
       <c r="EY47" s="115"/>
       <c r="EZ47" s="115"/>
       <c r="FA47" s="115"/>
       <c r="FB47" s="115">
-        <v>0</v>
+        <v>-0.35</v>
       </c>
       <c r="FC47" s="115"/>
       <c r="FD47" s="115"/>
       <c r="FE47" s="115"/>
       <c r="FF47" s="115">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="FG47" s="115"/>
       <c r="FH47" s="115"/>
       <c r="FI47" s="115"/>
-      <c r="FJ47" s="161"/>
-      <c r="FK47" s="161"/>
-      <c r="FL47" s="161"/>
-      <c r="FM47" s="161"/>
-    </row>
-    <row r="48" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ47" s="115">
+        <v>-0.1</v>
+      </c>
+      <c r="FK47" s="115"/>
+      <c r="FL47" s="115"/>
+      <c r="FM47" s="115"/>
+      <c r="FN47" s="161"/>
+      <c r="FO47" s="161"/>
+      <c r="FP47" s="161"/>
+      <c r="FQ47" s="161"/>
+    </row>
+    <row r="48" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="64" t="s">
         <v>329</v>
       </c>
@@ -17350,7 +17677,7 @@
       <c r="EJ48" s="115"/>
       <c r="EK48" s="115"/>
       <c r="EL48" s="115">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="EM48" s="115"/>
       <c r="EN48" s="115"/>
@@ -17368,13 +17695,13 @@
       <c r="EV48" s="115"/>
       <c r="EW48" s="115"/>
       <c r="EX48" s="115">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="EY48" s="115"/>
       <c r="EZ48" s="115"/>
       <c r="FA48" s="115"/>
       <c r="FB48" s="115">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="FC48" s="115"/>
       <c r="FD48" s="115"/>
@@ -17385,12 +17712,18 @@
       <c r="FG48" s="115"/>
       <c r="FH48" s="115"/>
       <c r="FI48" s="115"/>
-      <c r="FJ48" s="161"/>
-      <c r="FK48" s="161"/>
-      <c r="FL48" s="161"/>
-      <c r="FM48" s="161"/>
-    </row>
-    <row r="49" spans="1:169" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ48" s="115">
+        <v>0</v>
+      </c>
+      <c r="FK48" s="115"/>
+      <c r="FL48" s="115"/>
+      <c r="FM48" s="115"/>
+      <c r="FN48" s="161"/>
+      <c r="FO48" s="161"/>
+      <c r="FP48" s="161"/>
+      <c r="FQ48" s="161"/>
+    </row>
+    <row r="49" spans="1:173" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="64" t="s">
         <v>636</v>
       </c>
@@ -17594,12 +17927,18 @@
       <c r="FG49" s="115"/>
       <c r="FH49" s="115"/>
       <c r="FI49" s="115"/>
-      <c r="FJ49" s="161"/>
-      <c r="FK49" s="161"/>
-      <c r="FL49" s="161"/>
-      <c r="FM49" s="161"/>
-    </row>
-    <row r="50" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ49" s="115">
+        <v>0</v>
+      </c>
+      <c r="FK49" s="115"/>
+      <c r="FL49" s="115"/>
+      <c r="FM49" s="115"/>
+      <c r="FN49" s="161"/>
+      <c r="FO49" s="161"/>
+      <c r="FP49" s="161"/>
+      <c r="FQ49" s="161"/>
+    </row>
+    <row r="50" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="63" t="s">
         <v>607</v>
       </c>
@@ -17953,7 +18292,7 @@
       <c r="EK50" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL50" s="70"/>
+      <c r="EL50" s="110"/>
       <c r="EM50" s="110" t="s">
         <v>362</v>
       </c>
@@ -17983,7 +18322,7 @@
       <c r="EW50" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX50" s="112"/>
+      <c r="EX50" s="70"/>
       <c r="EY50" s="110" t="s">
         <v>362</v>
       </c>
@@ -18013,18 +18352,28 @@
       <c r="FI50" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ50" s="158"/>
-      <c r="FK50" s="158" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL50" s="158" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM50" s="158" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="51" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ50" s="112"/>
+      <c r="FK50" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL50" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM50" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN50" s="158"/>
+      <c r="FO50" s="158" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP50" s="158" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ50" s="158" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="51" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="65" t="s">
         <v>115</v>
       </c>
@@ -18179,7 +18528,7 @@
       <c r="EI51" s="113"/>
       <c r="EJ51" s="113"/>
       <c r="EK51" s="113"/>
-      <c r="EL51" s="71"/>
+      <c r="EL51" s="113"/>
       <c r="EM51" s="113"/>
       <c r="EN51" s="113"/>
       <c r="EO51" s="113"/>
@@ -18191,7 +18540,7 @@
       <c r="EU51" s="113"/>
       <c r="EV51" s="113"/>
       <c r="EW51" s="113"/>
-      <c r="EX51" s="113"/>
+      <c r="EX51" s="71"/>
       <c r="EY51" s="113"/>
       <c r="EZ51" s="113"/>
       <c r="FA51" s="113"/>
@@ -18203,12 +18552,16 @@
       <c r="FG51" s="113"/>
       <c r="FH51" s="113"/>
       <c r="FI51" s="113"/>
-      <c r="FJ51" s="163"/>
-      <c r="FK51" s="163"/>
-      <c r="FL51" s="163"/>
-      <c r="FM51" s="163"/>
-    </row>
-    <row r="52" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ51" s="113"/>
+      <c r="FK51" s="113"/>
+      <c r="FL51" s="113"/>
+      <c r="FM51" s="113"/>
+      <c r="FN51" s="163"/>
+      <c r="FO51" s="163"/>
+      <c r="FP51" s="163"/>
+      <c r="FQ51" s="163"/>
+    </row>
+    <row r="52" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="63" t="s">
         <v>604</v>
       </c>
@@ -18562,7 +18915,7 @@
       <c r="EK52" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL52" s="70"/>
+      <c r="EL52" s="110"/>
       <c r="EM52" s="110" t="s">
         <v>362</v>
       </c>
@@ -18592,7 +18945,7 @@
       <c r="EW52" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX52" s="112"/>
+      <c r="EX52" s="70"/>
       <c r="EY52" s="110" t="s">
         <v>362</v>
       </c>
@@ -18622,18 +18975,28 @@
       <c r="FI52" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ52" s="158"/>
-      <c r="FK52" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL52" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM52" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="53" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ52" s="112"/>
+      <c r="FK52" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL52" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM52" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN52" s="158"/>
+      <c r="FO52" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP52" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ52" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="53" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="65" t="s">
         <v>115</v>
       </c>
@@ -18788,7 +19151,7 @@
       <c r="EI53" s="113"/>
       <c r="EJ53" s="113"/>
       <c r="EK53" s="113"/>
-      <c r="EL53" s="71"/>
+      <c r="EL53" s="113"/>
       <c r="EM53" s="113"/>
       <c r="EN53" s="113"/>
       <c r="EO53" s="113"/>
@@ -18800,7 +19163,7 @@
       <c r="EU53" s="113"/>
       <c r="EV53" s="113"/>
       <c r="EW53" s="113"/>
-      <c r="EX53" s="113"/>
+      <c r="EX53" s="71"/>
       <c r="EY53" s="113"/>
       <c r="EZ53" s="113"/>
       <c r="FA53" s="113"/>
@@ -18812,12 +19175,16 @@
       <c r="FG53" s="113"/>
       <c r="FH53" s="113"/>
       <c r="FI53" s="113"/>
-      <c r="FJ53" s="163"/>
-      <c r="FK53" s="163"/>
-      <c r="FL53" s="163"/>
-      <c r="FM53" s="163"/>
-    </row>
-    <row r="54" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ53" s="113"/>
+      <c r="FK53" s="113"/>
+      <c r="FL53" s="113"/>
+      <c r="FM53" s="113"/>
+      <c r="FN53" s="163"/>
+      <c r="FO53" s="163"/>
+      <c r="FP53" s="163"/>
+      <c r="FQ53" s="163"/>
+    </row>
+    <row r="54" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="63" t="s">
         <v>603</v>
       </c>
@@ -19171,7 +19538,7 @@
       <c r="EK54" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL54" s="70"/>
+      <c r="EL54" s="110"/>
       <c r="EM54" s="110" t="s">
         <v>362</v>
       </c>
@@ -19201,7 +19568,7 @@
       <c r="EW54" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX54" s="112"/>
+      <c r="EX54" s="70"/>
       <c r="EY54" s="110" t="s">
         <v>362</v>
       </c>
@@ -19231,18 +19598,28 @@
       <c r="FI54" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ54" s="158"/>
-      <c r="FK54" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL54" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM54" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="55" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ54" s="112"/>
+      <c r="FK54" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL54" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM54" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN54" s="158"/>
+      <c r="FO54" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP54" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ54" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="55" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="65" t="s">
         <v>115</v>
       </c>
@@ -19397,7 +19774,7 @@
       <c r="EI55" s="113"/>
       <c r="EJ55" s="113"/>
       <c r="EK55" s="113"/>
-      <c r="EL55" s="71"/>
+      <c r="EL55" s="113"/>
       <c r="EM55" s="113"/>
       <c r="EN55" s="113"/>
       <c r="EO55" s="113"/>
@@ -19409,7 +19786,7 @@
       <c r="EU55" s="113"/>
       <c r="EV55" s="113"/>
       <c r="EW55" s="113"/>
-      <c r="EX55" s="113"/>
+      <c r="EX55" s="71"/>
       <c r="EY55" s="113"/>
       <c r="EZ55" s="113"/>
       <c r="FA55" s="113"/>
@@ -19421,12 +19798,16 @@
       <c r="FG55" s="113"/>
       <c r="FH55" s="113"/>
       <c r="FI55" s="113"/>
-      <c r="FJ55" s="163"/>
-      <c r="FK55" s="163"/>
-      <c r="FL55" s="163"/>
-      <c r="FM55" s="163"/>
-    </row>
-    <row r="56" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ55" s="113"/>
+      <c r="FK55" s="113"/>
+      <c r="FL55" s="113"/>
+      <c r="FM55" s="113"/>
+      <c r="FN55" s="163"/>
+      <c r="FO55" s="163"/>
+      <c r="FP55" s="163"/>
+      <c r="FQ55" s="163"/>
+    </row>
+    <row r="56" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="63" t="s">
         <v>608</v>
       </c>
@@ -19780,7 +20161,7 @@
       <c r="EK56" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL56" s="70"/>
+      <c r="EL56" s="110"/>
       <c r="EM56" s="110" t="s">
         <v>362</v>
       </c>
@@ -19810,7 +20191,7 @@
       <c r="EW56" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX56" s="112"/>
+      <c r="EX56" s="70"/>
       <c r="EY56" s="110" t="s">
         <v>362</v>
       </c>
@@ -19840,18 +20221,28 @@
       <c r="FI56" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ56" s="158"/>
-      <c r="FK56" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL56" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM56" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="57" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ56" s="112"/>
+      <c r="FK56" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL56" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM56" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN56" s="158"/>
+      <c r="FO56" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP56" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ56" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="57" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="65" t="s">
         <v>115</v>
       </c>
@@ -20006,7 +20397,7 @@
       <c r="EI57" s="113"/>
       <c r="EJ57" s="113"/>
       <c r="EK57" s="113"/>
-      <c r="EL57" s="71"/>
+      <c r="EL57" s="113"/>
       <c r="EM57" s="113"/>
       <c r="EN57" s="113"/>
       <c r="EO57" s="113"/>
@@ -20018,7 +20409,7 @@
       <c r="EU57" s="113"/>
       <c r="EV57" s="113"/>
       <c r="EW57" s="113"/>
-      <c r="EX57" s="113"/>
+      <c r="EX57" s="71"/>
       <c r="EY57" s="113"/>
       <c r="EZ57" s="113"/>
       <c r="FA57" s="113"/>
@@ -20030,12 +20421,16 @@
       <c r="FG57" s="113"/>
       <c r="FH57" s="113"/>
       <c r="FI57" s="113"/>
-      <c r="FJ57" s="163"/>
-      <c r="FK57" s="163"/>
-      <c r="FL57" s="163"/>
-      <c r="FM57" s="163"/>
-    </row>
-    <row r="58" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ57" s="113"/>
+      <c r="FK57" s="113"/>
+      <c r="FL57" s="113"/>
+      <c r="FM57" s="113"/>
+      <c r="FN57" s="163"/>
+      <c r="FO57" s="163"/>
+      <c r="FP57" s="163"/>
+      <c r="FQ57" s="163"/>
+    </row>
+    <row r="58" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="63" t="s">
         <v>613</v>
       </c>
@@ -20389,7 +20784,7 @@
       <c r="EK58" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL58" s="70"/>
+      <c r="EL58" s="110"/>
       <c r="EM58" s="110" t="s">
         <v>362</v>
       </c>
@@ -20419,7 +20814,7 @@
       <c r="EW58" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX58" s="112"/>
+      <c r="EX58" s="70"/>
       <c r="EY58" s="110" t="s">
         <v>362</v>
       </c>
@@ -20449,18 +20844,28 @@
       <c r="FI58" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ58" s="158"/>
-      <c r="FK58" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL58" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM58" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="59" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ58" s="112"/>
+      <c r="FK58" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL58" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM58" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN58" s="158"/>
+      <c r="FO58" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP58" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ58" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="59" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="65" t="s">
         <v>115</v>
       </c>
@@ -20615,7 +21020,7 @@
       <c r="EI59" s="113"/>
       <c r="EJ59" s="113"/>
       <c r="EK59" s="113"/>
-      <c r="EL59" s="71"/>
+      <c r="EL59" s="113"/>
       <c r="EM59" s="113"/>
       <c r="EN59" s="113"/>
       <c r="EO59" s="113"/>
@@ -20627,7 +21032,7 @@
       <c r="EU59" s="113"/>
       <c r="EV59" s="113"/>
       <c r="EW59" s="113"/>
-      <c r="EX59" s="113"/>
+      <c r="EX59" s="71"/>
       <c r="EY59" s="113"/>
       <c r="EZ59" s="113"/>
       <c r="FA59" s="113"/>
@@ -20639,12 +21044,16 @@
       <c r="FG59" s="113"/>
       <c r="FH59" s="113"/>
       <c r="FI59" s="113"/>
-      <c r="FJ59" s="163"/>
-      <c r="FK59" s="163"/>
-      <c r="FL59" s="163"/>
-      <c r="FM59" s="163"/>
-    </row>
-    <row r="60" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ59" s="113"/>
+      <c r="FK59" s="113"/>
+      <c r="FL59" s="113"/>
+      <c r="FM59" s="113"/>
+      <c r="FN59" s="163"/>
+      <c r="FO59" s="163"/>
+      <c r="FP59" s="163"/>
+      <c r="FQ59" s="163"/>
+    </row>
+    <row r="60" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="63" t="s">
         <v>614</v>
       </c>
@@ -20998,7 +21407,7 @@
       <c r="EK60" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL60" s="70"/>
+      <c r="EL60" s="110"/>
       <c r="EM60" s="110" t="s">
         <v>362</v>
       </c>
@@ -21028,7 +21437,7 @@
       <c r="EW60" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX60" s="112"/>
+      <c r="EX60" s="70"/>
       <c r="EY60" s="110" t="s">
         <v>362</v>
       </c>
@@ -21058,18 +21467,28 @@
       <c r="FI60" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ60" s="158"/>
-      <c r="FK60" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL60" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM60" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="61" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ60" s="112"/>
+      <c r="FK60" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL60" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM60" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN60" s="158"/>
+      <c r="FO60" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP60" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ60" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="61" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="65" t="s">
         <v>115</v>
       </c>
@@ -21224,7 +21643,7 @@
       <c r="EI61" s="113"/>
       <c r="EJ61" s="113"/>
       <c r="EK61" s="113"/>
-      <c r="EL61" s="71"/>
+      <c r="EL61" s="113"/>
       <c r="EM61" s="113"/>
       <c r="EN61" s="113"/>
       <c r="EO61" s="113"/>
@@ -21236,7 +21655,7 @@
       <c r="EU61" s="113"/>
       <c r="EV61" s="113"/>
       <c r="EW61" s="113"/>
-      <c r="EX61" s="113"/>
+      <c r="EX61" s="71"/>
       <c r="EY61" s="113"/>
       <c r="EZ61" s="113"/>
       <c r="FA61" s="113"/>
@@ -21248,12 +21667,16 @@
       <c r="FG61" s="113"/>
       <c r="FH61" s="113"/>
       <c r="FI61" s="113"/>
-      <c r="FJ61" s="163"/>
-      <c r="FK61" s="163"/>
-      <c r="FL61" s="163"/>
-      <c r="FM61" s="163"/>
-    </row>
-    <row r="62" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ61" s="113"/>
+      <c r="FK61" s="113"/>
+      <c r="FL61" s="113"/>
+      <c r="FM61" s="113"/>
+      <c r="FN61" s="163"/>
+      <c r="FO61" s="163"/>
+      <c r="FP61" s="163"/>
+      <c r="FQ61" s="163"/>
+    </row>
+    <row r="62" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="63" t="s">
         <v>610</v>
       </c>
@@ -21607,7 +22030,7 @@
       <c r="EK62" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL62" s="70"/>
+      <c r="EL62" s="110"/>
       <c r="EM62" s="110" t="s">
         <v>362</v>
       </c>
@@ -21637,7 +22060,7 @@
       <c r="EW62" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX62" s="112"/>
+      <c r="EX62" s="70"/>
       <c r="EY62" s="110" t="s">
         <v>362</v>
       </c>
@@ -21667,18 +22090,28 @@
       <c r="FI62" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ62" s="158"/>
-      <c r="FK62" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL62" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM62" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="63" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ62" s="112"/>
+      <c r="FK62" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL62" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM62" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN62" s="158"/>
+      <c r="FO62" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP62" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ62" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="63" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="65" t="s">
         <v>115</v>
       </c>
@@ -21833,7 +22266,7 @@
       <c r="EI63" s="113"/>
       <c r="EJ63" s="113"/>
       <c r="EK63" s="113"/>
-      <c r="EL63" s="71"/>
+      <c r="EL63" s="113"/>
       <c r="EM63" s="113"/>
       <c r="EN63" s="113"/>
       <c r="EO63" s="113"/>
@@ -21845,7 +22278,7 @@
       <c r="EU63" s="113"/>
       <c r="EV63" s="113"/>
       <c r="EW63" s="113"/>
-      <c r="EX63" s="113"/>
+      <c r="EX63" s="71"/>
       <c r="EY63" s="113"/>
       <c r="EZ63" s="113"/>
       <c r="FA63" s="113"/>
@@ -21857,12 +22290,16 @@
       <c r="FG63" s="113"/>
       <c r="FH63" s="113"/>
       <c r="FI63" s="113"/>
-      <c r="FJ63" s="163"/>
-      <c r="FK63" s="163"/>
-      <c r="FL63" s="163"/>
-      <c r="FM63" s="163"/>
-    </row>
-    <row r="64" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ63" s="113"/>
+      <c r="FK63" s="113"/>
+      <c r="FL63" s="113"/>
+      <c r="FM63" s="113"/>
+      <c r="FN63" s="163"/>
+      <c r="FO63" s="163"/>
+      <c r="FP63" s="163"/>
+      <c r="FQ63" s="163"/>
+    </row>
+    <row r="64" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="63" t="s">
         <v>605</v>
       </c>
@@ -22216,7 +22653,7 @@
       <c r="EK64" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL64" s="70"/>
+      <c r="EL64" s="110"/>
       <c r="EM64" s="110" t="s">
         <v>362</v>
       </c>
@@ -22246,7 +22683,7 @@
       <c r="EW64" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX64" s="112"/>
+      <c r="EX64" s="70"/>
       <c r="EY64" s="110" t="s">
         <v>362</v>
       </c>
@@ -22276,18 +22713,28 @@
       <c r="FI64" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ64" s="158"/>
-      <c r="FK64" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL64" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM64" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="65" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ64" s="112"/>
+      <c r="FK64" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL64" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM64" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN64" s="158"/>
+      <c r="FO64" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP64" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ64" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="65" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="65" t="s">
         <v>115</v>
       </c>
@@ -22442,7 +22889,7 @@
       <c r="EI65" s="113"/>
       <c r="EJ65" s="113"/>
       <c r="EK65" s="113"/>
-      <c r="EL65" s="71"/>
+      <c r="EL65" s="113"/>
       <c r="EM65" s="113"/>
       <c r="EN65" s="113"/>
       <c r="EO65" s="113"/>
@@ -22454,7 +22901,7 @@
       <c r="EU65" s="113"/>
       <c r="EV65" s="113"/>
       <c r="EW65" s="113"/>
-      <c r="EX65" s="113"/>
+      <c r="EX65" s="71"/>
       <c r="EY65" s="113"/>
       <c r="EZ65" s="113"/>
       <c r="FA65" s="113"/>
@@ -22466,12 +22913,16 @@
       <c r="FG65" s="113"/>
       <c r="FH65" s="113"/>
       <c r="FI65" s="113"/>
-      <c r="FJ65" s="163"/>
-      <c r="FK65" s="163"/>
-      <c r="FL65" s="163"/>
-      <c r="FM65" s="163"/>
-    </row>
-    <row r="66" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ65" s="113"/>
+      <c r="FK65" s="113"/>
+      <c r="FL65" s="113"/>
+      <c r="FM65" s="113"/>
+      <c r="FN65" s="163"/>
+      <c r="FO65" s="163"/>
+      <c r="FP65" s="163"/>
+      <c r="FQ65" s="163"/>
+    </row>
+    <row r="66" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="63" t="s">
         <v>602</v>
       </c>
@@ -22825,7 +23276,7 @@
       <c r="EK66" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL66" s="70"/>
+      <c r="EL66" s="110"/>
       <c r="EM66" s="110" t="s">
         <v>362</v>
       </c>
@@ -22855,7 +23306,7 @@
       <c r="EW66" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX66" s="112"/>
+      <c r="EX66" s="70"/>
       <c r="EY66" s="110" t="s">
         <v>362</v>
       </c>
@@ -22885,18 +23336,28 @@
       <c r="FI66" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ66" s="158"/>
-      <c r="FK66" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL66" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM66" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="67" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ66" s="112"/>
+      <c r="FK66" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL66" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM66" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN66" s="158"/>
+      <c r="FO66" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP66" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ66" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="67" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="65" t="s">
         <v>115</v>
       </c>
@@ -23051,7 +23512,7 @@
       <c r="EI67" s="113"/>
       <c r="EJ67" s="113"/>
       <c r="EK67" s="113"/>
-      <c r="EL67" s="71"/>
+      <c r="EL67" s="113"/>
       <c r="EM67" s="113"/>
       <c r="EN67" s="113"/>
       <c r="EO67" s="113"/>
@@ -23063,7 +23524,7 @@
       <c r="EU67" s="113"/>
       <c r="EV67" s="113"/>
       <c r="EW67" s="113"/>
-      <c r="EX67" s="113"/>
+      <c r="EX67" s="71"/>
       <c r="EY67" s="113"/>
       <c r="EZ67" s="113"/>
       <c r="FA67" s="113"/>
@@ -23075,12 +23536,16 @@
       <c r="FG67" s="113"/>
       <c r="FH67" s="113"/>
       <c r="FI67" s="113"/>
-      <c r="FJ67" s="163"/>
-      <c r="FK67" s="163"/>
-      <c r="FL67" s="163"/>
-      <c r="FM67" s="163"/>
-    </row>
-    <row r="68" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ67" s="113"/>
+      <c r="FK67" s="113"/>
+      <c r="FL67" s="113"/>
+      <c r="FM67" s="113"/>
+      <c r="FN67" s="163"/>
+      <c r="FO67" s="163"/>
+      <c r="FP67" s="163"/>
+      <c r="FQ67" s="163"/>
+    </row>
+    <row r="68" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="63" t="s">
         <v>611</v>
       </c>
@@ -23434,7 +23899,7 @@
       <c r="EK68" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL68" s="70"/>
+      <c r="EL68" s="110"/>
       <c r="EM68" s="110" t="s">
         <v>362</v>
       </c>
@@ -23464,7 +23929,7 @@
       <c r="EW68" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX68" s="112"/>
+      <c r="EX68" s="70"/>
       <c r="EY68" s="110" t="s">
         <v>362</v>
       </c>
@@ -23494,18 +23959,28 @@
       <c r="FI68" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ68" s="158"/>
-      <c r="FK68" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL68" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM68" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="69" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ68" s="112"/>
+      <c r="FK68" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL68" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM68" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN68" s="158"/>
+      <c r="FO68" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP68" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ68" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="69" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="65" t="s">
         <v>115</v>
       </c>
@@ -23660,7 +24135,7 @@
       <c r="EI69" s="113"/>
       <c r="EJ69" s="113"/>
       <c r="EK69" s="113"/>
-      <c r="EL69" s="71"/>
+      <c r="EL69" s="113"/>
       <c r="EM69" s="113"/>
       <c r="EN69" s="113"/>
       <c r="EO69" s="113"/>
@@ -23672,7 +24147,7 @@
       <c r="EU69" s="113"/>
       <c r="EV69" s="113"/>
       <c r="EW69" s="113"/>
-      <c r="EX69" s="113"/>
+      <c r="EX69" s="71"/>
       <c r="EY69" s="113"/>
       <c r="EZ69" s="113"/>
       <c r="FA69" s="113"/>
@@ -23684,12 +24159,16 @@
       <c r="FG69" s="113"/>
       <c r="FH69" s="113"/>
       <c r="FI69" s="113"/>
-      <c r="FJ69" s="163"/>
-      <c r="FK69" s="163"/>
-      <c r="FL69" s="163"/>
-      <c r="FM69" s="163"/>
-    </row>
-    <row r="70" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ69" s="113"/>
+      <c r="FK69" s="113"/>
+      <c r="FL69" s="113"/>
+      <c r="FM69" s="113"/>
+      <c r="FN69" s="163"/>
+      <c r="FO69" s="163"/>
+      <c r="FP69" s="163"/>
+      <c r="FQ69" s="163"/>
+    </row>
+    <row r="70" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="63" t="s">
         <v>612</v>
       </c>
@@ -24043,7 +24522,7 @@
       <c r="EK70" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL70" s="70"/>
+      <c r="EL70" s="110"/>
       <c r="EM70" s="110" t="s">
         <v>362</v>
       </c>
@@ -24073,7 +24552,7 @@
       <c r="EW70" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX70" s="112"/>
+      <c r="EX70" s="70"/>
       <c r="EY70" s="110" t="s">
         <v>362</v>
       </c>
@@ -24103,18 +24582,28 @@
       <c r="FI70" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ70" s="158"/>
-      <c r="FK70" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL70" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM70" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="71" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ70" s="112"/>
+      <c r="FK70" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL70" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM70" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN70" s="158"/>
+      <c r="FO70" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP70" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ70" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="71" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="65" t="s">
         <v>115</v>
       </c>
@@ -24269,7 +24758,7 @@
       <c r="EI71" s="113"/>
       <c r="EJ71" s="113"/>
       <c r="EK71" s="113"/>
-      <c r="EL71" s="71"/>
+      <c r="EL71" s="113"/>
       <c r="EM71" s="113"/>
       <c r="EN71" s="113"/>
       <c r="EO71" s="113"/>
@@ -24281,7 +24770,7 @@
       <c r="EU71" s="113"/>
       <c r="EV71" s="113"/>
       <c r="EW71" s="113"/>
-      <c r="EX71" s="113"/>
+      <c r="EX71" s="71"/>
       <c r="EY71" s="113"/>
       <c r="EZ71" s="113"/>
       <c r="FA71" s="113"/>
@@ -24293,12 +24782,16 @@
       <c r="FG71" s="113"/>
       <c r="FH71" s="113"/>
       <c r="FI71" s="113"/>
-      <c r="FJ71" s="163"/>
-      <c r="FK71" s="163"/>
-      <c r="FL71" s="163"/>
-      <c r="FM71" s="163"/>
-    </row>
-    <row r="72" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ71" s="113"/>
+      <c r="FK71" s="113"/>
+      <c r="FL71" s="113"/>
+      <c r="FM71" s="113"/>
+      <c r="FN71" s="163"/>
+      <c r="FO71" s="163"/>
+      <c r="FP71" s="163"/>
+      <c r="FQ71" s="163"/>
+    </row>
+    <row r="72" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="63" t="s">
         <v>606</v>
       </c>
@@ -24652,7 +25145,7 @@
       <c r="EK72" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL72" s="70"/>
+      <c r="EL72" s="110"/>
       <c r="EM72" s="110" t="s">
         <v>362</v>
       </c>
@@ -24682,7 +25175,7 @@
       <c r="EW72" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX72" s="112"/>
+      <c r="EX72" s="70"/>
       <c r="EY72" s="110" t="s">
         <v>362</v>
       </c>
@@ -24712,18 +25205,28 @@
       <c r="FI72" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ72" s="158"/>
-      <c r="FK72" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL72" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM72" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="73" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ72" s="112"/>
+      <c r="FK72" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL72" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM72" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN72" s="158"/>
+      <c r="FO72" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP72" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ72" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="73" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="65" t="s">
         <v>115</v>
       </c>
@@ -24878,7 +25381,7 @@
       <c r="EI73" s="113"/>
       <c r="EJ73" s="113"/>
       <c r="EK73" s="113"/>
-      <c r="EL73" s="71"/>
+      <c r="EL73" s="113"/>
       <c r="EM73" s="113"/>
       <c r="EN73" s="113"/>
       <c r="EO73" s="113"/>
@@ -24890,7 +25393,7 @@
       <c r="EU73" s="113"/>
       <c r="EV73" s="113"/>
       <c r="EW73" s="113"/>
-      <c r="EX73" s="113"/>
+      <c r="EX73" s="71"/>
       <c r="EY73" s="113"/>
       <c r="EZ73" s="113"/>
       <c r="FA73" s="113"/>
@@ -24902,12 +25405,16 @@
       <c r="FG73" s="113"/>
       <c r="FH73" s="113"/>
       <c r="FI73" s="113"/>
-      <c r="FJ73" s="163"/>
-      <c r="FK73" s="163"/>
-      <c r="FL73" s="163"/>
-      <c r="FM73" s="163"/>
-    </row>
-    <row r="74" spans="1:169" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="FJ73" s="113"/>
+      <c r="FK73" s="113"/>
+      <c r="FL73" s="113"/>
+      <c r="FM73" s="113"/>
+      <c r="FN73" s="163"/>
+      <c r="FO73" s="163"/>
+      <c r="FP73" s="163"/>
+      <c r="FQ73" s="163"/>
+    </row>
+    <row r="74" spans="1:173" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="63" t="s">
         <v>609</v>
       </c>
@@ -25261,7 +25768,7 @@
       <c r="EK74" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EL74" s="70"/>
+      <c r="EL74" s="110"/>
       <c r="EM74" s="110" t="s">
         <v>362</v>
       </c>
@@ -25291,7 +25798,7 @@
       <c r="EW74" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="EX74" s="112"/>
+      <c r="EX74" s="70"/>
       <c r="EY74" s="110" t="s">
         <v>362</v>
       </c>
@@ -25321,18 +25828,28 @@
       <c r="FI74" s="110" t="s">
         <v>364</v>
       </c>
-      <c r="FJ74" s="158"/>
-      <c r="FK74" s="159" t="s">
-        <v>362</v>
-      </c>
-      <c r="FL74" s="159" t="s">
-        <v>363</v>
-      </c>
-      <c r="FM74" s="159" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="75" spans="1:169" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FJ74" s="112"/>
+      <c r="FK74" s="110" t="s">
+        <v>362</v>
+      </c>
+      <c r="FL74" s="110" t="s">
+        <v>363</v>
+      </c>
+      <c r="FM74" s="110" t="s">
+        <v>364</v>
+      </c>
+      <c r="FN74" s="158"/>
+      <c r="FO74" s="159" t="s">
+        <v>362</v>
+      </c>
+      <c r="FP74" s="159" t="s">
+        <v>363</v>
+      </c>
+      <c r="FQ74" s="159" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="75" spans="1:173" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="65" t="s">
         <v>115</v>
       </c>
@@ -25487,7 +26004,7 @@
       <c r="EI75" s="113"/>
       <c r="EJ75" s="113"/>
       <c r="EK75" s="113"/>
-      <c r="EL75" s="71"/>
+      <c r="EL75" s="113"/>
       <c r="EM75" s="113"/>
       <c r="EN75" s="113"/>
       <c r="EO75" s="113"/>
@@ -25499,7 +26016,7 @@
       <c r="EU75" s="113"/>
       <c r="EV75" s="113"/>
       <c r="EW75" s="113"/>
-      <c r="EX75" s="113"/>
+      <c r="EX75" s="71"/>
       <c r="EY75" s="113"/>
       <c r="EZ75" s="113"/>
       <c r="FA75" s="113"/>
@@ -25511,10 +26028,14 @@
       <c r="FG75" s="113"/>
       <c r="FH75" s="113"/>
       <c r="FI75" s="113"/>
-      <c r="FJ75" s="163"/>
-      <c r="FK75" s="163"/>
-      <c r="FL75" s="163"/>
-      <c r="FM75" s="163"/>
+      <c r="FJ75" s="113"/>
+      <c r="FK75" s="113"/>
+      <c r="FL75" s="113"/>
+      <c r="FM75" s="113"/>
+      <c r="FN75" s="163"/>
+      <c r="FO75" s="163"/>
+      <c r="FP75" s="163"/>
+      <c r="FQ75" s="163"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update new vtach and vfib rhythms Fix a bit of logic for vtach rhythms
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04371603-DAF2-489B-9A1D-9D3E4E563D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B48499-7B53-4CF1-8DAA-5C667C921373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2350,16 +2350,16 @@
     <t>Type</t>
   </si>
   <si>
-    <t>0.905,0.975,1,0.96,0.975,1.205,1.255,1.275,1.145,0.85,0.715,0.74,0.8,0.775,0.655,0.475,0.315,0.255,0.19,0.15,0.135,0.085,0.075,-0.03,-0.125,-0.245,-0.245,-0.215,-0.215,-0.255,-0.37,-0.44,-0.365,-0.345,-0.375,-0.47,-0.67,-0.78,-0.69,-0.66,-0.7,-0.725,-0.8,-0.84,-0.725,-0.61,-0.575,-0.52,-0.42,-0.36,-0.26,-0.21,-0.185,-0.12,-0.05,0.115,0.31,0.455,0.655,0.81,0.785,0.785,0.77,0.795,0.93,1.05,1.11,1.07,1.045,1,1.015,1.04,1.08,1.03,1.035,0.99,0.93,0.855,0.75,0.59,0.47,0.385,0.285,0.34,0.39,0.255,0.12,-0.1,-0.3,-0.26,-0.12,-0.035,-0.085,-0.225,-0.365,-0.49,-0.47,-0.41,-0.46,-0.595,-0.705,-0.79,-0.86,-0.675,-0.655,-0.7,-0.725,-0.89,-0.895,-0.885,-0.885,-0.865,-0.77,-0.71,-0.585,-0.5,-0.52,-0.535,-0.42,-0.405,-0.28,-0.225,-0.215,-0.125,0,0.065,0.24,0.255,0.42,0.665,0.74,0.765,0.72,0.54,0.555,0.73,0.82,0.855,0.815,0.76,0.77,0.86,0.855,0.94,0.805,0.69,0.575,0.45,0.31,0.29,0.23,0.075,0.01,0.07,0.1,0.16,0.12,-0.05,-0.205,-0.365,-0.47,-0.31,-0.22,-0.14,-0.11,-0.21,-0.375,-0.49,-0.485,-0.385,-0.43,-0.415,-0.485,-0.7,-0.715,-0.67,-0.535,-0.385,-0.29,-0.235,-0.235,-0.245,-0.225,-0.19,-0.125,-0.08,-0.075,-0.075,-0.12,-0.025,0.025,0.075,0.11,0.155,0.22,0.24,0.365,0.415,0.37,0.535,0.57,0.58,0.705,0.81,0.805,0.755,0.805,0.86,0.93,0.96,0.81,0.65,0.585,0.6,0.67,0.6,0.38,0.19,0.045,0.05,0.12,0.24,0.195,0.08,-0.05,-0.16,-0.13,0,0.06,0.05,0.16,0.175,0.19,0.185,-0.035,-0.21,-0.23,-0.315,-0.33,-0.32,-0.365,-0.3,-0.25,-0.2,-0.37,-0.425,-0.51,-0.55,-0.535,-0.445,-0.32,-0.19,-0.04,-0.16,-0.2,-0.225,-0.295,-0.22,-0.21,-0.345,-0.295,-0.2,-0.12,0.045,0.11,0.18,0.23,0.325,0.425,0.645,0.71,0.755,0.72,0.645,0.645,0.73,0.725,0.65,0.475,0.345,0.265,0.27,0.28,0.23,0.22,0.24,0.27,0.26,0.255,0.17,0.1,0.095,0.16,0.21,0.24,0.255,0.2,0.135,0.175,0.215,0.285,0.335,0.32,0.34,0.25,0.325,0.36,0.455,0.46,0.28,0.115,-0.08,-0.155,-0.07,-0.045,0.095,0.145,0.06,0.045,-0.035,-0.11,-0.11,-0.105,-0.125,-0.05,0.095,0.27,0.18,0.11,0,-0.08,0.065,0.245,0.22,0.26,0.35,0.425,0.485,0.51,0.435,0.47,0.515,0.615,0.545,0.555,0.495,0.475,0.595,0.55,0.485,0.435,0.27,0.145,0.05,0.085,0.13,0.11,0.1,0.055,0.16,0.175,0.165,0.11,-0.065,-0.07,0.035,0.14,0.075,-0.08,-0.205,-0.3,-0.285,-0.235,-0.19,-0.23,-0.235,-0.175,-0.11,0.07,0.12,0.1,0.005,-0.125,-0.13,-0.08,0.14,0.31,0.27,0.215,0.07,-0.1,-0.08,0.18,0.24,0.23,0.22,0.14,0.095,0.245,0.39,0.4,0.445,0.47,0.5,0.545,0.645,0.72,0.775,0.865,0.86,0.76,0.67,0.555,0.44,0.47,0.49,0.455,0.365,0.265,0.145,0.15,0.2,0.27,0.285,0.25,0.255,0.295,0.335,0.345,0.405,0.455,0.415,0.33,0.155,-0.08,-0.115,-0.075,-0.07,-0.155,-0.32,-0.435,-0.465,-0.46,-0.465,-0.515,-0.48,-0.395,-0.445,-0.415,-0.435,-0.46,-0.385,-0.31,-0.33,-0.41,-0.4,-0.36,-0.3,-0.17,-0.1,-0.065,-0.045,-0.075,0,0.115,0.17,0.205,0.19,0.175,0.25,0.37,0.435,0.455,0.46,0.53,0.63,0.74,0.74,0.65,0.525,0.38,0.29,0.275,0.215,0.32,0.32,0.24,0.17,-0.05,-0.18,-0.18,-0.115,-0.07,-0.065,-0.08,-0.055,0,-0.025,-0.1,-0.115,-0.17,-0.13,0.01,-0.135,-0.325,-0.52,-0.72,-0.72,-0.55,-0.45,-0.45,-0.445,-0.5,-0.49,-0.49,-0.51,-0.53,-0.515,-0.43,-0.36,-0.345,-0.325,-0.3,-0.305,-0.195,-0.105,-0.06,0,0,-0.085,-0.145,-0.16,-0.12,-0.035,0.155,0.255,0.27,0.315,0.355,0.37,0.435,0.42,0.455,0.56,0.76,0.84,0.795,0.64,0.425,0.3,0.335,0.425,0.44,0.46,0.455,0.33,0.21,0.195,0.1,0.09,0.24,0.32,0.325,0.3,0.205,0.115,0.13,0.165,0.115,0.085,0.045,-0.09,-0.145,-0.21,-0.25,-0.32,-0.25,-0.24,-0.34,-0.465,-0.525,-0.65,-0.72,-0.66,-0.625,-0.62,-0.545,-0.49,-0.45,-0.33,-0.315,-0.33,-0.38,-0.455,-0.43,-0.335,-0.215,-0.13,-0.08,-0.09,-0.095,-0.085,-0.065,0.04,0.12,0.195,0.315,0.385,0.455,0.55,0.48,0.445,0.475,0.415,0.41,0.42,0.395,0.4,0.475,0.485,0.435,0.35,0.26,0.3,0.275,0.2,0.15,0.005,-0.145,-0.185,-0.25,-0.345,-0.43,-0.54,-0.66,-0.665,-0.685,-0.66,-0.6,-0.55,-0.49,-0.495,-0.565,-0.61,-0.605,-0.555,-0.54,-0.47,-0.45,-0.415,-0.3,-0.335,-0.365,-0.385,-0.445,-0.365,-0.34,-0.28,-0.235,-0.25,-0.2,-0.17,-0.11,-0.035,0.03,0.035,0.1,0.105,0.165,0.195,0.205,0.27,0.31,0.435,0.55,0.475,0.395,0.305,0.295,0.425,0.65,0.76,0.78,0.715,0.755,0.88,0.905,0.87,0.715,0.48,0.31,0.215,0.145,0.04,-0.1,-0.14,-0.185,-0.14,-0.155,-0.33,-0.5,-0.67,-0.74,-0.58,-0.43,-0.425,-0.445,-0.6,-0.74,-0.7,-0.585,-0.43,-0.305,-0.275,-0.275,-0.295,-0.275,-0.21,-0.195,-0.205,-0.085,-0.17,-0.28,-0.265,-0.305,-0.205,0.005,0.13,0.14,0.095,0.075,0.02,0.045,0.07,0.06,0.135,0.175,0.355,0.475,0.425,0.33,0.185,0.135,0.245,0.405,0.45,0.445,0.415,0.395,0.48,0.675,0.845,0.865,0.77,0.47,0.165,0.135,0.34,0.39,0.345,0.16,-0.13,-0.255,-0.235,-0.205,-0.325,-0.445,-0.53,-0.63,-0.74,-0.795,-0.8,-0.8,-0.795,-0.7,-0.73,-0.81,-0.825,-0.845,-0.76,-0.72,-0.58,-0.49,-0.505,-0.5,-0.48,-0.47,-0.38,-0.265,-0.22,-0.265,-0.32,-0.35,-0.26,-0.09,0.07,0.235,0.33,0.4,0.36,0.265,0.155,0.12,0.255,0.445,0.48,0.44,0.38,0.305,0.38,0.45,0.45,0.375,0.425,0.67,0.79,0.855,0.7,0.44,0.265,0.245,0.3,0.26,0.235,0.285,0.345,0.36,0.355,0.24,0.165,0.21,0.175,0.205,0.165,0.06,-0.07,-0.19,-0.305,-0.365,-0.32,-0.26,-0.33,-0.41,-0.5,-0.56,-0.49,-0.345,-0.3,-0.24,-0.145,-0.125,-0.15,-0.175,-0.17,-0.165,-0.045,0.085,0.04,0,-0.065,-0.07,0,0.055,0.08,0.12,0.195,0.17,0.155,0.135,0.09,0.21,0.2,0.195,0.34,0.285,0.28,0.28,0.085,-0.025,0.065,0.165,0.29,0.33,0.25,0.11,0.02,-0.065,-0.045,0.075,0.105,0.16,0.28,0.4,0.36,0.37,0.23,0.06,0.11,0.205,0.26,0.27,0.18,0.115,0.125,0.19,0.245,0.29,0.295,0.31,0.33,0.32,0.335,0.34,0.34,0.32,0.27,0.25,0.195,0.175,0.15,0.09,0.08,0.035,-0.08,-0.19,-0.325,-0.385,-0.32,-0.145,-0.05,0.06,0.035,0.045,0.09,0.105,0.14,0.12,0.135,0.195,0.24,0.24,0.235,0.155,0.135,0.19,0.19,0.18,0.08,-0.065,-0.2,-0.33,-0.405,-0.41,-0.37,-0.37,-0.38,-0.445,-0.485,-0.525,-0.47,-0.4,-0.37,-0.315,-0.24,-0.225,-0.14,-0.11,-0.09,-0.04,0.035,0.095,0.155,0.155,0.13,0.145,0.165,0.21,0.225,0.2,0.185,0.205,0.27,0.305,0.305,0.275,0.24,0.27,0.335,0.365,0.375,0.32,0.25,0.215,0.24,0.28,0.345,0.42,0.405,0.395,0.365,0.28,0.245,0.245,0.28,0.255,0.26,0.22,0.165,0.125,0.155,0.115,0,-0.165,-0.375,-0.575,-0.69,-0.81,-0.86,-0.915,-0.935,-0.92,-0.89,-0.895,-0.915,-0.95,-1.03,-1.045,-0.995,-0.91,-0.885,-0.845,-0.83,-0.795,-0.69,-0.635,-0.63,-0.64,-0.585,-0.5,-0.385,-0.305,-0.34,-0.38,-0.375,-0.365,-0.31,-0.24,-0.17,-0.075,0.07,0.18,0.255,0.32,0.395,0.44,0.505,0.555,0.54,0.535,0.535,0.52,0.56,0.57,0.565,0.54,0.485,0.5,0.47,0.475,0.405,0.305,0.18,0.105,0.05,-0.025,-0.165,-0.27,-0.36,-0.405,-0.33,-0.35,-0.36,-0.345,-0.405,-0.44,-0.48,-0.565,-0.595,-0.595,-0.62,-0.605,-0.535,-0.515,-0.435,-0.41,-0.44,-0.45,-0.46,-0.425,-0.415,-0.42,-0.435,-0.465,-0.5,-0.51,-0.495,-0.435,-0.355,-0.285,-0.25,-0.225,-0.175,-0.105,-0.065,-0.065,-0.095,-0.1,-0.085,-0.04,0.025,0.045,0.09,0.2,0.28,0.405,0.425,0.395,0.415,0.43,0.49,0.6,0.675,0.785,0.795,0.755,0.7,0.65,0.66,0.675,0.59,0.435,0.27,0.115,0.085,0.065,0.015,-0.105,-0.18,-0.225,-0.28,-0.295,-0.315,-0.295,-0.275,-0.305,-0.32,-0.34,-0.34,-0.295,-0.245,-0.22,-0.205,-0.21,-0.24,-0.235,-0.205,-0.125,-0.025,0.07,0.095,0.08,0.115,0.095,0.115,0.155,0.215,0.285,0.39,0.41,0.38,0.37,0.31,0.355,0.405,0.47,0.5,0.475,0.475,0.425,0.37,0.395,0.46,0.495,0.57,0.645,0.6,0.58,0.64,0.71,0.795,0.81,0.72,0.59,0.47,0.395,0.345,0.29,0.235,0.105,0.055,0.015,-0.02,0.01,0.045,0.045,0.04,0.04,0.055,0.05,0.095,0.14,0.135,0.135,0.165,0.15,0.18,0.215,0.195,0.22,0.22,0.195,0.195,0.135,0.045,0.01,-0.125,-0.185,-0.23,-0.285,-0.32,-0.34,-0.28,-0.245,-0.2,-0.105,0.015,0.095,0.185,0.185,0.15,0.13,0.095,0.075,0.08,0.07,0.1,0.16,0.23,0.3,0.365,0.425,0.52,0.615,0.7,0.765,0.78,0.755,0.655,0.51,0.38,0.28,0.195,0.145,0.06,-0.03,-0.1,-0.14,-0.2,-0.22,-0.245,-0.26,-0.25,-0.28,-0.28,-0.285,-0.27,-0.235,-0.22,-0.185,-0.175,-0.145,-0.115,-0.11,-0.065,-0.07,-0.07,-0.055,-0.035,-0.02,0.01,0,-0.055,-0.13,-0.22,-0.265,-0.34,-0.36,-0.33,-0.315,-0.285,-0.27,-0.265,-0.26,-0.24,-0.21,-0.19,-0.18,-0.195,-0.19,-0.135,-0.09,-0.05,-0.04,-0.035,-0.065,-0.065,-0.03,0,0.045,0.08,0.095,0.1,0.115,0.145,0.175,0.215,0.22,0.195,0.195,0.205,0.195,0.17,0.1,-0.04,-0.165,-0.27,-0.355,-0.34,-0.28,-0.245,-0.22,-0.2,-0.15,0.025,0.135,0.165,-0.025,-0.29,-0.53,-0.685,-0.66,-0.53,-0.41,-0.34,-0.27,-0.25,-0.21,-0.205,-0.24,-0.305,-0.305,-0.285,-0.225,-0.22,-0.24,-0.3,-0.325,-0.36,-0.315,-0.275,-0.225,-0.195,-0.2,-0.16,-0.155,-0.1,0.04,0.055,0.1,0.085,0.045,-0.03,-0.1,-0.18,-0.22,-0.2,-0.195,-0.12,-0.075,0,0.03,0.125,0.1,0.115,0.145,0.185,0.27,0.35,0.375,0.36,0.46,0.49,0.52,0.54,0.46,0.395,0.36,0.315,0.285,0.24,0.205,0.175,0.13,0.085,0.07,0.01,0.03,0.055,0.08,0.04,0.01,0.015,0.025,0.065,0.125,0.105,0.04,0,0,-0.03,-0.055,-0.08,-0.15,-0.16,-0.155,-0.065,0.06,0.115,0.095,0.065,-0.05,-0.1,-0.085,-0.1,-0.15,-0.26,-0.4,-0.41,-0.37,-0.325,-0.265,-0.28,-0.365,-0.405,-0.4,-0.355,-0.27,-0.175,-0.105,0,0.045,0.12,0.195,0.24,0.315,0.38,0.47,0.58,0.68,0.73,0.78,0.82,0.82,0.795,0.77,0.685,0.665,0.63,0.605,0.57,0.465,0.395,0.33,0.32,0.325,0.36,0.355,0.37,0.35,0.32,0.25,0.205,0.195,0.215,0.24,0.195,0.17,0.135,0.09,0.1,0.06,0.06,0,-0.02,0,0,-0.035,-0.075,-0.16,-0.26,-0.34,-0.385,-0.435,-0.49,-0.53,-0.59,-0.635,-0.665,-0.67,-0.7,-0.695,-0.7,-0.7,-0.71,-0.685,-0.62,-0.505,-0.36,-0.23,-0.075,0.035,0.175,0.31,0.425,0.49,0.595,0.665,0.71,0.755,0.78,0.775,0.79,0.86,0.89,0.93,0.935,0.865,0.84,0.77,0.715,0.655,0.545,0.475,0.425,0.42,0.375,0.33,0.225,0.12,0.035,-0.055,-0.13,-0.18,-0.26,-0.33,-0.425,-0.525,-0.605,-0.66,-0.66,-0.67,-0.715,-0.775,-0.845,-0.905,-0.96,-0.955,-0.955,-0.985,-1.05,-1.09,-1.115,-1.08,-0.995,-0.925,-0.915,-0.89,-0.825,-0.79,-0.7,-0.655,-0.605,-0.47,-0.445,-0.38,-0.305,-0.27,-0.16,-0.045,0.05,0.085,0.08,0.11,0.115,0.175,0.235,0.28,0.33,0.335,0.37,0.385,0.435,0.44,0.44,0.41,0.385,0.385,0.455,0.555,0.58,0.515,0.44,0.275,0.175,0.175,0.155,0.115,0.04,-0.03,-0.09,-0.11,-0.13,-0.165,-0.28,-0.325,-0.405,-0.52,-0.6,-0.72,-0.815,-0.895,-0.945,-0.925,-0.905,-0.925,-0.95,-1.06,-1.085,-1.045,-0.925,-0.8,-0.685,-0.605,-0.5,-0.405,-0.355,-0.31,-0.225,-0.06,0.14,0.36,0.475,0.47,0.39,0.355,0.36,0.395,0.44,0.52,0.53,0.545,0.615,0.66,0.655,0.725,0.675,0.645,0.69,0.66,0.705,0.69,0.705,0.645,0.635,0.645,0.59,0.605,0.555,0.475,0.47,0.505,0.475,0.385,0.315,0.235,0.225,0.295,0.355,0.24,0.085,-0.08,-0.145,-0.235,-0.32,-0.37,-0.6,-0.82,-0.885,-0.955,-0.91,-0.84,-0.77,-0.755,-0.71,-0.695,-0.65,-0.57,-0.475,-0.35,-0.22,-0.06,0.065,0.22,0.395,0.525,0.67,0.795,0.895,1.005,1.12,1.2,1.27,1.265,1.22,1.195,1.165,1.145,1.125,1.075,1.005,0.915,0.8,0.7,0.56,0.49,0.425,0.4,0.385,0.37,0.38,0.375,0.39,0.38,0.375,0.335,0.265,0.19,0.16,0.11,0.085,0.05,0.005,-0.04,-0.09,-0.175,-0.315,-0.435,-0.53,-0.525,-0.6,-0.655,-0.76,-0.885,-0.94,-0.98,-0.99,-0.97,-0.915,-0.875,-0.87,-0.865,-0.835,-0.81,-0.7,-0.665,-0.57,-0.5,-0.45,-0.355,-0.27,-0.205,-0.185,-0.115,-0.07,-0.02,0.085,0.165,0.235,0.26,0.29,0.315,0.315,0.345,0.34,0.305,0.295,0.31,0.3,0.265,0.22,0.15,0.14,0.16,0.125,0.105,0.015,-0.065,-0.11,-0.09,-0.165,-0.18,-0.245,-0.355,-0.435,-0.51,-0.63,-0.685,-0.67,-0.695,-0.685,-0.69,-0.68,-0.65,-0.615,-0.61,-0.605,-0.58,-0.515,-0.45,-0.29,-0.24,-0.195,-0.12,-0.115,-0.145,-0.09,-0.125,-0.17,-0.185,-0.17,-0.16,-0.09,-0.08,-0.085,-0.065,-0.085,-0.105,-0.095,-0.09,-0.055,0.015,0.005,0.03,0.125,0.28,0.395,0.4,0.29,0.11,0.095,0.13,0.21,0.28,0.31,0.265,0.22,0.17,0.115,0.015,0.03,0.055,0.04,-0.04,-0.135,-0.32,-0.44,-0.49,-0.495,-0.525,-0.52,-0.59,-0.58,-0.61,-0.675,-0.75,-0.84,-0.875,-0.78,-0.6,-0.45,-0.395,-0.45,-0.385,-0.35,-0.395,-0.42,-0.495,-0.495,-0.37,-0.21,-0.14,-0.125,-0.055,0.03,0.085,0.095,0.11,0.19,0.275,0.3,0.355,0.32,0.315,0.33,0.31,0.315,0.34,0.38,0.465,0.51,0.54,0.605,0.65,0.67,0.675,0.7,0.7,0.74,0.695,0.66,0.565,0.42,0.3,0.25,0.2,0.395,0.565,0.595,0.495,0.095,-0.275,-0.505,-0.6,-0.59,-0.595,-0.68,-0.73,-0.79,-0.79,-0.815,-0.785,-0.735,-0.67,-0.595,-0.49,-0.44,-0.42,-0.405,-0.46,-0.46,-0.45,-0.405,-0.33,-0.295,-0.28,-0.23,-0.215,-0.255,-0.215,-0.21,-0.175,-0.04,0.075,0.125,0.16,0.19,0.18,0.205,0.205,0.12,-0.03,-0.13,-0.225,-0.265,-0.225,-0.2,-0.245,-0.285,-0.35,-0.41,-0.42,-0.41,-0.4,-0.375,-0.405,-0.45,-0.45,-0.445,-0.44,-0.42,-0.415,-0.425,-0.415,-0.425,-0.485,-0.505,-0.59,-0.655,-0.7,-0.73,-0.7,-0.67,-0.635,-0.555,-0.485,-0.44,-0.35,-0.28,-0.21,-0.095,-0.075,-0.065,-0.125,-0.135,-0.07,0.055,0.215,0.325,0.395,0.31,0.18,0.115,0.095,0.2,0.3,0.31,0.275,0.18,0.22,0.305,0.295,0.335,0.325,0.225,0.295,0.38,0.435,0.4,0.365,0.38,0.33,0.335,0.36,0.32,0.275,0.19,0.02,-0.305,-0.555,-0.7,-0.78,-0.765,-0.725,-0.705,-0.765,-0.78,-0.83,-0.9,-0.965,-1.025,-1.065,-1.04,-0.925,-0.76,-0.555,-0.375,-0.195,-0.145,-0.26,-0.335,-0.39,-0.32,-0.185,-0.12,0,0.07,0.155,0.195,0.225,0.16,0.23,0.37,0.455,0.47,0.54,0.47,0.55,0.61,0.62,0.505,0.34,0.295,-0.195,-0.12,-0.305,-0.29,-0.08,0,0.07,0.145,0.15,0.215,0.355,0.57,0.7,0.765,0.75,0.655,0.595,0.685,0.705,0.545,0.34,0.08,-0.085,-0.065,-0.08,-0.13,-0.2,-0.31,-0.32,-0.37,-0.45,-0.58,-0.725,-0.875,-0.815,-0.71,-0.58,-0.42,-0.36,-0.375,-0.325,-0.24,-0.105,0.04,0.12,0.145,0.155,0.12,0.165,0.23,0.295,0.34,0.425,0.45,0.49,0.535,0.575,0.655,0.675,0.72,0.805,0.87,0.895,0.915,0.855,0.755,0.71,0.695,0.64,0.51,0.405,0.355,0.245,0.17,0.1,-0.11,-0.21,-0.175,-0.145,-0.16,-0.18,-0.265,-0.37,-0.44,-0.495,-0.525,-0.6,-0.645,-0.735,-0.78,-0.835,-0.805,-0.865,-0.78,-0.785,-0.785,-0.69,-0.71,-0.735,-0.695,-0.72,-0.675,-0.635,-0.6,-0.54,-0.53,-0.49,-0.465,-0.36,-0.27,-0.14,-0.06,0.01,0.035,0.11,0.165,0.235,0.295,0.375,0.435,0.49,0.5,0.605,0.71,0.74,0.79,0.695,0.64,0.63,0.67,0.72,0.775,0.76,0.8,0.77,0.67,0.595,0.515,0.435,0.345,0.315,0.325,0.315,0.29,0.205,0.02,-0.145,-0.18,-0.24,-0.35,-0.5,-0.69,-0.81,-0.87,-0.835,-0.825,-0.945,-0.93,-0.83,-0.72,-0.585,-0.56,-0.61,-0.7,-0.67,-0.625,-0.595,-0.595,-0.5,-0.295,-0.14,-0.04,-0.035,-0.1,-0.18,-0.15,-0.08,0.025,0.075,0.075,0.045,0.045,0.155,0.345,0.44,0.57,0.595,0.6,0.67,0.655,0.63,0.67,0.615,0.7,0.74,0.715,0.725,0.68,0.615,0.54,0.5,0.5,0.55,0.56,0.53,0.5,0.355,0.24,0.16,0,-0.13,-0.15,-0.29,-0.335,-0.29,-0.255,-0.145,-0.095,-0.14,-0.305,-0.41,-0.405,-0.345,-0.16,-0.02,-0.125,-0.2,-0.4,-0.5,-0.405,-0.275,-0.15,0,0.085,0.13,0.135,0.01,-0.135,-0.19,-0.125,0,0.105,0.165,0.16,0.21,0.32,0.4,0.505,0.515,0.37,0.24,0.15,0.23,0.34,0.46,0.495,0.69,0.79,0.91,0.99,0.805,0.585,0.47,0.375,0.42,0.625,0.67,0.785,0.8,0.515,0.315,0.07,-0.14,-0.085,0.06,0.14,0.14,0.08,0,-0.09,-0.195,-0.205,-0.235,-0.27,-0.275,-0.26,-0.3,-0.28,-0.2,-0.15,-0.16,-0.13,-0.08,-0.055,0.02,0.015,-0.155,-0.245,-0.25,-0.235,-0.155,-0.18,-0.2,-0.205,-0.12,-0.02,0.095,0.135,0.125,0.1,0.155,0.175,0.155,0.135,0.12,0.055,0.055,0.09,0.075,0.07,0.035,0.02,-0.05,-0.145,-0.19,-0.27,-0.285,-0.225,-0.16,-0.16,-0.19,-0.23,-0.26,-0.255,-0.215,-0.205,-0.19,-0.245,-0.245,-0.285,-0.27,-0.24,-0.225,-0.255,-0.245,-0.275,-0.265,-0.25,-0.195,-0.2,-0.195,-0.165,-0.18,-0.16,-0.11,-0.055,0.005,0.08,0.145,0.195,0.235,0.195,0.18,0.15,0.21,0.23,0.21,0.235,0.225,0.22,0.23,0.155,0.04,0.005,-0.055,-0.135,-0.215,-0.23,-0.14,-0.085,-0.05,-0.115,-0.295,-0.385,-0.41,-0.34,-0.33,-0.41,-0.54,-0.655,-0.76,-0.695,-0.645,-0.71,-0.805,-0.83,-0.785,-0.685,-0.575,-0.62,-0.72,-0.755,-0.705,-0.62,-0.545,-0.405,-0.36,-0.38,-0.34,-0.32,-0.33,-0.26,-0.16,-0.055,0,0.035,-0.075,-0.15,-0.1,0.01,0.25,0.355,0.295,0.255,0.195,0.18,0.3,0.455,0.49,0.485,0.455,0.515,0.54,0.55,0.55,0.53,0.525,0.6,0.665,0.69,0.795,1.2,1.24,1.165,0.87,0.365,0.095,-0.25,-0.36,-0.63,-0.76,-0.595,-0.53,-0.605,-0.845,-1.135,-1.265,-1.185,-1.195,-1.275,-1.33,-1.395,-1.26,-1.025,-0.93,-0.85,-0.915,-0.88,-0.825,-0.82,-0.695,-0.65,-0.6,-0.45,-0.375,-0.385,-0.325,-0.395,-0.295,-0.06,0.155,0.285,0.335,0.35,0.365,0.44,0.44,0.395,0.385,0.415,0.44,0.48,0.425,0.385,0.49,0.59,0.665,0.67,0.635,0.58,0.52,0.485,0.44,0.39,0.345,0.3,0.22,0.13,0.045,0.015,-0.05,-0.065,-0.085,-0.14,-0.19,-0.245,-0.325,-0.385,-0.46,-0.56,-0.675,-0.745,-0.79,-0.82,-0.81,-0.84,-0.84,-0.845,-0.83,-0.77,-0.7,-0.67,-0.605,-0.62,-0.675,-0.64,-0.595,-0.5,-0.39,-0.275,-0.2,-0.105,0.02,0.055,0.125,0.14,0.155,0.155,0.2,0.255,0.27,0.37,0.435,0.475,0.56,0.575,0.56,0.56,0.53,0.55,0.515,0.51,0.455,0.455,0.395,0.37,0.315,0.285,0.225,0.2,0.15,0.045,0,-0.085,-0.165,-0.265,-0.32,-0.38,-0.415,-0.44,-0.5,-0.58,-0.595,-0.6,-0.595,-0.605,-0.64,-0.68,-0.7,-0.725,-0.73,-0.755,-0.77,-0.79,-0.795,-0.79,-0.78,-0.74,-0.705,-0.7,-0.675,-0.64,-0.59,-0.525,-0.46,-0.42,-0.4,-0.37,-0.34,-0.31,-0.265,-0.225,-0.205,-0.145,-0.105,-0.075,-0.045,0.01,0.035,0.095,0.13,0.18,0.225,0.295,0.315,0.325,0.3,0.26,0.23,0.175,0.145,0.13,0.09,0.02,-0.045,-0.085,-0.1,-0.075,-0.03,-0.05,-0.045,-0.04,-0.04,-0.085,-0.105,-0.16,-0.16,-0.125,-0.07,-0.045,-0.07,-0.125,-0.14,-0.18,-0.19,-0.19,-0.145,-0.14,-0.095,-0.075,-0.13,-0.2,-0.275,-0.33,-0.385,-0.42,-0.43,-0.475,-0.45,-0.38,-0.33,-0.3,-0.315,-0.365,-0.4,-0.365,-0.31,-0.27,-0.32,-0.355,-0.345,-0.335,-0.345,-0.365,-0.5,-0.58,-0.61,-0.59,-0.49,-0.405,-0.335,-0.26,-0.245,-0.215,-0.205,-0.18,-0.165,-0.14,-0.06,0,0.05,0.11,0.135,0.17,0.255,0.205,0.2,0.265,0.245,0.32,0.37,0.32,0.32,0.305,0.34,0.305,0.255,0.255,0.19,0.21,0.195,0.165,0.165,0.195,0.23,0.24,0.2,0.135,0.035,-0.07,-0.18,-0.32,-0.44,-0.54,-0.575,-0.615,-0.62,-0.62,-0.615,-0.6,-0.56,-0.55,-0.53,-0.515,-0.505,-0.5,-0.48,-0.455,-0.405,-0.365,-0.325,-0.265,-0.245,-0.21,-0.225,-0.195,-0.2,-0.16,-0.09,-0.04,0.03,0.095,0.155,0.225,0.27,0.365,0.42,0.49,0.55,0.585,0.57,0.6,0.64,0.695,0.7,0.735,0.71,0.695,0.7,0.715,0.695,0.67,0.64,0.62,0.62,0.63,0.655,0.665,0.665,0.655,0.645,0.59,0.535,0.495,0.425,0.345,0.275,0.175,0.05,-0.1,-0.215,-0.29,-0.385,-0.43,-0.525,-0.66,-0.77,-0.83,-0.885,-0.875,-0.855,-0.82,-0.805,-0.755,-0.74,-0.69,-0.65,-0.605,-0.58,-0.555,-0.505,-0.46,-0.405,-0.33,-0.315,-0.29,-0.25,-0.22,-0.18,-0.16,-0.14,-0.105,-0.04,0.06,0.14,0.22,0.3,0.37,0.415,0.44,0.48,0.52,0.58,0.625,0.67,0.7,0.74,0.76,0.775,0.755,0.72,0.7,0.68,0.675,0.66,0.635,0.6,0.56,0.515,0.47,0.42,0.41,0.355,0.315,0.26,0.19,0.125,0.05,-0.055,-0.15,-0.22,-0.28,-0.335,-0.39,-0.495,-0.585,-0.655,-0.685,-0.725,-0.73,-0.77,-0.775,-0.775,-0.71,-0.64,-0.57,-0.505,-0.475,-0.49,-0.495,-0.505,-0.48,-0.395,-0.335,-0.295,-0.26,-0.235,-0.2,-0.105,-0.065,-0.025,0.035,0.065,0.085,0.155,0.175,0.22,0.29,0.35,0.4,0.45,0.485,0.505,0.515,0.515,0.46,0.4,0.365,0.31,0.265,0.225,0.155,0.075,0.07,0.02,-0.04,-0.09,-0.13,-0.235,-0.275,-0.275,-0.305,-0.34,-0.345,-0.32,-0.29,-0.255,-0.255,-0.33,-0.41,-0.415,-0.4,-0.405,-0.41,-0.445,-0.48,-0.485,-0.475,-0.43,-0.4,-0.33,-0.285,-0.265,-0.245,-0.24,-0.24,-0.22,-0.22,-0.21,-0.175,-0.15,-0.095,-0.045,0.005,0.025,0.07,0.07,0.115,0.075,0.125,0.14,0.17,0.2,0.21,0.195,0.175,0.205,0.22,0.255,0.295,0.29,0.295,0.27,0.21,0.15,0.06,0.02,-0.035,0,-0.035,-0.035,-0.05,-0.045,-0.045,0,0.06,0.045,0.105,0.165,0.21,0.18,0.22,0.135,0.16,0.12,0.145,0.15,0.14,0.165,0.195,0.18,0.175,0.11,0.115,0.085,0.085,0.095,0.045,0.025,0,0.015,-0.04,0.04,0.07,0.05,0.06,0,-0.075,-0.05,-0.07,-0.085,-0.08,-0.14,-0.155,-0.19,-0.225,-0.265,-0.3,-0.315,-0.33,-0.28,-0.29,-0.27,-0.32,-0.35,-0.335,-0.37,-0.3,-0.23,-0.185,-0.08,-0.07,0.01,0.055,0.03,0.03,0.03,0.05,0.095,0.175,0.23,0.26,0.265,0.29,0.265,0.29,0.33,0.29,0.35,0.315,0.335,0.35,0.33,0.325,0.29,0.24,0.18,0.145,0.125,0.13,0.135,0.105,0.08,0.065,0.06,0.07,0.095,0.14,0.16,0.175,0.175,0.145,0.115,0.115,0.13,0.15,0.16,0.145,0.1,0.03,-0.05,-0.1,-0.125,-0.155,-0.175,-0.21,-0.25,-0.28,-0.305,-0.335,-0.35,-0.365,-0.375,-0.375,-0.37,-0.365,-0.35,-0.345,-0.32,-0.285,-0.24,-0.175,-0.115,-0.05,0.02,0.085,0.14,0.21,0.305,0.45,0.675,0.88,1.04,0.87,0.695,0.415,0.245,0.23,0.27,0.26,0.22,0.165,0.155,0.125,0.145,0.16,0.18,0.18,0.18,0.16,0.145,0.125,0.105,0.08,0.06,0.055,0.05,0.035,0,-0.055,-0.08,-0.08,-0.075,-0.065,-0.07,-0.045,-0.025,0.02,0.055,0.05,0.025,0,-0.055,-0.08,-0.095,-0.105,-0.09,-0.07,-0.055,-0.055,-0.06,-0.09,-0.07,-0.035,0.045,0.115,0.155,0.165,0.135,0.14,0.215,0.275,0.375,0.435,0.46,0.435,0.44,0.44,0.395,0.335,0.265,0.175,0.09,0.065,0,-0.085,-0.12,-0.16,-0.185,-0.165,-0.175,-0.205,-0.19,-0.2,-0.24,-0.21,-0.195,-0.215,-0.195,-0.2,-0.245,-0.2,-0.18,-0.2,-0.235,-0.285,-0.39,-0.47,-0.47,-0.415,-0.39,-0.33,-0.38,-0.445,-0.46,-0.41,-0.34,-0.325,-0.305,-0.31,-0.28,-0.265,-0.22,-0.24,-0.225,-0.19,-0.17,-0.12,-0.07,-0.055,0.02,0.01,-0.02,-0.025,0.035,0.1,0.205,0.26,0.28,0.28,0.245,0.265,0.295,0.355,0.375,0.38,0.36,0.325,0.335,0.41,0.455,0.49,0.51,0.455,0.415,0.4,0.375,0.31,0.295,0.24,0.165,0.09,0,-0.105,-0.16,-0.18,-0.185,-0.2,-0.215,-0.22,-0.21,-0.215,-0.22,-0.25,-0.295,-0.31,-0.34,-0.33,-0.305,-0.28,-0.22,-0.14,-0.07,0.03,0.11,0.165,0.185,0.21,0.215,0.255,0.3,0.34,0.39,0.415,0.435,0.47,0.5,0.505,0.545,0.575,0.585,0.655,0.695,0.75,0.765,0.77,0.72,0.69,0.705,0.71,0.75,0.765,0.76,0.755,0.74,0.735,0.715,0.645,0.605,0.54,0.465,0.35,0.23,0.085,-0.045,-0.125,-0.19,-0.24,-0.26,-0.285,-0.325,-0.355,-0.405,-0.41,-0.4,-0.385,-0.36,-0.34,-0.305,-0.3,-0.27,-0.24,-0.24,-0.225,-0.195,-0.175,-0.14,-0.125,-0.14,-0.12,-0.095,0.005,0.065,0.095,0.11,0.135,0.185,0.25,0.315,0.36,0.395,0.41,0.41,0.415,0.41,0.4,0.41,0.435,0.475,0.53,0.61,0.68,0.74,0.78,0.815,0.84,0.86,0.895,0.92,0.925,0.91,0.86,0.795,0.72,0.665,0.615,0.555,0.495,0.415,0.335,0.25,0.195,0.125,0.06,0,-0.05,-0.08,-0.1,-0.11,-0.14,-0.16,-0.18,-0.17,-0.15,-0.13,-0.1,-0.065,-0.02,0.05,0.065,0.08,0.075,0.09,0.095,0.115,0.13,0.165,0.195,0.27,0.28,0.285,0.245,0.27,0.34,0.51,0.79,1.075,1.155,1.14,0.895,0.485,0.26,0.12,0.055,0.05,-0.035,-0.07,-0.065,-0.085,-0.125,-0.245,-0.365,-0.405,-0.385,-0.38,-0.35,-0.425,-0.455,-0.455,-0.465,-0.455,-0.435,-0.37,-0.29,-0.225,-0.19,-0.175,-0.16,-0.125,-0.115,-0.08,-0.075,-0.08,-0.095,-0.19,-0.3,-0.38,-0.405,-0.43,-0.4,-0.345,-0.405,-0.385,-0.395,-0.43,-0.43,-0.39,-0.39,-0.365,-0.335,-0.375,-0.4,-0.45,-0.5,-0.505,-0.485,-0.48,-0.49,-0.505,-0.53,-0.495,-0.44,-0.415,-0.35,-0.285,-0.225,-0.15,-0.09,-0.035,0,0.005,-0.075,-0.135,-0.19,-0.195,-0.15,-0.075,0,0.025,0.04,0.035,0.025,0.06,0.135,0.205,0.275,0.36,0.4,0.425,0.45,0.48,0.475,0.51,0.51,0.54,0.55,0.55,0.59,0.6,0.615,0.655,0.68,0.7,0.715,0.73,0.715,0.725,0.715,0.75,0.745,0.755,0.78,0.785,0.785,0.805,0.775,0.735,0.68,0.595,0.545,0.51,0.485,0.42,0.335,0.25,0.195,0.135,0.09,0.05,-0.03,-0.1,-0.14,-0.17,-0.25,-0.31,-0.355,-0.365,-0.345,-0.305,-0.285,-0.305,-0.305,-0.305,-0.305,-0.25,-0.225,-0.185,-0.145,-0.08,-0.065,0.015,0.08,0.12,0.17,0.19,0.235,0.24,0.265,0.325,0.33,0.325,0.315,0.275,0.26,0.27,0.285,0.275,0.26,0.27,0.265,0.275,0.275,0.26,0.235,0.2,0.145,0.08,0.025,-0.025,-0.05,-0.055,-0.045,-0.05,-0.06,-0.06,-0.07,-0.07,-0.095,-0.15,-0.205,-0.26,-0.28,-0.29,-0.29,-0.33,-0.405,-0.485,-0.555,-0.58,-0.59,-0.59,-0.58,-0.565,-0.515,-0.45,-0.375,-0.3,-0.22,-0.135,-0.05,0.05,0.12,0.175,0.225,0.265,0.315,0.355,0.4,0.44,0.49,0.535,0.585,0.635,0.675,0.705,0.74,0.775,0.8,0.82,0.81,0.785,0.735,0.7,0.68,0.675,0.685,0.715,0.77,0.795,0.79,0.765,0.705,0.74,0.84,1.125,1.335,1.435,1.37,1.06,0.805,0.64,0.595,0.585,0.46,0.22,-0.1,-0.305,-0.45,-0.535,-0.635,-0.72,-0.805,-0.85,-0.85,-0.83,-0.74,-0.665,-0.53,-0.47,-0.43,-0.465,-0.455,-0.435,-0.425,-0.415,-0.37,-0.305,-0.21,-0.065,0.005,0,0,0.005,0.015,0.065,0.11,0.125,0.155,0.165,0.225,0.325,0.4,0.455,0.425,0.46,0.465,0.515,0.615,0.615,0.645,0.655,0.69,0.735,0.78,0.82,0.815,0.85,0.84,0.82,0.83,0.84,0.86,0.91,0.96,0.97,0.895,0.74,0.555,0.36,0.205,0.085,0,-0.075,-0.125,-0.155,-0.19,-0.225,-0.3,-0.36,-0.425,-0.465,-0.48,-0.46,-0.445,-0.44,-0.41,-0.385,-0.355,-0.335,-0.37,-0.395,-0.435,-0.47,-0.465,-0.44,-0.425,-0.385,-0.345,-0.285,-0.185,-0.1,0,0.07,0.105,0.125,0.155,0.155,0.19,0.235,0.28,0.32,0.35,0.345,0.375,0.375,0.41,0.435,0.475,0.48,0.5,0.53,0.56,0.6,0.59,0.53,0.435,0.3,0.19,0.105,0.035,-0.045,-0.095,-0.12,-0.155,-0.13,-0.14,-0.14,-0.185,-0.2,-0.225,-0.22,-0.23,-0.275,-0.355,-0.46,-0.52,-0.495,-0.49,-0.48,-0.44,-0.495,-0.63,-0.655,-0.69,-0.65,-0.545,-0.47,-0.445,-0.43,-0.395,-0.355,-0.355,-0.34,-0.335,-0.305,-0.245,-0.185,-0.13,-0.055,0.035,0.115,0.17,0.225,0.255,0.305,0.355,0.395,0.445,0.49,0.53,0.565,0.575,0.57,0.53,0.48,0.44,0.41,0.37,0.34,0.3,0.28,0.27,0.265,0.275,0.28,0.275,0.27,0.255,0.23,0.2,0.19,0.165,0.14,0.1,0.05,-0.045,-0.13,-0.2,-0.26,-0.305,-0.345,-0.38,-0.425,-0.46,-0.465,-0.435,-0.425,-0.4,-0.39,-0.36,-0.35,-0.335,-0.31,-0.28,-0.235,-0.16,-0.08,-0.02,0.025,0.04,0.06,0.07,0.115,0.165,0.21,0.25,0.285,0.32,0.33,0.33,0.325,0.315,0.31,0.26,0.23,0.135,0.07,0.02,-0.02,-0.04,0.015,0.015,0.035,0.02,0.025,0.04,0.015,0.035,0.005,-0.045,-0.07,-0.08,-0.115,-0.17,-0.21,-0.315,-0.36,-0.34,-0.325,-0.24,-0.155,-0.17,-0.17,-0.225,-0.255,-0.23,-0.16,-0.065,-0.04,-0.035,-0.09,-0.16,-0.245,-0.28,-0.305,-0.285,-0.21,-0.14,-0.065,-0.035,0.015,0.015,0.085,0.175,0.265,0.27,0.255,0.145,0.07,0,-0.085,-0.225,-0.265,-0.305,-0.255,-0.15,-0.1,-0.12,-0.135,-0.17,-0.18,-0.105,-0.08,-0.05,-0.045,-0.09,-0.045,-0.07,-0.085,0.01,-0.045,-0.075,-0.03,-0.09,-0.165,-0.215,-0.295,-0.375,-0.33,-0.3,-0.25,-0.235,-0.24,-0.395,-0.475,-0.545,-0.565,-0.46,-0.33,-0.27,-0.23,-0.185,-0.14,-0.075,-0.03,-0.03,-0.035,-0.035,0,0.005,-0.03,-0.07,-0.12,-0.135,-0.135,-0.135,-0.175,-0.23,-0.31,-0.4,-0.47,-0.51,-0.54,-0.525,-0.5,-0.43,-0.37,-0.325,-0.295,-0.275,-0.255,-0.245,-0.21,-0.16,-0.13,-0.065,-0.015,0.035,0.06,0.09,0.095,0.11,0.12,0.105,0.115,0.11,0.115,0.15,0.15,0.115,0.115,0.1,0.12,0.13,0.11,0.06,-0.03,-0.05,-0.045,-0.04,0.015,0.035,0.03,0.075,0.07,0.07,0.095,0.105,0.13,0.16,0.18,0.2,0.185,0.215,0.24,0.195,0.15,0.065,-0.045,-0.115,-0.175,-0.25,-0.29,-0.34,-0.33,-0.34,-0.315,-0.315,-0.295,-0.245,-0.24,-0.22,-0.225,-0.26,-0.26,-0.22,-0.21,-0.2,-0.23,-0.235,-0.24,-0.25,-0.265,-0.31,-0.33,-0.34,-0.315,-0.33,-0.31,-0.28,-0.23,-0.16,-0.135,-0.14,-0.15,-0.16,-0.16,-0.16,-0.16,-0.15,-0.16,-0.125,-0.105,-0.08,0,0.05,0.115,0.16,0.155,0.175,0.17,0.16,0.14,0.09,0,-0.1,-0.155,-0.185,-0.17,-0.165,-0.15,-0.14,-0.105,-0.07,-0.04,0.005,0.03,0.06,0.09,0.12,0.165,0.185,0.19,0.2,0.195,0.175,0.145,0.105,0.06,0.035,0.015,0.015,0.005,0,-0.03,-0.05,-0.08,-0.09,-0.12,-0.15,-0.18,-0.21,-0.25,-0.28,-0.305,-0.32,-0.33,-0.33,-0.335,-0.375,-0.435,-0.52,-0.57,-0.59,-0.585,-0.565,-0.53,-0.505,-0.465,-0.415,-0.385,-0.405,-0.435,-0.475,-0.495,-0.495,-0.465,-0.45,-0.425,-0.395,-0.355,-0.41,-0.48,-0.54,-0.635,-0.675,-0.67,-0.66,-0.645,-0.57,-0.4,-0.26,-0.06,0.1,0.135,0.18,0.215,0.22,0.345,0.395,0.43,0.46,0.485,0.5,0.54,0.545,0.455,0.32,0.205,0.095,0.03,0,-0.065,-0.09,-0.125,-0.17,-0.165,-0.21,-0.275,-0.355,-0.51,-0.64,-0.71,-0.715,-0.72,-0.73,-0.77,-0.85,-0.91,-0.99,-1.065,-1.18,-1.28,-1.305,-1.31,-1.245,-1.14,-1.075,-1.025,-1.005,-0.97,-0.925,-0.825,-0.695,-0.67,-0.625,-0.57,-0.525,-0.425,-0.26,-0.155,0.005,0.07,0.12,0.165,0.255,0.355,0.48,0.595,0.645,0.715,0.73,0.755,0.775,0.78,0.855,0.835,0.905,0.915,0.95,0.94,0.915,0.85,0.775,0.78,0.82,0.785,0.69,0.58,0.455,0.355,0.29,0.19,0.14,0.1,0.035,-0.09,-0.295,-0.555,-0.72,-0.84,-0.905,-1,-1.105,-1.25,-1.315,-1.4,-1.39,-1.395,-1.395,-1.395,-1.31,-1.265,-1.155,-1.075,-1.04,-1.045,-0.98,-0.885,-0.82,-0.68,-0.62,-0.66,-0.615,-0.545,-0.28,-0.09,0.08,0.14,0.135,0.18,0.315,0.43,0.46,0.465,0.455,0.505,0.56,0.63,0.685,0.74,0.775,0.81,0.845,0.89,0.95,1,1.015,1.015,1,0.995,1.005,0.97,0.91,0.815,0.715,0.59,0.515,0.395,0.335,0.255,0.16,0.075,-0.06,-0.17,-0.285,-0.39,-0.485,-0.55,-0.615,-0.66,-0.71,-0.77,-0.79,-0.825,-0.84,-0.825,-0.82,-0.755,-0.68,-0.595,-0.53,-0.45,-0.41,-0.33,-0.255,-0.16,-0.065,0.04,0.095,0.14,0.15,0.145,0.155,0.18,0.185,0.25,0.315,0.41,0.515,0.59,0.665,0.715,0.775,0.815,0.875,0.895,0.94,0.99,0.95,0.94,0.88,0.87,0.815,0.775,0.69,0.59,0.505,0.45,0.39,0.32,0.24,0.16,0.105,0.07,0.015,-0.04,-0.09,-0.17,-0.27,-0.38,-0.445,-0.565,-0.645,-0.665,-0.73,-0.74,-0.705,-0.725,-0.725,-0.72,-0.69,-0.68,-0.64,-0.595,-0.585,-0.52,-0.475,-0.4,-0.33,-0.265,-0.225,-0.16,-0.085,0,0.085,0.13,0.18,0.22,0.255,0.295,0.33,0.355,0.42,0.425,0.39,0.365,0.3,0.265,0.26,0.255,0.275,0.31,0.32,0.325,0.315,0.29,0.3,0.315,0.325,0.32,0.31,0.33,0.355,0.395,0.42,0.43,0.435,0.46,0.495,0.51,0.495,0.46,0.4,0.35,0.3,0.255,0.205,0.165,0.115,0.035,-0.065,-0.185,-0.31,-0.44,-0.56,-0.655,-0.71,-0.745,-0.73,-0.68,-0.605,-0.535,-0.48,-0.46,-0.46,-0.46,-0.44,-0.38,-0.3,-0.24,-0.18,-0.15,-0.16,-0.175,-0.2,-0.24,-0.245,-0.19,-0.09,0.08,0.165,0.24,0.245,0.215,0.2,0.155,0.09,0.035,-0.03,-0.025,0.005,-0.03,-0.05,-0.06,-0.06,0,0.02,0.055,0.075,0.095,0.145,0.18,0.205,0.195,0.185,0.18,0.16,0.155,0.155,0.105,0.065,-0.035,-0.11,-0.125,-0.17,-0.165,-0.155,-0.2,-0.275,-0.34,-0.39,-0.4,-0.405,-0.37,-0.35,-0.295,-0.235,-0.2,-0.175,-0.235,-0.215,-0.2,-0.165,-0.17,-0.265,-0.32,-0.445,-0.41,-0.425,-0.435,-0.495,-0.495,-0.45,-0.38,-0.31,-0.28,-0.325,-0.365,-0.29,-0.18,-0.09,0.04,0.1,0.125,0.15,0.265,0.3,0.225,0.15,0.065,0.005,-0.03,0,-0.105,-0.135,-0.12,-0.03,0.13,0.24,0.22,0.15,0.035,-0.035,0.035,0.125,0.14,0.14,0.065,0.03,0.02,0.045,-0.05,-0.02,-0.04,-0.03,0.05,0.02,-0.1,-0.07,0,0.125,0.26,0.21,0.11,-0.045,-0.07,0.075,0.16,0.235,0.335,0.285,0.275,0.35,0.28,0.255,0.305,0.325,0.355,0.39,0.38,0.355,0.38,0.4,0.45,0.48,0.475,0.475,0.5,0.52,0.535,0.52,0.475,0.435,0.415,0.375,0.345,0.285,0.25,0.235,0.24,0.245,0.27,0.3,0.36,0.38,0.365,0.325,0.25,0.19,0.16,0.115,0.105,0.1,0.1,0.08,0.06,0.05,0.015,0.03,0.04,0.075,0.12,0.19,0.21,0.26,0.265,0.26,0.25,0.235,0.19,0.185,0.205,0.255,0.315,0.31,0.3,0.26,0.24,0.26,0.255,0.215,0.17,0.125,0.09,0.06,0.015,-0.035,-0.05,-0.07,-0.05,-0.07,-0.08,-0.1,-0.08,-0.05,0.01,0.1,0.155,0.21,0.255,0.26,0.305,0.315,0.335,0.315,0.305,0.28,0.29,0.3,0.285,0.25,0.23,0.175,0.17,0.155,0.135,0.155,0.15,0.135,0.125,0.09 mV</t>
-  </si>
-  <si>
-    <t>0,0.004,0.008,0.012,0.016,0.02,0.024,0.028,0.032,0.036,0.04,0.044,0.048,0.052,0.056,0.06,0.064,0.068,0.072,0.076,0.08,0.084,0.088,0.092,0.096,0.1,0.104,0.108,0.112,0.116,0.12,0.124,0.128,0.132,0.136,0.14,0.144,0.148,0.152,0.156,0.16,0.164,0.168,0.172,0.176,0.18,0.184,0.188,0.192,0.196,0.2,0.204,0.208,0.212,0.216,0.22,0.224,0.228,0.232,0.236,0.24,0.244,0.248,0.252,0.256,0.26,0.264,0.268,0.272,0.276,0.28,0.284,0.288,0.292,0.296,0.3,0.304,0.308,0.312,0.316,0.32,0.324,0.328,0.332,0.336,0.34,0.344,0.348,0.352,0.356,0.36,0.364,0.368,0.372,0.376,0.38,0.384,0.388,0.392,0.396,0.4,0.404,0.408,0.412,0.416,0.42,0.424,0.428,0.432,0.436,0.44,0.444,0.448,0.452,0.456,0.46,0.464,0.468,0.472,0.476,0.48,0.484,0.488,0.492,0.496,0.5,0.504,0.508,0.512,0.516 s</t>
-  </si>
-  <si>
-    <t>-0.425,-0.42,-0.41,-0.395,-0.395,-0.38,-0.365,-0.345,-0.345,-0.32,-0.3,-0.28,-0.28,-0.255,-0.23,-0.205,-0.2,-0.18,-0.16,-0.145,-0.135,-0.13,-0.12,-0.1,-0.085,-0.08,-0.06,-0.03,0,-0.035,-0.05,-0.075,-0.09,-0.11,-0.1,-0.08,-0.1,-0.14,-0.16,-0.165,-0.16,-0.16,-0.195,-0.24,-0.28,-0.31,-0.32,-0.29,-0.275,-0.25,-0.245,-0.22,-0.2,-0.18,-0.18,-0.15,-0.135,-0.12,-0.12,-0.105,-0.085,-0.065,-0.08,-0.065,-0.05,-0.04,-0.035,-0.02,0.015,0.04,0.045,0.065,0.145,0.27,0.4,0.52,0.67,0.8,0.905,0.975,1.055,1.09,1.115,1.1,1.04,0.995,0.95,0.87,0.785,0.71,0.675,0.66,0.67,0.71,0.71,0.66,0.6,0.62,0.625,0.61,0.58,0.58,0.525,0.455,0.33,0.17,0.015,-0.095,-0.185,-0.24,-0.31,-0.365,-0.4,-0.395,-0.39,-0.4,-0.41,-0.4,-0.4,-0.4,-0.405,-0.41,-0.415,-0.41,-0.405,-0.42,-0.42,-0.405,-0.4,-0.4 mV</t>
-  </si>
-  <si>
-    <t>0,0.004,0.008,0.012,0.016,0.02,0.024,0.028,0.032,0.036,0.04,0.044,0.048,0.052,0.056,0.06,0.064,0.068,0.072,0.076,0.08,0.084,0.088,0.092,0.096,0.1,0.104,0.108,0.112,0.116,0.12,0.124,0.128,0.132,0.136,0.14,0.144,0.148,0.152,0.156,0.16,0.164,0.168,0.172,0.176,0.18,0.184,0.188,0.192,0.196,0.2,0.204,0.208,0.212,0.216,0.22,0.224,0.228,0.232,0.236,0.24,0.244,0.248,0.252,0.256,0.26,0.264,0.268,0.272,0.276,0.28,0.284,0.288,0.292,0.296,0.3,0.304,0.308,0.312,0.316,0.32,0.324,0.328,0.332,0.336,0.34,0.344,0.348,0.352,0.356,0.36,0.364,0.368,0.372,0.376,0.38,0.384,0.388,0.392,0.396,0.4,0.404,0.408,0.412,0.416,0.42,0.424,0.428,0.432,0.436,0.44,0.444,0.448,0.452,0.456,0.46,0.464,0.468,0.472,0.476,0.48,0.484,0.488,0.492,0.496,0.5,0.504,0.508,0.512,0.516,0.52,0.524,0.528,0.532,0.536,0.54,0.544,0.548,0.552,0.556,0.56,0.564,0.568,0.572,0.576,0.58,0.584,0.588,0.592,0.596,0.6,0.604,0.608,0.612,0.616,0.62,0.624,0.628,0.632,0.636,0.64,0.644,0.648,0.652,0.656,0.66,0.664,0.668,0.672,0.676,0.68,0.684,0.688,0.692,0.696,0.7,0.704,0.708,0.712,0.716,0.72,0.724,0.728,0.732,0.736,0.74,0.744,0.748,0.752,0.756,0.76,0.764,0.768,0.772,0.776,0.78,0.784,0.788,0.792,0.796,0.8,0.804,0.808,0.812,0.816,0.82,0.824,0.828,0.832,0.836,0.84,0.844,0.848,0.852,0.856,0.86,0.864,0.868,0.872,0.876,0.88,0.884,0.888,0.892,0.896,0.9,0.904,0.908,0.912,0.916,0.92,0.924,0.928,0.932,0.936,0.94,0.944,0.948,0.952,0.956,0.96,0.964,0.968,0.972,0.976,0.98,0.984,0.988,0.992,0.996,1,1.004,1.008,1.012,1.016,1.02,1.024,1.028,1.032,1.036,1.04,1.044,1.048,1.052,1.056,1.06,1.064,1.068,1.072,1.076,1.08,1.084,1.088,1.092,1.096,1.1,1.104,1.108,1.112,1.116,1.12,1.124,1.128,1.132,1.136,1.14,1.144,1.148,1.152,1.156,1.16,1.164,1.168,1.172,1.176,1.18,1.184,1.188,1.192,1.196,1.2,1.204,1.208,1.212,1.216,1.22,1.224,1.228,1.232,1.236,1.24,1.244,1.248,1.252,1.256,1.26,1.264,1.268,1.272,1.276,1.28,1.284,1.288,1.292,1.296,1.3,1.304,1.308,1.312,1.316,1.32,1.324,1.328,1.332,1.336,1.34,1.344,1.348,1.352,1.356,1.36,1.364,1.368,1.372,1.376,1.38,1.384,1.388,1.392,1.396,1.4,1.404,1.408,1.412,1.416,1.42,1.424,1.428,1.432,1.436,1.44,1.444,1.448,1.452,1.456,1.46,1.464,1.468,1.472,1.476,1.48,1.484,1.488,1.492,1.496,1.5,1.504,1.508,1.512,1.516,1.52,1.524,1.528,1.532,1.536,1.54,1.544,1.548,1.552,1.556,1.56,1.564,1.568,1.572,1.576,1.58,1.584,1.588,1.592,1.596,1.6,1.604,1.608,1.612,1.616,1.62,1.624,1.628,1.632,1.636,1.64,1.644,1.648,1.652,1.656,1.66,1.664,1.668,1.672,1.676,1.68,1.684,1.688,1.692,1.696,1.7,1.704,1.708,1.712,1.716,1.72,1.724,1.728,1.732,1.736,1.74,1.744,1.748,1.752,1.756,1.76,1.764,1.768,1.772,1.776,1.78,1.784,1.788,1.792,1.796,1.8,1.804,1.808,1.812,1.816,1.82,1.824,1.828,1.832,1.836,1.84,1.844,1.848,1.852,1.856,1.86,1.864,1.868,1.872,1.876,1.88,1.884,1.888,1.892,1.896,1.9,1.904,1.908,1.912,1.916,1.92,1.924,1.928,1.932,1.936,1.94,1.944,1.948,1.952,1.956,1.96,1.964,1.968,1.972,1.976,1.98,1.984,1.988,1.992,1.996,2,2.004,2.008,2.012,2.016,2.02,2.024,2.028,2.032,2.036,2.04,2.044,2.048,2.052,2.056,2.06,2.064,2.068,2.072,2.076,2.08,2.084,2.088,2.092,2.096,2.1,2.104,2.108,2.112,2.116,2.12,2.124,2.128,2.132,2.136,2.14,2.144,2.148,2.152,2.156,2.16,2.164,2.168,2.172,2.176,2.18,2.184,2.188,2.192,2.196,2.2,2.204,2.208,2.212,2.216,2.22,2.224,2.228,2.232,2.236,2.24,2.244,2.248,2.252,2.256,2.26,2.264,2.268,2.272,2.276,2.28,2.284,2.288,2.292,2.296,2.3,2.304,2.308,2.312,2.316,2.32,2.324,2.328,2.332,2.336,2.34,2.344,2.348,2.352,2.356,2.36,2.364,2.368,2.372,2.376,2.38,2.384,2.388,2.392,2.396,2.4,2.404,2.408,2.412,2.416,2.42,2.424,2.428,2.432,2.436,2.44,2.444,2.448,2.452,2.456,2.46,2.464,2.468,2.472,2.476,2.48,2.484,2.488,2.492,2.496,2.5,2.504,2.508,2.512,2.516,2.52,2.524,2.528,2.532,2.536,2.54,2.544,2.548,2.552,2.556,2.56,2.564,2.568,2.572,2.576,2.58,2.584,2.588,2.592,2.596,2.6,2.604,2.608,2.612,2.616,2.62,2.624,2.628,2.632,2.636,2.64,2.644,2.648,2.652,2.656,2.66,2.664,2.668,2.672,2.676,2.68,2.684,2.688,2.692,2.696,2.7,2.704,2.708,2.712,2.716,2.72,2.724,2.728,2.732,2.736,2.74,2.744,2.748,2.752,2.756,2.76,2.764,2.768,2.772,2.776,2.78,2.784,2.788,2.792,2.796,2.8,2.804,2.808,2.812,2.816,2.82,2.824,2.828,2.832,2.836,2.84,2.844,2.848,2.852,2.856,2.86,2.864,2.868,2.872,2.876,2.88,2.884,2.888,2.892,2.896,2.9,2.904,2.908,2.912,2.916,2.92,2.924,2.928,2.932,2.936,2.94,2.944,2.948,2.952,2.956,2.96,2.964,2.968,2.972,2.976,2.98,2.984,2.988,2.992,2.996,3,3.004,3.008,3.012,3.016,3.02,3.024,3.028,3.032,3.036,3.04,3.044,3.048,3.052,3.056,3.06,3.064,3.068,3.072,3.076,3.08,3.084,3.088,3.092,3.096,3.1,3.104,3.108,3.112,3.116,3.12,3.124,3.128,3.132,3.136,3.14,3.144,3.148,3.152,3.156,3.16,3.164,3.168,3.172,3.176,3.18,3.184,3.188,3.192,3.196,3.2,3.204,3.208,3.212,3.216,3.22,3.224,3.228,3.232,3.236,3.24,3.244,3.248,3.252,3.256,3.26,3.264,3.268,3.272,3.276,3.28,3.284,3.288,3.292,3.296,3.3,3.304,3.308,3.312,3.316,3.32,3.324,3.328,3.332,3.336,3.34,3.344,3.348,3.352,3.356,3.36,3.364,3.368,3.372,3.376,3.38,3.384,3.388,3.392,3.396,3.4,3.404,3.408,3.412,3.416,3.42,3.424,3.428,3.432,3.436,3.44,3.444,3.448,3.452,3.456,3.46,3.464,3.468,3.472,3.476,3.48,3.484,3.488,3.492,3.496,3.5,3.504,3.508,3.512,3.516,3.52,3.524,3.528,3.532,3.536,3.54,3.544,3.548,3.552,3.556,3.56,3.564,3.568,3.572,3.576,3.58,3.584,3.588,3.592,3.596,3.6,3.604,3.608,3.612,3.616,3.62,3.624,3.628,3.632,3.636,3.64,3.644,3.648,3.652,3.656,3.66,3.664,3.668,3.672,3.676,3.68,3.684,3.688,3.692,3.696,3.7,3.704,3.708,3.712,3.716,3.72,3.724,3.728,3.732,3.736,3.74,3.744,3.748,3.752,3.756,3.76,3.764,3.768,3.772,3.776,3.78,3.784,3.788,3.792,3.796,3.8,3.804,3.808,3.812,3.816,3.82,3.824,3.828,3.832,3.836,3.84,3.844,3.848,3.852,3.856,3.86,3.864,3.868,3.872,3.876,3.88,3.884,3.888,3.892,3.896,3.9,3.904,3.908,3.912,3.916,3.92,3.924,3.928,3.932,3.936,3.94,3.944,3.948,3.952,3.956,3.96,3.964,3.968,3.972,3.976,3.98,3.984,3.988,3.992,3.996,4,4.004,4.008,4.012,4.016,4.02,4.024,4.028,4.032,4.036,4.04,4.044,4.048,4.052,4.056,4.06,4.064,4.068,4.072,4.076,4.08,4.084,4.088,4.092,4.096,4.1,4.104,4.108,4.112,4.116,4.12,4.124,4.128,4.132,4.136,4.14,4.144,4.148,4.152,4.156,4.16,4.164,4.168,4.172,4.176,4.18,4.184,4.188,4.192,4.196,4.2,4.204,4.208,4.212,4.216,4.22,4.224,4.228,4.232,4.236,4.24,4.244,4.248,4.252,4.256,4.26,4.264,4.268,4.272,4.276,4.28,4.284,4.288,4.292,4.296,4.3,4.304,4.308,4.312,4.316,4.32,4.324,4.328,4.332,4.336,4.34,4.344,4.348,4.352,4.356,4.36,4.364,4.368,4.372,4.376,4.38,4.384,4.388,4.392,4.396,4.4,4.404,4.408,4.412,4.416,4.42,4.424,4.428,4.432,4.436,4.44,4.444,4.448,4.452,4.456,4.46,4.464,4.468,4.472,4.476,4.48,4.484,4.488,4.492,4.496,4.5,4.504,4.508,4.512,4.516,4.52,4.524,4.528,4.532,4.536,4.54,4.544,4.548,4.552,4.556,4.56,4.564,4.568,4.572,4.576,4.58,4.584,4.588,4.592,4.596,4.6,4.604,4.608,4.612,4.616,4.62,4.624,4.628,4.632,4.636,4.64,4.644,4.648,4.652,4.656,4.66,4.664,4.668,4.672,4.676,4.68,4.684,4.688,4.692,4.696,4.7,4.704,4.708,4.712,4.716,4.72,4.724,4.728,4.732,4.736,4.74,4.744,4.748,4.752,4.756,4.76,4.764,4.768,4.772,4.776,4.78,4.784,4.788,4.792,4.796,4.8,4.804,4.808,4.812,4.816,4.82,4.824,4.828,4.832,4.836,4.84,4.844,4.848,4.852,4.856,4.86,4.864,4.868,4.872,4.876,4.88,4.884,4.888,4.892,4.896,4.9,4.904,4.908,4.912,4.916,4.92,4.924,4.928,4.932,4.936,4.94,4.944,4.948,4.952,4.956,4.96,4.964,4.968,4.972,4.976,4.98,4.984,4.988,4.992,4.996,5,5.004,5.008,5.012,5.016,5.02,5.024,5.028,5.032,5.036,5.04,5.044,5.048,5.052,5.056,5.06,5.064,5.068,5.072,5.076,5.08,5.084,5.088,5.092,5.096,5.1,5.104,5.108,5.112,5.116,5.12,5.124,5.128,5.132,5.136,5.14,5.144,5.148,5.152,5.156,5.16,5.164,5.168,5.172,5.176,5.18,5.184,5.188,5.192,5.196,5.2,5.204,5.208,5.212,5.216,5.22,5.224,5.228,5.232,5.236,5.24,5.244,5.248,5.252,5.256,5.26,5.264,5.268,5.272,5.276,5.28,5.284,5.288,5.292,5.296,5.3,5.304,5.308,5.312,5.316,5.32,5.324,5.328,5.332,5.336,5.34,5.344,5.348,5.352,5.356,5.36,5.364,5.368,5.372,5.376,5.38,5.384,5.388,5.392,5.396,5.4,5.404,5.408,5.412,5.416,5.42,5.424,5.428,5.432,5.436,5.44,5.444,5.448,5.452,5.456,5.46,5.464,5.468,5.472,5.476,5.48,5.484,5.488,5.492,5.496,5.5,5.504,5.508,5.512,5.516,5.52,5.524,5.528,5.532,5.536,5.54,5.544,5.548,5.552,5.556,5.56,5.564,5.568,5.572,5.576,5.58,5.584,5.588,5.592,5.596,5.6,5.604,5.608,5.612,5.616,5.62,5.624,5.628,5.632,5.636,5.64,5.644,5.648,5.652,5.656,5.66,5.664,5.668,5.672,5.676,5.68,5.684,5.688,5.692,5.696,5.7,5.704,5.708,5.712,5.716,5.72,5.724,5.728,5.732,5.736,5.74,5.744,5.748,5.752,5.756,5.76,5.764,5.768,5.772,5.776,5.78,5.784,5.788,5.792,5.796,5.8,5.804,5.808,5.812,5.816,5.82,5.824,5.828,5.832,5.836,5.84,5.844,5.848,5.852,5.856,5.86,5.864,5.868,5.872,5.876,5.88,5.884,5.888,5.892,5.896,5.9,5.904,5.908,5.912,5.916,5.92,5.924,5.928,5.932,5.936,5.94,5.944,5.948,5.952,5.956,5.96,5.964,5.968,5.972,5.976,5.98,5.984,5.988,5.992,5.996,6,6.004,6.008,6.012,6.016,6.02,6.024,6.028,6.032,6.036,6.04,6.044,6.048,6.052,6.056,6.06,6.064,6.068,6.072,6.076,6.08,6.084,6.088,6.092,6.096,6.1,6.104,6.108,6.112,6.116,6.12,6.124,6.128,6.132,6.136,6.14,6.144,6.148,6.152,6.156,6.16,6.164,6.168,6.172,6.176,6.18,6.184,6.188,6.192,6.196,6.2,6.204,6.208,6.212,6.216,6.22,6.224,6.228,6.232,6.236,6.24,6.244,6.248,6.252,6.256,6.26,6.264,6.268,6.272,6.276,6.28,6.284,6.288,6.292,6.296,6.3,6.304,6.308,6.312,6.316,6.32,6.324,6.328,6.332,6.336,6.34,6.344,6.348,6.352,6.356,6.36,6.364,6.368,6.372,6.376,6.38,6.384,6.388,6.392,6.396,6.4,6.404,6.408,6.412,6.416,6.42,6.424,6.428,6.432,6.436,6.44,6.444,6.448,6.452,6.456,6.46,6.464,6.468,6.472,6.476,6.48,6.484,6.488,6.492,6.496,6.5,6.504,6.508,6.512,6.516,6.52,6.524,6.528,6.532,6.536,6.54,6.544,6.548,6.552,6.556,6.56,6.564,6.568,6.572,6.576,6.58,6.584,6.588,6.592,6.596,6.6,6.604,6.608,6.612,6.616,6.62,6.624,6.628,6.632,6.636,6.64,6.644,6.648,6.652,6.656,6.66,6.664,6.668,6.672,6.676,6.68,6.684,6.688,6.692,6.696,6.7,6.704,6.708,6.712,6.716,6.72,6.724,6.728,6.732,6.736,6.74,6.744,6.748,6.752,6.756,6.76,6.764,6.768,6.772,6.776,6.78,6.784,6.788,6.792,6.796,6.8,6.804,6.808,6.812,6.816,6.82,6.824,6.828,6.832,6.836,6.84,6.844,6.848,6.852,6.856,6.86,6.864,6.868,6.872,6.876,6.88,6.884,6.888,6.892,6.896,6.9,6.904,6.908,6.912,6.916,6.92,6.924,6.928,6.932,6.936,6.94,6.944,6.948,6.952,6.956,6.96,6.964,6.968,6.972,6.976,6.98,6.984,6.988,6.992,6.996,7,7.004,7.008,7.012,7.016,7.02,7.024,7.028,7.032,7.036,7.04,7.044,7.048,7.052,7.056,7.06,7.064,7.068,7.072,7.076,7.08,7.084,7.088,7.092,7.096,7.1,7.104,7.108,7.112,7.116,7.12,7.124,7.128,7.132,7.136,7.14,7.144,7.148,7.152,7.156,7.16,7.164,7.168,7.172,7.176,7.18,7.184,7.188,7.192,7.196,7.2,7.204,7.208,7.212,7.216,7.22,7.224,7.228,7.232,7.236,7.24,7.244,7.248,7.252,7.256,7.26,7.264,7.268,7.272,7.276,7.28,7.284,7.288,7.292,7.296,7.3,7.304,7.308,7.312,7.316,7.32,7.324,7.328,7.332,7.336,7.34,7.344,7.348,7.352,7.356,7.36,7.364,7.368,7.372,7.376,7.38,7.384,7.388,7.392,7.396,7.4,7.404,7.408,7.412,7.416,7.42,7.424,7.428,7.432,7.436,7.44,7.444,7.448,7.452,7.456,7.46,7.464,7.468,7.472,7.476,7.48,7.484,7.488,7.492,7.496,7.5,7.504,7.508,7.512,7.516,7.52,7.524,7.528,7.532,7.536,7.54,7.544,7.548,7.552,7.556,7.56,7.564,7.568,7.572,7.576,7.58,7.584,7.588,7.592,7.596,7.6,7.604,7.608,7.612,7.616,7.62,7.624,7.628,7.632,7.636,7.64,7.644,7.648,7.652,7.656,7.66,7.664,7.668,7.672,7.676,7.68,7.684,7.688,7.692,7.696,7.7,7.704,7.708,7.712,7.716,7.72,7.724,7.728,7.732,7.736,7.74,7.744,7.748,7.752,7.756,7.76,7.764,7.768,7.772,7.776,7.78,7.784,7.788,7.792,7.796,7.8,7.804,7.808,7.812,7.816,7.82,7.824,7.828,7.832,7.836,7.84,7.844,7.848,7.852,7.856,7.86,7.864,7.868,7.872,7.876,7.88,7.884,7.888,7.892,7.896,7.9,7.904,7.908,7.912,7.916,7.92,7.924,7.928,7.932,7.936,7.94,7.944,7.948,7.952,7.956,7.96,7.964,7.968,7.972,7.976,7.98,7.984,7.988,7.992,7.996,8,8.004,8.008,8.012,8.016,8.02,8.024,8.028,8.032,8.036,8.04,8.044,8.048,8.052,8.056,8.06,8.064,8.068,8.072,8.076,8.08,8.084,8.088,8.092,8.096,8.1,8.104,8.108,8.112,8.116,8.12,8.124,8.128,8.132,8.136,8.14,8.144,8.148,8.152,8.156,8.16,8.164,8.168,8.172,8.176,8.18,8.184,8.188,8.192,8.196,8.2,8.204,8.208,8.212,8.216,8.22,8.224,8.228,8.232,8.236,8.24,8.244,8.248,8.252,8.256,8.26,8.264,8.268,8.272,8.276,8.28,8.284,8.288,8.292,8.296,8.3,8.304,8.308,8.312,8.316,8.32,8.324,8.328,8.332,8.336,8.34,8.344,8.348,8.352,8.356,8.36,8.364,8.368,8.372,8.376,8.38,8.384,8.388,8.392,8.396,8.4,8.404,8.408,8.412,8.416,8.42,8.424,8.428,8.432,8.436,8.44,8.444,8.448,8.452,8.456,8.46,8.464,8.468,8.472,8.476,8.48,8.484,8.488,8.492,8.496,8.5,8.504,8.508,8.512,8.516,8.52,8.524,8.528,8.532,8.536,8.54,8.544,8.548,8.552,8.556,8.56,8.564,8.568,8.572,8.576,8.58,8.584,8.588,8.592,8.596,8.6,8.604,8.608,8.612,8.616,8.62,8.624,8.628,8.632,8.636,8.64,8.644,8.648,8.652,8.656,8.66,8.664,8.668,8.672,8.676,8.68,8.684,8.688,8.692,8.696,8.7,8.704,8.708,8.712,8.716,8.72,8.724,8.728,8.732,8.736,8.74,8.744,8.748,8.752,8.756,8.76,8.764,8.768,8.772,8.776,8.78,8.784,8.788,8.792,8.796,8.8,8.804,8.808,8.812,8.816,8.82,8.824,8.828,8.832,8.836,8.84,8.844,8.848,8.852,8.856,8.86,8.864,8.868,8.872,8.876,8.88,8.884,8.888,8.892,8.896,8.9,8.904,8.908,8.912,8.916,8.92,8.924,8.928,8.932,8.936,8.94,8.944,8.948,8.952,8.956,8.96,8.964,8.968,8.972,8.976,8.98,8.984,8.988,8.992,8.996,9,9.004,9.008,9.012,9.016,9.02,9.024,9.028,9.032,9.036,9.04,9.044,9.048,9.052,9.056,9.06,9.064,9.068,9.072,9.076,9.08,9.084,9.088,9.092,9.096,9.1,9.104,9.108,9.112,9.116,9.12,9.124,9.128,9.132,9.136,9.14,9.144,9.148,9.152,9.156,9.16,9.164,9.168,9.172,9.176,9.18,9.184,9.188,9.192,9.196,9.2,9.204,9.208,9.212,9.216,9.22,9.224,9.228,9.232,9.236,9.24,9.244,9.248,9.252,9.256,9.26,9.264,9.268,9.272,9.276,9.28,9.284,9.288,9.292,9.296,9.3,9.304,9.308,9.312,9.316,9.32,9.324,9.328,9.332,9.336,9.34,9.344,9.348,9.352,9.356,9.36,9.364,9.368,9.372,9.376,9.38,9.384,9.388,9.392,9.396,9.4,9.404,9.408,9.412,9.416,9.42,9.424,9.428,9.432,9.436,9.44,9.444,9.448,9.452,9.456,9.46,9.464,9.468,9.472,9.476,9.48,9.484,9.488,9.492,9.496,9.5,9.504,9.508,9.512,9.516,9.52,9.524,9.528,9.532,9.536,9.54,9.544,9.548,9.552,9.556,9.56,9.564,9.568,9.572,9.576,9.58,9.584,9.588,9.592,9.596,9.6,9.604,9.608,9.612,9.616,9.62,9.624,9.628,9.632,9.636,9.64,9.644,9.648,9.652,9.656,9.66,9.664,9.668,9.672,9.676,9.68,9.684,9.688,9.692,9.696,9.7,9.704,9.708,9.712,9.716,9.72,9.724,9.728,9.732,9.736,9.74,9.744,9.748,9.752,9.756,9.76,9.764,9.768,9.772,9.776,9.78,9.784,9.788,9.792,9.796,9.8,9.804,9.808,9.812,9.816,9.82,9.824,9.828,9.832,9.836,9.84,9.844,9.848,9.852,9.856,9.86,9.864,9.868,9.872,9.876,9.88,9.884,9.888,9.892,9.896,9.9,9.904,9.908,9.912,9.916,9.92,9.924,9.928,9.932,9.936,9.94,9.944,9.948,9.952,9.956,9.96,9.964,9.968,9.972,9.976,9.98,9.984,9.988,9.992,9.996,10,10.004,10.008,10.012,10.016,10.02,10.024,10.028,10.032,10.036,10.04,10.044,10.048,10.052,10.056,10.06,10.064,10.068,10.072,10.076,10.08,10.084,10.088,10.092,10.096,10.1,10.104,10.108,10.112,10.116,10.12,10.124,10.128,10.132,10.136,10.14,10.144,10.148,10.152,10.156,10.16,10.164,10.168,10.172,10.176,10.18,10.184,10.188,10.192,10.196,10.2,10.204,10.208,10.212,10.216,10.22,10.224,10.228,10.232,10.236,10.24,10.244,10.248,10.252,10.256,10.26,10.264,10.268,10.272,10.276,10.28,10.284,10.288,10.292,10.296,10.3,10.304,10.308,10.312,10.316,10.32,10.324,10.328,10.332,10.336,10.34,10.344,10.348,10.352,10.356,10.36,10.364,10.368,10.372,10.376,10.38,10.384,10.388,10.392,10.396,10.4,10.404,10.408,10.412,10.416,10.42,10.424,10.428,10.432,10.436,10.44,10.444,10.448,10.452,10.456,10.46,10.464,10.468,10.472,10.476,10.48,10.484,10.488,10.492,10.496,10.5,10.504,10.508,10.512,10.516,10.52,10.524,10.528,10.532,10.536,10.54,10.544,10.548,10.552,10.556,10.56,10.564,10.568,10.572,10.576,10.58,10.584,10.588,10.592,10.596,10.6,10.604,10.608,10.612,10.616,10.62,10.624,10.628,10.632,10.636,10.64,10.644,10.648,10.652,10.656,10.66,10.664,10.668,10.672,10.676,10.68,10.684,10.688,10.692,10.696,10.7,10.704,10.708,10.712,10.716,10.72,10.724,10.728,10.732,10.736,10.74,10.744,10.748,10.752,10.756,10.76,10.764,10.768,10.772,10.776,10.78,10.784,10.788,10.792,10.796,10.8,10.804,10.808,10.812,10.816,10.82,10.824,10.828,10.832,10.836,10.84,10.844,10.848,10.852,10.856,10.86,10.864,10.868,10.872,10.876,10.88,10.884,10.888,10.892,10.896,10.9,10.904,10.908,10.912,10.916,10.92,10.924,10.928,10.932,10.936,10.94,10.944,10.948,10.952,10.956,10.96,10.964,10.968,10.972,10.976,10.98,10.984,10.988,10.992,10.996,11,11.004,11.008,11.012,11.016,11.02,11.024,11.028,11.032,11.036,11.04,11.044,11.048,11.052,11.056,11.06,11.064,11.068,11.072,11.076,11.08,11.084,11.088,11.092,11.096,11.1,11.104,11.108,11.112,11.116,11.12,11.124,11.128,11.132,11.136,11.14,11.144,11.148,11.152,11.156,11.16,11.164,11.168,11.172,11.176,11.18,11.184,11.188,11.192,11.196,11.2,11.204,11.208,11.212,11.216,11.22,11.224,11.228,11.232,11.236,11.24,11.244,11.248,11.252,11.256,11.26,11.264,11.268,11.272,11.276,11.28,11.284,11.288,11.292,11.296,11.3,11.304,11.308,11.312,11.316,11.32,11.324,11.328,11.332,11.336,11.34,11.344,11.348,11.352,11.356,11.36,11.364,11.368,11.372,11.376,11.38,11.384,11.388,11.392,11.396,11.4,11.404,11.408,11.412,11.416,11.42,11.424,11.428,11.432,11.436,11.44,11.444,11.448,11.452,11.456,11.46,11.464,11.468,11.472,11.476,11.48,11.484,11.488,11.492,11.496,11.5,11.504,11.508,11.512,11.516,11.52,11.524,11.528,11.532,11.536,11.54,11.544,11.548,11.552,11.556,11.56,11.564,11.568,11.572,11.576,11.58,11.584,11.588,11.592,11.596,11.6,11.604,11.608,11.612,11.616,11.62,11.624,11.628,11.632,11.636,11.64,11.644,11.648,11.652,11.656,11.66,11.664,11.668,11.672,11.676,11.68,11.684,11.688,11.692,11.696,11.7,11.704,11.708,11.712,11.716,11.72,11.724,11.728,11.732,11.736,11.74,11.744,11.748,11.752,11.756,11.76,11.764,11.768,11.772,11.776,11.78,11.784,11.788,11.792,11.796,11.8,11.804,11.808,11.812,11.816,11.82,11.824,11.828,11.832,11.836,11.84,11.844,11.848,11.852,11.856,11.86,11.864,11.868,11.872,11.876,11.88,11.884,11.888,11.892,11.896,11.9,11.904,11.908,11.912,11.916,11.92,11.924,11.928,11.932,11.936,11.94,11.944,11.948,11.952,11.956,11.96,11.964,11.968,11.972,11.976,11.98,11.984,11.988,11.992,11.996,12,12.004,12.008,12.012,12.016,12.02,12.024,12.028,12.032,12.036,12.04,12.044,12.048,12.052,12.056,12.06,12.064,12.068,12.072,12.076,12.08,12.084,12.088,12.092,12.096,12.1,12.104,12.108,12.112,12.116,12.12,12.124,12.128,12.132,12.136,12.14,12.144,12.148,12.152,12.156,12.16,12.164,12.168,12.172,12.176,12.18,12.184,12.188,12.192,12.196,12.2,12.204,12.208,12.212,12.216,12.22,12.224,12.228,12.232,12.236,12.24,12.244,12.248,12.252,12.256,12.26,12.264,12.268,12.272,12.276,12.28,12.284,12.288,12.292,12.296,12.3,12.304,12.308,12.312,12.316,12.32,12.324,12.328,12.332,12.336,12.34,12.344,12.348,12.352,12.356,12.36,12.364,12.368,12.372,12.376,12.38,12.384,12.388,12.392,12.396,12.4,12.404,12.408,12.412,12.416,12.42,12.424,12.428,12.432,12.436,12.44,12.444,12.448,12.452,12.456,12.46,12.464,12.468,12.472,12.476,12.48,12.484,12.488,12.492,12.496,12.5,12.504,12.508,12.512,12.516,12.52,12.524,12.528,12.532,12.536,12.54,12.544,12.548,12.552,12.556,12.56,12.564,12.568,12.572,12.576,12.58,12.584,12.588,12.592,12.596,12.6,12.604,12.608,12.612,12.616,12.62,12.624,12.628,12.632,12.636,12.64,12.644,12.648,12.652,12.656,12.66,12.664,12.668,12.672,12.676,12.68,12.684,12.688,12.692,12.696,12.7,12.704,12.708,12.712,12.716,12.72,12.724,12.728,12.732,12.736,12.74,12.744,12.748,12.752,12.756,12.76,12.764,12.768,12.772,12.776,12.78,12.784,12.788,12.792,12.796,12.8,12.804,12.808,12.812,12.816,12.82,12.824,12.828,12.832,12.836,12.84,12.844,12.848,12.852,12.856,12.86,12.864,12.868,12.872,12.876,12.88,12.884,12.888,12.892,12.896,12.9,12.904,12.908,12.912,12.916,12.92,12.924,12.928,12.932,12.936,12.94,12.944,12.948,12.952,12.956,12.96,12.964,12.968,12.972,12.976,12.98,12.984,12.988,12.992,12.996,13,13.004,13.008,13.012,13.016,13.02,13.024,13.028,13.032,13.036,13.04,13.044,13.048,13.052,13.056,13.06,13.064,13.068,13.072,13.076,13.08,13.084,13.088,13.092,13.096,13.1,13.104,13.108,13.112,13.116,13.12,13.124,13.128,13.132,13.136,13.14,13.144,13.148,13.152,13.156,13.16,13.164,13.168,13.172,13.176,13.18,13.184,13.188,13.192,13.196,13.2,13.204,13.208,13.212,13.216,13.22,13.224,13.228,13.232,13.236,13.24,13.244,13.248,13.252,13.256,13.26,13.264,13.268,13.272,13.276,13.28,13.284,13.288,13.292,13.296,13.3,13.304,13.308,13.312,13.316,13.32,13.324,13.328,13.332,13.336,13.34,13.344,13.348,13.352,13.356,13.36,13.364,13.368,13.372,13.376,13.38,13.384,13.388,13.392,13.396,13.4,13.404,13.408,13.412,13.416,13.42,13.424,13.428,13.432,13.436,13.44,13.444,13.448,13.452,13.456,13.46,13.464,13.468,13.472,13.476,13.48,13.484,13.488,13.492,13.496,13.5,13.504,13.508,13.512,13.516,13.52,13.524,13.528,13.532,13.536,13.54,13.544,13.548,13.552,13.556,13.56,13.564,13.568,13.572,13.576,13.58,13.584,13.588,13.592,13.596,13.6,13.604,13.608,13.612,13.616,13.62,13.624,13.628,13.632,13.636,13.64,13.644,13.648,13.652,13.656,13.66,13.664,13.668,13.672,13.676,13.68,13.684,13.688,13.692,13.696,13.7,13.704,13.708,13.712,13.716,13.72,13.724,13.728,13.732,13.736,13.74,13.744,13.748,13.752,13.756,13.76,13.764,13.768,13.772,13.776,13.78,13.784,13.788,13.792,13.796,13.8,13.804,13.808,13.812,13.816,13.82,13.824,13.828,13.832,13.836,13.84,13.844,13.848,13.852,13.856,13.86,13.864,13.868,13.872,13.876,13.88,13.884,13.888,13.892,13.896,13.9,13.904,13.908,13.912,13.916,13.92,13.924,13.928,13.932,13.936,13.94,13.944,13.948,13.952,13.956,13.96,13.964,13.968,13.972,13.976,13.98,13.984,13.988,13.992,13.996,14,14.004,14.008,14.012,14.016,14.02,14.024,14.028,14.032,14.036,14.04,14.044,14.048,14.052,14.056,14.06,14.064,14.068,14.072,14.076,14.08,14.084,14.088,14.092,14.096,14.1,14.104,14.108,14.112,14.116,14.12,14.124,14.128,14.132,14.136,14.14,14.144,14.148,14.152,14.156,14.16,14.164,14.168,14.172,14.176,14.18,14.184,14.188,14.192,14.196,14.2,14.204,14.208,14.212,14.216,14.22,14.224,14.228,14.232,14.236,14.24,14.244,14.248,14.252,14.256,14.26,14.264,14.268,14.272,14.276,14.28,14.284,14.288,14.292,14.296,14.3,14.304,14.308,14.312,14.316,14.32,14.324,14.328,14.332,14.336,14.34,14.344,14.348,14.352,14.356,14.36,14.364,14.368,14.372,14.376,14.38,14.384,14.388,14.392,14.396,14.4,14.404,14.408,14.412,14.416,14.42,14.424,14.428,14.432,14.436,14.44,14.444,14.448,14.452,14.456,14.46,14.464,14.468,14.472,14.476,14.48,14.484,14.488,14.492,14.496,14.5,14.504,14.508,14.512,14.516,14.52,14.524,14.528,14.532,14.536,14.54,14.544,14.548,14.552,14.556,14.56,14.564,14.568,14.572,14.576,14.58,14.584,14.588,14.592,14.596,14.6,14.604,14.608,14.612,14.616,14.62,14.624,14.628,14.632,14.636,14.64,14.644,14.648,14.652,14.656,14.66,14.664,14.668,14.672,14.676,14.68,14.684,14.688,14.692,14.696,14.7,14.704,14.708,14.712,14.716,14.72,14.724,14.728,14.732,14.736,14.74,14.744,14.748,14.752,14.756,14.76,14.764,14.768,14.772,14.776,14.78,14.784,14.788,14.792,14.796,14.8,14.804,14.808,14.812,14.816,14.82,14.824,14.828,14.832,14.836,14.84,14.844,14.848,14.852,14.856,14.86,14.864,14.868,14.872,14.876,14.88,14.884,14.888,14.892,14.896,14.9,14.904,14.908,14.912,14.916,14.92,14.924,14.928,14.932,14.936,14.94,14.944,14.948,14.952,14.956,14.96,14.964,14.968,14.972,14.976,14.98,14.984,14.988,14.992,14.996,15,15.004,15.008,15.012,15.016,15.02,15.024,15.028,15.032,15.036,15.04,15.044,15.048,15.052,15.056,15.06,15.064,15.068,15.072,15.076,15.08,15.084,15.088,15.092,15.096,15.1,15.104,15.108,15.112,15.116,15.12,15.124,15.128,15.132,15.136,15.14,15.144,15.148,15.152,15.156,15.16,15.164,15.168,15.172,15.176,15.18,15.184,15.188,15.192,15.196,15.2,15.204,15.208,15.212,15.216,15.22,15.224,15.228,15.232,15.236,15.24,15.244,15.248,15.252,15.256,15.26,15.264,15.268,15.272,15.276,15.28,15.284,15.288,15.292,15.296,15.3,15.304,15.308,15.312,15.316,15.32,15.324,15.328,15.332,15.336,15.34,15.344,15.348,15.352,15.356,15.36,15.364,15.368,15.372,15.376,15.38,15.384,15.388,15.392,15.396,15.4,15.404,15.408,15.412,15.416,15.42,15.424,15.428,15.432,15.436,15.44,15.444,15.448,15.452,15.456,15.46,15.464,15.468,15.472,15.476,15.48,15.484,15.488,15.492,15.496,15.5,15.504,15.508,15.512,15.516,15.52,15.524,15.528,15.532,15.536,15.54,15.544,15.548,15.552,15.556,15.56,15.564,15.568,15.572,15.576,15.58,15.584,15.588,15.592,15.596,15.6,15.604,15.608,15.612,15.616,15.62,15.624,15.628,15.632,15.636,15.64,15.644,15.648,15.652,15.656,15.66,15.664,15.668,15.672,15.676,15.68,15.684,15.688,15.692,15.696,15.7,15.704,15.708,15.712,15.716,15.72,15.724,15.728,15.732,15.736,15.74,15.744,15.748,15.752,15.756,15.76,15.764,15.768,15.772,15.776,15.78,15.784,15.788,15.792,15.796,15.8,15.804,15.808,15.812,15.816,15.82,15.824,15.828,15.832,15.836,15.84,15.844,15.848,15.852,15.856,15.86,15.864,15.868,15.872,15.876,15.88,15.884,15.888,15.892,15.896,15.9,15.904,15.908,15.912,15.916,15.92,15.924,15.928,15.932,15.936,15.94,15.944,15.948,15.952,15.956,15.96,15.964,15.968,15.972,15.976,15.98,15.984,15.988,15.992,15.996,16,16.004,16.008,16.012,16.016,16.02,16.024,16.028,16.032,16.036,16.04,16.044,16.048,16.052,16.056,16.06,16.064,16.068,16.072,16.076,16.08,16.084,16.088,16.092,16.096,16.1,16.104,16.108,16.112,16.116,16.12,16.124,16.128,16.132,16.136,16.14,16.144,16.148,16.152,16.156,16.16,16.164,16.168,16.172,16.176,16.18,16.184,16.188,16.192,16.196,16.2,16.204,16.208,16.212,16.216,16.22,16.224,16.228,16.232,16.236,16.24,16.244,16.248,16.252,16.256,16.26,16.264,16.268,16.272,16.276,16.28,16.284,16.288,16.292,16.296,16.3,16.304,16.308,16.312,16.316,16.32,16.324,16.328,16.332,16.336,16.34,16.344,16.348,16.352,16.356,16.36,16.364,16.368,16.372,16.376,16.38,16.384,16.388,16.392,16.396,16.4,16.404,16.408,16.412,16.416,16.42,16.424,16.428,16.432,16.436,16.44,16.444,16.448,16.452,16.456,16.46,16.464,16.468,16.472,16.476,16.48,16.484,16.488,16.492,16.496,16.5,16.504,16.508,16.512,16.516,16.52,16.524,16.528,16.532,16.536,16.54,16.544,16.548,16.552,16.556,16.56,16.564,16.568,16.572,16.576,16.58,16.584,16.588,16.592,16.596,16.6,16.604,16.608,16.612,16.616,16.62,16.624,16.628,16.632,16.636,16.64,16.644,16.648,16.652,16.656,16.66,16.664,16.668,16.672,16.676,16.68,16.684,16.688,16.692,16.696,16.7,16.704,16.708,16.712,16.716,16.72,16.724,16.728,16.732,16.736,16.74,16.744,16.748,16.752,16.756,16.76,16.764,16.768,16.772,16.776,16.78,16.784,16.788,16.792,16.796,16.8,16.804,16.808,16.812,16.816,16.82,16.824,16.828,16.832,16.836,16.84,16.844,16.848,16.852,16.856,16.86,16.864,16.868,16.872,16.876,16.88,16.884,16.888,16.892,16.896,16.9,16.904,16.908,16.912,16.916,16.92,16.924,16.928,16.932,16.936,16.94,16.944,16.948,16.952,16.956,16.96,16.964,16.968,16.972,16.976,16.98,16.984,16.988,16.992,16.996,17,17.004,17.008,17.012,17.016,17.02,17.024,17.028,17.032,17.036,17.04,17.044,17.048,17.052,17.056,17.06,17.064,17.068,17.072,17.076,17.08,17.084,17.088,17.092,17.096,17.1,17.104,17.108,17.112,17.116,17.12,17.124,17.128,17.132,17.136,17.14,17.144,17.148,17.152,17.156,17.16,17.164,17.168,17.172,17.176,17.18,17.184,17.188,17.192,17.196,17.2,17.204,17.208,17.212,17.216,17.22,17.224,17.228,17.232,17.236,17.24,17.244,17.248,17.252,17.256,17.26,17.264,17.268,17.272,17.276,17.28,17.284,17.288,17.292,17.296,17.3,17.304,17.308,17.312,17.316,17.32,17.324,17.328,17.332,17.336,17.34,17.344,17.348,17.352,17.356,17.36,17.364,17.368,17.372,17.376,17.38,17.384,17.388,17.392,17.396,17.4,17.404,17.408,17.412,17.416,17.42,17.424,17.428,17.432,17.436,17.44,17.444,17.448,17.452,17.456,17.46,17.464,17.468,17.472,17.476,17.48,17.484,17.488,17.492,17.496,17.5,17.504,17.508,17.512,17.516,17.52,17.524,17.528,17.532,17.536,17.54,17.544,17.548,17.552,17.556,17.56,17.564,17.568,17.572,17.576,17.58,17.584,17.588,17.592,17.596,17.6,17.604,17.608,17.612,17.616,17.62,17.624,17.628,17.632,17.636,17.64,17.644,17.648,17.652,17.656,17.66,17.664,17.668,17.672,17.676,17.68,17.684,17.688,17.692,17.696,17.7,17.704,17.708,17.712,17.716,17.72,17.724,17.728,17.732,17.736,17.74,17.744,17.748,17.752,17.756,17.76,17.764,17.768,17.772,17.776,17.78,17.784,17.788,17.792,17.796,17.8,17.804,17.808,17.812,17.816,17.82,17.824,17.828,17.832,17.836,17.84,17.844,17.848,17.852,17.856,17.86,17.864,17.868,17.872,17.876,17.88,17.884,17.888,17.892,17.896,17.9,17.904,17.908,17.912,17.916,17.92,17.924,17.928,17.932,17.936,17.94,17.944,17.948,17.952,17.956,17.96,17.964,17.968,17.972,17.976,17.98,17.984,17.988,17.992,17.996,18,18.004,18.008,18.012,18.016,18.02,18.024,18.028,18.032,18.036,18.04,18.044,18.048,18.052,18.056,18.06,18.064,18.068,18.072,18.076,18.08,18.084,18.088,18.092,18.096,18.1,18.104,18.108,18.112,18.116,18.12,18.124,18.128,18.132,18.136,18.14,18.144,18.148,18.152,18.156,18.16,18.164,18.168,18.172,18.176,18.18,18.184,18.188,18.192,18.196,18.2,18.204,18.208,18.212,18.216,18.22,18.224,18.228,18.232,18.236,18.24,18.244,18.248,18.252,18.256,18.26,18.264,18.268,18.272,18.276,18.28,18.284,18.288,18.292,18.296,18.3,18.304,18.308,18.312,18.316,18.32,18.324,18.328,18.332,18.336,18.34,18.344,18.348,18.352,18.356,18.36,18.364,18.368,18.372,18.376,18.38,18.384,18.388,18.392,18.396,18.4,18.404,18.408,18.412,18.416,18.42,18.424,18.428,18.432,18.436,18.44,18.444,18.448,18.452,18.456,18.46,18.464,18.468,18.472,18.476,18.48,18.484,18.488,18.492,18.496,18.5,18.504,18.508,18.512,18.516,18.52,18.524,18.528,18.532,18.536,18.54,18.544,18.548,18.552,18.556,18.56,18.564,18.568,18.572,18.576,18.58,18.584,18.588,18.592,18.596,18.6,18.604,18.608,18.612,18.616,18.62,18.624,18.628,18.632,18.636,18.64,18.644,18.648,18.652,18.656,18.66,18.664,18.668,18.672,18.676,18.68,18.684,18.688,18.692,18.696,18.7,18.704,18.708,18.712,18.716,18.72,18.724,18.728,18.732,18.736,18.74,18.744,18.748,18.752,18.756,18.76,18.764,18.768,18.772,18.776,18.78,18.784,18.788,18.792,18.796,18.8,18.804,18.808,18.812,18.816,18.82,18.824,18.828,18.832,18.836,18.84,18.844,18.848,18.852,18.856,18.86,18.864,18.868,18.872,18.876,18.88,18.884,18.888,18.892,18.896,18.9,18.904,18.908,18.912,18.916,18.92,18.924,18.928,18.932,18.936,18.94,18.944,18.948,18.952,18.956,18.96,18.964,18.968,18.972,18.976,18.98,18.984,18.988,18.992,18.996,19,19.004,19.008,19.012,19.016,19.02,19.024,19.028,19.032,19.036,19.04,19.044,19.048,19.052,19.056,19.06,19.064,19.068,19.072,19.076,19.08,19.084,19.088,19.092,19.096,19.1,19.104,19.108,19.112,19.116,19.12,19.124,19.128,19.132,19.136,19.14,19.144,19.148,19.152,19.156,19.16,19.164,19.168,19.172,19.176,19.18,19.184,19.188,19.192,19.196,19.2,19.204,19.208,19.212,19.216,19.22,19.224,19.228,19.232,19.236,19.24,19.244,19.248,19.252,19.256,19.26,19.264,19.268,19.272,19.276,19.28,19.284,19.288,19.292,19.296,19.3,19.304,19.308,19.312,19.316,19.32,19.324,19.328,19.332,19.336,19.34,19.344,19.348,19.352,19.356,19.36,19.364,19.368,19.372,19.376,19.38,19.384,19.388,19.392,19.396,19.4,19.404,19.408,19.412,19.416,19.42,19.424,19.428,19.432,19.436,19.44,19.444,19.448,19.452,19.456,19.46,19.464,19.468,19.472,19.476,19.48,19.484,19.488,19.492,19.496,19.5,19.504,19.508,19.512,19.516,19.52,19.524,19.528,19.532,19.536,19.54,19.544,19.548,19.552,19.556,19.56,19.564,19.568,19.572,19.576,19.58,19.584,19.588,19.592,19.596,19.6,19.604,19.608,19.612,19.616,19.62,19.624,19.628,19.632,19.636,19.64,19.644,19.648,19.652,19.656,19.66,19.664,19.668,19.672,19.676,19.68,19.684,19.688,19.692,19.696,19.7,19.704,19.708,19.712,19.716,19.72,19.724,19.728,19.732 s</t>
+    <t>0.795271692,0.855778355,0.946528036,0.866051904,0.775446631,0.674794735,0.543941082,0.453377068,0.413190576,0.493811115,0.614618146,0.705223419,0.785823328,0.876449231,0.967137022,1.017514544,1.098155712,1.078103726,0.997606965,0.927136197,0.866732681,0.786194661,0.715723893,0.615051368,0.554647852,0.484238973,0.4339646,0.454222882,0.544828155,0.60527293,0.685852209,0.796633247,0.857036762,0.957791806,0.998102075,0.998267112,0.947992738,0.857346206,0.817097826,0.726513182,0.656042414,0.595659529,0.52523002,0.444692,0.474996906,0.53542105,0.626046953,0.696497091,0.726822627,0.757189421,0.817634196,0.878161489,0.80775261,0.737281842,0.646676569,0.596319677,0.606551966,0.656908858,0.576453356,0.536266865,0.556545777,0.606943929,0.687481949,0.687626356,0.768226266,0.818624417,0.869043198,0.808742831,0.72822544,0.677889178,0.60741841,0.526942278,0.607562817,0.577464208,0.517101952,0.567541362,0.648058753,0.738643396,0.809155424,0.87970871,0.829454966,0.789289103,0.718818336,0.638280315,0.587944052,0.567974584,0.497524446,0.457317325,0.517844618,0.588294756,0.678920658,0.729277551,0.80985683,0.860254982,0.870446012,0.810063127,0.739716136,0.689421133,0.608945001,0.538494863,0.447868961,0.3673722,0.286896068,0.367516607,0.448054627,0.528633907,0.609213186,0.730040847,0.800511614,0.891158147,0.941576928,0.891281924,0.871312456,0.770639931,0.700169163,0.609605149,0.529067129,0.448549738,0.368094236,0.327866485,0.408487024,0.489086933,0.569624954,0.670338738,0.740809506,0.821409415,0.92214383,1.012810991,1.073214507,1.13372117,1.083467426,0.972707018,0.851899988,0.771361967,0.690823947,0.610285926,0.529830425,0.459400916,0.378862896,0.308474646,0.36896068,0.459607212,0.530139869,0.650967529,0.751660684,0.832260593,0.892746627,0.842534142,0.751928869,0.641209721,0.530573091,0.61119363,0.681746916,0.732248216,0.812951273,0.76263564,0.682118249,0.61168874,0.531233238,0.541403639,0.622024178,0.702562198,0.813322606,0.883834633,0.974522424,1.014873953,0.96455832,0.894087552,0.833684037,0.743099393,0.692845649,0.632524652,0.572203656,0.532037793,0.602611709,0.693237612,0.773816892,0.834261666,0.773961299,0.723645666,0.653174898,0.572657507,0.482052234,0.411684614,0.51237777,0.592998308,0.653484342,0.703965012,0.653773157,0.583384907,0.492800264,0.412282873,0.331744853,0.271444486,0.331951149,0.45275818,0.523228947,0.623901473,0.694454759,0.775095928,0.825514709,0.75512646,0.694784833,0.614329331,0.53381194,0.433201304,0.332652556,0.413273095,0.524054132,0.584540166,0.655093452,0.735713991 mV</t>
+  </si>
+  <si>
+    <t>0,0.018731691,0.047668166,0.059743368,0.059495812,0.063319168,0.067060005,0.075009283,0.091292927,0.107906644,0.108236718,0.108484273,0.120999574,0.125345546,0.14198677,0.150321134,0.171033269,0.187371924,0.195348709,0.195156166,0.194991129,0.19477108,0.194578537,0.194303475,0.194138438,0.206241146,0.218398867,0.243044381,0.243291937,0.251653808,0.260070691,0.268570093,0.268735129,0.285403859,0.293710718,0.326498054,0.338655774,0.330211385,0.334199777,0.338050639,0.337858096,0.341791476,0.349795767,0.349575718,0.370150321,0.374413775,0.378759747,0.374853874,0.399526894,0.432396749,0.44075862,0.465514159,0.477616867,0.477424324,0.477176768,0.472940821,0.505755663,0.509991611,0.526165229,0.542448873,0.571192804,0.583625586,0.583845635,0.612534555,0.625049855,0.637482637,0.654013836,0.674340884,0.678219252,0.678081721,0.677889178,0.68996438,0.706578097,0.726987663,0.735019461,0.755649076,0.751770709,0.747919847,0.756309224,0.772895435,0.789151573,0.809533633,0.80934109,0.809121041,0.80898351,0.841715834,0.845621708,0.857806934,0.882562473,0.878656599,0.883002572,0.88723852,0.895655403,0.908088185,0.932706193,0.936639573,0.961037532,0.969096835,0.981172037,0.985077911,0.980731939,0.988708724,1.000783925,1.017397643,1.017617692,1.026034575,1.034451459,1.038879949,1.039072492,1.047516882,1.064048081,1.072107384,1.104839708,1.104564646,1.104372103,1.112321382,1.112101333,1.1159797,1.132153319,1.140240129,1.156853846,1.169369146,1.169589196,1.178061091,1.178253634,1.190768935,1.203339247,1.215882054,1.216047091,1.236704213,1.25296035,1.248559365,1.248229291,1.248009242,1.247789193,1.247569144,1.263742762,1.271747053,1.271527004,1.287728129,1.304286834,1.312731224,1.325219018,1.329647509,1.334020987,1.346536287,1.363094993,1.387547964,1.387300408,1.391096258,1.411285775,1.427899493,1.444485704,1.477410571,1.510417956,1.514378842,1.51825721,1.526261501,1.54243512,1.562954711,1.579568428,1.579788478,1.584189462,1.59257884,1.609220063,1.625723756,1.629684642,1.629492099,1.629327062,1.633177924,1.649434061,1.665662692,1.681891323,1.702273384,1.722958012,1.727303984,1.735720868,1.744082739,1.764409787,1.768370673,1.76817813,1.772056498,1.771808942,1.792108484,1.796481963,1.81309568,1.829654385,1.858480835,1.887032223,1.903233348,1.90708421,1.910962578,1.910742529,1.931069577,1.951726699,1.952056773,1.952249316,1.952524377,1.969110588,1.989822723,2.006353922,2.022555047,2.034685261,2.05085888,2.054737247,2.066757437,2.091072878,2.107686595,2.116185997,2.132744702,2.149330913,2.16594463 s</t>
+  </si>
+  <si>
+    <t>0,0.003,0.005,0.008,0.011,0.014,0.017,0.019,0.022,0.025,0.028,0.03,0.033,0.036,0.039,0.042,0.044,0.047,0.05,0.053,0.055,0.058,0.061,0.064,0.067,0.069,0.072,0.075,0.078,0.08,0.083,0.086,0.089,0.092,0.094,0.097,0.1,0.103,0.105,0.108,0.111,0.114,0.117,0.119,0.122,0.125,0.128,0.13,0.133,0.136,0.139,0.142,0.144,0.147,0.15,0.153,0.155,0.158,0.161,0.164,0.167,0.169,0.172,0.175,0.178,0.18,0.183,0.186,0.189,0.192,0.194,0.197,0.2,0.203,0.205,0.208,0.211,0.214,0.217,0.219,0.222,0.225,0.228,0.23,0.233,0.236,0.239,0.242,0.244,0.247,0.25,0.253,0.255,0.258,0.261,0.264,0.267,0.269,0.272,0.275,0.278,0.28,0.283,0.286,0.289,0.292,0.294,0.297,0.3,0.303,0.305,0.308,0.311,0.314,0.317,0.319,0.322,0.325,0.328,0.33,0.333,0.336,0.339,0.342,0.344,0.347,0.35,0.353,0.355,0.358,0.361,0.364,0.367,0.369,0.372,0.375,0.378,0.38,0.383,0.386,0.389,0.392,0.394,0.397,0.4,0.403,0.405,0.408,0.411,0.414,0.417,0.419,0.422,0.425,0.428,0.43,0.433,0.436,0.439,0.442,0.444,0.447,0.45,0.453,0.455,0.458,0.461,0.464,0.467,0.469,0.472,0.475,0.478,0.48,0.483,0.486,0.489,0.492,0.494,0.497,0.5,0.503,0.505,0.508,0.511,0.514,0.517,0.519,0.522,0.525,0.528,0.53,0.533,0.536,0.539,0.542,0.544 s</t>
+  </si>
+  <si>
+    <t>-0.39,-0.38,-0.365,-0.345,-0.335,-0.325,-0.32,-0.315,-0.295,-0.285,-0.275,-0.285,-0.295,-0.31,-0.32,-0.305,-0.295,-0.275,-0.265,-0.29,-0.31,-0.335,-0.345,-0.355,-0.36,-0.36,-0.37,-0.37,-0.375,-0.38,-0.385,-0.385,-0.38,-0.39,-0.41,-0.425,-0.43,-0.435,-0.44,-0.44,-0.44,-0.43,-0.43,-0.435,-0.43,-0.425,-0.425,-0.43,-0.445,-0.435,-0.44,-0.435,-0.425,-0.425,-0.43,-0.43,-0.43,-0.43,-0.43,-0.445,-0.445,-0.46,-0.45,-0.445,-0.445,-0.435,-0.42,-0.425,-0.425,-0.425,-0.44,-0.45,-0.445,-0.445,-0.43,-0.405,-0.395,-0.395,-0.385,-0.38,-0.38,-0.385,-0.39,-0.39,-0.39,-0.385,-0.38,-0.38,-0.38,-0.37,-0.36,-0.37,-0.37,-0.4,-0.405,-0.415,-0.435,-0.445,-0.445,-0.43,-0.415,-0.405,-0.41,-0.43,-0.455,-0.485,-0.49,-0.49,-0.49,-0.49,-0.475,-0.48,-0.485,-0.475,-0.465,-0.47,-0.46,-0.455,-0.445,-0.465,-0.475,-0.48,-0.495,-0.505,-0.525,-0.535,-0.545,-0.505,-0.445,-0.345,-0.21,-0.05,0.16,0.39,0.62,0.8,0.885,0.835,0.62,0.305,-0.035,-0.34,-0.545,-0.615,-0.585,-0.525,-0.45,-0.395,-0.365,-0.355,-0.355,-0.375,-0.405,-0.435,-0.45,-0.465,-0.465,-0.465,-0.465,-0.45,-0.445,-0.45,-0.44,-0.43,-0.43,-0.43,-0.435,-0.43,-0.445,-0.45,-0.445,-0.445,-0.435,-0.42,-0.41,-0.42,-0.42,-0.425,-0.42,-0.425,-0.41,-0.41,-0.405,-0.4,-0.41,-0.395,-0.39,-0.39,-0.38,-0.38,-0.385,-0.4,-0.4,-0.405,-0.4,-0.39,-0.39 mV</t>
   </si>
 </sst>
 </file>
@@ -28154,7 +28154,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28296,7 +28296,7 @@
         <v>677</v>
       </c>
       <c r="B9" s="170" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
@@ -28307,20 +28307,20 @@
         <v>764</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="168" t="s">
         <v>676</v>
       </c>
       <c r="B11" s="169" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="168" t="s">
         <v>677</v>
       </c>
       <c r="B12" s="170" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved vtac and vfib waveforms
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B48499-7B53-4CF1-8DAA-5C667C921373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C03FBFE-943D-4366-83CB-A7D054448DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2350,16 +2350,16 @@
     <t>Type</t>
   </si>
   <si>
-    <t>0.795271692,0.855778355,0.946528036,0.866051904,0.775446631,0.674794735,0.543941082,0.453377068,0.413190576,0.493811115,0.614618146,0.705223419,0.785823328,0.876449231,0.967137022,1.017514544,1.098155712,1.078103726,0.997606965,0.927136197,0.866732681,0.786194661,0.715723893,0.615051368,0.554647852,0.484238973,0.4339646,0.454222882,0.544828155,0.60527293,0.685852209,0.796633247,0.857036762,0.957791806,0.998102075,0.998267112,0.947992738,0.857346206,0.817097826,0.726513182,0.656042414,0.595659529,0.52523002,0.444692,0.474996906,0.53542105,0.626046953,0.696497091,0.726822627,0.757189421,0.817634196,0.878161489,0.80775261,0.737281842,0.646676569,0.596319677,0.606551966,0.656908858,0.576453356,0.536266865,0.556545777,0.606943929,0.687481949,0.687626356,0.768226266,0.818624417,0.869043198,0.808742831,0.72822544,0.677889178,0.60741841,0.526942278,0.607562817,0.577464208,0.517101952,0.567541362,0.648058753,0.738643396,0.809155424,0.87970871,0.829454966,0.789289103,0.718818336,0.638280315,0.587944052,0.567974584,0.497524446,0.457317325,0.517844618,0.588294756,0.678920658,0.729277551,0.80985683,0.860254982,0.870446012,0.810063127,0.739716136,0.689421133,0.608945001,0.538494863,0.447868961,0.3673722,0.286896068,0.367516607,0.448054627,0.528633907,0.609213186,0.730040847,0.800511614,0.891158147,0.941576928,0.891281924,0.871312456,0.770639931,0.700169163,0.609605149,0.529067129,0.448549738,0.368094236,0.327866485,0.408487024,0.489086933,0.569624954,0.670338738,0.740809506,0.821409415,0.92214383,1.012810991,1.073214507,1.13372117,1.083467426,0.972707018,0.851899988,0.771361967,0.690823947,0.610285926,0.529830425,0.459400916,0.378862896,0.308474646,0.36896068,0.459607212,0.530139869,0.650967529,0.751660684,0.832260593,0.892746627,0.842534142,0.751928869,0.641209721,0.530573091,0.61119363,0.681746916,0.732248216,0.812951273,0.76263564,0.682118249,0.61168874,0.531233238,0.541403639,0.622024178,0.702562198,0.813322606,0.883834633,0.974522424,1.014873953,0.96455832,0.894087552,0.833684037,0.743099393,0.692845649,0.632524652,0.572203656,0.532037793,0.602611709,0.693237612,0.773816892,0.834261666,0.773961299,0.723645666,0.653174898,0.572657507,0.482052234,0.411684614,0.51237777,0.592998308,0.653484342,0.703965012,0.653773157,0.583384907,0.492800264,0.412282873,0.331744853,0.271444486,0.331951149,0.45275818,0.523228947,0.623901473,0.694454759,0.775095928,0.825514709,0.75512646,0.694784833,0.614329331,0.53381194,0.433201304,0.332652556,0.413273095,0.524054132,0.584540166,0.655093452,0.735713991 mV</t>
-  </si>
-  <si>
-    <t>0,0.018731691,0.047668166,0.059743368,0.059495812,0.063319168,0.067060005,0.075009283,0.091292927,0.107906644,0.108236718,0.108484273,0.120999574,0.125345546,0.14198677,0.150321134,0.171033269,0.187371924,0.195348709,0.195156166,0.194991129,0.19477108,0.194578537,0.194303475,0.194138438,0.206241146,0.218398867,0.243044381,0.243291937,0.251653808,0.260070691,0.268570093,0.268735129,0.285403859,0.293710718,0.326498054,0.338655774,0.330211385,0.334199777,0.338050639,0.337858096,0.341791476,0.349795767,0.349575718,0.370150321,0.374413775,0.378759747,0.374853874,0.399526894,0.432396749,0.44075862,0.465514159,0.477616867,0.477424324,0.477176768,0.472940821,0.505755663,0.509991611,0.526165229,0.542448873,0.571192804,0.583625586,0.583845635,0.612534555,0.625049855,0.637482637,0.654013836,0.674340884,0.678219252,0.678081721,0.677889178,0.68996438,0.706578097,0.726987663,0.735019461,0.755649076,0.751770709,0.747919847,0.756309224,0.772895435,0.789151573,0.809533633,0.80934109,0.809121041,0.80898351,0.841715834,0.845621708,0.857806934,0.882562473,0.878656599,0.883002572,0.88723852,0.895655403,0.908088185,0.932706193,0.936639573,0.961037532,0.969096835,0.981172037,0.985077911,0.980731939,0.988708724,1.000783925,1.017397643,1.017617692,1.026034575,1.034451459,1.038879949,1.039072492,1.047516882,1.064048081,1.072107384,1.104839708,1.104564646,1.104372103,1.112321382,1.112101333,1.1159797,1.132153319,1.140240129,1.156853846,1.169369146,1.169589196,1.178061091,1.178253634,1.190768935,1.203339247,1.215882054,1.216047091,1.236704213,1.25296035,1.248559365,1.248229291,1.248009242,1.247789193,1.247569144,1.263742762,1.271747053,1.271527004,1.287728129,1.304286834,1.312731224,1.325219018,1.329647509,1.334020987,1.346536287,1.363094993,1.387547964,1.387300408,1.391096258,1.411285775,1.427899493,1.444485704,1.477410571,1.510417956,1.514378842,1.51825721,1.526261501,1.54243512,1.562954711,1.579568428,1.579788478,1.584189462,1.59257884,1.609220063,1.625723756,1.629684642,1.629492099,1.629327062,1.633177924,1.649434061,1.665662692,1.681891323,1.702273384,1.722958012,1.727303984,1.735720868,1.744082739,1.764409787,1.768370673,1.76817813,1.772056498,1.771808942,1.792108484,1.796481963,1.81309568,1.829654385,1.858480835,1.887032223,1.903233348,1.90708421,1.910962578,1.910742529,1.931069577,1.951726699,1.952056773,1.952249316,1.952524377,1.969110588,1.989822723,2.006353922,2.022555047,2.034685261,2.05085888,2.054737247,2.066757437,2.091072878,2.107686595,2.116185997,2.132744702,2.149330913,2.16594463 s</t>
-  </si>
-  <si>
-    <t>0,0.003,0.005,0.008,0.011,0.014,0.017,0.019,0.022,0.025,0.028,0.03,0.033,0.036,0.039,0.042,0.044,0.047,0.05,0.053,0.055,0.058,0.061,0.064,0.067,0.069,0.072,0.075,0.078,0.08,0.083,0.086,0.089,0.092,0.094,0.097,0.1,0.103,0.105,0.108,0.111,0.114,0.117,0.119,0.122,0.125,0.128,0.13,0.133,0.136,0.139,0.142,0.144,0.147,0.15,0.153,0.155,0.158,0.161,0.164,0.167,0.169,0.172,0.175,0.178,0.18,0.183,0.186,0.189,0.192,0.194,0.197,0.2,0.203,0.205,0.208,0.211,0.214,0.217,0.219,0.222,0.225,0.228,0.23,0.233,0.236,0.239,0.242,0.244,0.247,0.25,0.253,0.255,0.258,0.261,0.264,0.267,0.269,0.272,0.275,0.278,0.28,0.283,0.286,0.289,0.292,0.294,0.297,0.3,0.303,0.305,0.308,0.311,0.314,0.317,0.319,0.322,0.325,0.328,0.33,0.333,0.336,0.339,0.342,0.344,0.347,0.35,0.353,0.355,0.358,0.361,0.364,0.367,0.369,0.372,0.375,0.378,0.38,0.383,0.386,0.389,0.392,0.394,0.397,0.4,0.403,0.405,0.408,0.411,0.414,0.417,0.419,0.422,0.425,0.428,0.43,0.433,0.436,0.439,0.442,0.444,0.447,0.45,0.453,0.455,0.458,0.461,0.464,0.467,0.469,0.472,0.475,0.478,0.48,0.483,0.486,0.489,0.492,0.494,0.497,0.5,0.503,0.505,0.508,0.511,0.514,0.517,0.519,0.522,0.525,0.528,0.53,0.533,0.536,0.539,0.542,0.544 s</t>
-  </si>
-  <si>
-    <t>-0.39,-0.38,-0.365,-0.345,-0.335,-0.325,-0.32,-0.315,-0.295,-0.285,-0.275,-0.285,-0.295,-0.31,-0.32,-0.305,-0.295,-0.275,-0.265,-0.29,-0.31,-0.335,-0.345,-0.355,-0.36,-0.36,-0.37,-0.37,-0.375,-0.38,-0.385,-0.385,-0.38,-0.39,-0.41,-0.425,-0.43,-0.435,-0.44,-0.44,-0.44,-0.43,-0.43,-0.435,-0.43,-0.425,-0.425,-0.43,-0.445,-0.435,-0.44,-0.435,-0.425,-0.425,-0.43,-0.43,-0.43,-0.43,-0.43,-0.445,-0.445,-0.46,-0.45,-0.445,-0.445,-0.435,-0.42,-0.425,-0.425,-0.425,-0.44,-0.45,-0.445,-0.445,-0.43,-0.405,-0.395,-0.395,-0.385,-0.38,-0.38,-0.385,-0.39,-0.39,-0.39,-0.385,-0.38,-0.38,-0.38,-0.37,-0.36,-0.37,-0.37,-0.4,-0.405,-0.415,-0.435,-0.445,-0.445,-0.43,-0.415,-0.405,-0.41,-0.43,-0.455,-0.485,-0.49,-0.49,-0.49,-0.49,-0.475,-0.48,-0.485,-0.475,-0.465,-0.47,-0.46,-0.455,-0.445,-0.465,-0.475,-0.48,-0.495,-0.505,-0.525,-0.535,-0.545,-0.505,-0.445,-0.345,-0.21,-0.05,0.16,0.39,0.62,0.8,0.885,0.835,0.62,0.305,-0.035,-0.34,-0.545,-0.615,-0.585,-0.525,-0.45,-0.395,-0.365,-0.355,-0.355,-0.375,-0.405,-0.435,-0.45,-0.465,-0.465,-0.465,-0.465,-0.45,-0.445,-0.45,-0.44,-0.43,-0.43,-0.43,-0.435,-0.43,-0.445,-0.45,-0.445,-0.445,-0.435,-0.42,-0.41,-0.42,-0.42,-0.425,-0.42,-0.425,-0.41,-0.41,-0.405,-0.4,-0.41,-0.395,-0.39,-0.39,-0.38,-0.38,-0.385,-0.4,-0.4,-0.405,-0.4,-0.39,-0.39 mV</t>
+    <t>0.146,0.179,0.195,0.163,0.138,0.098,0.147,0.196,0.236,0.285,0.326,0.285,0.253,0.196,0.155,0.115,0.074,0.058,0.05,0.123,0.172,0.229,0.278,0.319,0.343,0.376,0.327,0.278,0.246,0.213,0.181,0.149,0.149,0.141,0.141,0.166,0.214,0.263,0.312,0.345,0.361,0.361,0.362,0.345,0.329,0.321,0.297,0.248,0.216,0.184,0.216,0.249,0.29,0.33,0.379,0.412,0.445,0.445,0.421,0.396,0.372,0.323,0.283,0.242,0.185,0.145,0.104,0.056,0.04,0.04,0.072,0.121,0.154,0.195,0.252,0.3,0.366,0.415,0.463,0.496,0.512,0.488,0.472,0.448,0.44,0.399,0.343,0.294,0.245,0.205,0.164,0.123,0.091,0.075,0.091,0.116,0.14,0.214,0.271,0.32,0.352,0.393,0.393,0.377,0.353,0.328,0.28,0.239,0.199,0.142,0.085,0.061,0.093,0.158,0.215,0.272,0.321,0.37,0.394,0.338,0.289,0.232,0.167,0.118,0.159,0.192,0.24,0.306,0.354,0.387,0.42,0.355,0.29,0.233,0.168,0.095,0.054,0.03,-0.018,-0.034,-0.009,0.014,0.055,0.104,0.145,0.21,0.259,0.34,0.373,0.422,0.438,0.43,0.398,0.374,0.333,0.292,0.252,0.203,0.154,0.106,0.114,0.13,0.179,0.228,0.285,0.326,0.342,0.343,0.335,0.31,0.278,0.246,0.197,0.156,0.108,0.124,0.132,0.181,0.238,0.287,0.312,0.361,0.361,0.385,0.394,0.402,0.378,0.354,0.346,0.297,0.24,0.183,0.135,0.118,0.102,0.103,0.095,0.135,0.2,0.241,0.266,0.299,0.315,0.315,0.324,0.267,0.218,0.161,0.113,0.088,0.113,0.137,0.186,0.235,0.317,0.366,0.439,0.496,0.545,0.586,0.618,0.602,0.586,0.529,0.472,0.432,0.391,0.343,0.286,0.27,0.245,0.221,0.238,0.27,0.303,0.319,0.36,0.401,0.434,0.442,0.442,0.402,0.345,0.288,0.264,0.207,0.199,0.191,0.207,0.175,0.143,0.11,0.143,0.2,0.249,0.265,0.208,0.16,0.111,0.079,0.111,0.16,0.209,0.242,0.291,0.283,0.275,0.25,0.21,0.161,0.12,0.088,0.047,0.072,0.129,0.178,0.243,0.283,0.292,0.251,0.202,0.145,0.097,0.064 mV</t>
+  </si>
+  <si>
+    <t>0,0.015,0.024,0.034,0.046,0.062,0.08,0.077,0.08,0.095,0.113,0.123,0.132,0.13,0.136,0.149,0.161,0.18,0.202,0.208,0.211,0.216,0.222,0.222,0.231,0.247,0.259,0.263,0.272,0.285,0.294,0.31,0.329,0.347,0.363,0.381,0.39,0.406,0.418,0.433,0.452,0.476,0.501,0.52,0.542,0.557,0.576,0.589,0.605,0.62,0.636,0.651,0.657,0.669,0.687,0.697,0.712,0.734,0.749,0.759,0.774,0.79,0.8,0.813,0.825,0.838,0.851,0.863,0.885,0.901,0.919,0.931,0.95,0.956,0.968,0.983,0.998,1.013,1.029,1.041,1.059,1.081,1.097,1.116,1.134,1.15,1.163,1.169,1.179,1.185,1.195,1.202,1.217,1.233,1.251,1.27,1.291,1.297,1.309,1.328,1.334,1.346,1.361,1.383,1.405,1.421,1.427,1.437,1.443,1.447,1.453,1.475,1.491,1.503,1.508,1.511,1.517,1.526,1.538,1.542,1.542,1.546,1.552,1.562,1.577,1.586,1.592,1.607,1.616,1.628,1.65,1.653,1.663,1.676,1.676,1.683,1.69,1.708,1.733,1.749,1.771,1.795,1.814,1.826,1.844,1.856,1.859,1.862,1.883,1.898,1.923,1.948,1.967,1.983,1.986,1.995,2.005,2.005,2.015,2.025,2.043,2.062,2.071,2.08,2.089,2.107,2.135,2.16,2.178,2.197,2.216,2.232,2.245,2.251,2.261,2.279,2.298,2.316,2.328,2.346,2.371,2.383,2.408,2.427,2.458,2.482,2.501,2.523,2.545,2.558,2.564,2.574,2.58,2.599,2.621,2.646,2.658,2.67,2.685,2.695,2.719,2.75,2.775,2.797,2.821,2.831,2.841,2.85,2.863,2.876,2.9,2.916,2.925,2.946,2.964,2.992,3.001,3.022,3.041,3.059,3.071,3.09,3.109,3.121,3.131,3.141,3.156,3.166,3.173,3.191,3.201,3.22,3.241,3.266,3.284,3.309,3.334,3.352,3.373,3.398,3.417,3.423,3.439,3.446,3.462,3.468,3.493,3.515,3.539,3.558,3.577,3.596,3.608,3.614,3.62,3.645,3.648,3.658,3.677,3.689,3.702,3.711,3.723,3.735,3.756,3.781,3.797,3.813,3.816,3.819,3.82,3.829,3.851,3.863,3.869,3.869,3.872,3.887,3.899,3.909,3.912,3.919,3.925,3.932 s</t>
+  </si>
+  <si>
+    <t>0,0.02,0.04,0.06,0.08,0.1,0.12,0.14,0.16,0.18,0.20,0.22,0.24,0.26,0.28,0.3,0.32,0.34,0.36 s</t>
+  </si>
+  <si>
+    <t>0.0,0.007,0.024,0.033,0.247,0.938,1.273,1.353,1.423,1.417,1.209,1.024,0.740,0.638,0.325,0.033,0.027,0.007,0.0 mV</t>
   </si>
 </sst>
 </file>
@@ -28154,7 +28154,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28307,7 +28307,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="168" t="s">
         <v>676</v>
       </c>
@@ -28315,7 +28315,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="168" t="s">
         <v>677</v>
       </c>

</xml_diff>

<commit_message>
Convert ecg from a waveform with static cycle time to a waveform constructed dynamically based on the HR at the start of the cardiac cycle - Works ok, still needs more testing and the spline interpolate seems to be losing peaks...
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C03FBFE-943D-4366-83CB-A7D054448DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13B1D61-A776-4F29-888F-14D0AC820EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="29870" windowHeight="10590" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5330" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5324" uniqueCount="766">
   <si>
     <t>Name</t>
   </si>
@@ -2080,13 +2080,7 @@
     <t>ElectricPotential</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>-0.039,-0.032,-0.026,-0.021,-0.01,-0.001,0,0.006,0.009,-0.002,-0.004,0.006,0.006,0.01,0.022,0.043,0.052,0.054,0.062,0.071,0.068,0.061,0.057,0.061,0.06,0.046,0.042,0.035,0.017,0.004,-0.001,-0.009,-0.01,-0.012,-0.024,-0.031,-0.038,-0.048,-0.049,-0.051,-0.049,-0.048,-0.057,-0.062,-0.06,-0.059,-0.06,-0.065,-0.067,-0.067,-0.076,-0.089,-0.085,-0.074,-0.072,-0.073,-0.074,-0.077,-0.078,-0.079,-0.083,-0.084,-0.074,-0.078,-0.09,-0.083,-0.083,-0.084,-0.074,-0.073,-0.076,-0.077,-0.078,-0.065,-0.04,-0.01,0.033,0.081,0.12,0.157,0.193,0.243,0.319,0.396,0.461,0.513,0.568,0.629,0.658,0.668,0.623,0.453,0.232,0.106,0.063,0.017,-0.006,-0.011,-0.042,-0.077,-0.089,-0.087,-0.077,-0.066,-0.059,-0.052,-0.044,-0.039,-0.043,-0.038,-0.028,-0.028,-0.032,-0.032,-0.033,-0.035,-0.038,-0.042,-0.04,-0.035,-0.029,-0.031,-0.038,-0.035,-0.032,-0.037,-0.037,-0.034,-0.033,-0.033,-0.035,-0.029,-0.026,-0.029,-0.026,-0.023,-0.024,-0.021,-0.022,-0.018,-0.015,-0.016,-0.018,-0.024,-0.023,-0.021,-0.02,-0.011,-0.007,-0.007,-0.006,-0.002,0.002,0.001,0.002,0.006,0.004,0.001,0.007,0.013,0.017,0.018,0.022,0.022,0.02,0.023,0.022,0.021,0.031,0.034,0.033,0.037,0.04,0.045,0.044,0.042,0.049,0.055,0.06,0.066,0.068,0.071,0.073,0.074,0.083,0.087,0.085,0.093,0.093,0.098,0.114,0.115,0.117,0.125,0.126,0.128,0.133,0.142,0.145,0.145,0.153,0.161,0.161,0.161,0.17,0.173,0.176,0.181,0.183,0.19,0.194,0.195,0.2,0.203,0.205,0.204,0.206,0.206,0.201,0.204,0.209,0.21,0.214,0.212,0.2,0.2,0.205,0.206,0.209,0.204,0.198,0.193,0.178,0.17,0.167,0.162,0.157,0.147,0.139,0.131,0.111,0.1,0.093,0.081,0.077,0.071,0.062,0.061,0.05,0.039,0.032,0.018,0.012,0.007,-0.005,-0.007,-0.006,-0.013,-0.018,-0.02,-0.026,-0.028,-0.027,-0.034,-0.038,-0.039,-0.035,-0.033,-0.037,-0.042,-0.045,-0.045,-0.04,-0.043,-0.046,-0.037,-0.035,-0.039,-0.035,-0.037,-0.037,-0.035,-0.039 mV</t>
-  </si>
-  <si>
-    <t>0,0.002,0.004,0.006,0.008,0.01,0.012,0.014,0.016,0.018,0.02,0.022,0.024,0.026,0.028,0.03,0.032,0.034,0.036,0.038,0.04,0.043,0.045,0.047,0.049,0.051,0.053,0.055,0.057,0.059,0.061,0.063,0.065,0.067,0.069,0.071,0.073,0.075,0.077,0.079,0.081,0.083,0.085,0.087,0.089,0.091,0.093,0.095,0.097,0.099,0.101,0.103,0.105,0.107,0.109,0.111,0.113,0.115,0.117,0.119,0.121,0.123,0.125,0.127,0.129,0.131,0.133,0.135,0.137,0.139,0.141,0.143,0.145,0.147,0.149,0.151,0.153,0.155,0.157,0.159,0.161,0.163,0.165,0.168,0.17,0.172,0.174,0.176,0.178,0.18,0.182,0.184,0.186,0.188,0.19,0.192,0.194,0.196,0.198,0.2,0.202,0.204,0.206,0.208,0.21,0.212,0.214,0.216,0.218,0.22,0.222,0.224,0.226,0.228,0.23,0.232,0.234,0.236,0.238,0.24,0.242,0.244,0.246,0.248,0.25,0.252,0.254,0.256,0.258,0.26,0.262,0.264,0.266,0.268,0.27,0.272,0.274,0.276,0.278,0.28,0.282,0.284,0.286,0.288,0.29,0.293,0.295,0.297,0.299,0.301,0.303,0.305,0.307,0.309,0.311,0.313,0.315,0.317,0.319,0.321,0.323,0.325,0.327,0.329,0.331,0.333,0.335,0.337,0.339,0.341,0.343,0.345,0.347,0.349,0.351,0.353,0.355,0.357,0.359,0.361,0.363,0.365,0.367,0.369,0.371,0.373,0.375,0.377,0.379,0.381,0.383,0.385,0.387,0.389,0.391,0.393,0.395,0.397,0.399,0.401,0.403,0.405,0.407,0.409,0.411,0.413,0.415,0.418,0.42,0.422,0.424,0.426,0.428,0.43,0.432,0.434,0.436,0.438,0.44,0.442,0.444,0.446,0.448,0.45,0.452,0.454,0.456,0.458,0.46,0.462,0.464,0.466,0.468,0.47,0.472,0.474,0.476,0.478,0.48,0.482,0.484,0.486,0.488,0.49,0.492,0.494,0.496,0.498,0.5,0.502,0.504,0.506,0.508,0.51,0.512,0.514,0.516,0.518,0.52,0.522,0.524,0.526,0.528,0.53,0.532,0.534,0.536,0.538,0.54,0.543,0.545,0.547,0.549,0.551,0.553,0.555,0.557,0.559,0.561,0.563,0.565,0.567,0.569 s</t>
   </si>
   <si>
     <t>ECG consists of a Lead 3 Normal Sinus waveform retrieved from Physionet @cite goldberger2000physiobank.
@@ -2351,12 +2345,6 @@
   </si>
   <si>
     <t>0.146,0.179,0.195,0.163,0.138,0.098,0.147,0.196,0.236,0.285,0.326,0.285,0.253,0.196,0.155,0.115,0.074,0.058,0.05,0.123,0.172,0.229,0.278,0.319,0.343,0.376,0.327,0.278,0.246,0.213,0.181,0.149,0.149,0.141,0.141,0.166,0.214,0.263,0.312,0.345,0.361,0.361,0.362,0.345,0.329,0.321,0.297,0.248,0.216,0.184,0.216,0.249,0.29,0.33,0.379,0.412,0.445,0.445,0.421,0.396,0.372,0.323,0.283,0.242,0.185,0.145,0.104,0.056,0.04,0.04,0.072,0.121,0.154,0.195,0.252,0.3,0.366,0.415,0.463,0.496,0.512,0.488,0.472,0.448,0.44,0.399,0.343,0.294,0.245,0.205,0.164,0.123,0.091,0.075,0.091,0.116,0.14,0.214,0.271,0.32,0.352,0.393,0.393,0.377,0.353,0.328,0.28,0.239,0.199,0.142,0.085,0.061,0.093,0.158,0.215,0.272,0.321,0.37,0.394,0.338,0.289,0.232,0.167,0.118,0.159,0.192,0.24,0.306,0.354,0.387,0.42,0.355,0.29,0.233,0.168,0.095,0.054,0.03,-0.018,-0.034,-0.009,0.014,0.055,0.104,0.145,0.21,0.259,0.34,0.373,0.422,0.438,0.43,0.398,0.374,0.333,0.292,0.252,0.203,0.154,0.106,0.114,0.13,0.179,0.228,0.285,0.326,0.342,0.343,0.335,0.31,0.278,0.246,0.197,0.156,0.108,0.124,0.132,0.181,0.238,0.287,0.312,0.361,0.361,0.385,0.394,0.402,0.378,0.354,0.346,0.297,0.24,0.183,0.135,0.118,0.102,0.103,0.095,0.135,0.2,0.241,0.266,0.299,0.315,0.315,0.324,0.267,0.218,0.161,0.113,0.088,0.113,0.137,0.186,0.235,0.317,0.366,0.439,0.496,0.545,0.586,0.618,0.602,0.586,0.529,0.472,0.432,0.391,0.343,0.286,0.27,0.245,0.221,0.238,0.27,0.303,0.319,0.36,0.401,0.434,0.442,0.442,0.402,0.345,0.288,0.264,0.207,0.199,0.191,0.207,0.175,0.143,0.11,0.143,0.2,0.249,0.265,0.208,0.16,0.111,0.079,0.111,0.16,0.209,0.242,0.291,0.283,0.275,0.25,0.21,0.161,0.12,0.088,0.047,0.072,0.129,0.178,0.243,0.283,0.292,0.251,0.202,0.145,0.097,0.064 mV</t>
-  </si>
-  <si>
-    <t>0,0.015,0.024,0.034,0.046,0.062,0.08,0.077,0.08,0.095,0.113,0.123,0.132,0.13,0.136,0.149,0.161,0.18,0.202,0.208,0.211,0.216,0.222,0.222,0.231,0.247,0.259,0.263,0.272,0.285,0.294,0.31,0.329,0.347,0.363,0.381,0.39,0.406,0.418,0.433,0.452,0.476,0.501,0.52,0.542,0.557,0.576,0.589,0.605,0.62,0.636,0.651,0.657,0.669,0.687,0.697,0.712,0.734,0.749,0.759,0.774,0.79,0.8,0.813,0.825,0.838,0.851,0.863,0.885,0.901,0.919,0.931,0.95,0.956,0.968,0.983,0.998,1.013,1.029,1.041,1.059,1.081,1.097,1.116,1.134,1.15,1.163,1.169,1.179,1.185,1.195,1.202,1.217,1.233,1.251,1.27,1.291,1.297,1.309,1.328,1.334,1.346,1.361,1.383,1.405,1.421,1.427,1.437,1.443,1.447,1.453,1.475,1.491,1.503,1.508,1.511,1.517,1.526,1.538,1.542,1.542,1.546,1.552,1.562,1.577,1.586,1.592,1.607,1.616,1.628,1.65,1.653,1.663,1.676,1.676,1.683,1.69,1.708,1.733,1.749,1.771,1.795,1.814,1.826,1.844,1.856,1.859,1.862,1.883,1.898,1.923,1.948,1.967,1.983,1.986,1.995,2.005,2.005,2.015,2.025,2.043,2.062,2.071,2.08,2.089,2.107,2.135,2.16,2.178,2.197,2.216,2.232,2.245,2.251,2.261,2.279,2.298,2.316,2.328,2.346,2.371,2.383,2.408,2.427,2.458,2.482,2.501,2.523,2.545,2.558,2.564,2.574,2.58,2.599,2.621,2.646,2.658,2.67,2.685,2.695,2.719,2.75,2.775,2.797,2.821,2.831,2.841,2.85,2.863,2.876,2.9,2.916,2.925,2.946,2.964,2.992,3.001,3.022,3.041,3.059,3.071,3.09,3.109,3.121,3.131,3.141,3.156,3.166,3.173,3.191,3.201,3.22,3.241,3.266,3.284,3.309,3.334,3.352,3.373,3.398,3.417,3.423,3.439,3.446,3.462,3.468,3.493,3.515,3.539,3.558,3.577,3.596,3.608,3.614,3.62,3.645,3.648,3.658,3.677,3.689,3.702,3.711,3.723,3.735,3.756,3.781,3.797,3.813,3.816,3.819,3.82,3.829,3.851,3.863,3.869,3.869,3.872,3.887,3.899,3.909,3.912,3.919,3.925,3.932 s</t>
-  </si>
-  <si>
-    <t>0,0.02,0.04,0.06,0.08,0.1,0.12,0.14,0.16,0.18,0.20,0.22,0.24,0.26,0.28,0.3,0.32,0.34,0.36 s</t>
   </si>
   <si>
     <t>0.0,0.007,0.024,0.033,0.247,0.938,1.273,1.353,1.423,1.417,1.209,1.024,0.740,0.638,0.325,0.033,0.027,0.007,0.0 mV</t>
@@ -2990,7 +2978,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3415,9 +3403,6 @@
     <xf numFmtId="49" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3452,15 +3437,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3858,34 +3834,34 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="136"/>
-      <c r="B1" s="177" t="s">
+      <c r="B1" s="176" t="s">
         <v>591</v>
       </c>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="179"/>
-      <c r="F1" s="177" t="s">
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="176" t="s">
         <v>588</v>
       </c>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="179"/>
-      <c r="J1" s="177" t="s">
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="176" t="s">
         <v>589</v>
       </c>
-      <c r="K1" s="178"/>
-      <c r="L1" s="178"/>
-      <c r="M1" s="178"/>
-      <c r="N1" s="178"/>
-      <c r="O1" s="178"/>
-      <c r="P1" s="178"/>
-      <c r="Q1" s="178"/>
-      <c r="R1" s="178"/>
-      <c r="S1" s="179"/>
-      <c r="T1" s="177" t="s">
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
+      <c r="P1" s="177"/>
+      <c r="Q1" s="177"/>
+      <c r="R1" s="177"/>
+      <c r="S1" s="178"/>
+      <c r="T1" s="176" t="s">
         <v>590</v>
       </c>
-      <c r="U1" s="179"/>
+      <c r="U1" s="178"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="137" t="s">
@@ -4587,7 +4563,7 @@
         <v>289</v>
       </c>
       <c r="I16" s="153" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="J16" s="152" t="s">
         <v>71</v>
@@ -4620,7 +4596,7 @@
         <v>71</v>
       </c>
       <c r="T16" s="152" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="U16" s="153" t="s">
         <v>289</v>
@@ -4896,7 +4872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:FR75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="DB33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -5624,16 +5600,16 @@
         <v>15</v>
       </c>
       <c r="AP2" s="100" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="AQ2" s="100" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="AR2" s="100" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="AS2" s="100" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="AT2" s="100" t="s">
         <v>175</v>
@@ -5828,16 +5804,16 @@
         <v>51</v>
       </c>
       <c r="DF2" s="100" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="DG2" s="100" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="DH2" s="100" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="DI2" s="100" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="DJ2" s="100" t="s">
         <v>52</v>
@@ -5876,16 +5852,16 @@
         <v>45</v>
       </c>
       <c r="DV2" s="100" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="DW2" s="100" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="DX2" s="100" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="DY2" s="100" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="DZ2" s="100" t="s">
         <v>46</v>
@@ -5924,28 +5900,28 @@
         <v>48</v>
       </c>
       <c r="EL2" s="100" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="EM2" s="100" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="EN2" s="100" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="EO2" s="100" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="EP2" s="100" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="EQ2" s="100" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="ER2" s="100" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="ES2" s="100" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="ET2" s="100" t="s">
         <v>197</v>
@@ -6525,7 +6501,7 @@
       <c r="AQ4" s="106"/>
       <c r="AR4" s="106"/>
       <c r="AS4" s="106" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="AT4" s="92" t="s">
         <v>17</v>
@@ -7336,7 +7312,7 @@
       <c r="AN8" s="106"/>
       <c r="AO8" s="106"/>
       <c r="AP8" s="103" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="AQ8" s="106"/>
       <c r="AR8" s="106"/>
@@ -7436,13 +7412,13 @@
       <c r="DD8" s="111"/>
       <c r="DE8" s="111"/>
       <c r="DF8" s="111" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="DG8" s="111" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="DH8" s="111" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="DI8" s="111"/>
       <c r="DJ8" s="111" t="s">
@@ -7464,13 +7440,13 @@
       <c r="DT8" s="111"/>
       <c r="DU8" s="111"/>
       <c r="DV8" s="111" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="DW8" s="111">
         <v>321.15800000000002</v>
       </c>
       <c r="DX8" s="111" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="DY8" s="111"/>
       <c r="DZ8" s="111" t="s">
@@ -7492,17 +7468,17 @@
       <c r="EJ8" s="111"/>
       <c r="EK8" s="111"/>
       <c r="EL8" s="111" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="EM8" s="111"/>
       <c r="EN8" s="111"/>
       <c r="EO8" s="111"/>
       <c r="EP8" s="111" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="EQ8" s="111"/>
       <c r="ER8" s="111" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="ES8" s="111"/>
       <c r="ET8" s="111" t="s">
@@ -7542,7 +7518,7 @@
     </row>
     <row r="9" spans="1:173" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="62" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B9" s="106"/>
       <c r="C9" s="106"/>
@@ -9802,7 +9778,7 @@
       </c>
       <c r="AQ18" s="106"/>
       <c r="AR18" s="106" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="AS18" s="106"/>
       <c r="AT18" s="88">
@@ -9894,10 +9870,10 @@
         <v>0.215</v>
       </c>
       <c r="DH18" s="111" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="DI18" s="111" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="DJ18" s="111">
         <v>0.33600000000000002</v>
@@ -9921,10 +9897,10 @@
         <v>0.1</v>
       </c>
       <c r="DW18" s="111" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="DX18" s="111" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="DY18" s="111"/>
       <c r="DZ18" s="111">
@@ -10121,13 +10097,13 @@
       <c r="DD19" s="111"/>
       <c r="DE19" s="111"/>
       <c r="DF19" s="111" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="DG19" s="111" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="DH19" s="111" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="DI19" s="111"/>
       <c r="DJ19" s="111" t="s">
@@ -10153,7 +10129,7 @@
       </c>
       <c r="DW19" s="111"/>
       <c r="DX19" s="111" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="DY19" s="111"/>
       <c r="DZ19" s="111" t="s">
@@ -10175,19 +10151,19 @@
       <c r="EJ19" s="111"/>
       <c r="EK19" s="111"/>
       <c r="EL19" s="111" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="EM19" s="111"/>
       <c r="EN19" s="111"/>
       <c r="EO19" s="111"/>
       <c r="EP19" s="111" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="EQ19" s="111" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="ER19" s="111" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="ES19" s="111"/>
       <c r="ET19" s="111" t="s">
@@ -10378,7 +10354,7 @@
       <c r="DT20" s="111"/>
       <c r="DU20" s="111"/>
       <c r="DV20" s="111" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="DW20" s="111"/>
       <c r="DX20" s="111"/>
@@ -10408,7 +10384,7 @@
       <c r="EN20" s="111"/>
       <c r="EO20" s="111"/>
       <c r="EP20" s="111" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="EQ20" s="111"/>
       <c r="ER20" s="111"/>
@@ -10495,7 +10471,7 @@
       <c r="AN21" s="106"/>
       <c r="AO21" s="106"/>
       <c r="AP21" s="103" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="AQ21" s="106"/>
       <c r="AR21" s="106"/>
@@ -10543,7 +10519,7 @@
       <c r="BX21" s="92"/>
       <c r="BY21" s="92"/>
       <c r="BZ21" s="92" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="CA21" s="92"/>
       <c r="CB21" s="92"/>
@@ -10581,13 +10557,13 @@
       <c r="DD21" s="111"/>
       <c r="DE21" s="111"/>
       <c r="DF21" s="111" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="DG21" s="111" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="DH21" s="111" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="DI21" s="111"/>
       <c r="DJ21" s="111" t="s">
@@ -10609,11 +10585,11 @@
       <c r="DT21" s="111"/>
       <c r="DU21" s="111"/>
       <c r="DV21" s="111" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="DW21" s="111"/>
       <c r="DX21" s="111" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="DY21" s="111"/>
       <c r="DZ21" s="111" t="s">
@@ -10635,13 +10611,13 @@
       <c r="EJ21" s="111"/>
       <c r="EK21" s="111"/>
       <c r="EL21" s="111" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="EM21" s="111"/>
       <c r="EN21" s="111"/>
       <c r="EO21" s="111"/>
       <c r="EP21" s="111" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="EQ21" s="111"/>
       <c r="ER21" s="111"/>
@@ -13270,7 +13246,7 @@
         <v>9.41</v>
       </c>
       <c r="AR30" s="106" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="AS30" s="106"/>
       <c r="AT30" s="92"/>
@@ -13346,7 +13322,7 @@
         <v>4.2</v>
       </c>
       <c r="DH30" s="111" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="DI30" s="111"/>
       <c r="DJ30" s="111">
@@ -13370,7 +13346,7 @@
         <v>10.61</v>
       </c>
       <c r="DX30" s="111" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="DY30" s="111"/>
       <c r="DZ30" s="111">
@@ -13400,7 +13376,7 @@
       </c>
       <c r="EQ30" s="111"/>
       <c r="ER30" s="111" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="ES30" s="111"/>
       <c r="ET30" s="111">
@@ -13563,10 +13539,10 @@
         <v>114</v>
       </c>
       <c r="DH31" s="111" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="DI31" s="111" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="DJ31" s="111" t="s">
         <v>114</v>
@@ -13616,10 +13592,10 @@
         <v>114</v>
       </c>
       <c r="EQ31" s="111" t="s">
+        <v>734</v>
+      </c>
+      <c r="ER31" s="111" t="s">
         <v>736</v>
-      </c>
-      <c r="ER31" s="111" t="s">
-        <v>738</v>
       </c>
       <c r="ES31" s="111"/>
       <c r="ET31" s="111" t="s">
@@ -13802,7 +13778,7 @@
         <v>0.56699999999999995</v>
       </c>
       <c r="DX32" s="111" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="DY32" s="111"/>
       <c r="DZ32" s="111">
@@ -13833,7 +13809,7 @@
       <c r="EQ32" s="111"/>
       <c r="ER32" s="111"/>
       <c r="ES32" s="111" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="ET32" s="111">
         <v>1.5640000000000001</v>
@@ -14478,7 +14454,7 @@
         <v>-1.24</v>
       </c>
       <c r="AR35" s="106" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="AS35" s="106"/>
       <c r="AT35" s="92"/>
@@ -14554,7 +14530,7 @@
         <v>3.05</v>
       </c>
       <c r="DH35" s="111" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="DI35" s="111"/>
       <c r="DJ35" s="111">
@@ -14575,10 +14551,10 @@
       <c r="DU35" s="111"/>
       <c r="DV35" s="111"/>
       <c r="DW35" s="111" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="DX35" s="111" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="DY35" s="111"/>
       <c r="DZ35" s="111">
@@ -14608,7 +14584,7 @@
       </c>
       <c r="EQ35" s="111"/>
       <c r="ER35" s="111" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="ES35" s="111"/>
       <c r="ET35" s="111">
@@ -15216,7 +15192,7 @@
       </c>
       <c r="DG37" s="115"/>
       <c r="DH37" s="111" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="DI37" s="115"/>
       <c r="DJ37" s="115">
@@ -15433,7 +15409,7 @@
       </c>
       <c r="DG38" s="115"/>
       <c r="DH38" s="111" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="DI38" s="115"/>
       <c r="DJ38" s="115">
@@ -15572,7 +15548,7 @@
       <c r="AN39" s="114"/>
       <c r="AO39" s="114"/>
       <c r="AP39" s="114" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="AQ39" s="114"/>
       <c r="AR39" s="114"/>
@@ -15640,13 +15616,13 @@
       <c r="CZ39" s="115"/>
       <c r="DA39" s="115"/>
       <c r="DB39" s="115" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="DC39" s="115"/>
       <c r="DD39" s="115"/>
       <c r="DE39" s="115"/>
       <c r="DF39" s="115" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="DG39" s="115"/>
       <c r="DH39" s="115"/>
@@ -15670,13 +15646,13 @@
       <c r="DT39" s="115"/>
       <c r="DU39" s="115"/>
       <c r="DV39" s="115" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="DW39" s="115"/>
       <c r="DX39" s="115"/>
       <c r="DY39" s="115"/>
       <c r="DZ39" s="115" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="EA39" s="115"/>
       <c r="EB39" s="115"/>
@@ -15694,13 +15670,13 @@
       <c r="EJ39" s="115"/>
       <c r="EK39" s="115"/>
       <c r="EL39" s="115" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="EM39" s="115"/>
       <c r="EN39" s="115"/>
       <c r="EO39" s="115"/>
       <c r="EP39" s="115" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="EQ39" s="115"/>
       <c r="ER39" s="115"/>
@@ -16080,7 +16056,7 @@
       </c>
       <c r="DG41" s="115"/>
       <c r="DH41" s="111" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="DI41" s="115"/>
       <c r="DJ41" s="115">
@@ -16775,7 +16751,7 @@
       </c>
       <c r="DG44" s="115"/>
       <c r="DH44" s="115" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="DI44" s="115"/>
       <c r="DJ44" s="115">
@@ -17002,7 +16978,7 @@
       </c>
       <c r="DG45" s="115"/>
       <c r="DH45" s="111" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="DI45" s="115"/>
       <c r="DJ45" s="115">
@@ -17434,7 +17410,7 @@
       </c>
       <c r="DG47" s="115"/>
       <c r="DH47" s="111" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="DI47" s="115"/>
       <c r="DJ47" s="115">
@@ -26130,7 +26106,7 @@
       <c r="H2" s="73"/>
       <c r="I2" s="73"/>
       <c r="J2" s="73" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -26200,7 +26176,7 @@
       <c r="H5" s="75"/>
       <c r="I5" s="75"/>
       <c r="J5" s="75" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -26258,31 +26234,31 @@
         <v>54</v>
       </c>
       <c r="B8" s="75" t="s">
+        <v>684</v>
+      </c>
+      <c r="C8" s="75" t="s">
+        <v>690</v>
+      </c>
+      <c r="D8" s="75" t="s">
         <v>686</v>
       </c>
-      <c r="C8" s="75" t="s">
-        <v>692</v>
-      </c>
-      <c r="D8" s="75" t="s">
+      <c r="E8" s="175" t="s">
+        <v>687</v>
+      </c>
+      <c r="F8" s="75" t="s">
         <v>688</v>
       </c>
-      <c r="E8" s="176" t="s">
-        <v>689</v>
-      </c>
-      <c r="F8" s="75" t="s">
-        <v>690</v>
-      </c>
       <c r="G8" s="75" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="H8" s="75" t="s">
+        <v>686</v>
+      </c>
+      <c r="I8" s="175" t="s">
+        <v>687</v>
+      </c>
+      <c r="J8" s="75" t="s">
         <v>688</v>
-      </c>
-      <c r="I8" s="176" t="s">
-        <v>689</v>
-      </c>
-      <c r="J8" s="75" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -26340,31 +26316,31 @@
         <v>54</v>
       </c>
       <c r="B11" s="75" t="s">
+        <v>685</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>692</v>
+      </c>
+      <c r="D11" s="75" t="s">
+        <v>686</v>
+      </c>
+      <c r="E11" s="175" t="s">
         <v>687</v>
       </c>
-      <c r="C11" s="75" t="s">
-        <v>694</v>
-      </c>
-      <c r="D11" s="75" t="s">
-        <v>688</v>
-      </c>
-      <c r="E11" s="176" t="s">
+      <c r="F11" s="75" t="s">
         <v>689</v>
       </c>
-      <c r="F11" s="75" t="s">
-        <v>691</v>
-      </c>
       <c r="G11" s="75" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="H11" s="75" t="s">
-        <v>688</v>
-      </c>
-      <c r="I11" s="176" t="s">
+        <v>686</v>
+      </c>
+      <c r="I11" s="175" t="s">
+        <v>687</v>
+      </c>
+      <c r="J11" s="75" t="s">
         <v>689</v>
-      </c>
-      <c r="J11" s="75" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -26430,7 +26406,7 @@
       <c r="H14" s="75"/>
       <c r="I14" s="75"/>
       <c r="J14" s="75" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -28051,10 +28027,10 @@
         <v>191</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C5" s="72" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D5" s="46"/>
     </row>
@@ -28151,10 +28127,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28167,29 +28143,29 @@
   <sheetData>
     <row r="1" spans="1:15" s="38" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="38" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="42" customFormat="1" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="175" t="s">
-        <v>681</v>
-      </c>
-      <c r="B2" s="174" t="s">
-        <v>680</v>
-      </c>
-      <c r="C2" s="171"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="172"/>
-      <c r="F2" s="172"/>
-      <c r="G2" s="172"/>
-      <c r="H2" s="172"/>
-      <c r="I2" s="172"/>
-      <c r="J2" s="172"/>
-      <c r="K2" s="172"/>
-      <c r="L2" s="172"/>
-      <c r="M2" s="172"/>
-      <c r="N2" s="172"/>
-      <c r="O2" s="173"/>
+      <c r="A2" s="174" t="s">
+        <v>679</v>
+      </c>
+      <c r="B2" s="173" t="s">
+        <v>678</v>
+      </c>
+      <c r="C2" s="170"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="171"/>
+      <c r="H2" s="171"/>
+      <c r="I2" s="171"/>
+      <c r="J2" s="171"/>
+      <c r="K2" s="171"/>
+      <c r="L2" s="171"/>
+      <c r="M2" s="171"/>
+      <c r="N2" s="171"/>
+      <c r="O2" s="172"/>
     </row>
     <row r="3" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="42" t="s">
@@ -28198,134 +28174,97 @@
       <c r="B3" s="49">
         <v>3</v>
       </c>
-      <c r="C3" s="186"/>
-      <c r="D3" s="187"/>
-      <c r="E3" s="187"/>
-      <c r="F3" s="187"/>
-      <c r="G3" s="187"/>
-      <c r="H3" s="187"/>
-      <c r="I3" s="187"/>
-      <c r="J3" s="187"/>
-      <c r="K3" s="187"/>
-      <c r="L3" s="187"/>
-      <c r="M3" s="187"/>
-      <c r="N3" s="187"/>
-      <c r="O3" s="188"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="183"/>
+      <c r="J3" s="183"/>
+      <c r="K3" s="183"/>
+      <c r="L3" s="183"/>
+      <c r="M3" s="183"/>
+      <c r="N3" s="183"/>
+      <c r="O3" s="184"/>
     </row>
     <row r="4" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="42" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>762</v>
-      </c>
-      <c r="C4" s="189"/>
-      <c r="D4" s="190"/>
-      <c r="E4" s="190"/>
-      <c r="F4" s="190"/>
-      <c r="G4" s="190"/>
-      <c r="H4" s="190"/>
-      <c r="I4" s="190"/>
-      <c r="J4" s="190"/>
-      <c r="K4" s="190"/>
-      <c r="L4" s="190"/>
-      <c r="M4" s="190"/>
-      <c r="N4" s="190"/>
-      <c r="O4" s="191"/>
+        <v>760</v>
+      </c>
+      <c r="C4" s="185"/>
+      <c r="D4" s="186"/>
+      <c r="E4" s="186"/>
+      <c r="F4" s="186"/>
+      <c r="G4" s="186"/>
+      <c r="H4" s="186"/>
+      <c r="I4" s="186"/>
+      <c r="J4" s="186"/>
+      <c r="K4" s="186"/>
+      <c r="L4" s="186"/>
+      <c r="M4" s="186"/>
+      <c r="N4" s="186"/>
+      <c r="O4" s="187"/>
     </row>
     <row r="5" spans="1:15" s="36" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="168" t="s">
         <v>676</v>
       </c>
       <c r="B5" s="169" t="s">
-        <v>678</v>
-      </c>
-      <c r="C5" s="180"/>
-      <c r="D5" s="181"/>
-      <c r="E5" s="181"/>
-      <c r="F5" s="181"/>
-      <c r="G5" s="181"/>
-      <c r="H5" s="181"/>
-      <c r="I5" s="181"/>
-      <c r="J5" s="181"/>
-      <c r="K5" s="181"/>
-      <c r="L5" s="181"/>
-      <c r="M5" s="181"/>
-      <c r="N5" s="181"/>
-      <c r="O5" s="182"/>
-    </row>
-    <row r="6" spans="1:15" s="168" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A6" s="168" t="s">
         <v>677</v>
       </c>
-      <c r="B6" s="170" t="s">
-        <v>679</v>
-      </c>
-      <c r="C6" s="183"/>
-      <c r="D6" s="184"/>
-      <c r="E6" s="184"/>
-      <c r="F6" s="184"/>
-      <c r="G6" s="184"/>
-      <c r="H6" s="184"/>
-      <c r="I6" s="184"/>
-      <c r="J6" s="184"/>
-      <c r="K6" s="184"/>
-      <c r="L6" s="184"/>
-      <c r="M6" s="184"/>
-      <c r="N6" s="184"/>
-      <c r="O6" s="185"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="42" t="s">
+      <c r="C5" s="179"/>
+      <c r="D5" s="180"/>
+      <c r="E5" s="180"/>
+      <c r="F5" s="180"/>
+      <c r="G5" s="180"/>
+      <c r="H5" s="180"/>
+      <c r="I5" s="180"/>
+      <c r="J5" s="180"/>
+      <c r="K5" s="180"/>
+      <c r="L5" s="180"/>
+      <c r="M5" s="180"/>
+      <c r="N5" s="180"/>
+      <c r="O5" s="181"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="42" t="s">
+        <v>763</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="168" t="s">
+        <v>676</v>
+      </c>
+      <c r="B7" s="169" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="42" t="s">
+        <v>763</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="168" t="s">
+        <v>676</v>
+      </c>
+      <c r="B9" s="169" t="s">
         <v>765</v>
-      </c>
-      <c r="B7" s="49" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="168" t="s">
-        <v>676</v>
-      </c>
-      <c r="B8" s="169" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="168" t="s">
-        <v>677</v>
-      </c>
-      <c r="B9" s="170" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="42" t="s">
-        <v>765</v>
-      </c>
-      <c r="B10" s="49" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="168" t="s">
-        <v>676</v>
-      </c>
-      <c r="B11" s="169" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="168" t="s">
-        <v>677</v>
-      </c>
-      <c r="B12" s="170" t="s">
-        <v>768</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C5:O6"/>
+    <mergeCell ref="C5:O5"/>
     <mergeCell ref="C3:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28362,7 +28301,7 @@
         <v>143</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E1" s="39" t="s">
         <v>146</v>
@@ -28382,7 +28321,7 @@
         <v>149</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E2" s="42"/>
       <c r="F2" s="42"/>
@@ -28398,7 +28337,7 @@
         <v>150</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
@@ -28414,7 +28353,7 @@
         <v>151</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E4" s="43"/>
       <c r="F4" s="43"/>
@@ -28430,7 +28369,7 @@
         <v>152</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E5" s="43"/>
       <c r="F5" s="43"/>
@@ -28446,7 +28385,7 @@
         <v>153</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
@@ -28462,7 +28401,7 @@
         <v>154</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E7" s="43"/>
       <c r="F7" s="43"/>
@@ -28478,7 +28417,7 @@
         <v>270</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
@@ -28494,7 +28433,7 @@
         <v>271</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E9" s="43"/>
       <c r="F9" s="43"/>
@@ -28558,7 +28497,7 @@
         <v>143</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E14" s="39" t="s">
         <v>146</v>
@@ -28578,7 +28517,7 @@
         <v>149</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E15" s="42"/>
       <c r="F15" s="42"/>
@@ -28594,7 +28533,7 @@
         <v>150</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E16" s="43"/>
       <c r="F16" s="43"/>
@@ -28610,7 +28549,7 @@
         <v>151</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E17" s="43"/>
       <c r="F17" s="43"/>
@@ -28626,7 +28565,7 @@
         <v>152</v>
       </c>
       <c r="D18" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E18" s="43"/>
       <c r="F18" s="43"/>
@@ -28642,7 +28581,7 @@
         <v>153</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E19" s="43"/>
       <c r="F19" s="43"/>
@@ -28658,7 +28597,7 @@
         <v>154</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E20" s="43"/>
       <c r="F20" s="43"/>
@@ -28674,7 +28613,7 @@
         <v>594</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E21" s="43"/>
       <c r="F21" s="43"/>
@@ -28690,7 +28629,7 @@
         <v>595</v>
       </c>
       <c r="D22" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E22" s="43"/>
       <c r="F22" s="43"/>
@@ -28706,7 +28645,7 @@
         <v>270</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E23" s="43"/>
       <c r="F23" s="43"/>
@@ -28722,7 +28661,7 @@
         <v>271</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E24" s="43"/>
       <c r="F24" s="43"/>
@@ -28777,7 +28716,7 @@
     </row>
     <row r="29" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="34" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B29" s="35" t="s">
         <v>145</v>
@@ -28786,7 +28725,7 @@
         <v>143</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E29" s="35" t="s">
         <v>146</v>
@@ -28806,7 +28745,7 @@
         <v>149</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E30" s="42"/>
       <c r="F30" s="42"/>
@@ -28822,7 +28761,7 @@
         <v>150</v>
       </c>
       <c r="D31" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E31" s="43"/>
       <c r="F31" s="43"/>
@@ -28838,7 +28777,7 @@
         <v>151</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E32" s="43"/>
       <c r="F32" s="43"/>
@@ -28854,7 +28793,7 @@
         <v>152</v>
       </c>
       <c r="D33" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E33" s="43"/>
       <c r="F33" s="43"/>
@@ -28870,7 +28809,7 @@
         <v>153</v>
       </c>
       <c r="D34" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E34" s="43"/>
       <c r="F34" s="43"/>
@@ -28886,7 +28825,7 @@
         <v>154</v>
       </c>
       <c r="D35" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E35" s="43"/>
       <c r="F35" s="43"/>
@@ -28902,7 +28841,7 @@
         <v>594</v>
       </c>
       <c r="D36" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E36" s="43"/>
       <c r="F36" s="43"/>
@@ -28918,7 +28857,7 @@
         <v>595</v>
       </c>
       <c r="D37" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E37" s="43"/>
       <c r="F37" s="43"/>
@@ -28934,7 +28873,7 @@
         <v>270</v>
       </c>
       <c r="D38" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E38" s="43"/>
       <c r="F38" s="43"/>
@@ -28950,7 +28889,7 @@
         <v>271</v>
       </c>
       <c r="D39" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E39" s="43"/>
       <c r="F39" s="43"/>
@@ -29014,7 +28953,7 @@
         <v>143</v>
       </c>
       <c r="D44" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E44" s="35" t="s">
         <v>146</v>
@@ -29034,7 +28973,7 @@
         <v>149</v>
       </c>
       <c r="D45" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E45" s="42"/>
       <c r="F45" s="42"/>
@@ -29050,7 +28989,7 @@
         <v>150</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E46" s="43"/>
       <c r="F46" s="43"/>
@@ -29066,7 +29005,7 @@
         <v>151</v>
       </c>
       <c r="D47" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E47" s="43"/>
       <c r="F47" s="43"/>
@@ -29082,7 +29021,7 @@
         <v>152</v>
       </c>
       <c r="D48" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E48" s="43"/>
       <c r="F48" s="43"/>
@@ -29098,7 +29037,7 @@
         <v>153</v>
       </c>
       <c r="D49" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E49" s="43"/>
       <c r="F49" s="43"/>
@@ -29114,7 +29053,7 @@
         <v>154</v>
       </c>
       <c r="D50" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E50" s="43"/>
       <c r="F50" s="43"/>
@@ -29130,7 +29069,7 @@
         <v>594</v>
       </c>
       <c r="D51" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E51" s="43"/>
       <c r="F51" s="43"/>
@@ -29146,7 +29085,7 @@
         <v>595</v>
       </c>
       <c r="D52" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E52" s="43"/>
       <c r="F52" s="43"/>
@@ -29162,7 +29101,7 @@
         <v>270</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E53" s="43"/>
       <c r="F53" s="43"/>
@@ -29178,7 +29117,7 @@
         <v>271</v>
       </c>
       <c r="D54" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E54" s="43"/>
       <c r="F54" s="43"/>
@@ -29242,7 +29181,7 @@
         <v>143</v>
       </c>
       <c r="D59" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E59" s="39" t="s">
         <v>146</v>
@@ -29262,7 +29201,7 @@
         <v>149</v>
       </c>
       <c r="D60" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E60" s="42"/>
       <c r="F60" s="42"/>
@@ -29278,7 +29217,7 @@
         <v>150</v>
       </c>
       <c r="D61" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E61" s="42"/>
       <c r="F61" s="42"/>
@@ -29294,7 +29233,7 @@
         <v>151</v>
       </c>
       <c r="D62" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E62" s="42"/>
       <c r="F62" s="42"/>
@@ -29310,7 +29249,7 @@
         <v>152</v>
       </c>
       <c r="D63" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E63" s="43"/>
       <c r="F63" s="43"/>
@@ -29326,7 +29265,7 @@
         <v>153</v>
       </c>
       <c r="D64" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E64" s="43"/>
       <c r="F64" s="43"/>
@@ -29342,7 +29281,7 @@
         <v>154</v>
       </c>
       <c r="D65" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E65" s="43"/>
       <c r="F65" s="43"/>
@@ -29358,7 +29297,7 @@
         <v>594</v>
       </c>
       <c r="D66" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E66" s="43"/>
       <c r="F66" s="43"/>
@@ -29374,7 +29313,7 @@
         <v>595</v>
       </c>
       <c r="D67" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E67" s="43"/>
       <c r="F67" s="43"/>
@@ -29390,7 +29329,7 @@
         <v>270</v>
       </c>
       <c r="D68" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E68" s="43"/>
       <c r="F68" s="43"/>
@@ -29406,7 +29345,7 @@
         <v>271</v>
       </c>
       <c r="D69" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E69" s="43"/>
       <c r="F69" s="43"/>
@@ -29470,7 +29409,7 @@
         <v>143</v>
       </c>
       <c r="D74" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E74" s="35" t="s">
         <v>146</v>
@@ -29490,7 +29429,7 @@
         <v>149</v>
       </c>
       <c r="D75" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E75" s="42"/>
       <c r="F75" s="42"/>
@@ -29506,7 +29445,7 @@
         <v>150</v>
       </c>
       <c r="D76" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E76" s="43"/>
       <c r="F76" s="43"/>
@@ -29522,7 +29461,7 @@
         <v>151</v>
       </c>
       <c r="D77" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E77" s="43"/>
       <c r="F77" s="43"/>
@@ -29538,7 +29477,7 @@
         <v>152</v>
       </c>
       <c r="D78" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E78" s="43"/>
       <c r="F78" s="43"/>
@@ -29554,7 +29493,7 @@
         <v>153</v>
       </c>
       <c r="D79" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E79" s="43"/>
       <c r="F79" s="43"/>
@@ -29570,7 +29509,7 @@
         <v>154</v>
       </c>
       <c r="D80" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E80" s="43"/>
       <c r="F80" s="43"/>
@@ -29586,7 +29525,7 @@
         <v>594</v>
       </c>
       <c r="D81" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E81" s="43"/>
       <c r="F81" s="43"/>
@@ -29602,7 +29541,7 @@
         <v>595</v>
       </c>
       <c r="D82" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E82" s="43"/>
       <c r="F82" s="43"/>
@@ -29618,7 +29557,7 @@
         <v>270</v>
       </c>
       <c r="D83" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E83" s="43"/>
       <c r="F83" s="43"/>
@@ -29634,7 +29573,7 @@
         <v>271</v>
       </c>
       <c r="D84" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E84" s="43"/>
       <c r="F84" s="43"/>
@@ -29698,7 +29637,7 @@
         <v>143</v>
       </c>
       <c r="D89" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E89" s="35" t="s">
         <v>146</v>
@@ -29718,7 +29657,7 @@
         <v>149</v>
       </c>
       <c r="D90" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E90" s="42"/>
       <c r="F90" s="42"/>
@@ -29734,7 +29673,7 @@
         <v>150</v>
       </c>
       <c r="D91" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E91" s="43"/>
       <c r="F91" s="43"/>
@@ -29750,7 +29689,7 @@
         <v>151</v>
       </c>
       <c r="D92" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E92" s="43"/>
       <c r="F92" s="43"/>
@@ -29766,7 +29705,7 @@
         <v>152</v>
       </c>
       <c r="D93" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E93" s="43"/>
       <c r="F93" s="43"/>
@@ -29782,7 +29721,7 @@
         <v>153</v>
       </c>
       <c r="D94" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E94" s="43"/>
       <c r="F94" s="43"/>
@@ -29798,7 +29737,7 @@
         <v>154</v>
       </c>
       <c r="D95" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E95" s="43"/>
       <c r="F95" s="43"/>
@@ -29814,7 +29753,7 @@
         <v>594</v>
       </c>
       <c r="D96" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E96" s="43"/>
       <c r="F96" s="43"/>
@@ -29830,7 +29769,7 @@
         <v>595</v>
       </c>
       <c r="D97" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E97" s="43"/>
       <c r="F97" s="43"/>
@@ -29846,7 +29785,7 @@
         <v>270</v>
       </c>
       <c r="D98" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E98" s="43"/>
       <c r="F98" s="43"/>
@@ -29862,7 +29801,7 @@
         <v>271</v>
       </c>
       <c r="D99" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E99" s="43"/>
       <c r="F99" s="43"/>
@@ -29878,10 +29817,10 @@
         <v>54</v>
       </c>
       <c r="D100" s="43" t="s">
+        <v>705</v>
+      </c>
+      <c r="E100" s="43" t="s">
         <v>707</v>
-      </c>
-      <c r="E100" s="43" t="s">
-        <v>709</v>
       </c>
       <c r="F100" s="43" t="s">
         <v>133</v>
@@ -29898,10 +29837,10 @@
         <v>54</v>
       </c>
       <c r="D101" s="43" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="E101" s="43" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F101" s="43" t="s">
         <v>133</v>
@@ -29966,7 +29905,7 @@
         <v>143</v>
       </c>
       <c r="D106" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E106" s="35" t="s">
         <v>146</v>
@@ -29986,7 +29925,7 @@
         <v>149</v>
       </c>
       <c r="D107" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E107" s="42"/>
       <c r="F107" s="42"/>
@@ -30002,7 +29941,7 @@
         <v>150</v>
       </c>
       <c r="D108" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E108" s="43"/>
       <c r="F108" s="43"/>
@@ -30018,7 +29957,7 @@
         <v>151</v>
       </c>
       <c r="D109" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E109" s="43"/>
       <c r="F109" s="43"/>
@@ -30034,7 +29973,7 @@
         <v>152</v>
       </c>
       <c r="D110" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E110" s="43"/>
       <c r="F110" s="43"/>
@@ -30050,7 +29989,7 @@
         <v>153</v>
       </c>
       <c r="D111" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E111" s="43"/>
       <c r="F111" s="43"/>
@@ -30066,7 +30005,7 @@
         <v>154</v>
       </c>
       <c r="D112" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E112" s="43"/>
       <c r="F112" s="43"/>
@@ -30082,7 +30021,7 @@
         <v>594</v>
       </c>
       <c r="D113" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E113" s="43"/>
       <c r="F113" s="43"/>
@@ -30098,7 +30037,7 @@
         <v>595</v>
       </c>
       <c r="D114" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E114" s="43"/>
       <c r="F114" s="43"/>
@@ -30114,7 +30053,7 @@
         <v>270</v>
       </c>
       <c r="D115" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E115" s="43"/>
       <c r="F115" s="43"/>
@@ -30130,7 +30069,7 @@
         <v>271</v>
       </c>
       <c r="D116" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E116" s="43"/>
       <c r="F116" s="43"/>
@@ -30194,7 +30133,7 @@
         <v>143</v>
       </c>
       <c r="D121" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E121" s="39" t="s">
         <v>146</v>
@@ -30214,7 +30153,7 @@
         <v>149</v>
       </c>
       <c r="D122" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E122" s="42"/>
       <c r="F122" s="42"/>
@@ -30230,7 +30169,7 @@
         <v>150</v>
       </c>
       <c r="D123" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E123" s="43"/>
       <c r="F123" s="43"/>
@@ -30246,7 +30185,7 @@
         <v>151</v>
       </c>
       <c r="D124" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E124" s="43"/>
       <c r="F124" s="43"/>
@@ -30262,7 +30201,7 @@
         <v>152</v>
       </c>
       <c r="D125" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E125" s="43"/>
       <c r="F125" s="43"/>
@@ -30278,7 +30217,7 @@
         <v>153</v>
       </c>
       <c r="D126" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E126" s="43"/>
       <c r="F126" s="43"/>
@@ -30294,7 +30233,7 @@
         <v>154</v>
       </c>
       <c r="D127" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E127" s="43"/>
       <c r="F127" s="43"/>
@@ -30310,7 +30249,7 @@
         <v>594</v>
       </c>
       <c r="D128" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E128" s="43"/>
       <c r="F128" s="43"/>
@@ -30326,7 +30265,7 @@
         <v>595</v>
       </c>
       <c r="D129" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E129" s="43"/>
       <c r="F129" s="43"/>
@@ -30342,7 +30281,7 @@
         <v>270</v>
       </c>
       <c r="D130" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E130" s="43"/>
       <c r="F130" s="43"/>
@@ -30358,7 +30297,7 @@
         <v>271</v>
       </c>
       <c r="D131" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E131" s="43"/>
       <c r="F131" s="43"/>
@@ -30413,7 +30352,7 @@
     </row>
     <row r="136" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A136" s="38" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B136" s="39" t="s">
         <v>145</v>
@@ -30442,7 +30381,7 @@
         <v>149</v>
       </c>
       <c r="D137" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E137" s="42"/>
       <c r="F137" s="42"/>
@@ -30458,7 +30397,7 @@
         <v>150</v>
       </c>
       <c r="D138" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E138" s="43"/>
       <c r="F138" s="43"/>
@@ -30474,7 +30413,7 @@
         <v>151</v>
       </c>
       <c r="D139" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E139" s="43"/>
       <c r="F139" s="43"/>
@@ -30490,7 +30429,7 @@
         <v>152</v>
       </c>
       <c r="D140" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E140" s="43"/>
       <c r="F140" s="43"/>
@@ -30506,7 +30445,7 @@
         <v>153</v>
       </c>
       <c r="D141" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E141" s="43"/>
       <c r="F141" s="43"/>
@@ -30522,7 +30461,7 @@
         <v>154</v>
       </c>
       <c r="D142" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E142" s="43"/>
       <c r="F142" s="43"/>
@@ -30538,7 +30477,7 @@
         <v>594</v>
       </c>
       <c r="D143" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E143" s="43"/>
       <c r="F143" s="43"/>
@@ -30554,7 +30493,7 @@
         <v>595</v>
       </c>
       <c r="D144" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E144" s="43"/>
       <c r="F144" s="43"/>
@@ -30570,7 +30509,7 @@
         <v>270</v>
       </c>
       <c r="D145" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E145" s="43"/>
       <c r="F145" s="43"/>
@@ -30586,7 +30525,7 @@
         <v>271</v>
       </c>
       <c r="D146" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E146" s="43"/>
       <c r="F146" s="43"/>
@@ -30650,7 +30589,7 @@
         <v>143</v>
       </c>
       <c r="D151" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E151" s="39" t="s">
         <v>146</v>
@@ -30670,7 +30609,7 @@
         <v>149</v>
       </c>
       <c r="D152" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E152" s="42"/>
       <c r="F152" s="42"/>
@@ -30686,7 +30625,7 @@
         <v>150</v>
       </c>
       <c r="D153" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E153" s="42"/>
       <c r="F153" s="42"/>
@@ -30702,7 +30641,7 @@
         <v>151</v>
       </c>
       <c r="D154" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E154" s="42"/>
       <c r="F154" s="42"/>
@@ -30718,7 +30657,7 @@
         <v>152</v>
       </c>
       <c r="D155" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E155" s="42"/>
       <c r="F155" s="42"/>
@@ -30734,7 +30673,7 @@
         <v>153</v>
       </c>
       <c r="D156" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E156" s="43"/>
       <c r="F156" s="43"/>
@@ -30750,7 +30689,7 @@
         <v>154</v>
       </c>
       <c r="D157" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E157" s="43"/>
       <c r="F157" s="43"/>
@@ -30766,7 +30705,7 @@
         <v>594</v>
       </c>
       <c r="D158" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E158" s="43"/>
       <c r="F158" s="43"/>
@@ -30782,7 +30721,7 @@
         <v>595</v>
       </c>
       <c r="D159" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E159" s="43"/>
       <c r="F159" s="43"/>
@@ -30798,7 +30737,7 @@
         <v>270</v>
       </c>
       <c r="D160" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E160" s="43"/>
       <c r="F160" s="43"/>
@@ -30814,7 +30753,7 @@
         <v>271</v>
       </c>
       <c r="D161" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E161" s="43"/>
       <c r="F161" s="43"/>
@@ -30878,7 +30817,7 @@
         <v>143</v>
       </c>
       <c r="D166" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E166" s="39" t="s">
         <v>146</v>
@@ -30898,7 +30837,7 @@
         <v>149</v>
       </c>
       <c r="D167" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E167" s="42"/>
       <c r="F167" s="42"/>
@@ -30914,7 +30853,7 @@
         <v>150</v>
       </c>
       <c r="D168" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E168" s="42"/>
       <c r="F168" s="42"/>
@@ -30930,7 +30869,7 @@
         <v>151</v>
       </c>
       <c r="D169" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E169" s="42"/>
       <c r="F169" s="42"/>
@@ -30946,7 +30885,7 @@
         <v>152</v>
       </c>
       <c r="D170" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E170" s="42"/>
       <c r="F170" s="42"/>
@@ -30962,7 +30901,7 @@
         <v>153</v>
       </c>
       <c r="D171" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E171" s="43"/>
       <c r="F171" s="43"/>
@@ -30978,7 +30917,7 @@
         <v>154</v>
       </c>
       <c r="D172" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E172" s="43"/>
       <c r="F172" s="43"/>
@@ -30994,7 +30933,7 @@
         <v>594</v>
       </c>
       <c r="D173" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E173" s="43"/>
       <c r="F173" s="43"/>
@@ -31010,7 +30949,7 @@
         <v>595</v>
       </c>
       <c r="D174" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E174" s="43"/>
       <c r="F174" s="43"/>
@@ -31026,7 +30965,7 @@
         <v>270</v>
       </c>
       <c r="D175" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E175" s="43"/>
       <c r="F175" s="43"/>
@@ -31042,7 +30981,7 @@
         <v>271</v>
       </c>
       <c r="D176" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E176" s="43"/>
       <c r="F176" s="43"/>
@@ -31097,7 +31036,7 @@
     </row>
     <row r="181" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A181" s="38" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B181" s="39" t="s">
         <v>145</v>
@@ -31106,7 +31045,7 @@
         <v>143</v>
       </c>
       <c r="D181" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E181" s="39" t="s">
         <v>146</v>
@@ -31126,7 +31065,7 @@
         <v>149</v>
       </c>
       <c r="D182" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E182" s="42"/>
       <c r="F182" s="42"/>
@@ -31142,7 +31081,7 @@
         <v>150</v>
       </c>
       <c r="D183" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E183" s="42"/>
       <c r="F183" s="42"/>
@@ -31158,7 +31097,7 @@
         <v>151</v>
       </c>
       <c r="D184" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E184" s="42"/>
       <c r="F184" s="42"/>
@@ -31174,7 +31113,7 @@
         <v>152</v>
       </c>
       <c r="D185" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E185" s="42"/>
       <c r="F185" s="42"/>
@@ -31190,7 +31129,7 @@
         <v>153</v>
       </c>
       <c r="D186" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E186" s="43"/>
       <c r="F186" s="43"/>
@@ -31206,7 +31145,7 @@
         <v>154</v>
       </c>
       <c r="D187" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E187" s="43"/>
       <c r="F187" s="43"/>
@@ -31222,7 +31161,7 @@
         <v>594</v>
       </c>
       <c r="D188" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E188" s="43"/>
       <c r="F188" s="43"/>
@@ -31238,7 +31177,7 @@
         <v>595</v>
       </c>
       <c r="D189" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E189" s="43"/>
       <c r="F189" s="43"/>
@@ -31254,7 +31193,7 @@
         <v>270</v>
       </c>
       <c r="D190" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E190" s="43"/>
       <c r="F190" s="43"/>
@@ -31270,7 +31209,7 @@
         <v>271</v>
       </c>
       <c r="D191" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E191" s="43"/>
       <c r="F191" s="43"/>
@@ -31325,7 +31264,7 @@
     </row>
     <row r="196" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A196" s="38" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B196" s="39" t="s">
         <v>145</v>
@@ -31334,7 +31273,7 @@
         <v>143</v>
       </c>
       <c r="D196" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E196" s="39" t="s">
         <v>146</v>
@@ -31354,7 +31293,7 @@
         <v>149</v>
       </c>
       <c r="D197" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E197" s="42"/>
       <c r="F197" s="42"/>
@@ -31370,7 +31309,7 @@
         <v>150</v>
       </c>
       <c r="D198" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E198" s="42"/>
       <c r="F198" s="42"/>
@@ -31386,7 +31325,7 @@
         <v>151</v>
       </c>
       <c r="D199" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E199" s="42"/>
       <c r="F199" s="42"/>
@@ -31402,7 +31341,7 @@
         <v>152</v>
       </c>
       <c r="D200" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E200" s="42"/>
       <c r="F200" s="42"/>
@@ -31418,7 +31357,7 @@
         <v>153</v>
       </c>
       <c r="D201" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E201" s="43"/>
       <c r="F201" s="43"/>
@@ -31434,7 +31373,7 @@
         <v>154</v>
       </c>
       <c r="D202" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E202" s="43"/>
       <c r="F202" s="43"/>
@@ -31450,7 +31389,7 @@
         <v>594</v>
       </c>
       <c r="D203" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E203" s="43"/>
       <c r="F203" s="43"/>
@@ -31466,7 +31405,7 @@
         <v>595</v>
       </c>
       <c r="D204" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E204" s="43"/>
       <c r="F204" s="43"/>
@@ -31482,7 +31421,7 @@
         <v>270</v>
       </c>
       <c r="D205" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E205" s="43"/>
       <c r="F205" s="43"/>
@@ -31498,7 +31437,7 @@
         <v>271</v>
       </c>
       <c r="D206" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E206" s="43"/>
       <c r="F206" s="43"/>
@@ -31553,7 +31492,7 @@
     </row>
     <row r="211" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A211" s="38" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B211" s="39" t="s">
         <v>145</v>
@@ -31562,7 +31501,7 @@
         <v>143</v>
       </c>
       <c r="D211" s="39" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E211" s="39" t="s">
         <v>146</v>
@@ -31582,7 +31521,7 @@
         <v>149</v>
       </c>
       <c r="D212" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E212" s="42"/>
       <c r="F212" s="42"/>
@@ -31598,7 +31537,7 @@
         <v>150</v>
       </c>
       <c r="D213" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E213" s="42"/>
       <c r="F213" s="42"/>
@@ -31614,7 +31553,7 @@
         <v>151</v>
       </c>
       <c r="D214" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E214" s="42"/>
       <c r="F214" s="42"/>
@@ -31630,7 +31569,7 @@
         <v>152</v>
       </c>
       <c r="D215" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E215" s="42"/>
       <c r="F215" s="42"/>
@@ -31646,7 +31585,7 @@
         <v>153</v>
       </c>
       <c r="D216" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E216" s="43"/>
       <c r="F216" s="43"/>
@@ -31662,7 +31601,7 @@
         <v>154</v>
       </c>
       <c r="D217" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E217" s="43"/>
       <c r="F217" s="43"/>
@@ -31678,7 +31617,7 @@
         <v>594</v>
       </c>
       <c r="D218" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E218" s="43"/>
       <c r="F218" s="43"/>
@@ -31694,7 +31633,7 @@
         <v>595</v>
       </c>
       <c r="D219" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E219" s="43"/>
       <c r="F219" s="43"/>
@@ -31710,7 +31649,7 @@
         <v>270</v>
       </c>
       <c r="D220" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E220" s="43"/>
       <c r="F220" s="43"/>
@@ -31726,7 +31665,7 @@
         <v>271</v>
       </c>
       <c r="D221" s="42" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E221" s="43"/>
       <c r="F221" s="43"/>

</xml_diff>

<commit_message>
Added new vtach waveform Refactored CV a bit   - Calculate HR in BeginCardiacCycle now   - The HR is now associated with the current cycle (Rather than the previous as with all vitals in Record)   - ECG can now generate a waveform with a length using that current cycle HR This alleviated a mismatch where the current cycle and the last cycle were off by a few time steps, so the waveform went to 0 or cut off early ECG waveforms are looking good
TODO - test out vfib, and incorporate the waveform amplitude modifier
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13B1D61-A776-4F29-888F-14D0AC820EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA107A8-2613-41CD-B213-8EAE1DF042D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="2240" windowWidth="29870" windowHeight="10590" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2347,7 +2347,7 @@
     <t>0.146,0.179,0.195,0.163,0.138,0.098,0.147,0.196,0.236,0.285,0.326,0.285,0.253,0.196,0.155,0.115,0.074,0.058,0.05,0.123,0.172,0.229,0.278,0.319,0.343,0.376,0.327,0.278,0.246,0.213,0.181,0.149,0.149,0.141,0.141,0.166,0.214,0.263,0.312,0.345,0.361,0.361,0.362,0.345,0.329,0.321,0.297,0.248,0.216,0.184,0.216,0.249,0.29,0.33,0.379,0.412,0.445,0.445,0.421,0.396,0.372,0.323,0.283,0.242,0.185,0.145,0.104,0.056,0.04,0.04,0.072,0.121,0.154,0.195,0.252,0.3,0.366,0.415,0.463,0.496,0.512,0.488,0.472,0.448,0.44,0.399,0.343,0.294,0.245,0.205,0.164,0.123,0.091,0.075,0.091,0.116,0.14,0.214,0.271,0.32,0.352,0.393,0.393,0.377,0.353,0.328,0.28,0.239,0.199,0.142,0.085,0.061,0.093,0.158,0.215,0.272,0.321,0.37,0.394,0.338,0.289,0.232,0.167,0.118,0.159,0.192,0.24,0.306,0.354,0.387,0.42,0.355,0.29,0.233,0.168,0.095,0.054,0.03,-0.018,-0.034,-0.009,0.014,0.055,0.104,0.145,0.21,0.259,0.34,0.373,0.422,0.438,0.43,0.398,0.374,0.333,0.292,0.252,0.203,0.154,0.106,0.114,0.13,0.179,0.228,0.285,0.326,0.342,0.343,0.335,0.31,0.278,0.246,0.197,0.156,0.108,0.124,0.132,0.181,0.238,0.287,0.312,0.361,0.361,0.385,0.394,0.402,0.378,0.354,0.346,0.297,0.24,0.183,0.135,0.118,0.102,0.103,0.095,0.135,0.2,0.241,0.266,0.299,0.315,0.315,0.324,0.267,0.218,0.161,0.113,0.088,0.113,0.137,0.186,0.235,0.317,0.366,0.439,0.496,0.545,0.586,0.618,0.602,0.586,0.529,0.472,0.432,0.391,0.343,0.286,0.27,0.245,0.221,0.238,0.27,0.303,0.319,0.36,0.401,0.434,0.442,0.442,0.402,0.345,0.288,0.264,0.207,0.199,0.191,0.207,0.175,0.143,0.11,0.143,0.2,0.249,0.265,0.208,0.16,0.111,0.079,0.111,0.16,0.209,0.242,0.291,0.283,0.275,0.25,0.21,0.161,0.12,0.088,0.047,0.072,0.129,0.178,0.243,0.283,0.292,0.251,0.202,0.145,0.097,0.064 mV</t>
   </si>
   <si>
-    <t>0.0,0.007,0.024,0.033,0.247,0.938,1.273,1.353,1.423,1.417,1.209,1.024,0.740,0.638,0.325,0.033,0.027,0.007,0.0 mV</t>
+    <t>-1.855,-1.66,-1.47,-1.305,-1.145,-1.015,-0.89,-0.755,-0.61,-0.5,-0.385,-0.275,-0.175,-0.085,-0.035,0.03,0.11,0.165,0.18,0.2,0.225,0.255,0.29,0.315,0.32,0.35,0.38,0.41,0.435,0.465,0.47,0.48,0.5,0.515,0.505,0.505,0.52,0.52,0.525,0.505,0.495,0.51,0.515,0.49,0.485,0.46,0.445,0.42,0.41,0.38,0.36,0.335,0.34,0.32,0.315,0.29,0.28,0.26,0.275,0.285,0.32,0.345,0.355,0.39,0.4,0.4,0.4,0.385,0.345,0.33,0.32,0.295,0.255,0.19,0.11,0.075,0.035,0.005,-0.06,-0.14,-0.21,-0.265,-0.29,-0.29,-0.305,-0.32,-0.325,-0.345,-0.345,-0.355,-0.365,-0.385,-0.385,-0.405,-0.395,-0.385,-0.37,-0.38,-0.38,-0.395,-0.385,-0.38,-0.37,-0.37,-0.36,-0.33,-0.3,-0.345,-0.355,-0.395,-0.405,-0.41,-0.475,-0.59,-0.685,-0.715,-0.735,-0.735,-0.72,-0.705,-0.7,-0.745,-0.905,-1.095,-1.21,-1.275,-1.41,-1.64,-1.89,-2.065,-2.095,-1.975,-1.905,-1.88 mV</t>
   </si>
 </sst>
 </file>
@@ -28130,7 +28130,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28254,7 +28254,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="168" t="s">
         <v>676</v>
       </c>

</xml_diff>

<commit_message>
Update vtach We need to have uniform sampling for ECG waveforms
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA107A8-2613-41CD-B213-8EAE1DF042D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E3F274-022C-45F7-98C8-876B5E1ECBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="2240" windowWidth="29870" windowHeight="10590" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2347,7 +2347,7 @@
     <t>0.146,0.179,0.195,0.163,0.138,0.098,0.147,0.196,0.236,0.285,0.326,0.285,0.253,0.196,0.155,0.115,0.074,0.058,0.05,0.123,0.172,0.229,0.278,0.319,0.343,0.376,0.327,0.278,0.246,0.213,0.181,0.149,0.149,0.141,0.141,0.166,0.214,0.263,0.312,0.345,0.361,0.361,0.362,0.345,0.329,0.321,0.297,0.248,0.216,0.184,0.216,0.249,0.29,0.33,0.379,0.412,0.445,0.445,0.421,0.396,0.372,0.323,0.283,0.242,0.185,0.145,0.104,0.056,0.04,0.04,0.072,0.121,0.154,0.195,0.252,0.3,0.366,0.415,0.463,0.496,0.512,0.488,0.472,0.448,0.44,0.399,0.343,0.294,0.245,0.205,0.164,0.123,0.091,0.075,0.091,0.116,0.14,0.214,0.271,0.32,0.352,0.393,0.393,0.377,0.353,0.328,0.28,0.239,0.199,0.142,0.085,0.061,0.093,0.158,0.215,0.272,0.321,0.37,0.394,0.338,0.289,0.232,0.167,0.118,0.159,0.192,0.24,0.306,0.354,0.387,0.42,0.355,0.29,0.233,0.168,0.095,0.054,0.03,-0.018,-0.034,-0.009,0.014,0.055,0.104,0.145,0.21,0.259,0.34,0.373,0.422,0.438,0.43,0.398,0.374,0.333,0.292,0.252,0.203,0.154,0.106,0.114,0.13,0.179,0.228,0.285,0.326,0.342,0.343,0.335,0.31,0.278,0.246,0.197,0.156,0.108,0.124,0.132,0.181,0.238,0.287,0.312,0.361,0.361,0.385,0.394,0.402,0.378,0.354,0.346,0.297,0.24,0.183,0.135,0.118,0.102,0.103,0.095,0.135,0.2,0.241,0.266,0.299,0.315,0.315,0.324,0.267,0.218,0.161,0.113,0.088,0.113,0.137,0.186,0.235,0.317,0.366,0.439,0.496,0.545,0.586,0.618,0.602,0.586,0.529,0.472,0.432,0.391,0.343,0.286,0.27,0.245,0.221,0.238,0.27,0.303,0.319,0.36,0.401,0.434,0.442,0.442,0.402,0.345,0.288,0.264,0.207,0.199,0.191,0.207,0.175,0.143,0.11,0.143,0.2,0.249,0.265,0.208,0.16,0.111,0.079,0.111,0.16,0.209,0.242,0.291,0.283,0.275,0.25,0.21,0.161,0.12,0.088,0.047,0.072,0.129,0.178,0.243,0.283,0.292,0.251,0.202,0.145,0.097,0.064 mV</t>
   </si>
   <si>
-    <t>-1.855,-1.66,-1.47,-1.305,-1.145,-1.015,-0.89,-0.755,-0.61,-0.5,-0.385,-0.275,-0.175,-0.085,-0.035,0.03,0.11,0.165,0.18,0.2,0.225,0.255,0.29,0.315,0.32,0.35,0.38,0.41,0.435,0.465,0.47,0.48,0.5,0.515,0.505,0.505,0.52,0.52,0.525,0.505,0.495,0.51,0.515,0.49,0.485,0.46,0.445,0.42,0.41,0.38,0.36,0.335,0.34,0.32,0.315,0.29,0.28,0.26,0.275,0.285,0.32,0.345,0.355,0.39,0.4,0.4,0.4,0.385,0.345,0.33,0.32,0.295,0.255,0.19,0.11,0.075,0.035,0.005,-0.06,-0.14,-0.21,-0.265,-0.29,-0.29,-0.305,-0.32,-0.325,-0.345,-0.345,-0.355,-0.365,-0.385,-0.385,-0.405,-0.395,-0.385,-0.37,-0.38,-0.38,-0.395,-0.385,-0.38,-0.37,-0.37,-0.36,-0.33,-0.3,-0.345,-0.355,-0.395,-0.405,-0.41,-0.475,-0.59,-0.685,-0.715,-0.735,-0.735,-0.72,-0.705,-0.7,-0.745,-0.905,-1.095,-1.21,-1.275,-1.41,-1.64,-1.89,-2.065,-2.095,-1.975,-1.905,-1.88 mV</t>
+    <t>-0.888888889,-0.866775516,-0.844662144,-0.754008541,-0.619128193,-0.359613235,-0.029441884,0.237116059,0.64055495,0.699641178,0.933560091,1.256715507,1.338619537,1.386630711,1.404981145,1.397364637,1.385791715,1.35032944,1.287660976,1.214423414,1.115826445,0.932539683,0.788129745,0.659188034,0.512183404,0.361111111,0.219517175,-0.197374028,-0.844662144,-0.866775516,-0.888888889 mV</t>
   </si>
 </sst>
 </file>
@@ -28129,8 +28129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28254,7 +28254,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="168" t="s">
         <v>676</v>
       </c>

</xml_diff>

<commit_message>
Add some more fidelity to the vtach waveform
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E3F274-022C-45F7-98C8-876B5E1ECBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7136B9F4-163A-4BE0-A5FD-202E3FAD5921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="29870" windowHeight="10590" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="29870" windowHeight="10590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -2347,7 +2347,7 @@
     <t>0.146,0.179,0.195,0.163,0.138,0.098,0.147,0.196,0.236,0.285,0.326,0.285,0.253,0.196,0.155,0.115,0.074,0.058,0.05,0.123,0.172,0.229,0.278,0.319,0.343,0.376,0.327,0.278,0.246,0.213,0.181,0.149,0.149,0.141,0.141,0.166,0.214,0.263,0.312,0.345,0.361,0.361,0.362,0.345,0.329,0.321,0.297,0.248,0.216,0.184,0.216,0.249,0.29,0.33,0.379,0.412,0.445,0.445,0.421,0.396,0.372,0.323,0.283,0.242,0.185,0.145,0.104,0.056,0.04,0.04,0.072,0.121,0.154,0.195,0.252,0.3,0.366,0.415,0.463,0.496,0.512,0.488,0.472,0.448,0.44,0.399,0.343,0.294,0.245,0.205,0.164,0.123,0.091,0.075,0.091,0.116,0.14,0.214,0.271,0.32,0.352,0.393,0.393,0.377,0.353,0.328,0.28,0.239,0.199,0.142,0.085,0.061,0.093,0.158,0.215,0.272,0.321,0.37,0.394,0.338,0.289,0.232,0.167,0.118,0.159,0.192,0.24,0.306,0.354,0.387,0.42,0.355,0.29,0.233,0.168,0.095,0.054,0.03,-0.018,-0.034,-0.009,0.014,0.055,0.104,0.145,0.21,0.259,0.34,0.373,0.422,0.438,0.43,0.398,0.374,0.333,0.292,0.252,0.203,0.154,0.106,0.114,0.13,0.179,0.228,0.285,0.326,0.342,0.343,0.335,0.31,0.278,0.246,0.197,0.156,0.108,0.124,0.132,0.181,0.238,0.287,0.312,0.361,0.361,0.385,0.394,0.402,0.378,0.354,0.346,0.297,0.24,0.183,0.135,0.118,0.102,0.103,0.095,0.135,0.2,0.241,0.266,0.299,0.315,0.315,0.324,0.267,0.218,0.161,0.113,0.088,0.113,0.137,0.186,0.235,0.317,0.366,0.439,0.496,0.545,0.586,0.618,0.602,0.586,0.529,0.472,0.432,0.391,0.343,0.286,0.27,0.245,0.221,0.238,0.27,0.303,0.319,0.36,0.401,0.434,0.442,0.442,0.402,0.345,0.288,0.264,0.207,0.199,0.191,0.207,0.175,0.143,0.11,0.143,0.2,0.249,0.265,0.208,0.16,0.111,0.079,0.111,0.16,0.209,0.242,0.291,0.283,0.275,0.25,0.21,0.161,0.12,0.088,0.047,0.072,0.129,0.178,0.243,0.283,0.292,0.251,0.202,0.145,0.097,0.064 mV</t>
   </si>
   <si>
-    <t>-0.888888889,-0.866775516,-0.844662144,-0.754008541,-0.619128193,-0.359613235,-0.029441884,0.237116059,0.64055495,0.699641178,0.933560091,1.256715507,1.338619537,1.386630711,1.404981145,1.397364637,1.385791715,1.35032944,1.287660976,1.214423414,1.115826445,0.932539683,0.788129745,0.659188034,0.512183404,0.361111111,0.219517175,-0.197374028,-0.844662144,-0.866775516,-0.888888889 mV</t>
+    <t>-0.87037037,-0.87037037,-0.844608964,-0.822655766,-0.82220784,-0.768887363,-0.70764652,-0.614819727,-0.52892371,-0.480148781,-0.431191494,-0.376217822,-0.308852895,-0.117606594,0.011365573,0.346387061,0.420940171,0.482794761,0.515750794,0.578912467,0.689386257,0.746024058,0.805258268,1.002414409,1.104193829,1.24136119,1.301748698,1.366255851,1.396876272,1.400560652,1.403077707,1.405594762,1.407407407,1.407407407,1.407407407,1.404004432,1.394478079,1.384951725,1.372085541,1.354991524,1.337882835,1.320735399,1.291933761,1.203074033,1.156691749,1.110746466,1.035083637,0.987828826,0.94455454,0.89866332,0.858952572,0.829902799,0.744005507,0.691496613,0.574336482,0.534954811,0.506410256,0.477789201,0.445639405,0.40663102,0.322900955,0.217701898,0.094211344,-0.03049728,-0.271880342,-0.563069102,-0.82220784,-0.822655766,-0.844608964,-0.87037037,-0.87037037 mV</t>
   </si>
 </sst>
 </file>
@@ -4872,7 +4872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:FR75"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="DB33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -28129,8 +28129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28254,7 +28254,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="168" t="s">
         <v>676</v>
       </c>

</xml_diff>